<commit_message>
Updated okonomi spreadsheet after feedback 28/05
</commit_message>
<xml_diff>
--- a/doc/okonomi/Utbetaling.xlsx
+++ b/doc/okonomi/Utbetaling.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fred/src/nav/helse-spleis/doc/okonomi/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A1C0A23-43AD-0046-8D70-D6CBA9FBC72B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E80362C-98DF-CD4A-A9C3-EC2EDD89572A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9080" yWindow="1420" windowWidth="23940" windowHeight="17460" xr2:uid="{0C19B20D-83E0-4506-8A48-13513FAC2579}"/>
-    <workbookView xWindow="34560" yWindow="1400" windowWidth="28660" windowHeight="25500" activeTab="1" xr2:uid="{BB3196D1-BBA6-4B4B-8E55-37C48C2FF3A4}"/>
+    <workbookView xWindow="2360" yWindow="1420" windowWidth="22680" windowHeight="17460" xr2:uid="{0C19B20D-83E0-4506-8A48-13513FAC2579}"/>
+    <workbookView xWindow="25560" yWindow="1400" windowWidth="28660" windowHeight="25500" activeTab="1" xr2:uid="{BB3196D1-BBA6-4B4B-8E55-37C48C2FF3A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Terminology" sheetId="1" r:id="rId1"/>
     <sheet name="Multiple Employers" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="ScalingFactor">'Multiple Employers'!$C$13</definedName>
+    <definedName name="ScalingFactor">'Multiple Employers'!$C$16</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,10 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="58">
-  <si>
-    <t>Salary, usually monthly</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="59">
   <si>
     <t>Term</t>
   </si>
@@ -56,9 +53,6 @@
   </si>
   <si>
     <t>Integer</t>
-  </si>
-  <si>
-    <t>Daily salary</t>
   </si>
   <si>
     <t>Double</t>
@@ -102,9 +96,6 @@
     <t>100% for employers, 80% for self-employed, etc.</t>
   </si>
   <si>
-    <t>Dagsats</t>
-  </si>
-  <si>
     <t>Rebate percentage</t>
   </si>
   <si>
@@ -171,9 +162,6 @@
     <t>Personbeløp</t>
   </si>
   <si>
-    <t>Lønn</t>
-  </si>
-  <si>
     <t>Beløp</t>
   </si>
   <si>
@@ -232,6 +220,21 @@
   </si>
   <si>
     <t>Annual</t>
+  </si>
+  <si>
+    <t>Income monthly</t>
+  </si>
+  <si>
+    <t>Daily income</t>
+  </si>
+  <si>
+    <t>Sykepengegrunnlag</t>
+  </si>
+  <si>
+    <t>Monthly income</t>
+  </si>
+  <si>
+    <t>Income ratio</t>
   </si>
 </sst>
 </file>
@@ -322,7 +325,7 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -350,7 +353,6 @@
     <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -364,6 +366,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -683,13 +689,13 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.1640625" customWidth="1"/>
     <col min="2" max="2" width="28.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.1640625" style="3" customWidth="1"/>
     <col min="4" max="4" width="19.33203125" style="1" bestFit="1" customWidth="1"/>
@@ -698,19 +704,19 @@
   <sheetData>
     <row r="1" spans="1:5" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>3</v>
-      </c>
       <c r="E1" s="5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -718,10 +724,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>37</v>
+        <v>56</v>
       </c>
       <c r="B3" t="s">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>5</v>
@@ -733,76 +739,74 @@
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>55</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D4" s="2">
         <f>D3*12/260</f>
         <v>923.07692307692309</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D5" s="11">
         <v>80</v>
       </c>
       <c r="E5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
-        <v>14</v>
-      </c>
+      <c r="A6" s="4"/>
       <c r="B6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D6" s="2">
         <f>D4*ROUND(D5,0)/100</f>
         <v>738.46153846153845</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D7" s="11">
         <v>60</v>
       </c>
       <c r="E7" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="4"/>
       <c r="B8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D8" s="2">
         <f>D6*D7/100</f>
@@ -811,64 +815,64 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B9" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D9" s="11">
         <v>93634</v>
       </c>
-      <c r="E9" s="19">
+      <c r="E9" s="26">
         <v>43101</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B10" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D10" s="2">
         <f>6*D9/260</f>
         <v>2160.7846153846153</v>
       </c>
       <c r="E10" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
       <c r="B11" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D11" s="1">
         <f>ROUND(ROUND(D7,0)*D10/100,0)</f>
         <v>1296</v>
       </c>
       <c r="E11" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D12" s="2">
         <f>MIN(D8,D11)</f>
@@ -878,28 +882,28 @@
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D13" s="18">
         <f>100*2/3</f>
         <v>66.666666666666671</v>
       </c>
       <c r="E13" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="10" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D14" s="9">
         <f>ROUND(D12*D13/100, 0)</f>
@@ -908,29 +912,29 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D15" s="9">
         <f>ROUND(D12,0)-D14</f>
         <v>148</v>
       </c>
       <c r="E15" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
       <c r="B16" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D16" s="2">
         <f>D12-D14-D15</f>
@@ -940,17 +944,17 @@
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
       <c r="B17" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D17" s="2">
         <f>D16*260</f>
         <v>19.999999999989768</v>
       </c>
       <c r="E17" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -964,19 +968,19 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="13" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B21" s="14"/>
       <c r="C21" s="15"/>
       <c r="D21" s="16"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="B22" s="20"/>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
+      <c r="A22" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="19"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
@@ -990,18 +994,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBE9F233-0C57-4B39-8C81-6D2F9F1844A9}">
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="1">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="D25" sqref="D25:F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" customWidth="1"/>
     <col min="2" max="2" width="28.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
@@ -1013,28 +1017,28 @@
   <sheetData>
     <row r="1" spans="1:8" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>2</v>
-      </c>
       <c r="C1" s="5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D1" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>27</v>
-      </c>
       <c r="H1" s="8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -1042,10 +1046,10 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>37</v>
+        <v>56</v>
       </c>
       <c r="B3" t="s">
-        <v>0</v>
+        <v>57</v>
       </c>
       <c r="D3" s="11">
         <v>21000</v>
@@ -1066,453 +1070,496 @@
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="2">
-        <f>D3*12/260</f>
-        <v>969.23076923076928</v>
-      </c>
-      <c r="E4" s="2">
-        <f>E3*12/260</f>
-        <v>461.53846153846155</v>
-      </c>
-      <c r="F4" s="2">
-        <f>F3*12/260</f>
-        <v>1430.7692307692307</v>
-      </c>
-      <c r="G4" s="2">
-        <f>G3*12/260</f>
+        <v>58</v>
+      </c>
+      <c r="D4" s="22">
+        <f>D3/SUM($D$3:$G$3)</f>
+        <v>0.33870967741935482</v>
+      </c>
+      <c r="E4" s="22">
+        <f t="shared" ref="E4:G4" si="0">E3/SUM($D$3:$G$3)</f>
+        <v>0.16129032258064516</v>
+      </c>
+      <c r="F4" s="22">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="G4" s="22">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="22">
+        <v>55</v>
+      </c>
+      <c r="D5" s="2">
+        <f>D3*12/260</f>
+        <v>969.23076923076928</v>
+      </c>
+      <c r="E5" s="2">
+        <f>E3*12/260</f>
+        <v>461.53846153846155</v>
+      </c>
+      <c r="F5" s="2">
+        <f>F3*12/260</f>
+        <v>1430.7692307692307</v>
+      </c>
+      <c r="G5" s="2">
+        <f>G3*12/260</f>
+        <v>0</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="4"/>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="21">
         <v>1</v>
       </c>
-      <c r="E5" s="22">
+      <c r="E6" s="21">
         <v>1</v>
       </c>
-      <c r="F5" s="22">
+      <c r="F6" s="21">
         <v>1</v>
       </c>
-      <c r="G5" s="22">
+      <c r="G6" s="21">
         <v>1</v>
       </c>
-      <c r="H5" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
+      <c r="H6" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="4"/>
+      <c r="B7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="2">
+        <f>D5*D6</f>
+        <v>969.23076923076928</v>
+      </c>
+      <c r="E7" s="2">
+        <f t="shared" ref="E7:G7" si="1">E5*E6</f>
+        <v>461.53846153846155</v>
+      </c>
+      <c r="F7" s="2">
+        <f t="shared" si="1"/>
+        <v>1430.7692307692307</v>
+      </c>
+      <c r="G7" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="22">
+        <v>0.5</v>
+      </c>
+      <c r="E8" s="22">
+        <v>0.8</v>
+      </c>
+      <c r="F8" s="22">
+        <v>0.2</v>
+      </c>
+      <c r="G8" s="22">
+        <v>1</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="4"/>
+      <c r="B9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" s="2">
+        <f>D7*D8</f>
+        <v>484.61538461538464</v>
+      </c>
+      <c r="E9" s="2">
+        <f t="shared" ref="E9:G9" si="2">E7*E8</f>
+        <v>369.23076923076928</v>
+      </c>
+      <c r="F9" s="2">
+        <f t="shared" si="2"/>
+        <v>286.15384615384613</v>
+      </c>
+      <c r="G9" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="4"/>
+      <c r="B10" t="s">
         <v>14</v>
       </c>
-      <c r="B6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D6" s="2">
-        <f>D4*D5</f>
-        <v>969.23076923076928</v>
-      </c>
-      <c r="E6" s="2">
-        <f t="shared" ref="E6:G6" si="0">E4*E5</f>
-        <v>461.53846153846155</v>
-      </c>
-      <c r="F6" s="2">
-        <f t="shared" si="0"/>
-        <v>1430.7692307692307</v>
-      </c>
-      <c r="G6" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="D10" s="21">
+        <v>1</v>
+      </c>
+      <c r="E10" s="21">
+        <v>0.9</v>
+      </c>
+      <c r="F10" s="21">
+        <v>0.25</v>
+      </c>
+      <c r="G10" s="21">
+        <v>1</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="4"/>
+      <c r="B11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" s="17">
+        <f>D9*D10</f>
+        <v>484.61538461538464</v>
+      </c>
+      <c r="E11" s="17">
+        <f t="shared" ref="E11:G11" si="3">E9*E10</f>
+        <v>332.30769230769238</v>
+      </c>
+      <c r="F11" s="17">
+        <f t="shared" si="3"/>
+        <v>71.538461538461533</v>
+      </c>
+      <c r="G11" s="17">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="20">
+        <f>ROUND(SUM(D9:G9)/SUM(D7:G7),2)</f>
+        <v>0.4</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="23">
-        <v>0.5</v>
-      </c>
-      <c r="E7" s="23">
-        <v>0.8</v>
-      </c>
-      <c r="F7" s="23">
-        <v>0.2</v>
-      </c>
-      <c r="G7" s="23">
-        <v>1</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="4"/>
-      <c r="B8" t="s">
-        <v>49</v>
-      </c>
-      <c r="D8" s="2">
-        <f>D6*D7</f>
-        <v>484.61538461538464</v>
-      </c>
-      <c r="E8" s="2">
-        <f t="shared" ref="E8:G8" si="1">E6*E7</f>
-        <v>369.23076923076928</v>
-      </c>
-      <c r="F8" s="2">
-        <f t="shared" si="1"/>
-        <v>286.15384615384613</v>
-      </c>
-      <c r="G8" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B9" t="s">
-        <v>44</v>
-      </c>
-      <c r="C9" s="21">
-        <f>SUM(D8:G8)/SUM(D6:G6)</f>
-        <v>0.39838709677419348</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" s="11">
+      <c r="C13" s="11">
         <v>93634</v>
       </c>
-      <c r="H10" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" s="2">
-        <f>6*C10/260</f>
-        <v>2160.7846153846153</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="4"/>
-      <c r="B12" t="s">
-        <v>47</v>
-      </c>
-      <c r="C12" s="1">
-        <f>C9*C11</f>
-        <v>860.82870967741917</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="4"/>
-      <c r="B13" t="s">
-        <v>48</v>
-      </c>
-      <c r="C13" s="24">
-        <f>MIN(1, C12/SUM(D8:G8))</f>
-        <v>0.75511290322580626</v>
-      </c>
       <c r="H13" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
-      </c>
-      <c r="D14" s="17">
-        <f>D8*ScalingFactor</f>
-        <v>365.93933002481384</v>
-      </c>
-      <c r="E14" s="17">
-        <f>E8*ScalingFactor</f>
-        <v>278.81091811414387</v>
-      </c>
-      <c r="F14" s="17">
-        <f>F8*ScalingFactor</f>
-        <v>216.07846153846148</v>
-      </c>
-      <c r="G14" s="17">
-        <f>G8*ScalingFactor</f>
-        <v>0</v>
+        <v>30</v>
+      </c>
+      <c r="C14" s="2">
+        <f>6*C13/260</f>
+        <v>2160.7846153846153</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
       <c r="B15" t="s">
-        <v>17</v>
-      </c>
-      <c r="D15" s="18">
-        <v>100</v>
-      </c>
-      <c r="E15" s="18">
-        <v>90</v>
-      </c>
-      <c r="F15" s="18">
-        <v>25</v>
-      </c>
-      <c r="G15" s="18">
-        <v>100</v>
+        <v>43</v>
+      </c>
+      <c r="C15" s="1">
+        <f>C12*C14</f>
+        <v>864.31384615384616</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
       <c r="B16" t="s">
-        <v>52</v>
-      </c>
-      <c r="D16" s="17">
-        <f>D8*D15/100</f>
-        <v>484.61538461538458</v>
-      </c>
-      <c r="E16" s="17">
-        <f t="shared" ref="E16:G16" si="2">E8*E15/100</f>
-        <v>332.30769230769232</v>
-      </c>
-      <c r="F16" s="17">
-        <f t="shared" si="2"/>
-        <v>71.538461538461533</v>
-      </c>
-      <c r="G16" s="17">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>44</v>
+      </c>
+      <c r="C16" s="23">
+        <f>MIN(1, C15/SUM(D9:G9))</f>
+        <v>0.75817004048582992</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" s="4"/>
+      <c r="A17" s="4" t="s">
+        <v>34</v>
+      </c>
       <c r="B17" t="s">
-        <v>50</v>
+        <v>13</v>
       </c>
       <c r="D17" s="17">
-        <f>MIN(D14,D16)</f>
-        <v>365.93933002481384</v>
+        <f>D9*ScalingFactor</f>
+        <v>367.42086577390222</v>
       </c>
       <c r="E17" s="17">
-        <f t="shared" ref="E17:G17" si="3">MIN(E14,E16)</f>
-        <v>278.81091811414387</v>
+        <f>E9*ScalingFactor</f>
+        <v>279.93970725630646</v>
       </c>
       <c r="F17" s="17">
-        <f t="shared" si="3"/>
-        <v>71.538461538461533</v>
+        <f>F9*ScalingFactor</f>
+        <v>216.95327312363747</v>
       </c>
       <c r="G17" s="17">
-        <f t="shared" si="3"/>
+        <f>G9*ScalingFactor</f>
         <v>0</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="4"/>
       <c r="B18" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="D18" s="17">
-        <f>D17-D16</f>
-        <v>-118.67605459057074</v>
+        <f>MIN(D17,D11)</f>
+        <v>367.42086577390222</v>
       </c>
       <c r="E18" s="17">
-        <f t="shared" ref="E18:G18" si="4">E17-E16</f>
-        <v>-53.496774193548447</v>
+        <f t="shared" ref="E18:G18" si="4">MIN(E17,E11)</f>
+        <v>279.93970725630646</v>
       </c>
       <c r="F18" s="17">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>71.538461538461533</v>
       </c>
       <c r="G18" s="17">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="4"/>
       <c r="B19" t="s">
-        <v>54</v>
-      </c>
-      <c r="D19" s="21">
-        <f>D18/SUM($D$18:$G$18)</f>
-        <v>0.68928445579165121</v>
-      </c>
-      <c r="E19" s="21">
-        <f t="shared" ref="E19:G19" si="5">E18/SUM($D$18:$G$18)</f>
-        <v>0.31071554420834874</v>
-      </c>
-      <c r="F19" s="21">
+        <v>49</v>
+      </c>
+      <c r="D19" s="17">
+        <f>D18-D11</f>
+        <v>-117.19451884148242</v>
+      </c>
+      <c r="E19" s="17">
+        <f t="shared" ref="E19:G19" si="5">E18-E11</f>
+        <v>-52.367985051385915</v>
+      </c>
+      <c r="F19" s="17">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="G19" s="21">
+      <c r="G19" s="17">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="4"/>
-      <c r="B20" t="s">
-        <v>51</v>
-      </c>
-      <c r="D20" s="17">
-        <f t="shared" ref="D20" si="6">D14-D17</f>
-        <v>0</v>
-      </c>
-      <c r="E20" s="17">
-        <f t="shared" ref="E20" si="7">E14-E17</f>
-        <v>0</v>
-      </c>
-      <c r="F20" s="17">
-        <f>F14-F17</f>
-        <v>144.53999999999996</v>
-      </c>
-      <c r="G20" s="17">
-        <f>G14-G17</f>
-        <v>0</v>
-      </c>
+      <c r="D20" s="20">
+        <f>IF(D19 &lt; 0, D4, 0)</f>
+        <v>0.33870967741935482</v>
+      </c>
+      <c r="E20" s="20">
+        <f t="shared" ref="E20:F20" si="6">IF(E19 &lt; 0, E4, 0)</f>
+        <v>0.16129032258064516</v>
+      </c>
+      <c r="F20" s="20">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="G20" s="17"/>
       <c r="H20" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="4"/>
       <c r="B21" t="s">
-        <v>55</v>
-      </c>
-      <c r="D21" s="17">
-        <f>IF(SUM($D$18:$G$18)&gt;=0, 0, SUM($D$20:$G$20)*D19)</f>
-        <v>99.629175240125235</v>
-      </c>
-      <c r="E21" s="17">
-        <f t="shared" ref="E21:G21" si="8">IF(SUM($D$18:$G$18)&gt;=0, 0, SUM($D$20:$G$20)*E19)</f>
-        <v>44.910824759874714</v>
-      </c>
-      <c r="F21" s="17">
+        <v>50</v>
+      </c>
+      <c r="D21" s="20">
+        <f>D20/SUM($D$20:$G$20)</f>
+        <v>0.67741935483870963</v>
+      </c>
+      <c r="E21" s="20">
+        <f t="shared" ref="E21:G21" si="7">E20/SUM($D$20:$G$20)</f>
+        <v>0.32258064516129031</v>
+      </c>
+      <c r="F21" s="20">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="G21" s="20">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="4"/>
+      <c r="B22" t="s">
+        <v>47</v>
+      </c>
+      <c r="D22" s="17">
+        <f>D17-D18</f>
+        <v>0</v>
+      </c>
+      <c r="E22" s="17">
+        <f>E17-E18</f>
+        <v>0</v>
+      </c>
+      <c r="F22" s="17">
+        <f>F17-F18</f>
+        <v>145.41481158517593</v>
+      </c>
+      <c r="G22" s="17">
+        <f>G17-G18</f>
+        <v>0</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="4"/>
+      <c r="B23" t="s">
+        <v>51</v>
+      </c>
+      <c r="D23" s="17">
+        <f>IF(SUM($D$19:$G$19)&gt;=0, 0, SUM($D$22:$G$22)*D21)</f>
+        <v>98.50680784802239</v>
+      </c>
+      <c r="E23" s="17">
+        <f t="shared" ref="E23:G23" si="8">IF(SUM($D$19:$G$19)&gt;=0, 0, SUM($D$22:$G$22)*E21)</f>
+        <v>46.908003737153521</v>
+      </c>
+      <c r="F23" s="17">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="G21" s="17">
+      <c r="G23" s="17">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="H21" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B22" t="s">
-        <v>18</v>
-      </c>
-      <c r="D22" s="1">
-        <f>ROUND(D17+D21,0)</f>
+      <c r="H23" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24" t="s">
+        <v>15</v>
+      </c>
+      <c r="D24" s="1">
+        <f>ROUND(D18+D23,0)</f>
         <v>466</v>
       </c>
-      <c r="E22" s="1">
-        <f t="shared" ref="E22:G22" si="9">ROUND(E17+E21,0)</f>
-        <v>324</v>
-      </c>
-      <c r="F22" s="1">
+      <c r="E24" s="1">
+        <f t="shared" ref="E24:G24" si="9">ROUND(E18+E23,0)</f>
+        <v>327</v>
+      </c>
+      <c r="F24" s="1">
         <f t="shared" si="9"/>
         <v>72</v>
       </c>
-      <c r="G22" s="17">
+      <c r="G24" s="17">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="H22" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B23" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" s="4"/>
-      <c r="B24" t="s">
-        <v>21</v>
+      <c r="H24" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" s="4"/>
+      <c r="A25" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="B25" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A30" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="B30" s="26">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="4"/>
+      <c r="B26" t="s">
+        <v>18</v>
+      </c>
+      <c r="C26" s="27">
+        <f>C15-SUM(D24:G24)</f>
+        <v>-0.68615384615384301</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="4"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="B32" s="25">
         <v>1430.76</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A31" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="B31" s="26">
-        <f>ROUND(B30*260/12,0)</f>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="B33" s="25">
+        <f>ROUND(B32*260/12,0)</f>
         <v>31000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Another Økonomi spreadsheet update
</commit_message>
<xml_diff>
--- a/doc/okonomi/Utbetaling.xlsx
+++ b/doc/okonomi/Utbetaling.xlsx
@@ -8,9 +8,8 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fred/src/nav/helse-spleis/doc/okonomi/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E80362C-98DF-CD4A-A9C3-EC2EDD89572A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F99EAB1-E5AE-2646-BED4-1D5B1DBD1A18}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2360" yWindow="1420" windowWidth="22680" windowHeight="17460" xr2:uid="{0C19B20D-83E0-4506-8A48-13513FAC2579}"/>
     <workbookView xWindow="25560" yWindow="1400" windowWidth="28660" windowHeight="25500" activeTab="1" xr2:uid="{BB3196D1-BBA6-4B4B-8E55-37C48C2FF3A4}"/>
   </bookViews>
   <sheets>
@@ -688,10 +687,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{336B5C91-C43F-4BAE-BFBA-00152852E840}">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -996,11 +992,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBE9F233-0C57-4B39-8C81-6D2F9F1844A9}">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
-    </sheetView>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="1">
-      <selection activeCell="D25" sqref="D25:F25"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Updated Økonomi spreadsheet with Person Belop.
Co-authored-by: Marte Tårnes <marte.tarnes@nav.no>
</commit_message>
<xml_diff>
--- a/doc/okonomi/Utbetaling.xlsx
+++ b/doc/okonomi/Utbetaling.xlsx
@@ -1,23 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/david/dev/nav/helse/monorepo/helse-spleis/doc/okonomi/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fred/src/nav/helse-spleis/doc/okonomi/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B8A388F-CD40-F94C-8BA9-B7F2A380FB4C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5E2AE42-9FBB-C44D-82C6-8ADEA7B8FCAC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13040" yWindow="1280" windowWidth="43420" windowHeight="35960" activeTab="1" xr2:uid="{BB3196D1-BBA6-4B4B-8E55-37C48C2FF3A4}"/>
+    <workbookView xWindow="2020" yWindow="860" windowWidth="20220" windowHeight="14600" xr2:uid="{BB3196D1-BBA6-4B4B-8E55-37C48C2FF3A4}"/>
+    <workbookView xWindow="22440" yWindow="840" windowWidth="25260" windowHeight="16940" activeTab="1" xr2:uid="{84B3C1EA-5610-F945-853C-C9E087DDC0A8}"/>
   </bookViews>
   <sheets>
     <sheet name="Terminology" sheetId="1" r:id="rId1"/>
     <sheet name="Multiple Employers" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="AdjustmentArb">'Multiple Employers'!$D$23:$G$23</definedName>
     <definedName name="ScalingFactor">'Multiple Employers'!$C$16</definedName>
+    <definedName name="ShortfallIncomeRatioArb">'Multiple Employers'!$D$20:$G$20</definedName>
+    <definedName name="ShortfallIncomeRatioPerson">'Multiple Employers'!$D$24:$G$24</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="74">
   <si>
     <t>Term</t>
   </si>
@@ -206,9 +210,6 @@
     <t>Employer shortfall</t>
   </si>
   <si>
-    <t>Shortfall ratio</t>
-  </si>
-  <si>
     <t>Adjustment for employers</t>
   </si>
   <si>
@@ -270,6 +271,18 @@
   </si>
   <si>
     <t>Ekstra fordeling</t>
+  </si>
+  <si>
+    <t>Shortfall income ratio - person</t>
+  </si>
+  <si>
+    <t>Shortfall income ratio - arbeidsgiver</t>
+  </si>
+  <si>
+    <t>Shortfall ratio - arbeidsgiver</t>
+  </si>
+  <si>
+    <t>Shortfall ratio - person</t>
   </si>
 </sst>
 </file>
@@ -410,10 +423,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -732,9 +745,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{336B5C91-C43F-4BAE-BFBA-00152852E840}">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView zoomScale="244" zoomScaleNormal="244" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -767,10 +781,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>5</v>
@@ -782,7 +796,7 @@
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>5</v>
@@ -1018,12 +1032,12 @@
       <c r="D21" s="16"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="27" t="s">
+      <c r="A22" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="B22" s="27"/>
-      <c r="C22" s="27"/>
-      <c r="D22" s="27"/>
+      <c r="B22" s="28"/>
+      <c r="C22" s="28"/>
+      <c r="D22" s="28"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
@@ -1037,10 +1051,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBE9F233-0C57-4B39-8C81-6D2F9F1844A9}">
-  <dimension ref="A1:H33"/>
+  <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="249" zoomScaleNormal="249" workbookViewId="0">
+    <sheetView zoomScale="163" zoomScaleNormal="163" workbookViewId="0">
       <selection activeCell="A24" sqref="A24"/>
+    </sheetView>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="1">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1086,10 +1103,10 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D3" s="11">
         <v>21000</v>
@@ -1110,7 +1127,7 @@
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D4" s="21">
         <f>D3/SUM($D$3:$G$3)</f>
@@ -1133,11 +1150,11 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="28" t="s">
-        <v>65</v>
+      <c r="A5" s="27" t="s">
+        <v>64</v>
       </c>
       <c r="B5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D5" s="2">
         <f>D3*12/260</f>
@@ -1161,7 +1178,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B6" t="s">
         <v>12</v>
@@ -1184,7 +1201,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B7" t="s">
         <v>41</v>
@@ -1234,7 +1251,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B9" t="s">
         <v>44</v>
@@ -1261,7 +1278,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B10" t="s">
         <v>14</v>
@@ -1284,7 +1301,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B11" t="s">
         <v>47</v>
@@ -1311,7 +1328,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B12" t="s">
         <v>39</v>
@@ -1355,7 +1372,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B15" t="s">
         <v>42</v>
@@ -1370,7 +1387,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B16" t="s">
         <v>43</v>
@@ -1412,7 +1429,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B18" t="s">
         <v>45</v>
@@ -1464,6 +1481,9 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="4"/>
+      <c r="B20" t="s">
+        <v>71</v>
+      </c>
       <c r="D20" s="19">
         <f>IF(D19 &lt; 0, D4, 0)</f>
         <v>0.33870967741935482</v>
@@ -1483,25 +1503,25 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B21" t="s">
-        <v>49</v>
+        <v>72</v>
       </c>
       <c r="D21" s="19">
-        <f>D20/SUM($D$20:$G$20)</f>
+        <f>IF(SUM(ShortfallIncomeRatioArb)=0,0,D20/SUM(ShortfallIncomeRatioArb))</f>
         <v>0.67741935483870963</v>
       </c>
       <c r="E21" s="19">
-        <f t="shared" ref="E21:G21" si="7">E20/SUM($D$20:$G$20)</f>
+        <f>IF(SUM(ShortfallIncomeRatioArb)=0,0,E20/SUM(ShortfallIncomeRatioArb))</f>
         <v>0.32258064516129031</v>
       </c>
       <c r="F21" s="19">
-        <f t="shared" si="7"/>
+        <f>IF(SUM(ShortfallIncomeRatioArb)=0,0,F20/SUM(ShortfallIncomeRatioArb))</f>
         <v>0</v>
       </c>
       <c r="G21" s="19">
-        <f t="shared" si="7"/>
+        <f>IF(SUM(ShortfallIncomeRatioArb)=0,0,G20/SUM(ShortfallIncomeRatioArb))</f>
         <v>0</v>
       </c>
       <c r="H21" s="3" t="s">
@@ -1535,93 +1555,153 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B23" t="s">
+        <v>49</v>
+      </c>
+      <c r="D23" s="17">
+        <f>MIN(-D19,IF(SUM($D$19:$G$19)&gt;=0, 0, SUM($D$22:$G$22)*D21))</f>
+        <v>98.50680784802239</v>
+      </c>
+      <c r="E23" s="17">
+        <f t="shared" ref="E23:G23" si="7">MIN(-E19,IF(SUM($D$19:$G$19)&gt;=0, 0, SUM($D$22:$G$22)*E21))</f>
+        <v>46.908003737153521</v>
+      </c>
+      <c r="F23" s="17">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="G23" s="17">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="4"/>
+      <c r="B24" t="s">
         <v>70</v>
       </c>
-      <c r="B23" t="s">
-        <v>50</v>
-      </c>
-      <c r="D23" s="17">
-        <f>IF(SUM($D$19:$G$19)&gt;=0, 0, SUM($D$22:$G$22)*D21)</f>
-        <v>98.50680784802239</v>
-      </c>
-      <c r="E23" s="17">
-        <f t="shared" ref="E23:G23" si="8">IF(SUM($D$19:$G$19)&gt;=0, 0, SUM($D$22:$G$22)*E21)</f>
-        <v>46.908003737153521</v>
-      </c>
-      <c r="F23" s="17">
+      <c r="D24" s="19">
+        <f>IF(D22 = 0, 0, D4)</f>
+        <v>0</v>
+      </c>
+      <c r="E24" s="19">
+        <f t="shared" ref="E24:G24" si="8">IF(E22 = 0, 0, E4)</f>
+        <v>0</v>
+      </c>
+      <c r="F24" s="19">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="G23" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="G24" s="19">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="H23" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" s="4" t="s">
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" s="4"/>
+      <c r="B25" t="s">
+        <v>73</v>
+      </c>
+      <c r="D25" s="19">
+        <f>IF(SUM(ShortfallIncomeRatioPerson)= 0, 0, D24/SUM(ShortfallIncomeRatioPerson))</f>
+        <v>0</v>
+      </c>
+      <c r="E25" s="19">
+        <f>IF(SUM(ShortfallIncomeRatioPerson)= 0, 0, E24/SUM(ShortfallIncomeRatioPerson))</f>
+        <v>0</v>
+      </c>
+      <c r="F25" s="19">
+        <f>IF(SUM(ShortfallIncomeRatioPerson)= 0, 0, F24/SUM(ShortfallIncomeRatioPerson))</f>
+        <v>1</v>
+      </c>
+      <c r="G25" s="19">
+        <f>IF(SUM(ShortfallIncomeRatioPerson)= 0, 0, G24/SUM(ShortfallIncomeRatioPerson))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B26" t="s">
         <v>15</v>
       </c>
-      <c r="D24" s="1">
+      <c r="D26" s="1">
         <f>ROUND(D18+D23,0)</f>
         <v>466</v>
       </c>
-      <c r="E24" s="1">
-        <f t="shared" ref="E24:G24" si="9">ROUND(E18+E23,0)</f>
+      <c r="E26" s="1">
+        <f t="shared" ref="E26:G26" si="9">ROUND(E18+E23,0)</f>
         <v>327</v>
       </c>
-      <c r="F24" s="1">
+      <c r="F26" s="1">
         <f t="shared" si="9"/>
         <v>72</v>
       </c>
-      <c r="G24" s="17">
+      <c r="G26" s="17">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="H24" s="3" t="s">
+      <c r="H26" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" s="4" t="s">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B27" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" s="4"/>
-      <c r="B26" t="s">
+      <c r="D27">
+        <f>ROUND(D22-SUM(AdjustmentArb)*D25,0)</f>
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <f>ROUND(E22-SUM(AdjustmentArb)*E25,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <f>ROUND(F22-SUM(AdjustmentArb)*F25,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <f>ROUND(G22-SUM(AdjustmentArb)*G25,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="4"/>
+      <c r="B28" t="s">
         <v>18</v>
       </c>
-      <c r="C26" s="26">
-        <f>C15-SUM(D24:G24)</f>
+      <c r="C28" s="26">
+        <f>C15-SUM(D26:G27)</f>
         <v>-0.68615384615384301</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" s="4"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A32" s="23" t="s">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="4"/>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B34" s="24">
+        <v>1430.76</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="B32" s="24">
-        <v>1430.76</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="B33" s="24">
-        <f>ROUND(B32*260/12,0)</f>
+      <c r="B35" s="24">
+        <f>ROUND(B34*260/12,0)</f>
         <v>31000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Copying spreadsheet to this branch for ease of reference
Co-authored-by: Fred George <fredgeorge@acm.org>
Co-authored-by: Marte Tårnes <marte.tarnes@nav.no>
</commit_message>
<xml_diff>
--- a/doc/okonomi/Utbetaling.xlsx
+++ b/doc/okonomi/Utbetaling.xlsx
@@ -5,13 +5,13 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fred/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fred/src/nav/helse-spleis/doc/okonomi/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4128D7AA-40ED-E345-B4A4-AA1BFC1EBAC4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5E2AE42-9FBB-C44D-82C6-8ADEA7B8FCAC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2020" yWindow="860" windowWidth="27900" windowHeight="18840" xr2:uid="{BB3196D1-BBA6-4B4B-8E55-37C48C2FF3A4}"/>
-    <workbookView xWindow="32120" yWindow="1000" windowWidth="31580" windowHeight="23740" activeTab="1" xr2:uid="{84B3C1EA-5610-F945-853C-C9E087DDC0A8}"/>
+    <workbookView xWindow="2020" yWindow="860" windowWidth="20220" windowHeight="14600" xr2:uid="{BB3196D1-BBA6-4B4B-8E55-37C48C2FF3A4}"/>
+    <workbookView xWindow="22440" yWindow="840" windowWidth="25260" windowHeight="16940" activeTab="1" xr2:uid="{84B3C1EA-5610-F945-853C-C9E087DDC0A8}"/>
   </bookViews>
   <sheets>
     <sheet name="Terminology" sheetId="1" r:id="rId1"/>
@@ -19,8 +19,6 @@
   </sheets>
   <definedNames>
     <definedName name="AdjustmentArb">'Multiple Employers'!$D$23:$G$23</definedName>
-    <definedName name="MAKSBELOP">'Multiple Employers'!$C$15</definedName>
-    <definedName name="PersonRemainder">'Multiple Employers'!$C$34</definedName>
     <definedName name="ScalingFactor">'Multiple Employers'!$C$16</definedName>
     <definedName name="ShortfallIncomeRatioArb">'Multiple Employers'!$D$20:$G$20</definedName>
     <definedName name="ShortfallIncomeRatioPerson">'Multiple Employers'!$D$24:$G$24</definedName>
@@ -43,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="74">
   <si>
     <t>Term</t>
   </si>
@@ -52,6 +50,9 @@
   </si>
   <si>
     <t>Example</t>
+  </si>
+  <si>
+    <t>Format</t>
   </si>
   <si>
     <t>Integer</t>
@@ -282,27 +283,6 @@
   </si>
   <si>
     <t>Shortfall ratio - person</t>
-  </si>
-  <si>
-    <t>Precision</t>
-  </si>
-  <si>
-    <t>Ideal arbeidsgiver w/o 6G</t>
-  </si>
-  <si>
-    <t>Ideal person w/o 6G</t>
-  </si>
-  <si>
-    <t>Situation</t>
-  </si>
-  <si>
-    <t>Arbeidsgiverbeløp før 6g</t>
-  </si>
-  <si>
-    <t>Personbeløp før 6g</t>
-  </si>
-  <si>
-    <t>Remainder for employees</t>
   </si>
 </sst>
 </file>
@@ -355,7 +335,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -386,34 +366,13 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -422,7 +381,7 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -465,30 +424,7 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="6" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="6" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -809,8 +745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{336B5C91-C43F-4BAE-BFBA-00152852E840}">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
@@ -831,13 +767,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -845,13 +781,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D3" s="11">
         <v>20000</v>
@@ -860,74 +796,74 @@
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D4" s="2">
         <f>D3*12/260</f>
         <v>923.07692307692309</v>
       </c>
       <c r="E4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D5" s="11">
         <v>80</v>
       </c>
       <c r="E5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D6" s="2">
         <f>D4*ROUND(D5,0)/100</f>
         <v>738.46153846153845</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D7" s="11">
         <v>60</v>
       </c>
       <c r="E7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="4"/>
       <c r="B8" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D8" s="2">
         <f>D6*D7/100</f>
@@ -936,13 +872,13 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D9" s="11">
         <v>93634</v>
@@ -953,47 +889,47 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D10" s="2">
         <f>6*D9/260</f>
         <v>2160.7846153846153</v>
       </c>
       <c r="E10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D11" s="1">
         <f>ROUND(ROUND(D7,0)*D10/100,0)</f>
         <v>1296</v>
       </c>
       <c r="E11" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D12" s="2">
         <f>MIN(D8,D11)</f>
@@ -1003,28 +939,28 @@
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D13" s="18">
         <f>100*2/3</f>
         <v>66.666666666666671</v>
       </c>
       <c r="E13" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="10" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D14" s="9">
         <f>ROUND(D12*D13/100, 0)</f>
@@ -1033,29 +969,29 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D15" s="9">
         <f>ROUND(D12,0)-D14</f>
         <v>148</v>
       </c>
       <c r="E15" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
       <c r="B16" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D16" s="2">
         <f>D12-D14-D15</f>
@@ -1065,17 +1001,17 @@
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
       <c r="B17" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D17" s="2">
         <f>D16*260</f>
         <v>19.999999999989768</v>
       </c>
       <c r="E17" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -1089,19 +1025,19 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="13" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B21" s="14"/>
       <c r="C21" s="15"/>
       <c r="D21" s="16"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="42" t="s">
-        <v>8</v>
-      </c>
-      <c r="B22" s="42"/>
-      <c r="C22" s="42"/>
-      <c r="D22" s="42"/>
+      <c r="A22" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="28"/>
+      <c r="C22" s="28"/>
+      <c r="D22" s="28"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
@@ -1115,16 +1051,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBE9F233-0C57-4B39-8C81-6D2F9F1844A9}">
-  <dimension ref="A1:H41"/>
+  <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView zoomScale="163" zoomScaleNormal="163" workbookViewId="0">
       <selection activeCell="A24" sqref="A24"/>
     </sheetView>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="1">
-      <pane xSplit="8" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I1" sqref="I1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D33" sqref="D33:G35"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="1">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1147,22 +1080,22 @@
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>73</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -1170,10 +1103,10 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D3" s="11">
         <v>21000</v>
@@ -1188,40 +1121,40 @@
         <v>0</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" t="s">
-        <v>55</v>
-      </c>
-      <c r="D4" s="28">
+        <v>56</v>
+      </c>
+      <c r="D4" s="21">
         <f>D3/SUM($D$3:$G$3)</f>
         <v>0.33870967741935482</v>
       </c>
-      <c r="E4" s="28">
+      <c r="E4" s="21">
         <f t="shared" ref="E4:G4" si="0">E3/SUM($D$3:$G$3)</f>
         <v>0.16129032258064516</v>
       </c>
-      <c r="F4" s="28">
+      <c r="F4" s="21">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="G4" s="28">
+      <c r="G4" s="21">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="27" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D5" s="2">
         <f>D3*12/260</f>
@@ -1240,15 +1173,15 @@
         <v>0</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D6" s="20">
         <v>1</v>
@@ -1263,15 +1196,15 @@
         <v>1</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D7" s="2">
         <f>D5*D6</f>
@@ -1290,21 +1223,21 @@
         <v>0</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D8" s="21">
         <v>0.5</v>
       </c>
       <c r="E8" s="21">
-        <v>0.1</v>
+        <v>0.8</v>
       </c>
       <c r="F8" s="21">
         <v>0.2</v>
@@ -1313,15 +1246,15 @@
         <v>1</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D9" s="2">
         <f>D7*D8</f>
@@ -1329,7 +1262,7 @@
       </c>
       <c r="E9" s="2">
         <f t="shared" ref="E9:G9" si="2">E7*E8</f>
-        <v>46.15384615384616</v>
+        <v>369.23076923076928</v>
       </c>
       <c r="F9" s="2">
         <f t="shared" si="2"/>
@@ -1340,21 +1273,21 @@
         <v>0</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D10" s="20">
         <v>1</v>
       </c>
       <c r="E10" s="20">
-        <v>0.1</v>
+        <v>0.9</v>
       </c>
       <c r="F10" s="20">
         <v>0.25</v>
@@ -1363,15 +1296,15 @@
         <v>1</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B11" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D11" s="17">
         <f>D9*D10</f>
@@ -1379,7 +1312,7 @@
       </c>
       <c r="E11" s="17">
         <f t="shared" ref="E11:G11" si="3">E9*E10</f>
-        <v>4.6153846153846159</v>
+        <v>332.30769230769238</v>
       </c>
       <c r="F11" s="17">
         <f t="shared" si="3"/>
@@ -1390,562 +1323,389 @@
         <v>0</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B12" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C12" s="19">
         <f>ROUND(SUM(D9:G9)/SUM(D7:G7),2)</f>
-        <v>0.28999999999999998</v>
+        <v>0.4</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B13" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C13" s="11">
         <v>93634</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B14" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C14" s="2">
         <f>6*C13/260</f>
         <v>2160.7846153846153</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B15" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C15" s="1">
         <f>C12*C14</f>
-        <v>626.62753846153839</v>
+        <v>864.31384615384616</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B16" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C16" s="22">
         <f>MIN(1, C15/SUM(D9:G9))</f>
-        <v>0.76705819209039539</v>
+        <v>0.75817004048582992</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" s="29" t="s">
-        <v>33</v>
-      </c>
-      <c r="B17" s="30" t="s">
-        <v>12</v>
-      </c>
-      <c r="C17" s="30"/>
-      <c r="D17" s="31">
+      <c r="A17" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="17">
         <f>D9*ScalingFactor</f>
-        <v>371.72820078226857</v>
-      </c>
-      <c r="E17" s="31">
+        <v>367.42086577390222</v>
+      </c>
+      <c r="E17" s="17">
         <f>E9*ScalingFactor</f>
-        <v>35.402685788787487</v>
-      </c>
-      <c r="F17" s="31">
+        <v>279.93970725630646</v>
+      </c>
+      <c r="F17" s="17">
         <f>F9*ScalingFactor</f>
-        <v>219.49665189048235</v>
-      </c>
-      <c r="G17" s="31">
+        <v>216.95327312363747</v>
+      </c>
+      <c r="G17" s="17">
         <f>G9*ScalingFactor</f>
         <v>0</v>
       </c>
-      <c r="H17" s="32" t="s">
-        <v>4</v>
+      <c r="H17" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" s="29" t="s">
-        <v>66</v>
-      </c>
-      <c r="B18" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="C18" s="30"/>
-      <c r="D18" s="31">
+      <c r="A18" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18" s="17">
         <f>MIN(D17,D11)</f>
-        <v>371.72820078226857</v>
-      </c>
-      <c r="E18" s="31">
+        <v>367.42086577390222</v>
+      </c>
+      <c r="E18" s="17">
         <f t="shared" ref="E18:G18" si="4">MIN(E17,E11)</f>
-        <v>4.6153846153846159</v>
-      </c>
-      <c r="F18" s="31">
+        <v>279.93970725630646</v>
+      </c>
+      <c r="F18" s="17">
         <f t="shared" si="4"/>
         <v>71.538461538461533</v>
       </c>
-      <c r="G18" s="31">
+      <c r="G18" s="17">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="H18" s="32" t="s">
-        <v>4</v>
+      <c r="H18" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" s="29"/>
-      <c r="B19" s="30" t="s">
-        <v>47</v>
-      </c>
-      <c r="C19" s="30"/>
-      <c r="D19" s="31">
+      <c r="A19" s="4"/>
+      <c r="B19" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" s="17">
         <f>D18-D11</f>
-        <v>-112.88718383311607</v>
-      </c>
-      <c r="E19" s="31">
+        <v>-117.19451884148242</v>
+      </c>
+      <c r="E19" s="17">
         <f t="shared" ref="E19:G19" si="5">E18-E11</f>
-        <v>0</v>
-      </c>
-      <c r="F19" s="31">
+        <v>-52.367985051385915</v>
+      </c>
+      <c r="F19" s="17">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="G19" s="31">
+      <c r="G19" s="17">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="H19" s="32" t="s">
-        <v>4</v>
+      <c r="H19" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" s="29"/>
-      <c r="B20" s="30" t="s">
-        <v>70</v>
-      </c>
-      <c r="C20" s="30"/>
-      <c r="D20" s="33">
+      <c r="A20" s="4"/>
+      <c r="B20" t="s">
+        <v>71</v>
+      </c>
+      <c r="D20" s="19">
         <f>IF(D19 &lt; 0, D4, 0)</f>
         <v>0.33870967741935482</v>
       </c>
-      <c r="E20" s="33">
+      <c r="E20" s="19">
         <f t="shared" ref="E20:F20" si="6">IF(E19 &lt; 0, E4, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="F20" s="33">
+        <v>0.16129032258064516</v>
+      </c>
+      <c r="F20" s="19">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="G20" s="31"/>
-      <c r="H20" s="32" t="s">
-        <v>4</v>
+      <c r="G20" s="17"/>
+      <c r="H20" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" s="29" t="s">
-        <v>67</v>
-      </c>
-      <c r="B21" s="30" t="s">
-        <v>71</v>
-      </c>
-      <c r="C21" s="30"/>
-      <c r="D21" s="33">
+      <c r="A21" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B21" t="s">
+        <v>72</v>
+      </c>
+      <c r="D21" s="19">
         <f>IF(SUM(ShortfallIncomeRatioArb)=0,0,D20/SUM(ShortfallIncomeRatioArb))</f>
-        <v>1</v>
-      </c>
-      <c r="E21" s="33">
+        <v>0.67741935483870963</v>
+      </c>
+      <c r="E21" s="19">
         <f>IF(SUM(ShortfallIncomeRatioArb)=0,0,E20/SUM(ShortfallIncomeRatioArb))</f>
-        <v>0</v>
-      </c>
-      <c r="F21" s="33">
+        <v>0.32258064516129031</v>
+      </c>
+      <c r="F21" s="19">
         <f>IF(SUM(ShortfallIncomeRatioArb)=0,0,F20/SUM(ShortfallIncomeRatioArb))</f>
         <v>0</v>
       </c>
-      <c r="G21" s="33">
+      <c r="G21" s="19">
         <f>IF(SUM(ShortfallIncomeRatioArb)=0,0,G20/SUM(ShortfallIncomeRatioArb))</f>
         <v>0</v>
       </c>
-      <c r="H21" s="32" t="s">
-        <v>4</v>
+      <c r="H21" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" s="29"/>
-      <c r="B22" s="30" t="s">
-        <v>45</v>
-      </c>
-      <c r="C22" s="30"/>
-      <c r="D22" s="31">
+      <c r="A22" s="4"/>
+      <c r="B22" t="s">
+        <v>46</v>
+      </c>
+      <c r="D22" s="17">
         <f>D17-D18</f>
         <v>0</v>
       </c>
-      <c r="E22" s="31">
+      <c r="E22" s="17">
         <f>E17-E18</f>
-        <v>30.78730117340287</v>
-      </c>
-      <c r="F22" s="31">
+        <v>0</v>
+      </c>
+      <c r="F22" s="17">
         <f>F17-F18</f>
-        <v>147.95819035202084</v>
-      </c>
-      <c r="G22" s="31">
+        <v>145.41481158517593</v>
+      </c>
+      <c r="G22" s="17">
         <f>G17-G18</f>
         <v>0</v>
       </c>
-      <c r="H22" s="32" t="s">
-        <v>4</v>
+      <c r="H22" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="B23" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="C23" s="30"/>
-      <c r="D23" s="31">
+      <c r="A23" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B23" t="s">
+        <v>49</v>
+      </c>
+      <c r="D23" s="17">
         <f>MIN(-D19,IF(SUM($D$19:$G$19)&gt;=0, 0, SUM($D$22:$G$22)*D21))</f>
-        <v>112.88718383311607</v>
-      </c>
-      <c r="E23" s="31">
+        <v>98.50680784802239</v>
+      </c>
+      <c r="E23" s="17">
         <f t="shared" ref="E23:G23" si="7">MIN(-E19,IF(SUM($D$19:$G$19)&gt;=0, 0, SUM($D$22:$G$22)*E21))</f>
-        <v>0</v>
-      </c>
-      <c r="F23" s="31">
+        <v>46.908003737153521</v>
+      </c>
+      <c r="F23" s="17">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="G23" s="31">
+      <c r="G23" s="17">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="H23" s="32" t="s">
-        <v>4</v>
+      <c r="H23" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" s="29"/>
-      <c r="B24" s="30" t="s">
-        <v>69</v>
-      </c>
-      <c r="C24" s="30"/>
-      <c r="D24" s="33">
+      <c r="A24" s="4"/>
+      <c r="B24" t="s">
+        <v>70</v>
+      </c>
+      <c r="D24" s="19">
         <f>IF(D22 = 0, 0, D4)</f>
         <v>0</v>
       </c>
-      <c r="E24" s="33">
+      <c r="E24" s="19">
         <f t="shared" ref="E24:G24" si="8">IF(E22 = 0, 0, E4)</f>
-        <v>0.16129032258064516</v>
-      </c>
-      <c r="F24" s="33">
+        <v>0</v>
+      </c>
+      <c r="F24" s="19">
         <f t="shared" si="8"/>
         <v>0.5</v>
       </c>
-      <c r="G24" s="33">
+      <c r="G24" s="19">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="H24" s="32" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" s="29"/>
-      <c r="B25" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="C25" s="30"/>
-      <c r="D25" s="33">
+      <c r="A25" s="4"/>
+      <c r="B25" t="s">
+        <v>73</v>
+      </c>
+      <c r="D25" s="19">
         <f>IF(SUM(ShortfallIncomeRatioPerson)= 0, 0, D24/SUM(ShortfallIncomeRatioPerson))</f>
         <v>0</v>
       </c>
-      <c r="E25" s="33">
+      <c r="E25" s="19">
         <f>IF(SUM(ShortfallIncomeRatioPerson)= 0, 0, E24/SUM(ShortfallIncomeRatioPerson))</f>
-        <v>0.24390243902439024</v>
-      </c>
-      <c r="F25" s="33">
+        <v>0</v>
+      </c>
+      <c r="F25" s="19">
         <f>IF(SUM(ShortfallIncomeRatioPerson)= 0, 0, F24/SUM(ShortfallIncomeRatioPerson))</f>
-        <v>0.75609756097560976</v>
-      </c>
-      <c r="G25" s="33">
+        <v>1</v>
+      </c>
+      <c r="G25" s="19">
         <f>IF(SUM(ShortfallIncomeRatioPerson)= 0, 0, G24/SUM(ShortfallIncomeRatioPerson))</f>
         <v>0</v>
       </c>
-      <c r="H25" s="32" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" s="29" t="s">
-        <v>31</v>
-      </c>
-      <c r="B26" s="30" t="s">
-        <v>14</v>
-      </c>
-      <c r="C26" s="30"/>
-      <c r="D26" s="34">
+      <c r="A26" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B26" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26" s="1">
         <f>ROUND(D18+D23,0)</f>
-        <v>485</v>
-      </c>
-      <c r="E26" s="34">
+        <v>466</v>
+      </c>
+      <c r="E26" s="1">
         <f t="shared" ref="E26:G26" si="9">ROUND(E18+E23,0)</f>
-        <v>5</v>
-      </c>
-      <c r="F26" s="34">
+        <v>327</v>
+      </c>
+      <c r="F26" s="1">
         <f t="shared" si="9"/>
         <v>72</v>
       </c>
-      <c r="G26" s="31">
+      <c r="G26" s="17">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="H26" s="32" t="s">
-        <v>3</v>
+      <c r="H26" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="B27" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="C27" s="30"/>
-      <c r="D27" s="30">
+      <c r="A27" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B27" t="s">
+        <v>16</v>
+      </c>
+      <c r="D27">
         <f>ROUND(D22-SUM(AdjustmentArb)*D25,0)</f>
         <v>0</v>
       </c>
-      <c r="E27" s="30">
+      <c r="E27">
         <f>ROUND(E22-SUM(AdjustmentArb)*E25,0)</f>
-        <v>3</v>
-      </c>
-      <c r="F27" s="30">
+        <v>0</v>
+      </c>
+      <c r="F27">
         <f>ROUND(F22-SUM(AdjustmentArb)*F25,0)</f>
-        <v>63</v>
-      </c>
-      <c r="G27" s="30">
+        <v>0</v>
+      </c>
+      <c r="G27">
         <f>ROUND(G22-SUM(AdjustmentArb)*G25,0)</f>
         <v>0</v>
       </c>
-      <c r="H27" s="32" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" s="29"/>
-      <c r="B28" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="C28" s="35">
+      <c r="A28" s="4"/>
+      <c r="B28" t="s">
+        <v>18</v>
+      </c>
+      <c r="C28" s="26">
         <f>C15-SUM(D26:G27)</f>
-        <v>-1.3724615384616072</v>
-      </c>
-      <c r="D28" s="30"/>
-      <c r="E28" s="30"/>
-      <c r="F28" s="30"/>
-      <c r="G28" s="30"/>
-      <c r="H28" s="32" t="s">
-        <v>3</v>
+        <v>-0.68615384615384301</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="4"/>
-      <c r="C29" s="26"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A30" s="36" t="s">
-        <v>77</v>
-      </c>
-      <c r="B30" s="37" t="s">
-        <v>74</v>
-      </c>
-      <c r="C30" s="38"/>
-      <c r="D30" s="39">
-        <f>ROUND(D9*D10, 0)</f>
-        <v>485</v>
-      </c>
-      <c r="E30" s="39">
-        <f t="shared" ref="E30:G30" si="10">ROUND(E9*E10, 0)</f>
-        <v>5</v>
-      </c>
-      <c r="F30" s="39">
-        <f t="shared" si="10"/>
-        <v>72</v>
-      </c>
-      <c r="G30" s="39">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="H30" s="40" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A31" s="36" t="s">
-        <v>78</v>
-      </c>
-      <c r="B31" s="37" t="s">
-        <v>75</v>
-      </c>
-      <c r="C31" s="38"/>
-      <c r="D31" s="39">
-        <f>ROUND(D9,0) - D30</f>
-        <v>0</v>
-      </c>
-      <c r="E31" s="39">
-        <f t="shared" ref="E31:G31" si="11">ROUND(E9,0) - E30</f>
-        <v>41</v>
-      </c>
-      <c r="F31" s="39">
-        <f t="shared" si="11"/>
-        <v>214</v>
-      </c>
-      <c r="G31" s="39">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="H31" s="40" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A32" s="36"/>
-      <c r="B32" s="41" t="s">
-        <v>76</v>
-      </c>
-      <c r="C32" s="43" t="str">
-        <f>IF(SUM(D30:G31)&lt;=MAKSBELOP,"Everyone paid",IF(SUM(D30:G30)&lt;=MAKSBELOP,"Arbeidsgivere fully paid; Person partially paid by Dekningsfaktor", "Arbeidsgivere partial payment only by Dekningsfaktor"))</f>
-        <v>Arbeidsgivere fully paid; Person partially paid by Dekningsfaktor</v>
-      </c>
-      <c r="D32" s="43"/>
-      <c r="E32" s="43"/>
-      <c r="F32" s="43"/>
-      <c r="G32" s="43"/>
-      <c r="H32" s="40"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A33" s="36" t="s">
-        <v>31</v>
-      </c>
-      <c r="B33" s="37" t="s">
-        <v>14</v>
-      </c>
-      <c r="C33" s="38"/>
-      <c r="D33" s="37">
-        <f>IF(SUM($D$30:$G$31)&lt;=MAKSBELOP,D30,IF(SUM($D$30:$G$30)&lt;=MAKSBELOP,D30,ROUND(D30*ScalingFactor,0)))</f>
-        <v>485</v>
-      </c>
-      <c r="E33" s="37">
-        <f>IF(SUM($D$30:$G$31)&lt;=MAKSBELOP,E30,IF(SUM($D$30:$G$30)&lt;=MAKSBELOP,E30,ROUND(E30*ScalingFactor,0)))</f>
-        <v>5</v>
-      </c>
-      <c r="F33" s="37">
-        <f>IF(SUM($D$30:$G$31)&lt;=MAKSBELOP,F30,IF(SUM($D$30:$G$30)&lt;=MAKSBELOP,F30,ROUND(F30*ScalingFactor,0)))</f>
-        <v>72</v>
-      </c>
-      <c r="G33" s="37">
-        <f>IF(SUM($D$30:$G$31)&lt;=MAKSBELOP,G30,IF(SUM($D$30:$G$30)&lt;=MAKSBELOP,G30,ROUND(G30*ScalingFactor,0)))</f>
-        <v>0</v>
-      </c>
-      <c r="H33" s="40" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A34" s="36"/>
-      <c r="B34" s="37" t="s">
-        <v>79</v>
-      </c>
-      <c r="C34" s="38">
-        <f>MAKSBELOP-SUM(D33:G33)</f>
-        <v>64.627538461538393</v>
-      </c>
-      <c r="D34" s="37"/>
-      <c r="E34" s="37"/>
-      <c r="F34" s="37"/>
-      <c r="G34" s="37"/>
-      <c r="H34" s="40"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A35" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="B35" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="C35" s="37"/>
-      <c r="D35" s="37">
-        <f>ROUND(PersonRemainder*D31/SUM($D$31:$G$31),0)</f>
-        <v>0</v>
-      </c>
-      <c r="E35" s="37">
-        <f>ROUND(PersonRemainder*E31/SUM($D$31:$G$31),0)</f>
-        <v>10</v>
-      </c>
-      <c r="F35" s="37">
-        <f>ROUND(PersonRemainder*F31/SUM($D$31:$G$31),0)</f>
-        <v>54</v>
-      </c>
-      <c r="G35" s="37">
-        <f>ROUND(PersonRemainder*G31/SUM($D$31:$G$31),0)</f>
-        <v>0</v>
-      </c>
-      <c r="H35" s="40" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A40" s="23" t="s">
-        <v>49</v>
-      </c>
-      <c r="B40" s="24">
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B34" s="24">
         <v>1430.76</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A41" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="B41" s="24">
-        <f>ROUND(B40*260/12,0)</f>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="B35" s="24">
+        <f>ROUND(B34*260/12,0)</f>
         <v>31000</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="C32:G32"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated spreadsheet for showing both algorithms
</commit_message>
<xml_diff>
--- a/doc/okonomi/Utbetaling.xlsx
+++ b/doc/okonomi/Utbetaling.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fred/src/nav/helse-spleis/doc/okonomi/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5E2AE42-9FBB-C44D-82C6-8ADEA7B8FCAC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{397F8339-04CE-1E45-B951-8FB14660EC40}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2020" yWindow="860" windowWidth="20220" windowHeight="14600" xr2:uid="{BB3196D1-BBA6-4B4B-8E55-37C48C2FF3A4}"/>
-    <workbookView xWindow="22440" yWindow="840" windowWidth="25260" windowHeight="16940" activeTab="1" xr2:uid="{84B3C1EA-5610-F945-853C-C9E087DDC0A8}"/>
+    <workbookView xWindow="2020" yWindow="860" windowWidth="27900" windowHeight="18840" xr2:uid="{BB3196D1-BBA6-4B4B-8E55-37C48C2FF3A4}"/>
+    <workbookView xWindow="32120" yWindow="1000" windowWidth="31580" windowHeight="23740" activeTab="1" xr2:uid="{84B3C1EA-5610-F945-853C-C9E087DDC0A8}"/>
   </bookViews>
   <sheets>
     <sheet name="Terminology" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
   </sheets>
   <definedNames>
     <definedName name="AdjustmentArb">'Multiple Employers'!$D$23:$G$23</definedName>
+    <definedName name="MAKSBELOP">'Multiple Employers'!$C$15</definedName>
     <definedName name="ScalingFactor">'Multiple Employers'!$C$16</definedName>
     <definedName name="ShortfallIncomeRatioArb">'Multiple Employers'!$D$20:$G$20</definedName>
     <definedName name="ShortfallIncomeRatioPerson">'Multiple Employers'!$D$24:$G$24</definedName>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="79">
   <si>
     <t>Term</t>
   </si>
@@ -50,9 +51,6 @@
   </si>
   <si>
     <t>Example</t>
-  </si>
-  <si>
-    <t>Format</t>
   </si>
   <si>
     <t>Integer</t>
@@ -283,6 +281,24 @@
   </si>
   <si>
     <t>Shortfall ratio - person</t>
+  </si>
+  <si>
+    <t>Precision</t>
+  </si>
+  <si>
+    <t>Ideal arbeidsgiver w/o 6G</t>
+  </si>
+  <si>
+    <t>Ideal person w/o 6G</t>
+  </si>
+  <si>
+    <t>Situation</t>
+  </si>
+  <si>
+    <t>Arbeidsgiverbeløp før 6g</t>
+  </si>
+  <si>
+    <t>Personbeløp før 6g</t>
   </si>
 </sst>
 </file>
@@ -335,7 +351,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -366,13 +382,34 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -381,7 +418,7 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -424,8 +461,31 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="6" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -745,8 +805,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{336B5C91-C43F-4BAE-BFBA-00152852E840}">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
@@ -767,13 +827,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -781,13 +841,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D3" s="11">
         <v>20000</v>
@@ -796,74 +856,74 @@
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D4" s="2">
         <f>D3*12/260</f>
         <v>923.07692307692309</v>
       </c>
       <c r="E4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D5" s="11">
         <v>80</v>
       </c>
       <c r="E5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
       <c r="B6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D6" s="2">
         <f>D4*ROUND(D5,0)/100</f>
         <v>738.46153846153845</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s">
         <v>25</v>
       </c>
-      <c r="B7" t="s">
-        <v>26</v>
-      </c>
       <c r="C7" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D7" s="11">
         <v>60</v>
       </c>
       <c r="E7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="4"/>
       <c r="B8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D8" s="2">
         <f>D6*D7/100</f>
@@ -872,13 +932,13 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D9" s="11">
         <v>93634</v>
@@ -889,47 +949,47 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D10" s="2">
         <f>6*D9/260</f>
         <v>2160.7846153846153</v>
       </c>
       <c r="E10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
       <c r="B11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D11" s="1">
         <f>ROUND(ROUND(D7,0)*D10/100,0)</f>
         <v>1296</v>
       </c>
       <c r="E11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D12" s="2">
         <f>MIN(D8,D11)</f>
@@ -939,28 +999,28 @@
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D13" s="18">
         <f>100*2/3</f>
         <v>66.666666666666671</v>
       </c>
       <c r="E13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D14" s="9">
         <f>ROUND(D12*D13/100, 0)</f>
@@ -969,29 +1029,29 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D15" s="9">
         <f>ROUND(D12,0)-D14</f>
         <v>148</v>
       </c>
       <c r="E15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
       <c r="B16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D16" s="2">
         <f>D12-D14-D15</f>
@@ -1001,17 +1061,17 @@
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
       <c r="B17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D17" s="2">
         <f>D16*260</f>
         <v>19.999999999989768</v>
       </c>
       <c r="E17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -1025,19 +1085,19 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B21" s="14"/>
       <c r="C21" s="15"/>
       <c r="D21" s="16"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="B22" s="28"/>
-      <c r="C22" s="28"/>
-      <c r="D22" s="28"/>
+      <c r="A22" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="29"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="29"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
@@ -1051,13 +1111,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBE9F233-0C57-4B39-8C81-6D2F9F1844A9}">
-  <dimension ref="A1:H35"/>
+  <dimension ref="A1:H40"/>
   <sheetViews>
     <sheetView zoomScale="163" zoomScaleNormal="163" workbookViewId="0">
       <selection activeCell="A24" sqref="A24"/>
     </sheetView>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="1">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="1">
+      <pane xSplit="8" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="I1" sqref="I1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1080,22 +1143,22 @@
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D1" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="8" t="s">
-        <v>24</v>
-      </c>
       <c r="H1" s="8" t="s">
-        <v>3</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -1103,10 +1166,10 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D3" s="11">
         <v>21000</v>
@@ -1121,40 +1184,40 @@
         <v>0</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D4" s="21">
+        <v>55</v>
+      </c>
+      <c r="D4" s="28">
         <f>D3/SUM($D$3:$G$3)</f>
         <v>0.33870967741935482</v>
       </c>
-      <c r="E4" s="21">
+      <c r="E4" s="28">
         <f t="shared" ref="E4:G4" si="0">E3/SUM($D$3:$G$3)</f>
         <v>0.16129032258064516</v>
       </c>
-      <c r="F4" s="21">
+      <c r="F4" s="28">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="G4" s="21">
+      <c r="G4" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="27" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D5" s="2">
         <f>D3*12/260</f>
@@ -1173,15 +1236,15 @@
         <v>0</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D6" s="20">
         <v>1</v>
@@ -1196,15 +1259,15 @@
         <v>1</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D7" s="2">
         <f>D5*D6</f>
@@ -1223,15 +1286,15 @@
         <v>0</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" t="s">
         <v>25</v>
-      </c>
-      <c r="B8" t="s">
-        <v>26</v>
       </c>
       <c r="D8" s="21">
         <v>0.5</v>
@@ -1246,15 +1309,15 @@
         <v>1</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D9" s="2">
         <f>D7*D8</f>
@@ -1273,15 +1336,15 @@
         <v>0</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D10" s="20">
         <v>1</v>
@@ -1296,15 +1359,15 @@
         <v>1</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D11" s="17">
         <f>D9*D10</f>
@@ -1323,389 +1386,547 @@
         <v>0</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C12" s="19">
         <f>ROUND(SUM(D9:G9)/SUM(D7:G7),2)</f>
         <v>0.4</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C13" s="11">
         <v>93634</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C14" s="2">
         <f>6*C13/260</f>
         <v>2160.7846153846153</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C15" s="1">
         <f>C12*C14</f>
         <v>864.31384615384616</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C16" s="22">
         <f>MIN(1, C15/SUM(D9:G9))</f>
         <v>0.75817004048582992</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B17" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17" s="17">
+      <c r="A17" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="31"/>
+      <c r="D17" s="32">
         <f>D9*ScalingFactor</f>
         <v>367.42086577390222</v>
       </c>
-      <c r="E17" s="17">
+      <c r="E17" s="32">
         <f>E9*ScalingFactor</f>
         <v>279.93970725630646</v>
       </c>
-      <c r="F17" s="17">
+      <c r="F17" s="32">
         <f>F9*ScalingFactor</f>
         <v>216.95327312363747</v>
       </c>
-      <c r="G17" s="17">
+      <c r="G17" s="32">
         <f>G9*ScalingFactor</f>
         <v>0</v>
       </c>
-      <c r="H17" s="3" t="s">
-        <v>5</v>
+      <c r="H17" s="33" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="B18" t="s">
-        <v>45</v>
-      </c>
-      <c r="D18" s="17">
+      <c r="A18" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="B18" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="31"/>
+      <c r="D18" s="32">
         <f>MIN(D17,D11)</f>
         <v>367.42086577390222</v>
       </c>
-      <c r="E18" s="17">
+      <c r="E18" s="32">
         <f t="shared" ref="E18:G18" si="4">MIN(E17,E11)</f>
         <v>279.93970725630646</v>
       </c>
-      <c r="F18" s="17">
+      <c r="F18" s="32">
         <f t="shared" si="4"/>
         <v>71.538461538461533</v>
       </c>
-      <c r="G18" s="17">
+      <c r="G18" s="32">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="H18" s="3" t="s">
-        <v>5</v>
+      <c r="H18" s="33" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" s="4"/>
-      <c r="B19" t="s">
-        <v>48</v>
-      </c>
-      <c r="D19" s="17">
+      <c r="A19" s="30"/>
+      <c r="B19" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" s="31"/>
+      <c r="D19" s="32">
         <f>D18-D11</f>
         <v>-117.19451884148242</v>
       </c>
-      <c r="E19" s="17">
+      <c r="E19" s="32">
         <f t="shared" ref="E19:G19" si="5">E18-E11</f>
         <v>-52.367985051385915</v>
       </c>
-      <c r="F19" s="17">
+      <c r="F19" s="32">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="G19" s="17">
+      <c r="G19" s="32">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="H19" s="3" t="s">
-        <v>5</v>
+      <c r="H19" s="33" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" s="4"/>
-      <c r="B20" t="s">
-        <v>71</v>
-      </c>
-      <c r="D20" s="19">
+      <c r="A20" s="30"/>
+      <c r="B20" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20" s="31"/>
+      <c r="D20" s="34">
         <f>IF(D19 &lt; 0, D4, 0)</f>
         <v>0.33870967741935482</v>
       </c>
-      <c r="E20" s="19">
+      <c r="E20" s="34">
         <f t="shared" ref="E20:F20" si="6">IF(E19 &lt; 0, E4, 0)</f>
         <v>0.16129032258064516</v>
       </c>
-      <c r="F20" s="19">
+      <c r="F20" s="34">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="G20" s="17"/>
-      <c r="H20" s="3" t="s">
-        <v>5</v>
+      <c r="G20" s="32"/>
+      <c r="H20" s="33" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="B21" t="s">
-        <v>72</v>
-      </c>
-      <c r="D21" s="19">
+      <c r="A21" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="B21" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="C21" s="31"/>
+      <c r="D21" s="34">
         <f>IF(SUM(ShortfallIncomeRatioArb)=0,0,D20/SUM(ShortfallIncomeRatioArb))</f>
         <v>0.67741935483870963</v>
       </c>
-      <c r="E21" s="19">
+      <c r="E21" s="34">
         <f>IF(SUM(ShortfallIncomeRatioArb)=0,0,E20/SUM(ShortfallIncomeRatioArb))</f>
         <v>0.32258064516129031</v>
       </c>
-      <c r="F21" s="19">
+      <c r="F21" s="34">
         <f>IF(SUM(ShortfallIncomeRatioArb)=0,0,F20/SUM(ShortfallIncomeRatioArb))</f>
         <v>0</v>
       </c>
-      <c r="G21" s="19">
+      <c r="G21" s="34">
         <f>IF(SUM(ShortfallIncomeRatioArb)=0,0,G20/SUM(ShortfallIncomeRatioArb))</f>
         <v>0</v>
       </c>
-      <c r="H21" s="3" t="s">
-        <v>5</v>
+      <c r="H21" s="33" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" s="4"/>
-      <c r="B22" t="s">
-        <v>46</v>
-      </c>
-      <c r="D22" s="17">
+      <c r="A22" s="30"/>
+      <c r="B22" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" s="31"/>
+      <c r="D22" s="32">
         <f>D17-D18</f>
         <v>0</v>
       </c>
-      <c r="E22" s="17">
+      <c r="E22" s="32">
         <f>E17-E18</f>
         <v>0</v>
       </c>
-      <c r="F22" s="17">
+      <c r="F22" s="32">
         <f>F17-F18</f>
         <v>145.41481158517593</v>
       </c>
-      <c r="G22" s="17">
+      <c r="G22" s="32">
         <f>G17-G18</f>
         <v>0</v>
       </c>
-      <c r="H22" s="3" t="s">
-        <v>5</v>
+      <c r="H22" s="33" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="B23" t="s">
-        <v>49</v>
-      </c>
-      <c r="D23" s="17">
+      <c r="A23" s="30" t="s">
+        <v>68</v>
+      </c>
+      <c r="B23" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23" s="31"/>
+      <c r="D23" s="32">
         <f>MIN(-D19,IF(SUM($D$19:$G$19)&gt;=0, 0, SUM($D$22:$G$22)*D21))</f>
         <v>98.50680784802239</v>
       </c>
-      <c r="E23" s="17">
+      <c r="E23" s="32">
         <f t="shared" ref="E23:G23" si="7">MIN(-E19,IF(SUM($D$19:$G$19)&gt;=0, 0, SUM($D$22:$G$22)*E21))</f>
         <v>46.908003737153521</v>
       </c>
-      <c r="F23" s="17">
+      <c r="F23" s="32">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="G23" s="17">
+      <c r="G23" s="32">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="H23" s="3" t="s">
-        <v>5</v>
+      <c r="H23" s="33" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" s="4"/>
-      <c r="B24" t="s">
-        <v>70</v>
-      </c>
-      <c r="D24" s="19">
+      <c r="A24" s="30"/>
+      <c r="B24" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="C24" s="31"/>
+      <c r="D24" s="34">
         <f>IF(D22 = 0, 0, D4)</f>
         <v>0</v>
       </c>
-      <c r="E24" s="19">
+      <c r="E24" s="34">
         <f t="shared" ref="E24:G24" si="8">IF(E22 = 0, 0, E4)</f>
         <v>0</v>
       </c>
-      <c r="F24" s="19">
+      <c r="F24" s="34">
         <f t="shared" si="8"/>
         <v>0.5</v>
       </c>
-      <c r="G24" s="19">
+      <c r="G24" s="34">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
+      <c r="H24" s="33" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" s="4"/>
-      <c r="B25" t="s">
-        <v>73</v>
-      </c>
-      <c r="D25" s="19">
+      <c r="A25" s="30"/>
+      <c r="B25" s="31" t="s">
+        <v>72</v>
+      </c>
+      <c r="C25" s="31"/>
+      <c r="D25" s="34">
         <f>IF(SUM(ShortfallIncomeRatioPerson)= 0, 0, D24/SUM(ShortfallIncomeRatioPerson))</f>
         <v>0</v>
       </c>
-      <c r="E25" s="19">
+      <c r="E25" s="34">
         <f>IF(SUM(ShortfallIncomeRatioPerson)= 0, 0, E24/SUM(ShortfallIncomeRatioPerson))</f>
         <v>0</v>
       </c>
-      <c r="F25" s="19">
+      <c r="F25" s="34">
         <f>IF(SUM(ShortfallIncomeRatioPerson)= 0, 0, F24/SUM(ShortfallIncomeRatioPerson))</f>
         <v>1</v>
       </c>
-      <c r="G25" s="19">
+      <c r="G25" s="34">
         <f>IF(SUM(ShortfallIncomeRatioPerson)= 0, 0, G24/SUM(ShortfallIncomeRatioPerson))</f>
         <v>0</v>
       </c>
+      <c r="H25" s="33" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B26" t="s">
-        <v>15</v>
-      </c>
-      <c r="D26" s="1">
+      <c r="A26" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" s="31"/>
+      <c r="D26" s="35">
         <f>ROUND(D18+D23,0)</f>
         <v>466</v>
       </c>
-      <c r="E26" s="1">
+      <c r="E26" s="35">
         <f t="shared" ref="E26:G26" si="9">ROUND(E18+E23,0)</f>
         <v>327</v>
       </c>
-      <c r="F26" s="1">
+      <c r="F26" s="35">
         <f t="shared" si="9"/>
         <v>72</v>
       </c>
-      <c r="G26" s="17">
+      <c r="G26" s="32">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="H26" s="3" t="s">
-        <v>4</v>
+      <c r="H26" s="33" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B27" t="s">
-        <v>16</v>
-      </c>
-      <c r="D27">
+      <c r="A27" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="B27" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" s="31"/>
+      <c r="D27" s="31">
         <f>ROUND(D22-SUM(AdjustmentArb)*D25,0)</f>
         <v>0</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="31">
         <f>ROUND(E22-SUM(AdjustmentArb)*E25,0)</f>
         <v>0</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="31">
         <f>ROUND(F22-SUM(AdjustmentArb)*F25,0)</f>
         <v>0</v>
       </c>
-      <c r="G27">
+      <c r="G27" s="31">
         <f>ROUND(G22-SUM(AdjustmentArb)*G25,0)</f>
         <v>0</v>
       </c>
+      <c r="H27" s="33" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" s="4"/>
-      <c r="B28" t="s">
-        <v>18</v>
-      </c>
-      <c r="C28" s="26">
+      <c r="A28" s="30"/>
+      <c r="B28" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28" s="36">
         <f>C15-SUM(D26:G27)</f>
         <v>-0.68615384615384301</v>
       </c>
+      <c r="D28" s="31"/>
+      <c r="E28" s="31"/>
+      <c r="F28" s="31"/>
+      <c r="G28" s="31"/>
+      <c r="H28" s="33" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="4"/>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" s="23" t="s">
+      <c r="C29" s="26"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="37" t="s">
+        <v>77</v>
+      </c>
+      <c r="B30" s="38" t="s">
+        <v>74</v>
+      </c>
+      <c r="C30" s="39"/>
+      <c r="D30" s="40">
+        <f>ROUND(D9*D10, 0)</f>
+        <v>485</v>
+      </c>
+      <c r="E30" s="40">
+        <f t="shared" ref="E30:G30" si="10">ROUND(E9*E10, 0)</f>
+        <v>332</v>
+      </c>
+      <c r="F30" s="40">
+        <f t="shared" si="10"/>
+        <v>72</v>
+      </c>
+      <c r="G30" s="40">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="H30" s="41" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="37" t="s">
+        <v>78</v>
+      </c>
+      <c r="B31" s="38" t="s">
+        <v>75</v>
+      </c>
+      <c r="C31" s="39"/>
+      <c r="D31" s="40">
+        <f>ROUND(D9,0) - D30</f>
+        <v>0</v>
+      </c>
+      <c r="E31" s="40">
+        <f t="shared" ref="E31:G31" si="11">ROUND(E9,0) - E30</f>
+        <v>37</v>
+      </c>
+      <c r="F31" s="40">
+        <f t="shared" si="11"/>
+        <v>214</v>
+      </c>
+      <c r="G31" s="40">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="H31" s="41" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="37"/>
+      <c r="B32" s="43" t="s">
+        <v>76</v>
+      </c>
+      <c r="C32" s="42" t="str">
+        <f>IF(SUM(D30:G31)&lt;=MAKSBELOP,"Everyone paid",IF(SUM(D30:G30)&lt;=MAKSBELOP,"Arbeidsgivere fully paid; Person partially paid by Dekningsfaktor", "Arbeidsgivere partial payment only by Dekningsfaktor"))</f>
+        <v>Arbeidsgivere partial payment only by Dekningsfaktor</v>
+      </c>
+      <c r="D32" s="42"/>
+      <c r="E32" s="42"/>
+      <c r="F32" s="42"/>
+      <c r="G32" s="42"/>
+      <c r="H32" s="41"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="B33" s="38" t="s">
+        <v>14</v>
+      </c>
+      <c r="C33" s="39"/>
+      <c r="D33" s="38">
+        <f>IF(SUM($D$30:$G$31)&lt;=MAKSBELOP,D30,IF(SUM($D$30:$G$30)&lt;=MAKSBELOP,D30,ROUND(D30*ScalingFactor,0)))</f>
+        <v>368</v>
+      </c>
+      <c r="E33" s="38">
+        <f>IF(SUM($D$30:$G$31)&lt;=MAKSBELOP,E30,IF(SUM($D$30:$G$30)&lt;=MAKSBELOP,E30,ROUND(E30*ScalingFactor,0)))</f>
+        <v>252</v>
+      </c>
+      <c r="F33" s="38">
+        <f>IF(SUM($D$30:$G$31)&lt;=MAKSBELOP,F30,IF(SUM($D$30:$G$30)&lt;=MAKSBELOP,F30,ROUND(F30*ScalingFactor,0)))</f>
+        <v>55</v>
+      </c>
+      <c r="G33" s="38">
+        <f>IF(SUM($D$30:$G$31)&lt;=MAKSBELOP,G30,IF(SUM($D$30:$G$30)&lt;=MAKSBELOP,G30,ROUND(G30*ScalingFactor,0)))</f>
+        <v>0</v>
+      </c>
+      <c r="H33" s="41" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" s="37" t="s">
+        <v>32</v>
+      </c>
+      <c r="B34" s="38" t="s">
+        <v>15</v>
+      </c>
+      <c r="C34" s="38"/>
+      <c r="D34" s="38">
+        <f>IF(SUM($D$30:$G$31)&lt;=MAKSBELOP,D31,IF(SUM($D$30:$G$30)&lt;=MAKSBELOP,ROUND(D31*ScalingFactor,0),0))</f>
+        <v>0</v>
+      </c>
+      <c r="E34" s="38">
+        <f>IF(SUM($D$30:$G$31)&lt;=MAKSBELOP,E31,IF(SUM($D$30:$G$30)&lt;=MAKSBELOP,ROUND(E31*ScalingFactor,0),0))</f>
+        <v>0</v>
+      </c>
+      <c r="F34" s="38">
+        <f>IF(SUM($D$30:$G$31)&lt;=MAKSBELOP,F31,IF(SUM($D$30:$G$30)&lt;=MAKSBELOP,ROUND(F31*ScalingFactor,0),0))</f>
+        <v>0</v>
+      </c>
+      <c r="G34" s="38">
+        <f>IF(SUM($D$30:$G$31)&lt;=MAKSBELOP,G31,IF(SUM($D$30:$G$30)&lt;=MAKSBELOP,ROUND(G31*ScalingFactor,0),0))</f>
+        <v>0</v>
+      </c>
+      <c r="H34" s="41" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="B39" s="24">
+        <v>1430.76</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="B34" s="24">
-        <v>1430.76</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="B35" s="24">
-        <f>ROUND(B34*260/12,0)</f>
+      <c r="B40" s="24">
+        <f>ROUND(B39*260/12,0)</f>
         <v>31000</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C32:G32"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed Person calculation bug in spreadsheet
</commit_message>
<xml_diff>
--- a/doc/okonomi/Utbetaling.xlsx
+++ b/doc/okonomi/Utbetaling.xlsx
@@ -5,13 +5,13 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fred/src/nav/helse-spleis/doc/okonomi/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fred/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5E2AE42-9FBB-C44D-82C6-8ADEA7B8FCAC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4128D7AA-40ED-E345-B4A4-AA1BFC1EBAC4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2020" yWindow="860" windowWidth="20220" windowHeight="14600" xr2:uid="{BB3196D1-BBA6-4B4B-8E55-37C48C2FF3A4}"/>
-    <workbookView xWindow="22440" yWindow="840" windowWidth="25260" windowHeight="16940" activeTab="1" xr2:uid="{84B3C1EA-5610-F945-853C-C9E087DDC0A8}"/>
+    <workbookView xWindow="2020" yWindow="860" windowWidth="27900" windowHeight="18840" xr2:uid="{BB3196D1-BBA6-4B4B-8E55-37C48C2FF3A4}"/>
+    <workbookView xWindow="32120" yWindow="1000" windowWidth="31580" windowHeight="23740" activeTab="1" xr2:uid="{84B3C1EA-5610-F945-853C-C9E087DDC0A8}"/>
   </bookViews>
   <sheets>
     <sheet name="Terminology" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,8 @@
   </sheets>
   <definedNames>
     <definedName name="AdjustmentArb">'Multiple Employers'!$D$23:$G$23</definedName>
+    <definedName name="MAKSBELOP">'Multiple Employers'!$C$15</definedName>
+    <definedName name="PersonRemainder">'Multiple Employers'!$C$34</definedName>
     <definedName name="ScalingFactor">'Multiple Employers'!$C$16</definedName>
     <definedName name="ShortfallIncomeRatioArb">'Multiple Employers'!$D$20:$G$20</definedName>
     <definedName name="ShortfallIncomeRatioPerson">'Multiple Employers'!$D$24:$G$24</definedName>
@@ -41,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="80">
   <si>
     <t>Term</t>
   </si>
@@ -50,9 +52,6 @@
   </si>
   <si>
     <t>Example</t>
-  </si>
-  <si>
-    <t>Format</t>
   </si>
   <si>
     <t>Integer</t>
@@ -283,6 +282,27 @@
   </si>
   <si>
     <t>Shortfall ratio - person</t>
+  </si>
+  <si>
+    <t>Precision</t>
+  </si>
+  <si>
+    <t>Ideal arbeidsgiver w/o 6G</t>
+  </si>
+  <si>
+    <t>Ideal person w/o 6G</t>
+  </si>
+  <si>
+    <t>Situation</t>
+  </si>
+  <si>
+    <t>Arbeidsgiverbeløp før 6g</t>
+  </si>
+  <si>
+    <t>Personbeløp før 6g</t>
+  </si>
+  <si>
+    <t>Remainder for employees</t>
   </si>
 </sst>
 </file>
@@ -335,7 +355,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -366,13 +386,34 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -381,7 +422,7 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -424,7 +465,30 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="6" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -745,8 +809,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{336B5C91-C43F-4BAE-BFBA-00152852E840}">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
@@ -767,13 +831,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -781,13 +845,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D3" s="11">
         <v>20000</v>
@@ -796,74 +860,74 @@
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D4" s="2">
         <f>D3*12/260</f>
         <v>923.07692307692309</v>
       </c>
       <c r="E4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D5" s="11">
         <v>80</v>
       </c>
       <c r="E5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
       <c r="B6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D6" s="2">
         <f>D4*ROUND(D5,0)/100</f>
         <v>738.46153846153845</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s">
         <v>25</v>
       </c>
-      <c r="B7" t="s">
-        <v>26</v>
-      </c>
       <c r="C7" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D7" s="11">
         <v>60</v>
       </c>
       <c r="E7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="4"/>
       <c r="B8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D8" s="2">
         <f>D6*D7/100</f>
@@ -872,13 +936,13 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D9" s="11">
         <v>93634</v>
@@ -889,47 +953,47 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D10" s="2">
         <f>6*D9/260</f>
         <v>2160.7846153846153</v>
       </c>
       <c r="E10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
       <c r="B11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D11" s="1">
         <f>ROUND(ROUND(D7,0)*D10/100,0)</f>
         <v>1296</v>
       </c>
       <c r="E11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D12" s="2">
         <f>MIN(D8,D11)</f>
@@ -939,28 +1003,28 @@
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D13" s="18">
         <f>100*2/3</f>
         <v>66.666666666666671</v>
       </c>
       <c r="E13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D14" s="9">
         <f>ROUND(D12*D13/100, 0)</f>
@@ -969,29 +1033,29 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D15" s="9">
         <f>ROUND(D12,0)-D14</f>
         <v>148</v>
       </c>
       <c r="E15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
       <c r="B16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D16" s="2">
         <f>D12-D14-D15</f>
@@ -1001,17 +1065,17 @@
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
       <c r="B17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D17" s="2">
         <f>D16*260</f>
         <v>19.999999999989768</v>
       </c>
       <c r="E17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -1025,19 +1089,19 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B21" s="14"/>
       <c r="C21" s="15"/>
       <c r="D21" s="16"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="B22" s="28"/>
-      <c r="C22" s="28"/>
-      <c r="D22" s="28"/>
+      <c r="A22" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="42"/>
+      <c r="C22" s="42"/>
+      <c r="D22" s="42"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
@@ -1051,13 +1115,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBE9F233-0C57-4B39-8C81-6D2F9F1844A9}">
-  <dimension ref="A1:H35"/>
+  <dimension ref="A1:H41"/>
   <sheetViews>
     <sheetView zoomScale="163" zoomScaleNormal="163" workbookViewId="0">
       <selection activeCell="A24" sqref="A24"/>
     </sheetView>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="1">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="1">
+      <pane xSplit="8" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="I1" sqref="I1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="D33" sqref="D33:G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1080,22 +1147,22 @@
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D1" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="8" t="s">
-        <v>24</v>
-      </c>
       <c r="H1" s="8" t="s">
-        <v>3</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -1103,10 +1170,10 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D3" s="11">
         <v>21000</v>
@@ -1121,40 +1188,40 @@
         <v>0</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D4" s="21">
+        <v>55</v>
+      </c>
+      <c r="D4" s="28">
         <f>D3/SUM($D$3:$G$3)</f>
         <v>0.33870967741935482</v>
       </c>
-      <c r="E4" s="21">
+      <c r="E4" s="28">
         <f t="shared" ref="E4:G4" si="0">E3/SUM($D$3:$G$3)</f>
         <v>0.16129032258064516</v>
       </c>
-      <c r="F4" s="21">
+      <c r="F4" s="28">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="G4" s="21">
+      <c r="G4" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="27" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D5" s="2">
         <f>D3*12/260</f>
@@ -1173,15 +1240,15 @@
         <v>0</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D6" s="20">
         <v>1</v>
@@ -1196,15 +1263,15 @@
         <v>1</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D7" s="2">
         <f>D5*D6</f>
@@ -1223,21 +1290,21 @@
         <v>0</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" t="s">
         <v>25</v>
-      </c>
-      <c r="B8" t="s">
-        <v>26</v>
       </c>
       <c r="D8" s="21">
         <v>0.5</v>
       </c>
       <c r="E8" s="21">
-        <v>0.8</v>
+        <v>0.1</v>
       </c>
       <c r="F8" s="21">
         <v>0.2</v>
@@ -1246,15 +1313,15 @@
         <v>1</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D9" s="2">
         <f>D7*D8</f>
@@ -1262,7 +1329,7 @@
       </c>
       <c r="E9" s="2">
         <f t="shared" ref="E9:G9" si="2">E7*E8</f>
-        <v>369.23076923076928</v>
+        <v>46.15384615384616</v>
       </c>
       <c r="F9" s="2">
         <f t="shared" si="2"/>
@@ -1273,21 +1340,21 @@
         <v>0</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D10" s="20">
         <v>1</v>
       </c>
       <c r="E10" s="20">
-        <v>0.9</v>
+        <v>0.1</v>
       </c>
       <c r="F10" s="20">
         <v>0.25</v>
@@ -1296,15 +1363,15 @@
         <v>1</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D11" s="17">
         <f>D9*D10</f>
@@ -1312,7 +1379,7 @@
       </c>
       <c r="E11" s="17">
         <f t="shared" ref="E11:G11" si="3">E9*E10</f>
-        <v>332.30769230769238</v>
+        <v>4.6153846153846159</v>
       </c>
       <c r="F11" s="17">
         <f t="shared" si="3"/>
@@ -1323,389 +1390,562 @@
         <v>0</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C12" s="19">
         <f>ROUND(SUM(D9:G9)/SUM(D7:G7),2)</f>
-        <v>0.4</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C13" s="11">
         <v>93634</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C14" s="2">
         <f>6*C13/260</f>
         <v>2160.7846153846153</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C15" s="1">
         <f>C12*C14</f>
-        <v>864.31384615384616</v>
+        <v>626.62753846153839</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C16" s="22">
         <f>MIN(1, C15/SUM(D9:G9))</f>
-        <v>0.75817004048582992</v>
+        <v>0.76705819209039539</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B17" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17" s="17">
+      <c r="A17" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="30"/>
+      <c r="D17" s="31">
         <f>D9*ScalingFactor</f>
-        <v>367.42086577390222</v>
-      </c>
-      <c r="E17" s="17">
+        <v>371.72820078226857</v>
+      </c>
+      <c r="E17" s="31">
         <f>E9*ScalingFactor</f>
-        <v>279.93970725630646</v>
-      </c>
-      <c r="F17" s="17">
+        <v>35.402685788787487</v>
+      </c>
+      <c r="F17" s="31">
         <f>F9*ScalingFactor</f>
-        <v>216.95327312363747</v>
-      </c>
-      <c r="G17" s="17">
+        <v>219.49665189048235</v>
+      </c>
+      <c r="G17" s="31">
         <f>G9*ScalingFactor</f>
         <v>0</v>
       </c>
-      <c r="H17" s="3" t="s">
-        <v>5</v>
+      <c r="H17" s="32" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="B18" t="s">
-        <v>45</v>
-      </c>
-      <c r="D18" s="17">
+      <c r="A18" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="B18" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="30"/>
+      <c r="D18" s="31">
         <f>MIN(D17,D11)</f>
-        <v>367.42086577390222</v>
-      </c>
-      <c r="E18" s="17">
+        <v>371.72820078226857</v>
+      </c>
+      <c r="E18" s="31">
         <f t="shared" ref="E18:G18" si="4">MIN(E17,E11)</f>
-        <v>279.93970725630646</v>
-      </c>
-      <c r="F18" s="17">
+        <v>4.6153846153846159</v>
+      </c>
+      <c r="F18" s="31">
         <f t="shared" si="4"/>
         <v>71.538461538461533</v>
       </c>
-      <c r="G18" s="17">
+      <c r="G18" s="31">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="H18" s="3" t="s">
-        <v>5</v>
+      <c r="H18" s="32" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" s="4"/>
-      <c r="B19" t="s">
-        <v>48</v>
-      </c>
-      <c r="D19" s="17">
+      <c r="A19" s="29"/>
+      <c r="B19" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" s="30"/>
+      <c r="D19" s="31">
         <f>D18-D11</f>
-        <v>-117.19451884148242</v>
-      </c>
-      <c r="E19" s="17">
+        <v>-112.88718383311607</v>
+      </c>
+      <c r="E19" s="31">
         <f t="shared" ref="E19:G19" si="5">E18-E11</f>
-        <v>-52.367985051385915</v>
-      </c>
-      <c r="F19" s="17">
+        <v>0</v>
+      </c>
+      <c r="F19" s="31">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="G19" s="17">
+      <c r="G19" s="31">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="H19" s="3" t="s">
-        <v>5</v>
+      <c r="H19" s="32" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" s="4"/>
-      <c r="B20" t="s">
-        <v>71</v>
-      </c>
-      <c r="D20" s="19">
+      <c r="A20" s="29"/>
+      <c r="B20" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20" s="30"/>
+      <c r="D20" s="33">
         <f>IF(D19 &lt; 0, D4, 0)</f>
         <v>0.33870967741935482</v>
       </c>
-      <c r="E20" s="19">
+      <c r="E20" s="33">
         <f t="shared" ref="E20:F20" si="6">IF(E19 &lt; 0, E4, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="F20" s="33">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="G20" s="31"/>
+      <c r="H20" s="32" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="B21" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="C21" s="30"/>
+      <c r="D21" s="33">
+        <f>IF(SUM(ShortfallIncomeRatioArb)=0,0,D20/SUM(ShortfallIncomeRatioArb))</f>
+        <v>1</v>
+      </c>
+      <c r="E21" s="33">
+        <f>IF(SUM(ShortfallIncomeRatioArb)=0,0,E20/SUM(ShortfallIncomeRatioArb))</f>
+        <v>0</v>
+      </c>
+      <c r="F21" s="33">
+        <f>IF(SUM(ShortfallIncomeRatioArb)=0,0,F20/SUM(ShortfallIncomeRatioArb))</f>
+        <v>0</v>
+      </c>
+      <c r="G21" s="33">
+        <f>IF(SUM(ShortfallIncomeRatioArb)=0,0,G20/SUM(ShortfallIncomeRatioArb))</f>
+        <v>0</v>
+      </c>
+      <c r="H21" s="32" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="29"/>
+      <c r="B22" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" s="30"/>
+      <c r="D22" s="31">
+        <f>D17-D18</f>
+        <v>0</v>
+      </c>
+      <c r="E22" s="31">
+        <f>E17-E18</f>
+        <v>30.78730117340287</v>
+      </c>
+      <c r="F22" s="31">
+        <f>F17-F18</f>
+        <v>147.95819035202084</v>
+      </c>
+      <c r="G22" s="31">
+        <f>G17-G18</f>
+        <v>0</v>
+      </c>
+      <c r="H22" s="32" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="B23" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23" s="30"/>
+      <c r="D23" s="31">
+        <f>MIN(-D19,IF(SUM($D$19:$G$19)&gt;=0, 0, SUM($D$22:$G$22)*D21))</f>
+        <v>112.88718383311607</v>
+      </c>
+      <c r="E23" s="31">
+        <f t="shared" ref="E23:G23" si="7">MIN(-E19,IF(SUM($D$19:$G$19)&gt;=0, 0, SUM($D$22:$G$22)*E21))</f>
+        <v>0</v>
+      </c>
+      <c r="F23" s="31">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="G23" s="31">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="H23" s="32" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="29"/>
+      <c r="B24" s="30" t="s">
+        <v>69</v>
+      </c>
+      <c r="C24" s="30"/>
+      <c r="D24" s="33">
+        <f>IF(D22 = 0, 0, D4)</f>
+        <v>0</v>
+      </c>
+      <c r="E24" s="33">
+        <f t="shared" ref="E24:G24" si="8">IF(E22 = 0, 0, E4)</f>
         <v>0.16129032258064516</v>
       </c>
-      <c r="F20" s="19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="G20" s="17"/>
-      <c r="H20" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="B21" t="s">
-        <v>72</v>
-      </c>
-      <c r="D21" s="19">
-        <f>IF(SUM(ShortfallIncomeRatioArb)=0,0,D20/SUM(ShortfallIncomeRatioArb))</f>
-        <v>0.67741935483870963</v>
-      </c>
-      <c r="E21" s="19">
-        <f>IF(SUM(ShortfallIncomeRatioArb)=0,0,E20/SUM(ShortfallIncomeRatioArb))</f>
-        <v>0.32258064516129031</v>
-      </c>
-      <c r="F21" s="19">
-        <f>IF(SUM(ShortfallIncomeRatioArb)=0,0,F20/SUM(ShortfallIncomeRatioArb))</f>
-        <v>0</v>
-      </c>
-      <c r="G21" s="19">
-        <f>IF(SUM(ShortfallIncomeRatioArb)=0,0,G20/SUM(ShortfallIncomeRatioArb))</f>
-        <v>0</v>
-      </c>
-      <c r="H21" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" s="4"/>
-      <c r="B22" t="s">
-        <v>46</v>
-      </c>
-      <c r="D22" s="17">
-        <f>D17-D18</f>
-        <v>0</v>
-      </c>
-      <c r="E22" s="17">
-        <f>E17-E18</f>
-        <v>0</v>
-      </c>
-      <c r="F22" s="17">
-        <f>F17-F18</f>
-        <v>145.41481158517593</v>
-      </c>
-      <c r="G22" s="17">
-        <f>G17-G18</f>
-        <v>0</v>
-      </c>
-      <c r="H22" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="B23" t="s">
-        <v>49</v>
-      </c>
-      <c r="D23" s="17">
-        <f>MIN(-D19,IF(SUM($D$19:$G$19)&gt;=0, 0, SUM($D$22:$G$22)*D21))</f>
-        <v>98.50680784802239</v>
-      </c>
-      <c r="E23" s="17">
-        <f t="shared" ref="E23:G23" si="7">MIN(-E19,IF(SUM($D$19:$G$19)&gt;=0, 0, SUM($D$22:$G$22)*E21))</f>
-        <v>46.908003737153521</v>
-      </c>
-      <c r="F23" s="17">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="G23" s="17">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="H23" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" s="4"/>
-      <c r="B24" t="s">
-        <v>70</v>
-      </c>
-      <c r="D24" s="19">
-        <f>IF(D22 = 0, 0, D4)</f>
-        <v>0</v>
-      </c>
-      <c r="E24" s="19">
-        <f t="shared" ref="E24:G24" si="8">IF(E22 = 0, 0, E4)</f>
-        <v>0</v>
-      </c>
-      <c r="F24" s="19">
+      <c r="F24" s="33">
         <f t="shared" si="8"/>
         <v>0.5</v>
       </c>
-      <c r="G24" s="19">
+      <c r="G24" s="33">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
+      <c r="H24" s="32" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" s="4"/>
-      <c r="B25" t="s">
-        <v>73</v>
-      </c>
-      <c r="D25" s="19">
+      <c r="A25" s="29"/>
+      <c r="B25" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="C25" s="30"/>
+      <c r="D25" s="33">
         <f>IF(SUM(ShortfallIncomeRatioPerson)= 0, 0, D24/SUM(ShortfallIncomeRatioPerson))</f>
         <v>0</v>
       </c>
-      <c r="E25" s="19">
+      <c r="E25" s="33">
         <f>IF(SUM(ShortfallIncomeRatioPerson)= 0, 0, E24/SUM(ShortfallIncomeRatioPerson))</f>
-        <v>0</v>
-      </c>
-      <c r="F25" s="19">
+        <v>0.24390243902439024</v>
+      </c>
+      <c r="F25" s="33">
         <f>IF(SUM(ShortfallIncomeRatioPerson)= 0, 0, F24/SUM(ShortfallIncomeRatioPerson))</f>
-        <v>1</v>
-      </c>
-      <c r="G25" s="19">
+        <v>0.75609756097560976</v>
+      </c>
+      <c r="G25" s="33">
         <f>IF(SUM(ShortfallIncomeRatioPerson)= 0, 0, G24/SUM(ShortfallIncomeRatioPerson))</f>
         <v>0</v>
       </c>
+      <c r="H25" s="32" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B26" t="s">
-        <v>15</v>
-      </c>
-      <c r="D26" s="1">
+      <c r="A26" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" s="30"/>
+      <c r="D26" s="34">
         <f>ROUND(D18+D23,0)</f>
-        <v>466</v>
-      </c>
-      <c r="E26" s="1">
+        <v>485</v>
+      </c>
+      <c r="E26" s="34">
         <f t="shared" ref="E26:G26" si="9">ROUND(E18+E23,0)</f>
-        <v>327</v>
-      </c>
-      <c r="F26" s="1">
+        <v>5</v>
+      </c>
+      <c r="F26" s="34">
         <f t="shared" si="9"/>
         <v>72</v>
       </c>
-      <c r="G26" s="17">
+      <c r="G26" s="31">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="H26" s="3" t="s">
-        <v>4</v>
+      <c r="H26" s="32" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B27" t="s">
-        <v>16</v>
-      </c>
-      <c r="D27">
+      <c r="A27" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="B27" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" s="30"/>
+      <c r="D27" s="30">
         <f>ROUND(D22-SUM(AdjustmentArb)*D25,0)</f>
         <v>0</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="30">
         <f>ROUND(E22-SUM(AdjustmentArb)*E25,0)</f>
-        <v>0</v>
-      </c>
-      <c r="F27">
+        <v>3</v>
+      </c>
+      <c r="F27" s="30">
         <f>ROUND(F22-SUM(AdjustmentArb)*F25,0)</f>
-        <v>0</v>
-      </c>
-      <c r="G27">
+        <v>63</v>
+      </c>
+      <c r="G27" s="30">
         <f>ROUND(G22-SUM(AdjustmentArb)*G25,0)</f>
         <v>0</v>
       </c>
+      <c r="H27" s="32" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" s="4"/>
-      <c r="B28" t="s">
-        <v>18</v>
-      </c>
-      <c r="C28" s="26">
+      <c r="A28" s="29"/>
+      <c r="B28" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28" s="35">
         <f>C15-SUM(D26:G27)</f>
-        <v>-0.68615384615384301</v>
+        <v>-1.3724615384616072</v>
+      </c>
+      <c r="D28" s="30"/>
+      <c r="E28" s="30"/>
+      <c r="F28" s="30"/>
+      <c r="G28" s="30"/>
+      <c r="H28" s="32" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="4"/>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" s="23" t="s">
+      <c r="C29" s="26"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="36" t="s">
+        <v>77</v>
+      </c>
+      <c r="B30" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="C30" s="38"/>
+      <c r="D30" s="39">
+        <f>ROUND(D9*D10, 0)</f>
+        <v>485</v>
+      </c>
+      <c r="E30" s="39">
+        <f t="shared" ref="E30:G30" si="10">ROUND(E9*E10, 0)</f>
+        <v>5</v>
+      </c>
+      <c r="F30" s="39">
+        <f t="shared" si="10"/>
+        <v>72</v>
+      </c>
+      <c r="G30" s="39">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="H30" s="40" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="36" t="s">
+        <v>78</v>
+      </c>
+      <c r="B31" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="C31" s="38"/>
+      <c r="D31" s="39">
+        <f>ROUND(D9,0) - D30</f>
+        <v>0</v>
+      </c>
+      <c r="E31" s="39">
+        <f t="shared" ref="E31:G31" si="11">ROUND(E9,0) - E30</f>
+        <v>41</v>
+      </c>
+      <c r="F31" s="39">
+        <f t="shared" si="11"/>
+        <v>214</v>
+      </c>
+      <c r="G31" s="39">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="H31" s="40" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="36"/>
+      <c r="B32" s="41" t="s">
+        <v>76</v>
+      </c>
+      <c r="C32" s="43" t="str">
+        <f>IF(SUM(D30:G31)&lt;=MAKSBELOP,"Everyone paid",IF(SUM(D30:G30)&lt;=MAKSBELOP,"Arbeidsgivere fully paid; Person partially paid by Dekningsfaktor", "Arbeidsgivere partial payment only by Dekningsfaktor"))</f>
+        <v>Arbeidsgivere fully paid; Person partially paid by Dekningsfaktor</v>
+      </c>
+      <c r="D32" s="43"/>
+      <c r="E32" s="43"/>
+      <c r="F32" s="43"/>
+      <c r="G32" s="43"/>
+      <c r="H32" s="40"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="B33" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="C33" s="38"/>
+      <c r="D33" s="37">
+        <f>IF(SUM($D$30:$G$31)&lt;=MAKSBELOP,D30,IF(SUM($D$30:$G$30)&lt;=MAKSBELOP,D30,ROUND(D30*ScalingFactor,0)))</f>
+        <v>485</v>
+      </c>
+      <c r="E33" s="37">
+        <f>IF(SUM($D$30:$G$31)&lt;=MAKSBELOP,E30,IF(SUM($D$30:$G$30)&lt;=MAKSBELOP,E30,ROUND(E30*ScalingFactor,0)))</f>
+        <v>5</v>
+      </c>
+      <c r="F33" s="37">
+        <f>IF(SUM($D$30:$G$31)&lt;=MAKSBELOP,F30,IF(SUM($D$30:$G$30)&lt;=MAKSBELOP,F30,ROUND(F30*ScalingFactor,0)))</f>
+        <v>72</v>
+      </c>
+      <c r="G33" s="37">
+        <f>IF(SUM($D$30:$G$31)&lt;=MAKSBELOP,G30,IF(SUM($D$30:$G$30)&lt;=MAKSBELOP,G30,ROUND(G30*ScalingFactor,0)))</f>
+        <v>0</v>
+      </c>
+      <c r="H33" s="40" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" s="36"/>
+      <c r="B34" s="37" t="s">
+        <v>79</v>
+      </c>
+      <c r="C34" s="38">
+        <f>MAKSBELOP-SUM(D33:G33)</f>
+        <v>64.627538461538393</v>
+      </c>
+      <c r="D34" s="37"/>
+      <c r="E34" s="37"/>
+      <c r="F34" s="37"/>
+      <c r="G34" s="37"/>
+      <c r="H34" s="40"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="B35" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="C35" s="37"/>
+      <c r="D35" s="37">
+        <f>ROUND(PersonRemainder*D31/SUM($D$31:$G$31),0)</f>
+        <v>0</v>
+      </c>
+      <c r="E35" s="37">
+        <f>ROUND(PersonRemainder*E31/SUM($D$31:$G$31),0)</f>
+        <v>10</v>
+      </c>
+      <c r="F35" s="37">
+        <f>ROUND(PersonRemainder*F31/SUM($D$31:$G$31),0)</f>
+        <v>54</v>
+      </c>
+      <c r="G35" s="37">
+        <f>ROUND(PersonRemainder*G31/SUM($D$31:$G$31),0)</f>
+        <v>0</v>
+      </c>
+      <c r="H35" s="40" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="B40" s="24">
+        <v>1430.76</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="B34" s="24">
-        <v>1430.76</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="B35" s="24">
-        <f>ROUND(B34*260/12,0)</f>
+      <c r="B41" s="24">
+        <f>ROUND(B40*260/12,0)</f>
         <v>31000</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C32:G32"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Arbeidsgiverbelop bug in spreadsheet
</commit_message>
<xml_diff>
--- a/doc/okonomi/Utbetaling.xlsx
+++ b/doc/okonomi/Utbetaling.xlsx
@@ -5,13 +5,13 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fred/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fred/src/nav/helse-spleis/doc/okonomi/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4128D7AA-40ED-E345-B4A4-AA1BFC1EBAC4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59F8D189-477F-6442-BB3E-DFD8F9B51C8D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2020" yWindow="860" windowWidth="27900" windowHeight="18840" xr2:uid="{BB3196D1-BBA6-4B4B-8E55-37C48C2FF3A4}"/>
-    <workbookView xWindow="32120" yWindow="1000" windowWidth="31580" windowHeight="23740" activeTab="1" xr2:uid="{84B3C1EA-5610-F945-853C-C9E087DDC0A8}"/>
+    <workbookView xWindow="30700" yWindow="880" windowWidth="32120" windowHeight="22420" activeTab="1" xr2:uid="{4751B54A-2E15-734D-9A93-8E38B5748ECD}"/>
   </bookViews>
   <sheets>
     <sheet name="Terminology" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="80">
   <si>
     <t>Term</t>
   </si>
@@ -1120,11 +1120,8 @@
     <sheetView zoomScale="163" zoomScaleNormal="163" workbookViewId="0">
       <selection activeCell="A24" sqref="A24"/>
     </sheetView>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="1">
-      <pane xSplit="8" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I1" sqref="I1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D33" sqref="D33:G35"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="1">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1304,7 +1301,7 @@
         <v>0.5</v>
       </c>
       <c r="E8" s="21">
-        <v>0.1</v>
+        <v>0.8</v>
       </c>
       <c r="F8" s="21">
         <v>0.2</v>
@@ -1329,7 +1326,7 @@
       </c>
       <c r="E9" s="2">
         <f t="shared" ref="E9:G9" si="2">E7*E8</f>
-        <v>46.15384615384616</v>
+        <v>369.23076923076928</v>
       </c>
       <c r="F9" s="2">
         <f t="shared" si="2"/>
@@ -1354,7 +1351,7 @@
         <v>1</v>
       </c>
       <c r="E10" s="20">
-        <v>0.1</v>
+        <v>0.9</v>
       </c>
       <c r="F10" s="20">
         <v>0.25</v>
@@ -1379,7 +1376,7 @@
       </c>
       <c r="E11" s="17">
         <f t="shared" ref="E11:G11" si="3">E9*E10</f>
-        <v>4.6153846153846159</v>
+        <v>332.30769230769238</v>
       </c>
       <c r="F11" s="17">
         <f t="shared" si="3"/>
@@ -1402,7 +1399,7 @@
       </c>
       <c r="C12" s="19">
         <f>ROUND(SUM(D9:G9)/SUM(D7:G7),2)</f>
-        <v>0.28999999999999998</v>
+        <v>0.4</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>3</v>
@@ -1446,7 +1443,7 @@
       </c>
       <c r="C15" s="1">
         <f>C12*C14</f>
-        <v>626.62753846153839</v>
+        <v>864.31384615384616</v>
       </c>
       <c r="H15" s="3" t="s">
         <v>3</v>
@@ -1461,7 +1458,7 @@
       </c>
       <c r="C16" s="22">
         <f>MIN(1, C15/SUM(D9:G9))</f>
-        <v>0.76705819209039539</v>
+        <v>0.75817004048582992</v>
       </c>
       <c r="H16" s="3" t="s">
         <v>4</v>
@@ -1477,15 +1474,15 @@
       <c r="C17" s="30"/>
       <c r="D17" s="31">
         <f>D9*ScalingFactor</f>
-        <v>371.72820078226857</v>
+        <v>367.42086577390222</v>
       </c>
       <c r="E17" s="31">
         <f>E9*ScalingFactor</f>
-        <v>35.402685788787487</v>
+        <v>279.93970725630646</v>
       </c>
       <c r="F17" s="31">
         <f>F9*ScalingFactor</f>
-        <v>219.49665189048235</v>
+        <v>216.95327312363747</v>
       </c>
       <c r="G17" s="31">
         <f>G9*ScalingFactor</f>
@@ -1505,11 +1502,11 @@
       <c r="C18" s="30"/>
       <c r="D18" s="31">
         <f>MIN(D17,D11)</f>
-        <v>371.72820078226857</v>
+        <v>367.42086577390222</v>
       </c>
       <c r="E18" s="31">
         <f t="shared" ref="E18:G18" si="4">MIN(E17,E11)</f>
-        <v>4.6153846153846159</v>
+        <v>279.93970725630646</v>
       </c>
       <c r="F18" s="31">
         <f t="shared" si="4"/>
@@ -1531,11 +1528,11 @@
       <c r="C19" s="30"/>
       <c r="D19" s="31">
         <f>D18-D11</f>
-        <v>-112.88718383311607</v>
+        <v>-117.19451884148242</v>
       </c>
       <c r="E19" s="31">
         <f t="shared" ref="E19:G19" si="5">E18-E11</f>
-        <v>0</v>
+        <v>-52.367985051385915</v>
       </c>
       <c r="F19" s="31">
         <f t="shared" si="5"/>
@@ -1561,7 +1558,7 @@
       </c>
       <c r="E20" s="33">
         <f t="shared" ref="E20:F20" si="6">IF(E19 &lt; 0, E4, 0)</f>
-        <v>0</v>
+        <v>0.16129032258064516</v>
       </c>
       <c r="F20" s="33">
         <f t="shared" si="6"/>
@@ -1582,11 +1579,11 @@
       <c r="C21" s="30"/>
       <c r="D21" s="33">
         <f>IF(SUM(ShortfallIncomeRatioArb)=0,0,D20/SUM(ShortfallIncomeRatioArb))</f>
-        <v>1</v>
+        <v>0.67741935483870963</v>
       </c>
       <c r="E21" s="33">
         <f>IF(SUM(ShortfallIncomeRatioArb)=0,0,E20/SUM(ShortfallIncomeRatioArb))</f>
-        <v>0</v>
+        <v>0.32258064516129031</v>
       </c>
       <c r="F21" s="33">
         <f>IF(SUM(ShortfallIncomeRatioArb)=0,0,F20/SUM(ShortfallIncomeRatioArb))</f>
@@ -1612,11 +1609,11 @@
       </c>
       <c r="E22" s="31">
         <f>E17-E18</f>
-        <v>30.78730117340287</v>
+        <v>0</v>
       </c>
       <c r="F22" s="31">
         <f>F17-F18</f>
-        <v>147.95819035202084</v>
+        <v>145.41481158517593</v>
       </c>
       <c r="G22" s="31">
         <f>G17-G18</f>
@@ -1636,11 +1633,11 @@
       <c r="C23" s="30"/>
       <c r="D23" s="31">
         <f>MIN(-D19,IF(SUM($D$19:$G$19)&gt;=0, 0, SUM($D$22:$G$22)*D21))</f>
-        <v>112.88718383311607</v>
+        <v>98.50680784802239</v>
       </c>
       <c r="E23" s="31">
         <f t="shared" ref="E23:G23" si="7">MIN(-E19,IF(SUM($D$19:$G$19)&gt;=0, 0, SUM($D$22:$G$22)*E21))</f>
-        <v>0</v>
+        <v>46.908003737153521</v>
       </c>
       <c r="F23" s="31">
         <f t="shared" si="7"/>
@@ -1666,7 +1663,7 @@
       </c>
       <c r="E24" s="33">
         <f t="shared" ref="E24:G24" si="8">IF(E22 = 0, 0, E4)</f>
-        <v>0.16129032258064516</v>
+        <v>0</v>
       </c>
       <c r="F24" s="33">
         <f t="shared" si="8"/>
@@ -1692,11 +1689,11 @@
       </c>
       <c r="E25" s="33">
         <f>IF(SUM(ShortfallIncomeRatioPerson)= 0, 0, E24/SUM(ShortfallIncomeRatioPerson))</f>
-        <v>0.24390243902439024</v>
+        <v>0</v>
       </c>
       <c r="F25" s="33">
         <f>IF(SUM(ShortfallIncomeRatioPerson)= 0, 0, F24/SUM(ShortfallIncomeRatioPerson))</f>
-        <v>0.75609756097560976</v>
+        <v>1</v>
       </c>
       <c r="G25" s="33">
         <f>IF(SUM(ShortfallIncomeRatioPerson)= 0, 0, G24/SUM(ShortfallIncomeRatioPerson))</f>
@@ -1716,11 +1713,11 @@
       <c r="C26" s="30"/>
       <c r="D26" s="34">
         <f>ROUND(D18+D23,0)</f>
-        <v>485</v>
+        <v>466</v>
       </c>
       <c r="E26" s="34">
         <f t="shared" ref="E26:G26" si="9">ROUND(E18+E23,0)</f>
-        <v>5</v>
+        <v>327</v>
       </c>
       <c r="F26" s="34">
         <f t="shared" si="9"/>
@@ -1748,11 +1745,11 @@
       </c>
       <c r="E27" s="30">
         <f>ROUND(E22-SUM(AdjustmentArb)*E25,0)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F27" s="30">
         <f>ROUND(F22-SUM(AdjustmentArb)*F25,0)</f>
-        <v>63</v>
+        <v>0</v>
       </c>
       <c r="G27" s="30">
         <f>ROUND(G22-SUM(AdjustmentArb)*G25,0)</f>
@@ -1769,7 +1766,7 @@
       </c>
       <c r="C28" s="35">
         <f>C15-SUM(D26:G27)</f>
-        <v>-1.3724615384616072</v>
+        <v>-0.68615384615384301</v>
       </c>
       <c r="D28" s="30"/>
       <c r="E28" s="30"/>
@@ -1797,7 +1794,7 @@
       </c>
       <c r="E30" s="39">
         <f t="shared" ref="E30:G30" si="10">ROUND(E9*E10, 0)</f>
-        <v>5</v>
+        <v>332</v>
       </c>
       <c r="F30" s="39">
         <f t="shared" si="10"/>
@@ -1825,7 +1822,7 @@
       </c>
       <c r="E31" s="39">
         <f t="shared" ref="E31:G31" si="11">ROUND(E9,0) - E30</f>
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F31" s="39">
         <f t="shared" si="11"/>
@@ -1845,8 +1842,8 @@
         <v>76</v>
       </c>
       <c r="C32" s="43" t="str">
-        <f>IF(SUM(D30:G31)&lt;=MAKSBELOP,"Everyone paid",IF(SUM(D30:G30)&lt;=MAKSBELOP,"Arbeidsgivere fully paid; Person partially paid by Dekningsfaktor", "Arbeidsgivere partial payment only by Dekningsfaktor"))</f>
-        <v>Arbeidsgivere fully paid; Person partially paid by Dekningsfaktor</v>
+        <f>IF(SUM(D30:G31)&lt;=MAKSBELOP,"Everyone paid",IF(SUM(D30:G30)&lt;=MAKSBELOP,"Arbeidsgivere fully paid; Person partially paid by Person request", "Arbeidsgivere partial payment ratio by Arbeidsgiver request"))</f>
+        <v>Arbeidsgivere partial payment ratio by Arbeidsgiver request</v>
       </c>
       <c r="D32" s="43"/>
       <c r="E32" s="43"/>
@@ -1863,33 +1860,33 @@
       </c>
       <c r="C33" s="38"/>
       <c r="D33" s="37">
-        <f>IF(SUM($D$30:$G$31)&lt;=MAKSBELOP,D30,IF(SUM($D$30:$G$30)&lt;=MAKSBELOP,D30,ROUND(D30*ScalingFactor,0)))</f>
-        <v>485</v>
+        <f>IF(SUM($D$30:$G$31)&lt;=MAKSBELOP,D30,IF(SUM($D$30:$G$30)&lt;=MAKSBELOP,D30,ROUND(D30*MAKSBELOP/SUM($D$30:$G$30),0)))</f>
+        <v>472</v>
       </c>
       <c r="E33" s="37">
-        <f>IF(SUM($D$30:$G$31)&lt;=MAKSBELOP,E30,IF(SUM($D$30:$G$30)&lt;=MAKSBELOP,E30,ROUND(E30*ScalingFactor,0)))</f>
-        <v>5</v>
+        <f>IF(SUM($D$30:$G$31)&lt;=MAKSBELOP,E30,IF(SUM($D$30:$G$30)&lt;=MAKSBELOP,E30,ROUND(E30*MAKSBELOP/SUM($D$30:$G$30),0)))</f>
+        <v>323</v>
       </c>
       <c r="F33" s="37">
-        <f>IF(SUM($D$30:$G$31)&lt;=MAKSBELOP,F30,IF(SUM($D$30:$G$30)&lt;=MAKSBELOP,F30,ROUND(F30*ScalingFactor,0)))</f>
-        <v>72</v>
+        <f>IF(SUM($D$30:$G$31)&lt;=MAKSBELOP,F30,IF(SUM($D$30:$G$30)&lt;=MAKSBELOP,F30,ROUND(F30*MAKSBELOP/SUM($D$30:$G$30),0)))</f>
+        <v>70</v>
       </c>
       <c r="G33" s="37">
-        <f>IF(SUM($D$30:$G$31)&lt;=MAKSBELOP,G30,IF(SUM($D$30:$G$30)&lt;=MAKSBELOP,G30,ROUND(G30*ScalingFactor,0)))</f>
+        <f>IF(SUM($D$30:$G$31)&lt;=MAKSBELOP,G30,IF(SUM($D$30:$G$30)&lt;=MAKSBELOP,G30,ROUND(G30*MAKSBELOP/SUM($D$30:$G$30),0)))</f>
         <v>0</v>
       </c>
       <c r="H33" s="40" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="36"/>
       <c r="B34" s="37" t="s">
         <v>79</v>
       </c>
       <c r="C34" s="38">
         <f>MAKSBELOP-SUM(D33:G33)</f>
-        <v>64.627538461538393</v>
+        <v>-0.68615384615384301</v>
       </c>
       <c r="D34" s="37"/>
       <c r="E34" s="37"/>
@@ -1906,22 +1903,39 @@
       </c>
       <c r="C35" s="37"/>
       <c r="D35" s="37">
-        <f>ROUND(PersonRemainder*D31/SUM($D$31:$G$31),0)</f>
+        <f>IF(SUM($D$30:$G$31)&lt;=MAKSBELOP,D31,IF(SUM($D$30:$G$30)&lt;=MAKSBELOP,ROUND(PersonRemainder*D31/SUM($D$31:$G$31),0),0))</f>
         <v>0</v>
       </c>
       <c r="E35" s="37">
-        <f>ROUND(PersonRemainder*E31/SUM($D$31:$G$31),0)</f>
-        <v>10</v>
+        <f>IF(SUM($D$30:$G$31)&lt;=MAKSBELOP,E31,IF(SUM($D$30:$G$30)&lt;=MAKSBELOP,ROUND(PersonRemainder*E31/SUM($D$31:$G$31),0),0))</f>
+        <v>0</v>
       </c>
       <c r="F35" s="37">
-        <f>ROUND(PersonRemainder*F31/SUM($D$31:$G$31),0)</f>
-        <v>54</v>
+        <f>IF(SUM($D$30:$G$31)&lt;=MAKSBELOP,F31,IF(SUM($D$30:$G$30)&lt;=MAKSBELOP,ROUND(PersonRemainder*F31/SUM($D$31:$G$31),0),0))</f>
+        <v>0</v>
       </c>
       <c r="G35" s="37">
-        <f>ROUND(PersonRemainder*G31/SUM($D$31:$G$31),0)</f>
+        <f>IF(SUM($D$30:$G$31)&lt;=MAKSBELOP,G31,IF(SUM($D$30:$G$30)&lt;=MAKSBELOP,ROUND(PersonRemainder*G31/SUM($D$31:$G$31),0),0))</f>
         <v>0</v>
       </c>
       <c r="H35" s="40" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" s="36"/>
+      <c r="B36" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="C36" s="38">
+        <f>MAKSBELOP-SUM(D33:G35)</f>
+        <v>-0.68615384615384301</v>
+      </c>
+      <c r="D36" s="37"/>
+      <c r="E36" s="37"/>
+      <c r="F36" s="37"/>
+      <c r="G36" s="37"/>
+      <c r="H36" s="40" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fikser avrunding av dagsats for 6G, og gradert dagsats av 6G
Co-authored-by: Morten Tholander <morten.tholander@gmail.com>
Co-authored-by: Stephen Ramthun <stephen.ramthun@nav.no>
</commit_message>
<xml_diff>
--- a/doc/okonomi/Utbetaling.xlsx
+++ b/doc/okonomi/Utbetaling.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fred/src/nav/helse-spleis/doc/okonomi/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/david/dev/nav/helse/monorepo/helse-spleis/doc/okonomi/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59F8D189-477F-6442-BB3E-DFD8F9B51C8D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7690AA5-68EF-9B49-B5B0-D23DD1727BCC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2020" yWindow="860" windowWidth="27900" windowHeight="18840" xr2:uid="{BB3196D1-BBA6-4B4B-8E55-37C48C2FF3A4}"/>
     <workbookView xWindow="30700" yWindow="880" windowWidth="32120" windowHeight="22420" activeTab="1" xr2:uid="{4751B54A-2E15-734D-9A93-8E38B5748ECD}"/>
@@ -1121,7 +1121,7 @@
       <selection activeCell="A24" sqref="A24"/>
     </sheetView>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="1">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1427,8 +1427,8 @@
         <v>29</v>
       </c>
       <c r="C14" s="2">
-        <f>6*C13/260</f>
-        <v>2160.7846153846153</v>
+        <f>ROUND(6*C13/260, 0)</f>
+        <v>2161</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>4</v>
@@ -1442,8 +1442,8 @@
         <v>41</v>
       </c>
       <c r="C15" s="1">
-        <f>C12*C14</f>
-        <v>864.31384615384616</v>
+        <f>ROUND(C12*C14,0)</f>
+        <v>864</v>
       </c>
       <c r="H15" s="3" t="s">
         <v>3</v>
@@ -1458,7 +1458,7 @@
       </c>
       <c r="C16" s="22">
         <f>MIN(1, C15/SUM(D9:G9))</f>
-        <v>0.75817004048582992</v>
+        <v>0.75789473684210529</v>
       </c>
       <c r="H16" s="3" t="s">
         <v>4</v>
@@ -1474,15 +1474,15 @@
       <c r="C17" s="30"/>
       <c r="D17" s="31">
         <f>D9*ScalingFactor</f>
-        <v>367.42086577390222</v>
+        <v>367.28744939271257</v>
       </c>
       <c r="E17" s="31">
         <f>E9*ScalingFactor</f>
-        <v>279.93970725630646</v>
+        <v>279.83805668016197</v>
       </c>
       <c r="F17" s="31">
         <f>F9*ScalingFactor</f>
-        <v>216.95327312363747</v>
+        <v>216.87449392712549</v>
       </c>
       <c r="G17" s="31">
         <f>G9*ScalingFactor</f>
@@ -1502,11 +1502,11 @@
       <c r="C18" s="30"/>
       <c r="D18" s="31">
         <f>MIN(D17,D11)</f>
-        <v>367.42086577390222</v>
+        <v>367.28744939271257</v>
       </c>
       <c r="E18" s="31">
         <f t="shared" ref="E18:G18" si="4">MIN(E17,E11)</f>
-        <v>279.93970725630646</v>
+        <v>279.83805668016197</v>
       </c>
       <c r="F18" s="31">
         <f t="shared" si="4"/>
@@ -1528,11 +1528,11 @@
       <c r="C19" s="30"/>
       <c r="D19" s="31">
         <f>D18-D11</f>
-        <v>-117.19451884148242</v>
+        <v>-117.32793522267207</v>
       </c>
       <c r="E19" s="31">
         <f t="shared" ref="E19:G19" si="5">E18-E11</f>
-        <v>-52.367985051385915</v>
+        <v>-52.469635627530408</v>
       </c>
       <c r="F19" s="31">
         <f t="shared" si="5"/>
@@ -1613,7 +1613,7 @@
       </c>
       <c r="F22" s="31">
         <f>F17-F18</f>
-        <v>145.41481158517593</v>
+        <v>145.33603238866397</v>
       </c>
       <c r="G22" s="31">
         <f>G17-G18</f>
@@ -1633,11 +1633,11 @@
       <c r="C23" s="30"/>
       <c r="D23" s="31">
         <f>MIN(-D19,IF(SUM($D$19:$G$19)&gt;=0, 0, SUM($D$22:$G$22)*D21))</f>
-        <v>98.50680784802239</v>
+        <v>98.453441295546554</v>
       </c>
       <c r="E23" s="31">
         <f t="shared" ref="E23:G23" si="7">MIN(-E19,IF(SUM($D$19:$G$19)&gt;=0, 0, SUM($D$22:$G$22)*E21))</f>
-        <v>46.908003737153521</v>
+        <v>46.882591093117405</v>
       </c>
       <c r="F23" s="31">
         <f t="shared" si="7"/>
@@ -1766,7 +1766,7 @@
       </c>
       <c r="C28" s="35">
         <f>C15-SUM(D26:G27)</f>
-        <v>-0.68615384615384301</v>
+        <v>-1</v>
       </c>
       <c r="D28" s="30"/>
       <c r="E28" s="30"/>
@@ -1861,7 +1861,7 @@
       <c r="C33" s="38"/>
       <c r="D33" s="37">
         <f>IF(SUM($D$30:$G$31)&lt;=MAKSBELOP,D30,IF(SUM($D$30:$G$30)&lt;=MAKSBELOP,D30,ROUND(D30*MAKSBELOP/SUM($D$30:$G$30),0)))</f>
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="E33" s="37">
         <f>IF(SUM($D$30:$G$31)&lt;=MAKSBELOP,E30,IF(SUM($D$30:$G$30)&lt;=MAKSBELOP,E30,ROUND(E30*MAKSBELOP/SUM($D$30:$G$30),0)))</f>
@@ -1886,7 +1886,7 @@
       </c>
       <c r="C34" s="38">
         <f>MAKSBELOP-SUM(D33:G33)</f>
-        <v>-0.68615384615384301</v>
+        <v>0</v>
       </c>
       <c r="D34" s="37"/>
       <c r="E34" s="37"/>
@@ -1929,7 +1929,7 @@
       </c>
       <c r="C36" s="38">
         <f>MAKSBELOP-SUM(D33:G35)</f>
-        <v>-0.68615384615384301</v>
+        <v>0</v>
       </c>
       <c r="D36" s="37"/>
       <c r="E36" s="37"/>

</xml_diff>

<commit_message>
Modified spreadsheet to round daily rate assuming 100% sickness; change NOT in code yet pending reviews
</commit_message>
<xml_diff>
--- a/doc/okonomi/Utbetaling.xlsx
+++ b/doc/okonomi/Utbetaling.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/david/dev/nav/helse/monorepo/helse-spleis/doc/okonomi/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fred/src/nav/helse-spleis/doc/okonomi/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7690AA5-68EF-9B49-B5B0-D23DD1727BCC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54C42ECC-7C73-F348-8A82-62D244FB0A7A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2020" yWindow="860" windowWidth="27900" windowHeight="18840" xr2:uid="{BB3196D1-BBA6-4B4B-8E55-37C48C2FF3A4}"/>
     <workbookView xWindow="30700" yWindow="880" windowWidth="32120" windowHeight="22420" activeTab="1" xr2:uid="{4751B54A-2E15-734D-9A93-8E38B5748ECD}"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="81">
   <si>
     <t>Term</t>
   </si>
@@ -304,6 +304,9 @@
   <si>
     <t>Remainder for employees</t>
   </si>
+  <si>
+    <t>New: Rounding assuming 100% sickness</t>
+  </si>
 </sst>
 </file>
 
@@ -315,7 +318,7 @@
     <numFmt numFmtId="166" formatCode="_(* #,##0.0000000000_);_(* \(#,##0.0000000000\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="167" formatCode="_(* #,##0.0000000000_);_(* \(#,##0.0000000000\);_(* &quot;-&quot;??????????_);_(@_)"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -350,6 +353,13 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -422,7 +432,7 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -491,6 +501,7 @@
     <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1115,13 +1126,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBE9F233-0C57-4B39-8C81-6D2F9F1844A9}">
-  <dimension ref="A1:H41"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView zoomScale="163" zoomScaleNormal="163" workbookViewId="0">
       <selection activeCell="A24" sqref="A24"/>
     </sheetView>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="1">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1136,7 +1147,7 @@
     <col min="8" max="8" width="8.6640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1162,10 +1173,10 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="4"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>64</v>
       </c>
@@ -1188,7 +1199,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" t="s">
         <v>55</v>
@@ -1213,34 +1224,37 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="27" t="s">
         <v>63</v>
       </c>
       <c r="B5" t="s">
         <v>52</v>
       </c>
-      <c r="D5" s="2">
-        <f>D3*12/260</f>
-        <v>969.23076923076928</v>
-      </c>
-      <c r="E5" s="2">
-        <f>E3*12/260</f>
-        <v>461.53846153846155</v>
-      </c>
-      <c r="F5" s="2">
-        <f>F3*12/260</f>
-        <v>1430.7692307692307</v>
-      </c>
-      <c r="G5" s="2">
-        <f>G3*12/260</f>
+      <c r="D5" s="1">
+        <f>ROUND(D3*12/260,0)</f>
+        <v>969</v>
+      </c>
+      <c r="E5" s="1">
+        <f t="shared" ref="E5:G5" si="1">ROUND(E3*12/260,0)</f>
+        <v>462</v>
+      </c>
+      <c r="F5" s="1">
+        <f t="shared" si="1"/>
+        <v>1431</v>
+      </c>
+      <c r="G5" s="1">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="I5" s="44" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>56</v>
       </c>
@@ -1263,7 +1277,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>57</v>
       </c>
@@ -1272,25 +1286,25 @@
       </c>
       <c r="D7" s="2">
         <f>D5*D6</f>
-        <v>969.23076923076928</v>
+        <v>969</v>
       </c>
       <c r="E7" s="2">
-        <f t="shared" ref="E7:G7" si="1">E5*E6</f>
-        <v>461.53846153846155</v>
+        <f t="shared" ref="E7:G7" si="2">E5*E6</f>
+        <v>462</v>
       </c>
       <c r="F7" s="2">
-        <f t="shared" si="1"/>
-        <v>1430.7692307692307</v>
+        <f t="shared" si="2"/>
+        <v>1431</v>
       </c>
       <c r="G7" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H7" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>24</v>
       </c>
@@ -1313,7 +1327,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>58</v>
       </c>
@@ -1322,25 +1336,25 @@
       </c>
       <c r="D9" s="2">
         <f>D7*D8</f>
-        <v>484.61538461538464</v>
+        <v>484.5</v>
       </c>
       <c r="E9" s="2">
-        <f t="shared" ref="E9:G9" si="2">E7*E8</f>
-        <v>369.23076923076928</v>
+        <f t="shared" ref="E9:G9" si="3">E7*E8</f>
+        <v>369.6</v>
       </c>
       <c r="F9" s="2">
-        <f t="shared" si="2"/>
-        <v>286.15384615384613</v>
+        <f t="shared" si="3"/>
+        <v>286.2</v>
       </c>
       <c r="G9" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H9" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>59</v>
       </c>
@@ -1363,7 +1377,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>60</v>
       </c>
@@ -1372,25 +1386,25 @@
       </c>
       <c r="D11" s="17">
         <f>D9*D10</f>
-        <v>484.61538461538464</v>
+        <v>484.5</v>
       </c>
       <c r="E11" s="17">
-        <f t="shared" ref="E11:G11" si="3">E9*E10</f>
-        <v>332.30769230769238</v>
+        <f t="shared" ref="E11:G11" si="4">E9*E10</f>
+        <v>332.64000000000004</v>
       </c>
       <c r="F11" s="17">
-        <f t="shared" si="3"/>
-        <v>71.538461538461533</v>
+        <f t="shared" si="4"/>
+        <v>71.55</v>
       </c>
       <c r="G11" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>61</v>
       </c>
@@ -1405,7 +1419,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>30</v>
       </c>
@@ -1419,7 +1433,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>27</v>
       </c>
@@ -1434,7 +1448,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>62</v>
       </c>
@@ -1449,7 +1463,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>65</v>
       </c>
@@ -1458,7 +1472,7 @@
       </c>
       <c r="C16" s="22">
         <f>MIN(1, C15/SUM(D9:G9))</f>
-        <v>0.75789473684210529</v>
+        <v>0.75769534333070243</v>
       </c>
       <c r="H16" s="3" t="s">
         <v>4</v>
@@ -1474,15 +1488,15 @@
       <c r="C17" s="30"/>
       <c r="D17" s="31">
         <f>D9*ScalingFactor</f>
-        <v>367.28744939271257</v>
+        <v>367.10339384372531</v>
       </c>
       <c r="E17" s="31">
         <f>E9*ScalingFactor</f>
-        <v>279.83805668016197</v>
+        <v>280.04419889502765</v>
       </c>
       <c r="F17" s="31">
         <f>F9*ScalingFactor</f>
-        <v>216.87449392712549</v>
+        <v>216.85240726124704</v>
       </c>
       <c r="G17" s="31">
         <f>G9*ScalingFactor</f>
@@ -1502,18 +1516,18 @@
       <c r="C18" s="30"/>
       <c r="D18" s="31">
         <f>MIN(D17,D11)</f>
-        <v>367.28744939271257</v>
+        <v>367.10339384372531</v>
       </c>
       <c r="E18" s="31">
-        <f t="shared" ref="E18:G18" si="4">MIN(E17,E11)</f>
-        <v>279.83805668016197</v>
+        <f t="shared" ref="E18:G18" si="5">MIN(E17,E11)</f>
+        <v>280.04419889502765</v>
       </c>
       <c r="F18" s="31">
-        <f t="shared" si="4"/>
-        <v>71.538461538461533</v>
+        <f t="shared" si="5"/>
+        <v>71.55</v>
       </c>
       <c r="G18" s="31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="H18" s="32" t="s">
@@ -1528,18 +1542,18 @@
       <c r="C19" s="30"/>
       <c r="D19" s="31">
         <f>D18-D11</f>
-        <v>-117.32793522267207</v>
+        <v>-117.39660615627469</v>
       </c>
       <c r="E19" s="31">
-        <f t="shared" ref="E19:G19" si="5">E18-E11</f>
-        <v>-52.469635627530408</v>
+        <f t="shared" ref="E19:G19" si="6">E18-E11</f>
+        <v>-52.595801104972395</v>
       </c>
       <c r="F19" s="31">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="G19" s="31">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H19" s="32" t="s">
@@ -1557,11 +1571,11 @@
         <v>0.33870967741935482</v>
       </c>
       <c r="E20" s="33">
-        <f t="shared" ref="E20:F20" si="6">IF(E19 &lt; 0, E4, 0)</f>
+        <f t="shared" ref="E20:F20" si="7">IF(E19 &lt; 0, E4, 0)</f>
         <v>0.16129032258064516</v>
       </c>
       <c r="F20" s="33">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G20" s="31"/>
@@ -1613,7 +1627,7 @@
       </c>
       <c r="F22" s="31">
         <f>F17-F18</f>
-        <v>145.33603238866397</v>
+        <v>145.30240726124703</v>
       </c>
       <c r="G22" s="31">
         <f>G17-G18</f>
@@ -1633,18 +1647,18 @@
       <c r="C23" s="30"/>
       <c r="D23" s="31">
         <f>MIN(-D19,IF(SUM($D$19:$G$19)&gt;=0, 0, SUM($D$22:$G$22)*D21))</f>
-        <v>98.453441295546554</v>
+        <v>98.430662983425393</v>
       </c>
       <c r="E23" s="31">
-        <f t="shared" ref="E23:G23" si="7">MIN(-E19,IF(SUM($D$19:$G$19)&gt;=0, 0, SUM($D$22:$G$22)*E21))</f>
-        <v>46.882591093117405</v>
+        <f t="shared" ref="E23:G23" si="8">MIN(-E19,IF(SUM($D$19:$G$19)&gt;=0, 0, SUM($D$22:$G$22)*E21))</f>
+        <v>46.87174427782162</v>
       </c>
       <c r="F23" s="31">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G23" s="31">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="H23" s="32" t="s">
@@ -1662,15 +1676,15 @@
         <v>0</v>
       </c>
       <c r="E24" s="33">
-        <f t="shared" ref="E24:G24" si="8">IF(E22 = 0, 0, E4)</f>
+        <f t="shared" ref="E24:G24" si="9">IF(E22 = 0, 0, E4)</f>
         <v>0</v>
       </c>
       <c r="F24" s="33">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.5</v>
       </c>
       <c r="G24" s="33">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H24" s="32" t="s">
@@ -1716,15 +1730,15 @@
         <v>466</v>
       </c>
       <c r="E26" s="34">
-        <f t="shared" ref="E26:G26" si="9">ROUND(E18+E23,0)</f>
+        <f t="shared" ref="E26:G26" si="10">ROUND(E18+E23,0)</f>
         <v>327</v>
       </c>
       <c r="F26" s="34">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>72</v>
       </c>
       <c r="G26" s="31">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="H26" s="32" t="s">
@@ -1793,15 +1807,15 @@
         <v>485</v>
       </c>
       <c r="E30" s="39">
-        <f t="shared" ref="E30:G30" si="10">ROUND(E9*E10, 0)</f>
-        <v>332</v>
+        <f t="shared" ref="E30:G30" si="11">ROUND(E9*E10, 0)</f>
+        <v>333</v>
       </c>
       <c r="F30" s="39">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>72</v>
       </c>
       <c r="G30" s="39">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="H30" s="40" t="s">
@@ -1821,15 +1835,15 @@
         <v>0</v>
       </c>
       <c r="E31" s="39">
-        <f t="shared" ref="E31:G31" si="11">ROUND(E9,0) - E30</f>
+        <f t="shared" ref="E31:G31" si="12">ROUND(E9,0) - E30</f>
         <v>37</v>
       </c>
       <c r="F31" s="39">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>214</v>
       </c>
       <c r="G31" s="39">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="H31" s="40" t="s">

</xml_diff>

<commit_message>
Removed terminology page; it has served its purpose, and is no longer useful
</commit_message>
<xml_diff>
--- a/doc/okonomi/Utbetaling.xlsx
+++ b/doc/okonomi/Utbetaling.xlsx
@@ -8,14 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fred/src/nav/helse-spleis/doc/okonomi/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54C42ECC-7C73-F348-8A82-62D244FB0A7A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04B3C38E-65D5-EA4B-8856-975C572E501F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2020" yWindow="860" windowWidth="27900" windowHeight="18840" xr2:uid="{BB3196D1-BBA6-4B4B-8E55-37C48C2FF3A4}"/>
-    <workbookView xWindow="30700" yWindow="880" windowWidth="32120" windowHeight="22420" activeTab="1" xr2:uid="{4751B54A-2E15-734D-9A93-8E38B5748ECD}"/>
+    <workbookView xWindow="11340" yWindow="660" windowWidth="32120" windowHeight="22420" xr2:uid="{4751B54A-2E15-734D-9A93-8E38B5748ECD}"/>
   </bookViews>
   <sheets>
-    <sheet name="Terminology" sheetId="1" r:id="rId1"/>
-    <sheet name="Multiple Employers" sheetId="2" r:id="rId2"/>
+    <sheet name="Multiple Employers" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="AdjustmentArb">'Multiple Employers'!$D$23:$G$23</definedName>
@@ -43,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="66">
   <si>
     <t>Term</t>
   </si>
@@ -51,19 +49,10 @@
     <t>Meaning</t>
   </si>
   <si>
-    <t>Example</t>
-  </si>
-  <si>
     <t>Integer</t>
   </si>
   <si>
     <t>Double</t>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>Format*</t>
   </si>
   <si>
     <t>*Definitions</t>
@@ -92,12 +81,6 @@
     </r>
   </si>
   <si>
-    <t>Monthly * 12 / 260</t>
-  </si>
-  <si>
-    <t>100% for employers, 80% for self-employed, etc.</t>
-  </si>
-  <si>
     <t>Rebate percentage</t>
   </si>
   <si>
@@ -113,18 +96,9 @@
     <t>Amount to employee</t>
   </si>
   <si>
-    <t>Remainder after deducting Arbeidsgiverbelop</t>
-  </si>
-  <si>
     <t>Daily rounding error</t>
   </si>
   <si>
-    <t>Maximum yearly rounding error</t>
-  </si>
-  <si>
-    <t>Worse case is 260 * 0.5, or +/- 130 kr.</t>
-  </si>
-  <si>
     <t>Emp 1</t>
   </si>
   <si>
@@ -143,9 +117,6 @@
     <t>Percentage sick</t>
   </si>
   <si>
-    <t>Sykmelding is Integer, Soknad is ??</t>
-  </si>
-  <si>
     <t>6G</t>
   </si>
   <si>
@@ -167,18 +138,6 @@
     <t>Beløp</t>
   </si>
   <si>
-    <t>Grunnbeløp * 6 / 260</t>
-  </si>
-  <si>
-    <t>Grad * Daily 6G</t>
-  </si>
-  <si>
-    <t>Ratio from Inntektsmelding</t>
-  </si>
-  <si>
-    <t>Spleis current rounds this number!</t>
-  </si>
-  <si>
     <t>Weighted percentage sick</t>
   </si>
   <si>
@@ -218,13 +177,7 @@
     <t>Annual</t>
   </si>
   <si>
-    <t>Income monthly</t>
-  </si>
-  <si>
     <t>Daily income</t>
-  </si>
-  <si>
-    <t>Sykepengegrunnlag</t>
   </si>
   <si>
     <t>Monthly income</t>
@@ -365,7 +318,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -381,12 +334,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -432,7 +379,7 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -441,50 +388,39 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="10" fontId="0" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="6" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="6" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="5" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -495,7 +431,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -817,322 +753,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{336B5C91-C43F-4BAE-BFBA-00152852E840}">
-  <dimension ref="A1:E22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBE9F233-0C57-4B39-8C81-6D2F9F1844A9}">
+  <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="17.1640625" customWidth="1"/>
-    <col min="2" max="2" width="28.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.1640625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="19.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="41.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="4"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="11">
-        <v>20000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="4"/>
-      <c r="B4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="2">
-        <f>D3*12/260</f>
-        <v>923.07692307692309</v>
-      </c>
-      <c r="E4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="4"/>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="11">
-        <v>80</v>
-      </c>
-      <c r="E5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="4"/>
-      <c r="B6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="2">
-        <f>D4*ROUND(D5,0)/100</f>
-        <v>738.46153846153845</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="11">
-        <v>60</v>
-      </c>
-      <c r="E7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="4"/>
-      <c r="B8" t="s">
-        <v>43</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" s="2">
-        <f>D6*D7/100</f>
-        <v>443.07692307692304</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B9" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9" s="11">
-        <v>93634</v>
-      </c>
-      <c r="E9" s="25">
-        <v>43101</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" s="2">
-        <f>6*D9/260</f>
-        <v>2160.7846153846153</v>
-      </c>
-      <c r="E10" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="4"/>
-      <c r="B11" t="s">
-        <v>41</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D11" s="1">
-        <f>ROUND(ROUND(D7,0)*D10/100,0)</f>
-        <v>1296</v>
-      </c>
-      <c r="E11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" s="2">
-        <f>MIN(D8,D11)</f>
-        <v>443.07692307692304</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="4"/>
-      <c r="B13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" s="18">
-        <f>100*2/3</f>
-        <v>66.666666666666671</v>
-      </c>
-      <c r="E13" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="B14" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D14" s="9">
-        <f>ROUND(D12*D13/100, 0)</f>
-        <v>295</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="B15" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D15" s="9">
-        <f>ROUND(D12,0)-D14</f>
-        <v>148</v>
-      </c>
-      <c r="E15" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="4"/>
-      <c r="B16" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D16" s="2">
-        <f>D12-D14-D15</f>
-        <v>7.692307692303757E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="4"/>
-      <c r="B17" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D17" s="2">
-        <f>D16*260</f>
-        <v>19.999999999989768</v>
-      </c>
-      <c r="E17" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="4"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="4"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="4"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B21" s="14"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="16"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="42" t="s">
-        <v>8</v>
-      </c>
-      <c r="B22" s="42"/>
-      <c r="C22" s="42"/>
-      <c r="D22" s="42"/>
-    </row>
-  </sheetData>
-  <sheetProtection selectLockedCells="1"/>
-  <mergeCells count="1">
-    <mergeCell ref="A22:D22"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBE9F233-0C57-4B39-8C81-6D2F9F1844A9}">
-  <dimension ref="A1:I41"/>
-  <sheetViews>
-    <sheetView zoomScale="163" zoomScaleNormal="163" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
-    </sheetView>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="1">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1155,22 +780,22 @@
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>73</v>
+        <v>26</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -1178,58 +803,58 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="B3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D3" s="11">
+        <v>39</v>
+      </c>
+      <c r="D3" s="7">
         <v>21000</v>
       </c>
-      <c r="E3" s="11">
+      <c r="E3" s="7">
         <v>10000</v>
       </c>
-      <c r="F3" s="11">
+      <c r="F3" s="7">
         <v>31000</v>
       </c>
-      <c r="G3" s="11">
+      <c r="G3" s="7">
         <v>0</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" t="s">
-        <v>55</v>
-      </c>
-      <c r="D4" s="28">
+        <v>40</v>
+      </c>
+      <c r="D4" s="21">
         <f>D3/SUM($D$3:$G$3)</f>
         <v>0.33870967741935482</v>
       </c>
-      <c r="E4" s="28">
+      <c r="E4" s="21">
         <f t="shared" ref="E4:G4" si="0">E3/SUM($D$3:$G$3)</f>
         <v>0.16129032258064516</v>
       </c>
-      <c r="F4" s="28">
+      <c r="F4" s="21">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="G4" s="28">
+      <c r="G4" s="21">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="27" t="s">
-        <v>63</v>
+      <c r="A5" s="20" t="s">
+        <v>48</v>
       </c>
       <c r="B5" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D5" s="1">
         <f>ROUND(D3*12/260,0)</f>
@@ -1248,41 +873,41 @@
         <v>0</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="I5" s="44" t="s">
-        <v>80</v>
+        <v>2</v>
+      </c>
+      <c r="I5" s="37" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="20">
+        <v>6</v>
+      </c>
+      <c r="D6" s="14">
         <v>1</v>
       </c>
-      <c r="E6" s="20">
+      <c r="E6" s="14">
         <v>1</v>
       </c>
-      <c r="F6" s="20">
+      <c r="F6" s="14">
         <v>1</v>
       </c>
-      <c r="G6" s="20">
+      <c r="G6" s="14">
         <v>1</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="D7" s="2">
         <f>D5*D6</f>
@@ -1301,38 +926,38 @@
         <v>0</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" s="21">
+        <v>17</v>
+      </c>
+      <c r="D8" s="15">
         <v>0.5</v>
       </c>
-      <c r="E8" s="21">
+      <c r="E8" s="15">
         <v>0.8</v>
       </c>
-      <c r="F8" s="21">
+      <c r="F8" s="15">
         <v>0.2</v>
       </c>
-      <c r="G8" s="21">
+      <c r="G8" s="15">
         <v>1</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="B9" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="D9" s="2">
         <f>D7*D8</f>
@@ -1351,628 +976,645 @@
         <v>0</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="20">
+        <v>8</v>
+      </c>
+      <c r="D10" s="14">
         <v>1</v>
       </c>
-      <c r="E10" s="20">
+      <c r="E10" s="14">
         <v>0.9</v>
       </c>
-      <c r="F10" s="20">
+      <c r="F10" s="14">
         <v>0.25</v>
       </c>
-      <c r="G10" s="20">
+      <c r="G10" s="14">
         <v>1</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="B11" t="s">
-        <v>46</v>
-      </c>
-      <c r="D11" s="17">
+        <v>33</v>
+      </c>
+      <c r="D11" s="12">
         <f>D9*D10</f>
         <v>484.5</v>
       </c>
-      <c r="E11" s="17">
+      <c r="E11" s="12">
         <f t="shared" ref="E11:G11" si="4">E9*E10</f>
         <v>332.64000000000004</v>
       </c>
-      <c r="F11" s="17">
+      <c r="F11" s="12">
         <f t="shared" si="4"/>
         <v>71.55</v>
       </c>
-      <c r="G11" s="17">
+      <c r="G11" s="12">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="B12" t="s">
-        <v>38</v>
-      </c>
-      <c r="C12" s="19">
+        <v>25</v>
+      </c>
+      <c r="C12" s="13">
         <f>ROUND(SUM(D9:G9)/SUM(D7:G7),2)</f>
         <v>0.4</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="B13" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="11">
+        <v>19</v>
+      </c>
+      <c r="C13" s="7">
         <v>93634</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="C14" s="2">
         <f>ROUND(6*C13/260, 0)</f>
         <v>2161</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="B15" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C15" s="1">
         <f>ROUND(C12*C14,0)</f>
         <v>864</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="B16" t="s">
-        <v>42</v>
-      </c>
-      <c r="C16" s="22">
+        <v>29</v>
+      </c>
+      <c r="C16" s="16">
         <f>MIN(1, C15/SUM(D9:G9))</f>
         <v>0.75769534333070243</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" s="29" t="s">
-        <v>33</v>
-      </c>
-      <c r="B17" s="30" t="s">
-        <v>12</v>
-      </c>
-      <c r="C17" s="30"/>
-      <c r="D17" s="31">
+      <c r="A17" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="23"/>
+      <c r="D17" s="24">
         <f>D9*ScalingFactor</f>
         <v>367.10339384372531</v>
       </c>
-      <c r="E17" s="31">
+      <c r="E17" s="24">
         <f>E9*ScalingFactor</f>
         <v>280.04419889502765</v>
       </c>
-      <c r="F17" s="31">
+      <c r="F17" s="24">
         <f>F9*ScalingFactor</f>
         <v>216.85240726124704</v>
       </c>
-      <c r="G17" s="31">
+      <c r="G17" s="24">
         <f>G9*ScalingFactor</f>
         <v>0</v>
       </c>
-      <c r="H17" s="32" t="s">
-        <v>4</v>
+      <c r="H17" s="25" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" s="29" t="s">
-        <v>66</v>
-      </c>
-      <c r="B18" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="C18" s="30"/>
-      <c r="D18" s="31">
+      <c r="A18" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" s="23"/>
+      <c r="D18" s="24">
         <f>MIN(D17,D11)</f>
         <v>367.10339384372531</v>
       </c>
-      <c r="E18" s="31">
+      <c r="E18" s="24">
         <f t="shared" ref="E18:G18" si="5">MIN(E17,E11)</f>
         <v>280.04419889502765</v>
       </c>
-      <c r="F18" s="31">
+      <c r="F18" s="24">
         <f t="shared" si="5"/>
         <v>71.55</v>
       </c>
-      <c r="G18" s="31">
+      <c r="G18" s="24">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="H18" s="32" t="s">
-        <v>4</v>
+      <c r="H18" s="25" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" s="29"/>
-      <c r="B19" s="30" t="s">
-        <v>47</v>
-      </c>
-      <c r="C19" s="30"/>
-      <c r="D19" s="31">
+      <c r="A19" s="22"/>
+      <c r="B19" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="23"/>
+      <c r="D19" s="24">
         <f>D18-D11</f>
         <v>-117.39660615627469</v>
       </c>
-      <c r="E19" s="31">
+      <c r="E19" s="24">
         <f t="shared" ref="E19:G19" si="6">E18-E11</f>
         <v>-52.595801104972395</v>
       </c>
-      <c r="F19" s="31">
+      <c r="F19" s="24">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="G19" s="31">
+      <c r="G19" s="24">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="H19" s="32" t="s">
-        <v>4</v>
+      <c r="H19" s="25" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" s="29"/>
-      <c r="B20" s="30" t="s">
-        <v>70</v>
-      </c>
-      <c r="C20" s="30"/>
-      <c r="D20" s="33">
+      <c r="A20" s="22"/>
+      <c r="B20" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" s="23"/>
+      <c r="D20" s="26">
         <f>IF(D19 &lt; 0, D4, 0)</f>
         <v>0.33870967741935482</v>
       </c>
-      <c r="E20" s="33">
+      <c r="E20" s="26">
         <f t="shared" ref="E20:F20" si="7">IF(E19 &lt; 0, E4, 0)</f>
         <v>0.16129032258064516</v>
       </c>
-      <c r="F20" s="33">
+      <c r="F20" s="26">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="G20" s="31"/>
-      <c r="H20" s="32" t="s">
-        <v>4</v>
+      <c r="G20" s="24"/>
+      <c r="H20" s="25" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" s="29" t="s">
-        <v>67</v>
-      </c>
-      <c r="B21" s="30" t="s">
-        <v>71</v>
-      </c>
-      <c r="C21" s="30"/>
-      <c r="D21" s="33">
+      <c r="A21" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="C21" s="23"/>
+      <c r="D21" s="26">
         <f>IF(SUM(ShortfallIncomeRatioArb)=0,0,D20/SUM(ShortfallIncomeRatioArb))</f>
         <v>0.67741935483870963</v>
       </c>
-      <c r="E21" s="33">
+      <c r="E21" s="26">
         <f>IF(SUM(ShortfallIncomeRatioArb)=0,0,E20/SUM(ShortfallIncomeRatioArb))</f>
         <v>0.32258064516129031</v>
       </c>
-      <c r="F21" s="33">
+      <c r="F21" s="26">
         <f>IF(SUM(ShortfallIncomeRatioArb)=0,0,F20/SUM(ShortfallIncomeRatioArb))</f>
         <v>0</v>
       </c>
-      <c r="G21" s="33">
+      <c r="G21" s="26">
         <f>IF(SUM(ShortfallIncomeRatioArb)=0,0,G20/SUM(ShortfallIncomeRatioArb))</f>
         <v>0</v>
       </c>
-      <c r="H21" s="32" t="s">
-        <v>4</v>
+      <c r="H21" s="25" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" s="29"/>
-      <c r="B22" s="30" t="s">
-        <v>45</v>
-      </c>
-      <c r="C22" s="30"/>
-      <c r="D22" s="31">
+      <c r="A22" s="22"/>
+      <c r="B22" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" s="23"/>
+      <c r="D22" s="24">
         <f>D17-D18</f>
         <v>0</v>
       </c>
-      <c r="E22" s="31">
+      <c r="E22" s="24">
         <f>E17-E18</f>
         <v>0</v>
       </c>
-      <c r="F22" s="31">
+      <c r="F22" s="24">
         <f>F17-F18</f>
         <v>145.30240726124703</v>
       </c>
-      <c r="G22" s="31">
+      <c r="G22" s="24">
         <f>G17-G18</f>
         <v>0</v>
       </c>
-      <c r="H22" s="32" t="s">
-        <v>4</v>
+      <c r="H22" s="25" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="B23" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="C23" s="30"/>
-      <c r="D23" s="31">
+      <c r="A23" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="B23" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" s="23"/>
+      <c r="D23" s="24">
         <f>MIN(-D19,IF(SUM($D$19:$G$19)&gt;=0, 0, SUM($D$22:$G$22)*D21))</f>
         <v>98.430662983425393</v>
       </c>
-      <c r="E23" s="31">
+      <c r="E23" s="24">
         <f t="shared" ref="E23:G23" si="8">MIN(-E19,IF(SUM($D$19:$G$19)&gt;=0, 0, SUM($D$22:$G$22)*E21))</f>
         <v>46.87174427782162</v>
       </c>
-      <c r="F23" s="31">
+      <c r="F23" s="24">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="G23" s="31">
+      <c r="G23" s="24">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="H23" s="32" t="s">
-        <v>4</v>
+      <c r="H23" s="25" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" s="29"/>
-      <c r="B24" s="30" t="s">
-        <v>69</v>
-      </c>
-      <c r="C24" s="30"/>
-      <c r="D24" s="33">
+      <c r="A24" s="22"/>
+      <c r="B24" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24" s="23"/>
+      <c r="D24" s="26">
         <f>IF(D22 = 0, 0, D4)</f>
         <v>0</v>
       </c>
-      <c r="E24" s="33">
+      <c r="E24" s="26">
         <f t="shared" ref="E24:G24" si="9">IF(E22 = 0, 0, E4)</f>
         <v>0</v>
       </c>
-      <c r="F24" s="33">
+      <c r="F24" s="26">
         <f t="shared" si="9"/>
         <v>0.5</v>
       </c>
-      <c r="G24" s="33">
+      <c r="G24" s="26">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="H24" s="32" t="s">
-        <v>4</v>
+      <c r="H24" s="25" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" s="29"/>
-      <c r="B25" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="C25" s="30"/>
-      <c r="D25" s="33">
+      <c r="A25" s="22"/>
+      <c r="B25" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="C25" s="23"/>
+      <c r="D25" s="26">
         <f>IF(SUM(ShortfallIncomeRatioPerson)= 0, 0, D24/SUM(ShortfallIncomeRatioPerson))</f>
         <v>0</v>
       </c>
-      <c r="E25" s="33">
+      <c r="E25" s="26">
         <f>IF(SUM(ShortfallIncomeRatioPerson)= 0, 0, E24/SUM(ShortfallIncomeRatioPerson))</f>
         <v>0</v>
       </c>
-      <c r="F25" s="33">
+      <c r="F25" s="26">
         <f>IF(SUM(ShortfallIncomeRatioPerson)= 0, 0, F24/SUM(ShortfallIncomeRatioPerson))</f>
         <v>1</v>
       </c>
-      <c r="G25" s="33">
+      <c r="G25" s="26">
         <f>IF(SUM(ShortfallIncomeRatioPerson)= 0, 0, G24/SUM(ShortfallIncomeRatioPerson))</f>
         <v>0</v>
       </c>
-      <c r="H25" s="32" t="s">
-        <v>4</v>
+      <c r="H25" s="25" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" s="29" t="s">
-        <v>31</v>
-      </c>
-      <c r="B26" s="30" t="s">
-        <v>14</v>
-      </c>
-      <c r="C26" s="30"/>
-      <c r="D26" s="34">
+      <c r="A26" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="B26" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" s="23"/>
+      <c r="D26" s="27">
         <f>ROUND(D18+D23,0)</f>
         <v>466</v>
       </c>
-      <c r="E26" s="34">
+      <c r="E26" s="27">
         <f t="shared" ref="E26:G26" si="10">ROUND(E18+E23,0)</f>
         <v>327</v>
       </c>
-      <c r="F26" s="34">
+      <c r="F26" s="27">
         <f t="shared" si="10"/>
         <v>72</v>
       </c>
-      <c r="G26" s="31">
+      <c r="G26" s="24">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="H26" s="32" t="s">
-        <v>3</v>
+      <c r="H26" s="25" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="B27" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="C27" s="30"/>
-      <c r="D27" s="30">
+      <c r="A27" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="B27" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" s="23"/>
+      <c r="D27" s="23">
         <f>ROUND(D22-SUM(AdjustmentArb)*D25,0)</f>
         <v>0</v>
       </c>
-      <c r="E27" s="30">
+      <c r="E27" s="23">
         <f>ROUND(E22-SUM(AdjustmentArb)*E25,0)</f>
         <v>0</v>
       </c>
-      <c r="F27" s="30">
+      <c r="F27" s="23">
         <f>ROUND(F22-SUM(AdjustmentArb)*F25,0)</f>
         <v>0</v>
       </c>
-      <c r="G27" s="30">
+      <c r="G27" s="23">
         <f>ROUND(G22-SUM(AdjustmentArb)*G25,0)</f>
         <v>0</v>
       </c>
-      <c r="H27" s="32" t="s">
-        <v>3</v>
+      <c r="H27" s="25" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" s="29"/>
-      <c r="B28" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="C28" s="35">
+      <c r="A28" s="22"/>
+      <c r="B28" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28" s="28">
         <f>C15-SUM(D26:G27)</f>
         <v>-1</v>
       </c>
-      <c r="D28" s="30"/>
-      <c r="E28" s="30"/>
-      <c r="F28" s="30"/>
-      <c r="G28" s="30"/>
-      <c r="H28" s="32" t="s">
-        <v>3</v>
+      <c r="D28" s="23"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="23"/>
+      <c r="H28" s="25" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="4"/>
-      <c r="C29" s="26"/>
+      <c r="C29" s="19"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A30" s="36" t="s">
-        <v>77</v>
-      </c>
-      <c r="B30" s="37" t="s">
-        <v>74</v>
-      </c>
-      <c r="C30" s="38"/>
-      <c r="D30" s="39">
+      <c r="A30" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="B30" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="C30" s="31"/>
+      <c r="D30" s="32">
         <f>ROUND(D9*D10, 0)</f>
         <v>485</v>
       </c>
-      <c r="E30" s="39">
+      <c r="E30" s="32">
         <f t="shared" ref="E30:G30" si="11">ROUND(E9*E10, 0)</f>
         <v>333</v>
       </c>
-      <c r="F30" s="39">
+      <c r="F30" s="32">
         <f t="shared" si="11"/>
         <v>72</v>
       </c>
-      <c r="G30" s="39">
+      <c r="G30" s="32">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="H30" s="40" t="s">
-        <v>3</v>
+      <c r="H30" s="33" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A31" s="36" t="s">
-        <v>78</v>
-      </c>
-      <c r="B31" s="37" t="s">
-        <v>75</v>
-      </c>
-      <c r="C31" s="38"/>
-      <c r="D31" s="39">
+      <c r="A31" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="B31" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="C31" s="31"/>
+      <c r="D31" s="32">
         <f>ROUND(D9,0) - D30</f>
         <v>0</v>
       </c>
-      <c r="E31" s="39">
+      <c r="E31" s="32">
         <f t="shared" ref="E31:G31" si="12">ROUND(E9,0) - E30</f>
         <v>37</v>
       </c>
-      <c r="F31" s="39">
+      <c r="F31" s="32">
         <f t="shared" si="12"/>
         <v>214</v>
       </c>
-      <c r="G31" s="39">
+      <c r="G31" s="32">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="H31" s="40" t="s">
-        <v>3</v>
+      <c r="H31" s="33" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A32" s="36"/>
-      <c r="B32" s="41" t="s">
-        <v>76</v>
-      </c>
-      <c r="C32" s="43" t="str">
+      <c r="A32" s="29"/>
+      <c r="B32" s="34" t="s">
+        <v>61</v>
+      </c>
+      <c r="C32" s="36" t="str">
         <f>IF(SUM(D30:G31)&lt;=MAKSBELOP,"Everyone paid",IF(SUM(D30:G30)&lt;=MAKSBELOP,"Arbeidsgivere fully paid; Person partially paid by Person request", "Arbeidsgivere partial payment ratio by Arbeidsgiver request"))</f>
         <v>Arbeidsgivere partial payment ratio by Arbeidsgiver request</v>
       </c>
-      <c r="D32" s="43"/>
-      <c r="E32" s="43"/>
-      <c r="F32" s="43"/>
-      <c r="G32" s="43"/>
-      <c r="H32" s="40"/>
+      <c r="D32" s="36"/>
+      <c r="E32" s="36"/>
+      <c r="F32" s="36"/>
+      <c r="G32" s="36"/>
+      <c r="H32" s="33"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A33" s="36" t="s">
-        <v>31</v>
-      </c>
-      <c r="B33" s="37" t="s">
-        <v>14</v>
-      </c>
-      <c r="C33" s="38"/>
-      <c r="D33" s="37">
+      <c r="A33" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="B33" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33" s="31"/>
+      <c r="D33" s="30">
         <f>IF(SUM($D$30:$G$31)&lt;=MAKSBELOP,D30,IF(SUM($D$30:$G$30)&lt;=MAKSBELOP,D30,ROUND(D30*MAKSBELOP/SUM($D$30:$G$30),0)))</f>
         <v>471</v>
       </c>
-      <c r="E33" s="37">
+      <c r="E33" s="30">
         <f>IF(SUM($D$30:$G$31)&lt;=MAKSBELOP,E30,IF(SUM($D$30:$G$30)&lt;=MAKSBELOP,E30,ROUND(E30*MAKSBELOP/SUM($D$30:$G$30),0)))</f>
         <v>323</v>
       </c>
-      <c r="F33" s="37">
+      <c r="F33" s="30">
         <f>IF(SUM($D$30:$G$31)&lt;=MAKSBELOP,F30,IF(SUM($D$30:$G$30)&lt;=MAKSBELOP,F30,ROUND(F30*MAKSBELOP/SUM($D$30:$G$30),0)))</f>
         <v>70</v>
       </c>
-      <c r="G33" s="37">
+      <c r="G33" s="30">
         <f>IF(SUM($D$30:$G$31)&lt;=MAKSBELOP,G30,IF(SUM($D$30:$G$30)&lt;=MAKSBELOP,G30,ROUND(G30*MAKSBELOP/SUM($D$30:$G$30),0)))</f>
         <v>0</v>
       </c>
-      <c r="H33" s="40" t="s">
-        <v>3</v>
+      <c r="H33" s="33" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="34" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="36"/>
-      <c r="B34" s="37" t="s">
-        <v>79</v>
-      </c>
-      <c r="C34" s="38">
+      <c r="A34" s="29"/>
+      <c r="B34" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="C34" s="31">
         <f>MAKSBELOP-SUM(D33:G33)</f>
         <v>0</v>
       </c>
-      <c r="D34" s="37"/>
-      <c r="E34" s="37"/>
-      <c r="F34" s="37"/>
-      <c r="G34" s="37"/>
-      <c r="H34" s="40"/>
+      <c r="D34" s="30"/>
+      <c r="E34" s="30"/>
+      <c r="F34" s="30"/>
+      <c r="G34" s="30"/>
+      <c r="H34" s="33"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A35" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="B35" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="C35" s="37"/>
-      <c r="D35" s="37">
+      <c r="A35" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="B35" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="C35" s="30"/>
+      <c r="D35" s="30">
         <f>IF(SUM($D$30:$G$31)&lt;=MAKSBELOP,D31,IF(SUM($D$30:$G$30)&lt;=MAKSBELOP,ROUND(PersonRemainder*D31/SUM($D$31:$G$31),0),0))</f>
         <v>0</v>
       </c>
-      <c r="E35" s="37">
+      <c r="E35" s="30">
         <f>IF(SUM($D$30:$G$31)&lt;=MAKSBELOP,E31,IF(SUM($D$30:$G$30)&lt;=MAKSBELOP,ROUND(PersonRemainder*E31/SUM($D$31:$G$31),0),0))</f>
         <v>0</v>
       </c>
-      <c r="F35" s="37">
+      <c r="F35" s="30">
         <f>IF(SUM($D$30:$G$31)&lt;=MAKSBELOP,F31,IF(SUM($D$30:$G$30)&lt;=MAKSBELOP,ROUND(PersonRemainder*F31/SUM($D$31:$G$31),0),0))</f>
         <v>0</v>
       </c>
-      <c r="G35" s="37">
+      <c r="G35" s="30">
         <f>IF(SUM($D$30:$G$31)&lt;=MAKSBELOP,G31,IF(SUM($D$30:$G$30)&lt;=MAKSBELOP,ROUND(PersonRemainder*G31/SUM($D$31:$G$31),0),0))</f>
         <v>0</v>
       </c>
-      <c r="H35" s="40" t="s">
-        <v>3</v>
+      <c r="H35" s="33" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A36" s="36"/>
-      <c r="B36" s="37" t="s">
-        <v>17</v>
-      </c>
-      <c r="C36" s="38">
+      <c r="A36" s="29"/>
+      <c r="B36" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="C36" s="31">
         <f>MAKSBELOP-SUM(D33:G35)</f>
         <v>0</v>
       </c>
-      <c r="D36" s="37"/>
-      <c r="E36" s="37"/>
-      <c r="F36" s="37"/>
-      <c r="G36" s="37"/>
-      <c r="H36" s="40" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A40" s="23" t="s">
-        <v>49</v>
-      </c>
-      <c r="B40" s="24">
+      <c r="D36" s="30"/>
+      <c r="E36" s="30"/>
+      <c r="F36" s="30"/>
+      <c r="G36" s="30"/>
+      <c r="H36" s="33" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B38" s="9"/>
+      <c r="C38" s="10"/>
+      <c r="D38" s="11"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="B39" s="35"/>
+      <c r="C39" s="35"/>
+      <c r="D39" s="35"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B41" s="18">
         <v>1430.76</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A41" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="B41" s="24">
-        <f>ROUND(B40*260/12,0)</f>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A42" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B42" s="18">
+        <f>ROUND(B41*260/12,0)</f>
         <v>31000</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="C32:G32"/>
+    <mergeCell ref="A39:D39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Skeleton of next V22 migration test created; code still needed to enable it.
Co-authored-by: Marte Tårnes <marte.tarnes@nav.no>
</commit_message>
<xml_diff>
--- a/doc/okonomi/Utbetaling.xlsx
+++ b/doc/okonomi/Utbetaling.xlsx
@@ -8,20 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fred/src/nav/helse-spleis/doc/okonomi/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04B3C38E-65D5-EA4B-8856-975C572E501F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EE62673-1CFD-8C49-8149-0BC6767738E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11340" yWindow="660" windowWidth="32120" windowHeight="22420" xr2:uid="{4751B54A-2E15-734D-9A93-8E38B5748ECD}"/>
+    <workbookView xWindow="31160" yWindow="1500" windowWidth="32120" windowHeight="22420" xr2:uid="{4751B54A-2E15-734D-9A93-8E38B5748ECD}"/>
   </bookViews>
   <sheets>
     <sheet name="Multiple Employers" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="AdjustmentArb">'Multiple Employers'!$D$23:$G$23</definedName>
-    <definedName name="MAKSBELOP">'Multiple Employers'!$C$15</definedName>
-    <definedName name="PersonRemainder">'Multiple Employers'!$C$34</definedName>
-    <definedName name="ScalingFactor">'Multiple Employers'!$C$16</definedName>
-    <definedName name="ShortfallIncomeRatioArb">'Multiple Employers'!$D$20:$G$20</definedName>
-    <definedName name="ShortfallIncomeRatioPerson">'Multiple Employers'!$D$24:$G$24</definedName>
+    <definedName name="AdjustmentArb">'Multiple Employers'!$D$24:$G$24</definedName>
+    <definedName name="MAKSBELOP">'Multiple Employers'!$C$16</definedName>
+    <definedName name="PersonRemainder">'Multiple Employers'!$C$35</definedName>
+    <definedName name="ScalingFactor">'Multiple Employers'!$C$17</definedName>
+    <definedName name="ShortfallIncomeRatioArb">'Multiple Employers'!$D$21:$G$21</definedName>
+    <definedName name="ShortfallIncomeRatioPerson">'Multiple Employers'!$D$25:$G$25</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="68">
   <si>
     <t>Term</t>
   </si>
@@ -258,7 +258,13 @@
     <t>Remainder for employees</t>
   </si>
   <si>
-    <t>New: Rounding assuming 100% sickness</t>
+    <t>New: Fred 18-06</t>
+  </si>
+  <si>
+    <t>Dagsats</t>
+  </si>
+  <si>
+    <t>Maximum assuming 100% sick, only employer</t>
   </si>
 </sst>
 </file>
@@ -431,13 +437,13 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -754,16 +760,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBE9F233-0C57-4B39-8C81-6D2F9F1844A9}">
-  <dimension ref="A1:I42"/>
+  <dimension ref="A1:I43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="27" customWidth="1"/>
-    <col min="2" max="2" width="28.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.33203125" customWidth="1"/>
     <col min="3" max="3" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.33203125" bestFit="1" customWidth="1"/>
@@ -856,26 +862,26 @@
       <c r="B5" t="s">
         <v>38</v>
       </c>
-      <c r="D5" s="1">
-        <f>ROUND(D3*12/260,0)</f>
-        <v>969</v>
-      </c>
-      <c r="E5" s="1">
-        <f t="shared" ref="E5:G5" si="1">ROUND(E3*12/260,0)</f>
-        <v>462</v>
-      </c>
-      <c r="F5" s="1">
+      <c r="D5" s="2">
+        <f>D3*12/260</f>
+        <v>969.23076923076928</v>
+      </c>
+      <c r="E5" s="2">
+        <f t="shared" ref="E5:G5" si="1">E3*12/260</f>
+        <v>461.53846153846155</v>
+      </c>
+      <c r="F5" s="2">
         <f t="shared" si="1"/>
-        <v>1431</v>
-      </c>
-      <c r="G5" s="1">
+        <v>1430.7692307692307</v>
+      </c>
+      <c r="G5" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I5" s="37" t="s">
+        <v>3</v>
+      </c>
+      <c r="I5" s="35" t="s">
         <v>65</v>
       </c>
     </row>
@@ -909,71 +915,77 @@
       <c r="B7" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="2">
-        <f>D5*D6</f>
+      <c r="D7" s="1">
+        <f>ROUND(D5*D6,0)</f>
         <v>969</v>
       </c>
-      <c r="E7" s="2">
-        <f t="shared" ref="E7:G7" si="2">E5*E6</f>
+      <c r="E7" s="1">
+        <f t="shared" ref="E7:G7" si="2">ROUND(E5*E6,0)</f>
         <v>462</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="1">
         <f t="shared" si="2"/>
         <v>1431</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="1">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="I7" s="35" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>16</v>
+        <v>66</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="15">
-        <v>0.5</v>
-      </c>
-      <c r="E8" s="15">
-        <v>0.8</v>
-      </c>
-      <c r="F8" s="15">
-        <v>0.2</v>
-      </c>
-      <c r="G8" s="15">
-        <v>1</v>
+        <v>67</v>
+      </c>
+      <c r="D8" s="1">
+        <f>MIN(D7,$C$15)</f>
+        <v>969</v>
+      </c>
+      <c r="E8" s="1">
+        <f t="shared" ref="E8:G8" si="3">MIN(E7,$C$15)</f>
+        <v>462</v>
+      </c>
+      <c r="F8" s="1">
+        <f t="shared" si="3"/>
+        <v>1431</v>
+      </c>
+      <c r="G8" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="I8" s="35" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="2">
-        <f>D7*D8</f>
-        <v>484.5</v>
-      </c>
-      <c r="E9" s="2">
-        <f t="shared" ref="E9:G9" si="3">E7*E8</f>
-        <v>369.6</v>
-      </c>
-      <c r="F9" s="2">
-        <f t="shared" si="3"/>
-        <v>286.2</v>
-      </c>
-      <c r="G9" s="2">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>17</v>
+      </c>
+      <c r="D9" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="E9" s="15">
+        <v>0.8</v>
+      </c>
+      <c r="F9" s="15">
+        <v>0.2</v>
+      </c>
+      <c r="G9" s="15">
+        <v>1</v>
       </c>
       <c r="H9" s="3" t="s">
         <v>3</v>
@@ -981,22 +993,26 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="14">
-        <v>1</v>
-      </c>
-      <c r="E10" s="14">
-        <v>0.9</v>
-      </c>
-      <c r="F10" s="14">
-        <v>0.25</v>
-      </c>
-      <c r="G10" s="14">
-        <v>1</v>
+        <v>30</v>
+      </c>
+      <c r="D10" s="2">
+        <f>D7*D9</f>
+        <v>484.5</v>
+      </c>
+      <c r="E10" s="2">
+        <f t="shared" ref="E10:G10" si="4">E7*E9</f>
+        <v>369.6</v>
+      </c>
+      <c r="F10" s="2">
+        <f t="shared" si="4"/>
+        <v>286.2</v>
+      </c>
+      <c r="G10" s="2">
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>3</v>
@@ -1004,26 +1020,22 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B11" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" s="12">
-        <f>D9*D10</f>
-        <v>484.5</v>
-      </c>
-      <c r="E11" s="12">
-        <f t="shared" ref="E11:G11" si="4">E9*E10</f>
-        <v>332.64000000000004</v>
-      </c>
-      <c r="F11" s="12">
-        <f t="shared" si="4"/>
-        <v>71.55</v>
-      </c>
-      <c r="G11" s="12">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <v>8</v>
+      </c>
+      <c r="D11" s="14">
+        <v>1</v>
+      </c>
+      <c r="E11" s="14">
+        <v>0.9</v>
+      </c>
+      <c r="F11" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="G11" s="14">
+        <v>1</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>3</v>
@@ -1031,28 +1043,41 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="13">
-        <f>ROUND(SUM(D9:G9)/SUM(D7:G7),2)</f>
-        <v>0.4</v>
+        <v>33</v>
+      </c>
+      <c r="D12" s="12">
+        <f>D10*D11</f>
+        <v>484.5</v>
+      </c>
+      <c r="E12" s="12">
+        <f t="shared" ref="E12:G12" si="5">E10*E11</f>
+        <v>332.64000000000004</v>
+      </c>
+      <c r="F12" s="12">
+        <f t="shared" si="5"/>
+        <v>71.55</v>
+      </c>
+      <c r="G12" s="12">
+        <f t="shared" si="5"/>
+        <v>0</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="7">
-        <v>93634</v>
+        <v>25</v>
+      </c>
+      <c r="C13" s="13">
+        <f>ROUND(SUM(D10:G10)/SUM(D7:G7),2)</f>
+        <v>0.4</v>
       </c>
       <c r="H13" s="3" t="s">
         <v>2</v>
@@ -1060,99 +1085,88 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="2">
-        <f>ROUND(6*C13/260, 0)</f>
-        <v>2161</v>
+        <v>19</v>
+      </c>
+      <c r="C14" s="7">
+        <v>93634</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>47</v>
+        <v>18</v>
       </c>
       <c r="B15" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" s="1">
-        <f>ROUND(C12*C14,0)</f>
-        <v>864</v>
+        <v>20</v>
+      </c>
+      <c r="C15" s="2">
+        <f>ROUND(6*C14/260, 0)</f>
+        <v>2161</v>
       </c>
       <c r="H15" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="I15" s="35" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="1">
+        <f>ROUND(C13*C15,0)</f>
+        <v>864</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="16">
-        <f>MIN(1, C15/SUM(D9:G9))</f>
+      <c r="C17" s="16">
+        <f>MIN(1, C16/SUM(D10:G10))</f>
         <v>0.75769534333070243</v>
       </c>
-      <c r="H16" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="B17" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="C17" s="23"/>
-      <c r="D17" s="24">
-        <f>D9*ScalingFactor</f>
-        <v>367.10339384372531</v>
-      </c>
-      <c r="E17" s="24">
-        <f>E9*ScalingFactor</f>
-        <v>280.04419889502765</v>
-      </c>
-      <c r="F17" s="24">
-        <f>F9*ScalingFactor</f>
-        <v>216.85240726124704</v>
-      </c>
-      <c r="G17" s="24">
-        <f>G9*ScalingFactor</f>
-        <v>0</v>
-      </c>
-      <c r="H17" s="25" t="s">
+      <c r="H17" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="22" t="s">
-        <v>51</v>
+        <v>24</v>
       </c>
       <c r="B18" s="23" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="C18" s="23"/>
       <c r="D18" s="24">
-        <f>MIN(D17,D11)</f>
+        <f>D10*ScalingFactor</f>
         <v>367.10339384372531</v>
       </c>
       <c r="E18" s="24">
-        <f t="shared" ref="E18:G18" si="5">MIN(E17,E11)</f>
+        <f>E10*ScalingFactor</f>
         <v>280.04419889502765</v>
       </c>
       <c r="F18" s="24">
-        <f t="shared" si="5"/>
-        <v>71.55</v>
+        <f>F10*ScalingFactor</f>
+        <v>216.85240726124704</v>
       </c>
       <c r="G18" s="24">
-        <f t="shared" si="5"/>
+        <f>G10*ScalingFactor</f>
         <v>0</v>
       </c>
       <c r="H18" s="25" t="s">
@@ -1160,22 +1174,24 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" s="22"/>
+      <c r="A19" s="22" t="s">
+        <v>51</v>
+      </c>
       <c r="B19" s="23" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C19" s="23"/>
       <c r="D19" s="24">
-        <f>D18-D11</f>
-        <v>-117.39660615627469</v>
+        <f>MIN(D18,D12)</f>
+        <v>367.10339384372531</v>
       </c>
       <c r="E19" s="24">
-        <f t="shared" ref="E19:G19" si="6">E18-E11</f>
-        <v>-52.595801104972395</v>
+        <f t="shared" ref="E19:G19" si="6">MIN(E18,E12)</f>
+        <v>280.04419889502765</v>
       </c>
       <c r="F19" s="24">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>71.55</v>
       </c>
       <c r="G19" s="24">
         <f t="shared" si="6"/>
@@ -1188,74 +1204,74 @@
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="22"/>
       <c r="B20" s="23" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
       <c r="C20" s="23"/>
-      <c r="D20" s="26">
-        <f>IF(D19 &lt; 0, D4, 0)</f>
-        <v>0.33870967741935482</v>
-      </c>
-      <c r="E20" s="26">
-        <f t="shared" ref="E20:F20" si="7">IF(E19 &lt; 0, E4, 0)</f>
-        <v>0.16129032258064516</v>
-      </c>
-      <c r="F20" s="26">
+      <c r="D20" s="24">
+        <f>D19-D12</f>
+        <v>-117.39660615627469</v>
+      </c>
+      <c r="E20" s="24">
+        <f t="shared" ref="E20:G20" si="7">E19-E12</f>
+        <v>-52.595801104972395</v>
+      </c>
+      <c r="F20" s="24">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="G20" s="24"/>
+      <c r="G20" s="24">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
       <c r="H20" s="25" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" s="22" t="s">
-        <v>52</v>
-      </c>
+      <c r="A21" s="22"/>
       <c r="B21" s="23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C21" s="23"/>
       <c r="D21" s="26">
-        <f>IF(SUM(ShortfallIncomeRatioArb)=0,0,D20/SUM(ShortfallIncomeRatioArb))</f>
-        <v>0.67741935483870963</v>
+        <f>IF(D20 &lt; 0, D4, 0)</f>
+        <v>0.33870967741935482</v>
       </c>
       <c r="E21" s="26">
-        <f>IF(SUM(ShortfallIncomeRatioArb)=0,0,E20/SUM(ShortfallIncomeRatioArb))</f>
-        <v>0.32258064516129031</v>
+        <f t="shared" ref="E21:F21" si="8">IF(E20 &lt; 0, E4, 0)</f>
+        <v>0.16129032258064516</v>
       </c>
       <c r="F21" s="26">
-        <f>IF(SUM(ShortfallIncomeRatioArb)=0,0,F20/SUM(ShortfallIncomeRatioArb))</f>
-        <v>0</v>
-      </c>
-      <c r="G21" s="26">
-        <f>IF(SUM(ShortfallIncomeRatioArb)=0,0,G20/SUM(ShortfallIncomeRatioArb))</f>
-        <v>0</v>
-      </c>
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="G21" s="24"/>
       <c r="H21" s="25" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" s="22"/>
+      <c r="A22" s="22" t="s">
+        <v>52</v>
+      </c>
       <c r="B22" s="23" t="s">
-        <v>32</v>
+        <v>56</v>
       </c>
       <c r="C22" s="23"/>
-      <c r="D22" s="24">
-        <f>D17-D18</f>
-        <v>0</v>
-      </c>
-      <c r="E22" s="24">
-        <f>E17-E18</f>
-        <v>0</v>
-      </c>
-      <c r="F22" s="24">
-        <f>F17-F18</f>
-        <v>145.30240726124703</v>
-      </c>
-      <c r="G22" s="24">
-        <f>G17-G18</f>
+      <c r="D22" s="26">
+        <f>IF(SUM(ShortfallIncomeRatioArb)=0,0,D21/SUM(ShortfallIncomeRatioArb))</f>
+        <v>0.67741935483870963</v>
+      </c>
+      <c r="E22" s="26">
+        <f>IF(SUM(ShortfallIncomeRatioArb)=0,0,E21/SUM(ShortfallIncomeRatioArb))</f>
+        <v>0.32258064516129031</v>
+      </c>
+      <c r="F22" s="26">
+        <f>IF(SUM(ShortfallIncomeRatioArb)=0,0,F21/SUM(ShortfallIncomeRatioArb))</f>
+        <v>0</v>
+      </c>
+      <c r="G22" s="26">
+        <f>IF(SUM(ShortfallIncomeRatioArb)=0,0,G21/SUM(ShortfallIncomeRatioArb))</f>
         <v>0</v>
       </c>
       <c r="H22" s="25" t="s">
@@ -1263,27 +1279,25 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" s="22" t="s">
-        <v>53</v>
-      </c>
+      <c r="A23" s="22"/>
       <c r="B23" s="23" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C23" s="23"/>
       <c r="D23" s="24">
-        <f>MIN(-D19,IF(SUM($D$19:$G$19)&gt;=0, 0, SUM($D$22:$G$22)*D21))</f>
-        <v>98.430662983425393</v>
+        <f>D18-D19</f>
+        <v>0</v>
       </c>
       <c r="E23" s="24">
-        <f t="shared" ref="E23:G23" si="8">MIN(-E19,IF(SUM($D$19:$G$19)&gt;=0, 0, SUM($D$22:$G$22)*E21))</f>
-        <v>46.87174427782162</v>
+        <f>E18-E19</f>
+        <v>0</v>
       </c>
       <c r="F23" s="24">
-        <f t="shared" si="8"/>
-        <v>0</v>
+        <f>F18-F19</f>
+        <v>145.30240726124703</v>
       </c>
       <c r="G23" s="24">
-        <f t="shared" si="8"/>
+        <f>G18-G19</f>
         <v>0</v>
       </c>
       <c r="H23" s="25" t="s">
@@ -1291,24 +1305,26 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" s="22"/>
+      <c r="A24" s="22" t="s">
+        <v>53</v>
+      </c>
       <c r="B24" s="23" t="s">
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="C24" s="23"/>
-      <c r="D24" s="26">
-        <f>IF(D22 = 0, 0, D4)</f>
-        <v>0</v>
-      </c>
-      <c r="E24" s="26">
-        <f t="shared" ref="E24:G24" si="9">IF(E22 = 0, 0, E4)</f>
-        <v>0</v>
-      </c>
-      <c r="F24" s="26">
+      <c r="D24" s="24">
+        <f>MIN(-D20,IF(SUM($D$20:$G$20)&gt;=0, 0, SUM($D$23:$G$23)*D22))</f>
+        <v>98.430662983425393</v>
+      </c>
+      <c r="E24" s="24">
+        <f t="shared" ref="E24:G24" si="9">MIN(-E20,IF(SUM($D$20:$G$20)&gt;=0, 0, SUM($D$23:$G$23)*E22))</f>
+        <v>46.87174427782162</v>
+      </c>
+      <c r="F24" s="24">
         <f t="shared" si="9"/>
-        <v>0.5</v>
-      </c>
-      <c r="G24" s="26">
+        <v>0</v>
+      </c>
+      <c r="G24" s="24">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
@@ -1319,23 +1335,23 @@
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="22"/>
       <c r="B25" s="23" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C25" s="23"/>
       <c r="D25" s="26">
-        <f>IF(SUM(ShortfallIncomeRatioPerson)= 0, 0, D24/SUM(ShortfallIncomeRatioPerson))</f>
+        <f>IF(D23 = 0, 0, D4)</f>
         <v>0</v>
       </c>
       <c r="E25" s="26">
-        <f>IF(SUM(ShortfallIncomeRatioPerson)= 0, 0, E24/SUM(ShortfallIncomeRatioPerson))</f>
+        <f t="shared" ref="E25:G25" si="10">IF(E23 = 0, 0, E4)</f>
         <v>0</v>
       </c>
       <c r="F25" s="26">
-        <f>IF(SUM(ShortfallIncomeRatioPerson)= 0, 0, F24/SUM(ShortfallIncomeRatioPerson))</f>
-        <v>1</v>
+        <f t="shared" si="10"/>
+        <v>0.5</v>
       </c>
       <c r="G25" s="26">
-        <f>IF(SUM(ShortfallIncomeRatioPerson)= 0, 0, G24/SUM(ShortfallIncomeRatioPerson))</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="H25" s="25" t="s">
@@ -1343,55 +1359,53 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="A26" s="22"/>
       <c r="B26" s="23" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="C26" s="23"/>
-      <c r="D26" s="27">
-        <f>ROUND(D18+D23,0)</f>
-        <v>466</v>
-      </c>
-      <c r="E26" s="27">
-        <f t="shared" ref="E26:G26" si="10">ROUND(E18+E23,0)</f>
-        <v>327</v>
-      </c>
-      <c r="F26" s="27">
-        <f t="shared" si="10"/>
-        <v>72</v>
-      </c>
-      <c r="G26" s="24">
-        <f t="shared" si="10"/>
+      <c r="D26" s="26">
+        <f>IF(SUM(ShortfallIncomeRatioPerson)= 0, 0, D25/SUM(ShortfallIncomeRatioPerson))</f>
+        <v>0</v>
+      </c>
+      <c r="E26" s="26">
+        <f>IF(SUM(ShortfallIncomeRatioPerson)= 0, 0, E25/SUM(ShortfallIncomeRatioPerson))</f>
+        <v>0</v>
+      </c>
+      <c r="F26" s="26">
+        <f>IF(SUM(ShortfallIncomeRatioPerson)= 0, 0, F25/SUM(ShortfallIncomeRatioPerson))</f>
+        <v>1</v>
+      </c>
+      <c r="G26" s="26">
+        <f>IF(SUM(ShortfallIncomeRatioPerson)= 0, 0, G25/SUM(ShortfallIncomeRatioPerson))</f>
         <v>0</v>
       </c>
       <c r="H26" s="25" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B27" s="23" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C27" s="23"/>
-      <c r="D27" s="23">
-        <f>ROUND(D22-SUM(AdjustmentArb)*D25,0)</f>
-        <v>0</v>
-      </c>
-      <c r="E27" s="23">
-        <f>ROUND(E22-SUM(AdjustmentArb)*E25,0)</f>
-        <v>0</v>
-      </c>
-      <c r="F27" s="23">
-        <f>ROUND(F22-SUM(AdjustmentArb)*F25,0)</f>
-        <v>0</v>
-      </c>
-      <c r="G27" s="23">
-        <f>ROUND(G22-SUM(AdjustmentArb)*G25,0)</f>
+      <c r="D27" s="27">
+        <f>ROUND(D19+D24,0)</f>
+        <v>466</v>
+      </c>
+      <c r="E27" s="27">
+        <f t="shared" ref="E27:G27" si="11">ROUND(E19+E24,0)</f>
+        <v>327</v>
+      </c>
+      <c r="F27" s="27">
+        <f t="shared" si="11"/>
+        <v>72</v>
+      </c>
+      <c r="G27" s="24">
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="H27" s="25" t="s">
@@ -1399,73 +1413,73 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" s="22"/>
+      <c r="A28" s="22" t="s">
+        <v>23</v>
+      </c>
       <c r="B28" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="C28" s="28">
-        <f>C15-SUM(D26:G27)</f>
-        <v>-1</v>
-      </c>
-      <c r="D28" s="23"/>
-      <c r="E28" s="23"/>
-      <c r="F28" s="23"/>
-      <c r="G28" s="23"/>
+        <v>10</v>
+      </c>
+      <c r="C28" s="23"/>
+      <c r="D28" s="23">
+        <f>ROUND(D23-SUM(AdjustmentArb)*D26,0)</f>
+        <v>0</v>
+      </c>
+      <c r="E28" s="23">
+        <f>ROUND(E23-SUM(AdjustmentArb)*E26,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F28" s="23">
+        <f>ROUND(F23-SUM(AdjustmentArb)*F26,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G28" s="23">
+        <f>ROUND(G23-SUM(AdjustmentArb)*G26,0)</f>
+        <v>0</v>
+      </c>
       <c r="H28" s="25" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" s="4"/>
-      <c r="C29" s="19"/>
+      <c r="A29" s="22"/>
+      <c r="B29" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29" s="28">
+        <f>C16-SUM(D27:G28)</f>
+        <v>-1</v>
+      </c>
+      <c r="D29" s="23"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="23"/>
+      <c r="G29" s="23"/>
+      <c r="H29" s="25" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A30" s="29" t="s">
-        <v>62</v>
-      </c>
-      <c r="B30" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="C30" s="31"/>
-      <c r="D30" s="32">
-        <f>ROUND(D9*D10, 0)</f>
-        <v>485</v>
-      </c>
-      <c r="E30" s="32">
-        <f t="shared" ref="E30:G30" si="11">ROUND(E9*E10, 0)</f>
-        <v>333</v>
-      </c>
-      <c r="F30" s="32">
-        <f t="shared" si="11"/>
-        <v>72</v>
-      </c>
-      <c r="G30" s="32">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="H30" s="33" t="s">
-        <v>2</v>
-      </c>
+      <c r="A30" s="4"/>
+      <c r="C30" s="19"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="29" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B31" s="30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C31" s="31"/>
       <c r="D31" s="32">
-        <f>ROUND(D9,0) - D30</f>
-        <v>0</v>
+        <f>ROUND(D10*D11, 0)</f>
+        <v>485</v>
       </c>
       <c r="E31" s="32">
-        <f t="shared" ref="E31:G31" si="12">ROUND(E9,0) - E30</f>
-        <v>37</v>
+        <f t="shared" ref="E31:G31" si="12">ROUND(E10*E11, 0)</f>
+        <v>333</v>
       </c>
       <c r="F31" s="32">
         <f t="shared" si="12"/>
-        <v>214</v>
+        <v>72</v>
       </c>
       <c r="G31" s="32">
         <f t="shared" si="12"/>
@@ -1476,145 +1490,173 @@
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A32" s="29"/>
-      <c r="B32" s="34" t="s">
+      <c r="A32" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="B32" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="C32" s="31"/>
+      <c r="D32" s="32">
+        <f>ROUND(D10,0) - D31</f>
+        <v>0</v>
+      </c>
+      <c r="E32" s="32">
+        <f t="shared" ref="E32:G32" si="13">ROUND(E10,0) - E31</f>
+        <v>37</v>
+      </c>
+      <c r="F32" s="32">
+        <f t="shared" si="13"/>
+        <v>214</v>
+      </c>
+      <c r="G32" s="32">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="H32" s="33" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" s="29"/>
+      <c r="B33" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="C32" s="36" t="str">
-        <f>IF(SUM(D30:G31)&lt;=MAKSBELOP,"Everyone paid",IF(SUM(D30:G30)&lt;=MAKSBELOP,"Arbeidsgivere fully paid; Person partially paid by Person request", "Arbeidsgivere partial payment ratio by Arbeidsgiver request"))</f>
+      <c r="C33" s="36" t="str">
+        <f>IF(SUM(D31:G32)&lt;=MAKSBELOP,"Everyone paid",IF(SUM(D31:G31)&lt;=MAKSBELOP,"Arbeidsgivere fully paid; Person partially paid by Person request", "Arbeidsgivere partial payment ratio by Arbeidsgiver request"))</f>
         <v>Arbeidsgivere partial payment ratio by Arbeidsgiver request</v>
       </c>
-      <c r="D32" s="36"/>
-      <c r="E32" s="36"/>
-      <c r="F32" s="36"/>
-      <c r="G32" s="36"/>
-      <c r="H32" s="33"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A33" s="29" t="s">
+      <c r="D33" s="36"/>
+      <c r="E33" s="36"/>
+      <c r="F33" s="36"/>
+      <c r="G33" s="36"/>
+      <c r="H33" s="33"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="B33" s="30" t="s">
+      <c r="B34" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="C33" s="31"/>
-      <c r="D33" s="30">
-        <f>IF(SUM($D$30:$G$31)&lt;=MAKSBELOP,D30,IF(SUM($D$30:$G$30)&lt;=MAKSBELOP,D30,ROUND(D30*MAKSBELOP/SUM($D$30:$G$30),0)))</f>
+      <c r="C34" s="31"/>
+      <c r="D34" s="30">
+        <f>IF(SUM($D$31:$G$32)&lt;=MAKSBELOP,D31,IF(SUM($D$31:$G$31)&lt;=MAKSBELOP,D31,ROUND(D31*MAKSBELOP/SUM($D$31:$G$31),0)))</f>
         <v>471</v>
       </c>
-      <c r="E33" s="30">
-        <f>IF(SUM($D$30:$G$31)&lt;=MAKSBELOP,E30,IF(SUM($D$30:$G$30)&lt;=MAKSBELOP,E30,ROUND(E30*MAKSBELOP/SUM($D$30:$G$30),0)))</f>
+      <c r="E34" s="30">
+        <f>IF(SUM($D$31:$G$32)&lt;=MAKSBELOP,E31,IF(SUM($D$31:$G$31)&lt;=MAKSBELOP,E31,ROUND(E31*MAKSBELOP/SUM($D$31:$G$31),0)))</f>
         <v>323</v>
       </c>
-      <c r="F33" s="30">
-        <f>IF(SUM($D$30:$G$31)&lt;=MAKSBELOP,F30,IF(SUM($D$30:$G$30)&lt;=MAKSBELOP,F30,ROUND(F30*MAKSBELOP/SUM($D$30:$G$30),0)))</f>
+      <c r="F34" s="30">
+        <f>IF(SUM($D$31:$G$32)&lt;=MAKSBELOP,F31,IF(SUM($D$31:$G$31)&lt;=MAKSBELOP,F31,ROUND(F31*MAKSBELOP/SUM($D$31:$G$31),0)))</f>
         <v>70</v>
       </c>
-      <c r="G33" s="30">
-        <f>IF(SUM($D$30:$G$31)&lt;=MAKSBELOP,G30,IF(SUM($D$30:$G$30)&lt;=MAKSBELOP,G30,ROUND(G30*MAKSBELOP/SUM($D$30:$G$30),0)))</f>
-        <v>0</v>
-      </c>
-      <c r="H33" s="33" t="s">
+      <c r="G34" s="30">
+        <f>IF(SUM($D$31:$G$32)&lt;=MAKSBELOP,G31,IF(SUM($D$31:$G$31)&lt;=MAKSBELOP,G31,ROUND(G31*MAKSBELOP/SUM($D$31:$G$31),0)))</f>
+        <v>0</v>
+      </c>
+      <c r="H34" s="33" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="29"/>
-      <c r="B34" s="30" t="s">
+    <row r="35" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="29"/>
+      <c r="B35" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="C34" s="31">
-        <f>MAKSBELOP-SUM(D33:G33)</f>
-        <v>0</v>
-      </c>
-      <c r="D34" s="30"/>
-      <c r="E34" s="30"/>
-      <c r="F34" s="30"/>
-      <c r="G34" s="30"/>
-      <c r="H34" s="33"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A35" s="29" t="s">
+      <c r="C35" s="31">
+        <f>MAKSBELOP-SUM(D34:G34)</f>
+        <v>0</v>
+      </c>
+      <c r="D35" s="30"/>
+      <c r="E35" s="30"/>
+      <c r="F35" s="30"/>
+      <c r="G35" s="30"/>
+      <c r="H35" s="33"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="B35" s="30" t="s">
+      <c r="B36" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="C35" s="30"/>
-      <c r="D35" s="30">
-        <f>IF(SUM($D$30:$G$31)&lt;=MAKSBELOP,D31,IF(SUM($D$30:$G$30)&lt;=MAKSBELOP,ROUND(PersonRemainder*D31/SUM($D$31:$G$31),0),0))</f>
-        <v>0</v>
-      </c>
-      <c r="E35" s="30">
-        <f>IF(SUM($D$30:$G$31)&lt;=MAKSBELOP,E31,IF(SUM($D$30:$G$30)&lt;=MAKSBELOP,ROUND(PersonRemainder*E31/SUM($D$31:$G$31),0),0))</f>
-        <v>0</v>
-      </c>
-      <c r="F35" s="30">
-        <f>IF(SUM($D$30:$G$31)&lt;=MAKSBELOP,F31,IF(SUM($D$30:$G$30)&lt;=MAKSBELOP,ROUND(PersonRemainder*F31/SUM($D$31:$G$31),0),0))</f>
-        <v>0</v>
-      </c>
-      <c r="G35" s="30">
-        <f>IF(SUM($D$30:$G$31)&lt;=MAKSBELOP,G31,IF(SUM($D$30:$G$30)&lt;=MAKSBELOP,ROUND(PersonRemainder*G31/SUM($D$31:$G$31),0),0))</f>
-        <v>0</v>
-      </c>
-      <c r="H35" s="33" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A36" s="29"/>
-      <c r="B36" s="30" t="s">
-        <v>11</v>
-      </c>
-      <c r="C36" s="31">
-        <f>MAKSBELOP-SUM(D33:G35)</f>
-        <v>0</v>
-      </c>
-      <c r="D36" s="30"/>
-      <c r="E36" s="30"/>
-      <c r="F36" s="30"/>
-      <c r="G36" s="30"/>
+      <c r="C36" s="30"/>
+      <c r="D36" s="30">
+        <f>IF(SUM($D$31:$G$32)&lt;=MAKSBELOP,D32,IF(SUM($D$31:$G$31)&lt;=MAKSBELOP,ROUND(PersonRemainder*D32/SUM($D$32:$G$32),0),0))</f>
+        <v>0</v>
+      </c>
+      <c r="E36" s="30">
+        <f>IF(SUM($D$31:$G$32)&lt;=MAKSBELOP,E32,IF(SUM($D$31:$G$31)&lt;=MAKSBELOP,ROUND(PersonRemainder*E32/SUM($D$32:$G$32),0),0))</f>
+        <v>0</v>
+      </c>
+      <c r="F36" s="30">
+        <f>IF(SUM($D$31:$G$32)&lt;=MAKSBELOP,F32,IF(SUM($D$31:$G$31)&lt;=MAKSBELOP,ROUND(PersonRemainder*F32/SUM($D$32:$G$32),0),0))</f>
+        <v>0</v>
+      </c>
+      <c r="G36" s="30">
+        <f>IF(SUM($D$31:$G$32)&lt;=MAKSBELOP,G32,IF(SUM($D$31:$G$31)&lt;=MAKSBELOP,ROUND(PersonRemainder*G32/SUM($D$32:$G$32),0),0))</f>
+        <v>0</v>
+      </c>
       <c r="H36" s="33" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A38" s="8" t="s">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" s="29"/>
+      <c r="B37" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="C37" s="31">
+        <f>MAKSBELOP-SUM(D34:G36)</f>
+        <v>0</v>
+      </c>
+      <c r="D37" s="30"/>
+      <c r="E37" s="30"/>
+      <c r="F37" s="30"/>
+      <c r="G37" s="30"/>
+      <c r="H37" s="33" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B38" s="9"/>
-      <c r="C38" s="10"/>
-      <c r="D38" s="11"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A39" s="35" t="s">
+      <c r="B39" s="9"/>
+      <c r="C39" s="10"/>
+      <c r="D39" s="11"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="B39" s="35"/>
-      <c r="C39" s="35"/>
-      <c r="D39" s="35"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A41" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="B41" s="18">
-        <v>1430.76</v>
-      </c>
+      <c r="B40" s="37"/>
+      <c r="C40" s="37"/>
+      <c r="D40" s="37"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B42" s="18">
+        <v>1430.76</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A43" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="B42" s="18">
-        <f>ROUND(B41*260/12,0)</f>
+      <c r="B43" s="18">
+        <f>ROUND(B42*260/12,0)</f>
         <v>31000</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="A39:D39"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="A40:D40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated spreadsheet with some rounding adjustments
</commit_message>
<xml_diff>
--- a/doc/okonomi/Utbetaling.xlsx
+++ b/doc/okonomi/Utbetaling.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fred/src/nav/helse-spleis/doc/okonomi/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EE62673-1CFD-8C49-8149-0BC6767738E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9141110E-8969-654B-834F-5815260768D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="31160" yWindow="1500" windowWidth="32120" windowHeight="22420" xr2:uid="{4751B54A-2E15-734D-9A93-8E38B5748ECD}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="AdjustmentArb">'Multiple Employers'!$D$24:$G$24</definedName>
     <definedName name="MAKSBELOP">'Multiple Employers'!$C$16</definedName>
-    <definedName name="PersonRemainder">'Multiple Employers'!$C$35</definedName>
+    <definedName name="PersonRemainder">'Multiple Employers'!$C$36</definedName>
     <definedName name="ScalingFactor">'Multiple Employers'!$C$17</definedName>
     <definedName name="ShortfallIncomeRatioArb">'Multiple Employers'!$D$21:$G$21</definedName>
     <definedName name="ShortfallIncomeRatioPerson">'Multiple Employers'!$D$25:$G$25</definedName>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="69">
   <si>
     <t>Term</t>
   </si>
@@ -265,6 +265,9 @@
   </si>
   <si>
     <t>Maximum assuming 100% sick, only employer</t>
+  </si>
+  <si>
+    <t>New: Fred 26-06</t>
   </si>
 </sst>
 </file>
@@ -405,10 +408,8 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="10" fontId="0" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -444,6 +445,8 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -760,10 +763,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBE9F233-0C57-4B39-8C81-6D2F9F1844A9}">
-  <dimension ref="A1:I43"/>
+  <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -776,6 +780,7 @@
     <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.6640625" style="3"/>
+    <col min="9" max="9" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
@@ -835,19 +840,19 @@
       <c r="B4" t="s">
         <v>40</v>
       </c>
-      <c r="D4" s="21">
+      <c r="D4" s="19">
         <f>D3/SUM($D$3:$G$3)</f>
         <v>0.33870967741935482</v>
       </c>
-      <c r="E4" s="21">
+      <c r="E4" s="19">
         <f t="shared" ref="E4:G4" si="0">E3/SUM($D$3:$G$3)</f>
         <v>0.16129032258064516</v>
       </c>
-      <c r="F4" s="21">
+      <c r="F4" s="19">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="G4" s="21">
+      <c r="G4" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -856,7 +861,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="18" t="s">
         <v>48</v>
       </c>
       <c r="B5" t="s">
@@ -881,7 +886,7 @@
       <c r="H5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="I5" s="35" t="s">
+      <c r="I5" s="36" t="s">
         <v>65</v>
       </c>
     </row>
@@ -892,16 +897,16 @@
       <c r="B6" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="14">
+      <c r="D6" s="13">
         <v>1</v>
       </c>
-      <c r="E6" s="14">
+      <c r="E6" s="13">
         <v>1</v>
       </c>
-      <c r="F6" s="14">
+      <c r="F6" s="13">
         <v>1</v>
       </c>
-      <c r="G6" s="14">
+      <c r="G6" s="13">
         <v>1</v>
       </c>
       <c r="H6" s="3" t="s">
@@ -915,27 +920,27 @@
       <c r="B7" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="1">
-        <f>ROUND(D5*D6,0)</f>
-        <v>969</v>
-      </c>
-      <c r="E7" s="1">
-        <f t="shared" ref="E7:G7" si="2">ROUND(E5*E6,0)</f>
-        <v>462</v>
-      </c>
-      <c r="F7" s="1">
+      <c r="D7" s="2">
+        <f>D5*D6</f>
+        <v>969.23076923076928</v>
+      </c>
+      <c r="E7" s="2">
+        <f t="shared" ref="E7:G7" si="2">E5*E6</f>
+        <v>461.53846153846155</v>
+      </c>
+      <c r="F7" s="2">
         <f t="shared" si="2"/>
-        <v>1431</v>
-      </c>
-      <c r="G7" s="1">
+        <v>1430.7692307692307</v>
+      </c>
+      <c r="G7" s="2">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I7" s="35" t="s">
-        <v>65</v>
+        <v>3</v>
+      </c>
+      <c r="I7" s="33" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -947,15 +952,15 @@
       </c>
       <c r="D8" s="1">
         <f>MIN(D7,$C$15)</f>
-        <v>969</v>
+        <v>969.23076923076928</v>
       </c>
       <c r="E8" s="1">
         <f t="shared" ref="E8:G8" si="3">MIN(E7,$C$15)</f>
-        <v>462</v>
+        <v>461.53846153846155</v>
       </c>
       <c r="F8" s="1">
         <f t="shared" si="3"/>
-        <v>1431</v>
+        <v>1430.7692307692307</v>
       </c>
       <c r="G8" s="1">
         <f t="shared" si="3"/>
@@ -964,7 +969,7 @@
       <c r="H8" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="I8" s="35" t="s">
+      <c r="I8" s="36" t="s">
         <v>65</v>
       </c>
     </row>
@@ -975,16 +980,16 @@
       <c r="B9" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="15">
+      <c r="D9" s="14">
         <v>0.5</v>
       </c>
-      <c r="E9" s="15">
+      <c r="E9" s="14">
         <v>0.8</v>
       </c>
-      <c r="F9" s="15">
+      <c r="F9" s="14">
         <v>0.2</v>
       </c>
-      <c r="G9" s="15">
+      <c r="G9" s="14">
         <v>1</v>
       </c>
       <c r="H9" s="3" t="s">
@@ -1000,15 +1005,15 @@
       </c>
       <c r="D10" s="2">
         <f>D7*D9</f>
-        <v>484.5</v>
+        <v>484.61538461538464</v>
       </c>
       <c r="E10" s="2">
         <f t="shared" ref="E10:G10" si="4">E7*E9</f>
-        <v>369.6</v>
+        <v>369.23076923076928</v>
       </c>
       <c r="F10" s="2">
         <f t="shared" si="4"/>
-        <v>286.2</v>
+        <v>286.15384615384613</v>
       </c>
       <c r="G10" s="2">
         <f t="shared" si="4"/>
@@ -1025,16 +1030,16 @@
       <c r="B11" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="14">
+      <c r="D11" s="13">
         <v>1</v>
       </c>
-      <c r="E11" s="14">
+      <c r="E11" s="13">
         <v>0.9</v>
       </c>
-      <c r="F11" s="14">
+      <c r="F11" s="13">
         <v>0.25</v>
       </c>
-      <c r="G11" s="14">
+      <c r="G11" s="13">
         <v>1</v>
       </c>
       <c r="H11" s="3" t="s">
@@ -1050,15 +1055,15 @@
       </c>
       <c r="D12" s="12">
         <f>D10*D11</f>
-        <v>484.5</v>
+        <v>484.61538461538464</v>
       </c>
       <c r="E12" s="12">
         <f t="shared" ref="E12:G12" si="5">E10*E11</f>
-        <v>332.64000000000004</v>
+        <v>332.30769230769238</v>
       </c>
       <c r="F12" s="12">
         <f t="shared" si="5"/>
-        <v>71.55</v>
+        <v>71.538461538461533</v>
       </c>
       <c r="G12" s="12">
         <f t="shared" si="5"/>
@@ -1075,7 +1080,7 @@
       <c r="B13" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="13">
+      <c r="C13" s="37">
         <f>ROUND(SUM(D10:G10)/SUM(D7:G7),2)</f>
         <v>0.4</v>
       </c>
@@ -1104,14 +1109,14 @@
       <c r="B15" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="1">
         <f>ROUND(6*C14/260, 0)</f>
         <v>2161</v>
       </c>
       <c r="H15" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="I15" s="35" t="s">
+      <c r="I15" s="36" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1130,533 +1135,568 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="16">
+      <c r="C17" s="24">
         <f>MIN(1, C16/SUM(D10:G10))</f>
-        <v>0.75769534333070243</v>
-      </c>
-      <c r="H17" s="3" t="s">
+        <v>0.75789473684210529</v>
+      </c>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="23" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" s="22" t="s">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="23" t="s">
+      <c r="B18" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="23"/>
-      <c r="D18" s="24">
+      <c r="C18" s="21"/>
+      <c r="D18" s="22">
         <f>D10*ScalingFactor</f>
-        <v>367.10339384372531</v>
-      </c>
-      <c r="E18" s="24">
+        <v>367.28744939271257</v>
+      </c>
+      <c r="E18" s="22">
         <f>E10*ScalingFactor</f>
-        <v>280.04419889502765</v>
-      </c>
-      <c r="F18" s="24">
+        <v>279.83805668016197</v>
+      </c>
+      <c r="F18" s="22">
         <f>F10*ScalingFactor</f>
-        <v>216.85240726124704</v>
-      </c>
-      <c r="G18" s="24">
+        <v>216.87449392712549</v>
+      </c>
+      <c r="G18" s="22">
         <f>G10*ScalingFactor</f>
         <v>0</v>
       </c>
-      <c r="H18" s="25" t="s">
+      <c r="H18" s="23" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" s="22" t="s">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="B19" s="23" t="s">
+      <c r="B19" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="C19" s="23"/>
-      <c r="D19" s="24">
+      <c r="C19" s="21"/>
+      <c r="D19" s="22">
         <f>MIN(D18,D12)</f>
-        <v>367.10339384372531</v>
-      </c>
-      <c r="E19" s="24">
+        <v>367.28744939271257</v>
+      </c>
+      <c r="E19" s="22">
         <f t="shared" ref="E19:G19" si="6">MIN(E18,E12)</f>
-        <v>280.04419889502765</v>
-      </c>
-      <c r="F19" s="24">
+        <v>279.83805668016197</v>
+      </c>
+      <c r="F19" s="22">
         <f t="shared" si="6"/>
-        <v>71.55</v>
-      </c>
-      <c r="G19" s="24">
+        <v>71.538461538461533</v>
+      </c>
+      <c r="G19" s="22">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="H19" s="25" t="s">
+      <c r="H19" s="23" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" s="22"/>
-      <c r="B20" s="23" t="s">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="20"/>
+      <c r="B20" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="C20" s="23"/>
-      <c r="D20" s="24">
+      <c r="C20" s="21"/>
+      <c r="D20" s="22">
         <f>D19-D12</f>
-        <v>-117.39660615627469</v>
-      </c>
-      <c r="E20" s="24">
+        <v>-117.32793522267207</v>
+      </c>
+      <c r="E20" s="22">
         <f t="shared" ref="E20:G20" si="7">E19-E12</f>
-        <v>-52.595801104972395</v>
-      </c>
-      <c r="F20" s="24">
+        <v>-52.469635627530408</v>
+      </c>
+      <c r="F20" s="22">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="G20" s="24">
+      <c r="G20" s="22">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="H20" s="25" t="s">
+      <c r="H20" s="23" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" s="22"/>
-      <c r="B21" s="23" t="s">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="20"/>
+      <c r="B21" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="C21" s="23"/>
-      <c r="D21" s="26">
+      <c r="C21" s="21"/>
+      <c r="D21" s="24">
         <f>IF(D20 &lt; 0, D4, 0)</f>
         <v>0.33870967741935482</v>
       </c>
-      <c r="E21" s="26">
+      <c r="E21" s="24">
         <f t="shared" ref="E21:F21" si="8">IF(E20 &lt; 0, E4, 0)</f>
         <v>0.16129032258064516</v>
       </c>
-      <c r="F21" s="26">
+      <c r="F21" s="24">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="G21" s="24"/>
-      <c r="H21" s="25" t="s">
+      <c r="G21" s="22"/>
+      <c r="H21" s="23" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" s="22" t="s">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="B22" s="23" t="s">
+      <c r="B22" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="C22" s="23"/>
-      <c r="D22" s="26">
+      <c r="C22" s="21"/>
+      <c r="D22" s="24">
         <f>IF(SUM(ShortfallIncomeRatioArb)=0,0,D21/SUM(ShortfallIncomeRatioArb))</f>
         <v>0.67741935483870963</v>
       </c>
-      <c r="E22" s="26">
+      <c r="E22" s="24">
         <f>IF(SUM(ShortfallIncomeRatioArb)=0,0,E21/SUM(ShortfallIncomeRatioArb))</f>
         <v>0.32258064516129031</v>
       </c>
-      <c r="F22" s="26">
+      <c r="F22" s="24">
         <f>IF(SUM(ShortfallIncomeRatioArb)=0,0,F21/SUM(ShortfallIncomeRatioArb))</f>
         <v>0</v>
       </c>
-      <c r="G22" s="26">
+      <c r="G22" s="24">
         <f>IF(SUM(ShortfallIncomeRatioArb)=0,0,G21/SUM(ShortfallIncomeRatioArb))</f>
         <v>0</v>
       </c>
-      <c r="H22" s="25" t="s">
+      <c r="H22" s="23" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" s="22"/>
-      <c r="B23" s="23" t="s">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="20"/>
+      <c r="B23" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="C23" s="23"/>
-      <c r="D23" s="24">
+      <c r="C23" s="21"/>
+      <c r="D23" s="22">
         <f>D18-D19</f>
         <v>0</v>
       </c>
-      <c r="E23" s="24">
+      <c r="E23" s="22">
         <f>E18-E19</f>
         <v>0</v>
       </c>
-      <c r="F23" s="24">
+      <c r="F23" s="22">
         <f>F18-F19</f>
-        <v>145.30240726124703</v>
-      </c>
-      <c r="G23" s="24">
+        <v>145.33603238866397</v>
+      </c>
+      <c r="G23" s="22">
         <f>G18-G19</f>
         <v>0</v>
       </c>
-      <c r="H23" s="25" t="s">
+      <c r="H23" s="23" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" s="22" t="s">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="B24" s="23" t="s">
+      <c r="B24" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="C24" s="23"/>
-      <c r="D24" s="24">
+      <c r="C24" s="21"/>
+      <c r="D24" s="22">
         <f>MIN(-D20,IF(SUM($D$20:$G$20)&gt;=0, 0, SUM($D$23:$G$23)*D22))</f>
-        <v>98.430662983425393</v>
-      </c>
-      <c r="E24" s="24">
+        <v>98.453441295546554</v>
+      </c>
+      <c r="E24" s="22">
         <f t="shared" ref="E24:G24" si="9">MIN(-E20,IF(SUM($D$20:$G$20)&gt;=0, 0, SUM($D$23:$G$23)*E22))</f>
-        <v>46.87174427782162</v>
-      </c>
-      <c r="F24" s="24">
+        <v>46.882591093117405</v>
+      </c>
+      <c r="F24" s="22">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="G24" s="24">
+      <c r="G24" s="22">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="H24" s="25" t="s">
+      <c r="H24" s="23" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" s="22"/>
-      <c r="B25" s="23" t="s">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="20"/>
+      <c r="B25" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="C25" s="23"/>
-      <c r="D25" s="26">
+      <c r="C25" s="21"/>
+      <c r="D25" s="24">
         <f>IF(D23 = 0, 0, D4)</f>
         <v>0</v>
       </c>
-      <c r="E25" s="26">
+      <c r="E25" s="24">
         <f t="shared" ref="E25:G25" si="10">IF(E23 = 0, 0, E4)</f>
         <v>0</v>
       </c>
-      <c r="F25" s="26">
+      <c r="F25" s="24">
         <f t="shared" si="10"/>
         <v>0.5</v>
       </c>
-      <c r="G25" s="26">
+      <c r="G25" s="24">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="H25" s="25" t="s">
+      <c r="H25" s="23" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" s="22"/>
-      <c r="B26" s="23" t="s">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="20"/>
+      <c r="B26" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="C26" s="23"/>
-      <c r="D26" s="26">
+      <c r="C26" s="21"/>
+      <c r="D26" s="24">
         <f>IF(SUM(ShortfallIncomeRatioPerson)= 0, 0, D25/SUM(ShortfallIncomeRatioPerson))</f>
         <v>0</v>
       </c>
-      <c r="E26" s="26">
+      <c r="E26" s="24">
         <f>IF(SUM(ShortfallIncomeRatioPerson)= 0, 0, E25/SUM(ShortfallIncomeRatioPerson))</f>
         <v>0</v>
       </c>
-      <c r="F26" s="26">
+      <c r="F26" s="24">
         <f>IF(SUM(ShortfallIncomeRatioPerson)= 0, 0, F25/SUM(ShortfallIncomeRatioPerson))</f>
         <v>1</v>
       </c>
-      <c r="G26" s="26">
+      <c r="G26" s="24">
         <f>IF(SUM(ShortfallIncomeRatioPerson)= 0, 0, G25/SUM(ShortfallIncomeRatioPerson))</f>
         <v>0</v>
       </c>
-      <c r="H26" s="25" t="s">
+      <c r="H26" s="23" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" s="22" t="s">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="B27" s="23" t="s">
+      <c r="B27" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="C27" s="23"/>
-      <c r="D27" s="27">
+      <c r="C27" s="21"/>
+      <c r="D27" s="25">
         <f>ROUND(D19+D24,0)</f>
         <v>466</v>
       </c>
-      <c r="E27" s="27">
+      <c r="E27" s="25">
         <f t="shared" ref="E27:G27" si="11">ROUND(E19+E24,0)</f>
         <v>327</v>
       </c>
-      <c r="F27" s="27">
+      <c r="F27" s="25">
         <f t="shared" si="11"/>
         <v>72</v>
       </c>
-      <c r="G27" s="24">
+      <c r="G27" s="22">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="H27" s="25" t="s">
+      <c r="H27" s="23" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" s="22" t="s">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="B28" s="23" t="s">
+      <c r="B28" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="C28" s="23"/>
-      <c r="D28" s="23">
+      <c r="C28" s="21"/>
+      <c r="D28" s="21">
         <f>ROUND(D23-SUM(AdjustmentArb)*D26,0)</f>
         <v>0</v>
       </c>
-      <c r="E28" s="23">
+      <c r="E28" s="21">
         <f>ROUND(E23-SUM(AdjustmentArb)*E26,0)</f>
         <v>0</v>
       </c>
-      <c r="F28" s="23">
+      <c r="F28" s="21">
         <f>ROUND(F23-SUM(AdjustmentArb)*F26,0)</f>
         <v>0</v>
       </c>
-      <c r="G28" s="23">
+      <c r="G28" s="21">
         <f>ROUND(G23-SUM(AdjustmentArb)*G26,0)</f>
         <v>0</v>
       </c>
-      <c r="H28" s="25" t="s">
+      <c r="H28" s="23" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" s="22"/>
-      <c r="B29" s="23" t="s">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" s="20"/>
+      <c r="B29" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="C29" s="28">
+      <c r="C29" s="26">
         <f>C16-SUM(D27:G28)</f>
         <v>-1</v>
       </c>
-      <c r="D29" s="23"/>
-      <c r="E29" s="23"/>
-      <c r="F29" s="23"/>
-      <c r="G29" s="23"/>
-      <c r="H29" s="25" t="s">
+      <c r="D29" s="21"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="21"/>
+      <c r="G29" s="21"/>
+      <c r="H29" s="23" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="4"/>
-      <c r="C30" s="19"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A31" s="29" t="s">
+      <c r="C30" s="17"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="B31" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="C31" s="29"/>
+      <c r="D31" s="30">
+        <f>ROUND(D10,0)</f>
+        <v>485</v>
+      </c>
+      <c r="E31" s="30">
+        <f t="shared" ref="E31:G31" si="12">ROUND(E10,0)</f>
+        <v>369</v>
+      </c>
+      <c r="F31" s="30">
+        <f t="shared" si="12"/>
+        <v>286</v>
+      </c>
+      <c r="G31" s="30">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="H31" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="I31" s="33" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="B31" s="30" t="s">
+      <c r="B32" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="31"/>
-      <c r="D31" s="32">
-        <f>ROUND(D10*D11, 0)</f>
+      <c r="C32" s="29"/>
+      <c r="D32" s="30">
+        <f>ROUND(D12,0)</f>
         <v>485</v>
       </c>
-      <c r="E31" s="32">
-        <f t="shared" ref="E31:G31" si="12">ROUND(E10*E11, 0)</f>
-        <v>333</v>
-      </c>
-      <c r="F31" s="32">
-        <f t="shared" si="12"/>
+      <c r="E32" s="30">
+        <f t="shared" ref="E32:G32" si="13">ROUND(E12,0)</f>
+        <v>332</v>
+      </c>
+      <c r="F32" s="30">
+        <f t="shared" si="13"/>
         <v>72</v>
       </c>
-      <c r="G31" s="32">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="H31" s="33" t="s">
+      <c r="G32" s="30">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="H32" s="31" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A32" s="29" t="s">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="B32" s="30" t="s">
+      <c r="B33" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="31"/>
-      <c r="D32" s="32">
-        <f>ROUND(D10,0) - D31</f>
-        <v>0</v>
-      </c>
-      <c r="E32" s="32">
-        <f t="shared" ref="E32:G32" si="13">ROUND(E10,0) - E31</f>
+      <c r="C33" s="29"/>
+      <c r="D33" s="30">
+        <f>D31-D32</f>
+        <v>0</v>
+      </c>
+      <c r="E33" s="30">
+        <f t="shared" ref="E33:G33" si="14">E31-E32</f>
         <v>37</v>
       </c>
-      <c r="F32" s="32">
-        <f t="shared" si="13"/>
+      <c r="F33" s="30">
+        <f t="shared" si="14"/>
         <v>214</v>
       </c>
-      <c r="G32" s="32">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="H32" s="33" t="s">
+      <c r="G33" s="30">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="H33" s="31" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A33" s="29"/>
-      <c r="B33" s="34" t="s">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" s="27"/>
+      <c r="B34" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="36" t="str">
-        <f>IF(SUM(D31:G32)&lt;=MAKSBELOP,"Everyone paid",IF(SUM(D31:G31)&lt;=MAKSBELOP,"Arbeidsgivere fully paid; Person partially paid by Person request", "Arbeidsgivere partial payment ratio by Arbeidsgiver request"))</f>
+      <c r="C34" s="34" t="str">
+        <f>IF(SUM(D32:G33)&lt;=MAKSBELOP,"Everyone paid",IF(SUM(D32:G32)&lt;=MAKSBELOP,"Arbeidsgivere fully paid; Person partially paid by Person request", "Arbeidsgivere partial payment ratio by Arbeidsgiver request"))</f>
         <v>Arbeidsgivere partial payment ratio by Arbeidsgiver request</v>
       </c>
-      <c r="D33" s="36"/>
-      <c r="E33" s="36"/>
-      <c r="F33" s="36"/>
-      <c r="G33" s="36"/>
-      <c r="H33" s="33"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A34" s="29" t="s">
+      <c r="D34" s="34"/>
+      <c r="E34" s="34"/>
+      <c r="F34" s="34"/>
+      <c r="G34" s="34"/>
+      <c r="H34" s="31"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="B34" s="30" t="s">
+      <c r="B35" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="C34" s="31"/>
-      <c r="D34" s="30">
-        <f>IF(SUM($D$31:$G$32)&lt;=MAKSBELOP,D31,IF(SUM($D$31:$G$31)&lt;=MAKSBELOP,D31,ROUND(D31*MAKSBELOP/SUM($D$31:$G$31),0)))</f>
+      <c r="C35" s="29"/>
+      <c r="D35" s="28">
+        <f>IF(SUM($D$32:$G$33)&lt;=MAKSBELOP,D32,IF(SUM($D$32:$G$32)&lt;=MAKSBELOP,D32,ROUND(D32*MAKSBELOP/SUM($D$32:$G$32),0)))</f>
         <v>471</v>
       </c>
-      <c r="E34" s="30">
-        <f>IF(SUM($D$31:$G$32)&lt;=MAKSBELOP,E31,IF(SUM($D$31:$G$31)&lt;=MAKSBELOP,E31,ROUND(E31*MAKSBELOP/SUM($D$31:$G$31),0)))</f>
+      <c r="E35" s="28">
+        <f>IF(SUM($D$32:$G$33)&lt;=MAKSBELOP,E32,IF(SUM($D$32:$G$32)&lt;=MAKSBELOP,E32,ROUND(E32*MAKSBELOP/SUM($D$32:$G$32),0)))</f>
         <v>323</v>
       </c>
-      <c r="F34" s="30">
-        <f>IF(SUM($D$31:$G$32)&lt;=MAKSBELOP,F31,IF(SUM($D$31:$G$31)&lt;=MAKSBELOP,F31,ROUND(F31*MAKSBELOP/SUM($D$31:$G$31),0)))</f>
+      <c r="F35" s="28">
+        <f>IF(SUM($D$32:$G$33)&lt;=MAKSBELOP,F32,IF(SUM($D$32:$G$32)&lt;=MAKSBELOP,F32,ROUND(F32*MAKSBELOP/SUM($D$32:$G$32),0)))</f>
         <v>70</v>
       </c>
-      <c r="G34" s="30">
-        <f>IF(SUM($D$31:$G$32)&lt;=MAKSBELOP,G31,IF(SUM($D$31:$G$31)&lt;=MAKSBELOP,G31,ROUND(G31*MAKSBELOP/SUM($D$31:$G$31),0)))</f>
-        <v>0</v>
-      </c>
-      <c r="H34" s="33" t="s">
+      <c r="G35" s="28">
+        <f>IF(SUM($D$32:$G$33)&lt;=MAKSBELOP,G32,IF(SUM($D$32:$G$32)&lt;=MAKSBELOP,G32,ROUND(G32*MAKSBELOP/SUM($D$32:$G$32),0)))</f>
+        <v>0</v>
+      </c>
+      <c r="H35" s="31" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="29"/>
-      <c r="B35" s="30" t="s">
+    <row r="36" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="27"/>
+      <c r="B36" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="C35" s="31">
-        <f>MAKSBELOP-SUM(D34:G34)</f>
-        <v>0</v>
-      </c>
-      <c r="D35" s="30"/>
-      <c r="E35" s="30"/>
-      <c r="F35" s="30"/>
-      <c r="G35" s="30"/>
-      <c r="H35" s="33"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A36" s="29" t="s">
+      <c r="C36" s="29">
+        <f>MAKSBELOP-SUM(D35:G35)</f>
+        <v>0</v>
+      </c>
+      <c r="D36" s="28"/>
+      <c r="E36" s="28"/>
+      <c r="F36" s="28"/>
+      <c r="G36" s="28"/>
+      <c r="H36" s="31"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="B36" s="30" t="s">
+      <c r="B37" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="C36" s="30"/>
-      <c r="D36" s="30">
-        <f>IF(SUM($D$31:$G$32)&lt;=MAKSBELOP,D32,IF(SUM($D$31:$G$31)&lt;=MAKSBELOP,ROUND(PersonRemainder*D32/SUM($D$32:$G$32),0),0))</f>
-        <v>0</v>
-      </c>
-      <c r="E36" s="30">
-        <f>IF(SUM($D$31:$G$32)&lt;=MAKSBELOP,E32,IF(SUM($D$31:$G$31)&lt;=MAKSBELOP,ROUND(PersonRemainder*E32/SUM($D$32:$G$32),0),0))</f>
-        <v>0</v>
-      </c>
-      <c r="F36" s="30">
-        <f>IF(SUM($D$31:$G$32)&lt;=MAKSBELOP,F32,IF(SUM($D$31:$G$31)&lt;=MAKSBELOP,ROUND(PersonRemainder*F32/SUM($D$32:$G$32),0),0))</f>
-        <v>0</v>
-      </c>
-      <c r="G36" s="30">
-        <f>IF(SUM($D$31:$G$32)&lt;=MAKSBELOP,G32,IF(SUM($D$31:$G$31)&lt;=MAKSBELOP,ROUND(PersonRemainder*G32/SUM($D$32:$G$32),0),0))</f>
-        <v>0</v>
-      </c>
-      <c r="H36" s="33" t="s">
+      <c r="C37" s="28"/>
+      <c r="D37" s="28">
+        <f>IF(SUM($D$32:$G$33)&lt;=MAKSBELOP,D33,IF(SUM($D$32:$G$32)&lt;=MAKSBELOP,ROUND(PersonRemainder*D33/SUM($D$33:$G$33),0),0))</f>
+        <v>0</v>
+      </c>
+      <c r="E37" s="28">
+        <f>IF(SUM($D$32:$G$33)&lt;=MAKSBELOP,E33,IF(SUM($D$32:$G$32)&lt;=MAKSBELOP,ROUND(PersonRemainder*E33/SUM($D$33:$G$33),0),0))</f>
+        <v>0</v>
+      </c>
+      <c r="F37" s="28">
+        <f>IF(SUM($D$32:$G$33)&lt;=MAKSBELOP,F33,IF(SUM($D$32:$G$32)&lt;=MAKSBELOP,ROUND(PersonRemainder*F33/SUM($D$33:$G$33),0),0))</f>
+        <v>0</v>
+      </c>
+      <c r="G37" s="28">
+        <f>IF(SUM($D$32:$G$33)&lt;=MAKSBELOP,G33,IF(SUM($D$32:$G$32)&lt;=MAKSBELOP,ROUND(PersonRemainder*G33/SUM($D$33:$G$33),0),0))</f>
+        <v>0</v>
+      </c>
+      <c r="H37" s="31" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A37" s="29"/>
-      <c r="B37" s="30" t="s">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" s="27"/>
+      <c r="B38" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="C37" s="31">
-        <f>MAKSBELOP-SUM(D34:G36)</f>
-        <v>0</v>
-      </c>
-      <c r="D37" s="30"/>
-      <c r="E37" s="30"/>
-      <c r="F37" s="30"/>
-      <c r="G37" s="30"/>
-      <c r="H37" s="33" t="s">
+      <c r="C38" s="29">
+        <f>MAKSBELOP-SUM(D35:G37)</f>
+        <v>0</v>
+      </c>
+      <c r="D38" s="28"/>
+      <c r="E38" s="28"/>
+      <c r="F38" s="28"/>
+      <c r="G38" s="28"/>
+      <c r="H38" s="31" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A39" s="8" t="s">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B39" s="9"/>
-      <c r="C39" s="10"/>
-      <c r="D39" s="11"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A40" s="37" t="s">
+      <c r="B40" s="9"/>
+      <c r="C40" s="10"/>
+      <c r="D40" s="11"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="B40" s="37"/>
-      <c r="C40" s="37"/>
-      <c r="D40" s="37"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A42" s="17" t="s">
+      <c r="B41" s="35"/>
+      <c r="C41" s="35"/>
+      <c r="D41" s="35"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A43" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="B42" s="18">
+      <c r="B43" s="16">
         <v>1430.76</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A43" s="17" t="s">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A44" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="B43" s="18">
-        <f>ROUND(B42*260/12,0)</f>
+      <c r="B44" s="16">
+        <f>ROUND(B43*260/12,0)</f>
         <v>31000</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="A40:D40"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="A41:D41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Legger til fane med beregning uten avrunding underveis i excel-arket
</commit_message>
<xml_diff>
--- a/doc/okonomi/Utbetaling.xlsx
+++ b/doc/okonomi/Utbetaling.xlsx
@@ -1,24 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fred/src/nav/helse-spleis/doc/okonomi/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martetarnes/IdeaProjects/helse-spleis/doc/okonomi/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9141110E-8969-654B-834F-5815260768D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FFA8C1D-B8E4-9040-B9E3-3F26D03D32BA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31160" yWindow="1500" windowWidth="32120" windowHeight="22420" xr2:uid="{4751B54A-2E15-734D-9A93-8E38B5748ECD}"/>
+    <workbookView xWindow="28800" yWindow="-18160" windowWidth="76800" windowHeight="42700" activeTab="1" xr2:uid="{4751B54A-2E15-734D-9A93-8E38B5748ECD}"/>
   </bookViews>
   <sheets>
     <sheet name="Multiple Employers" sheetId="2" r:id="rId1"/>
+    <sheet name="Multiple Employers no rounding" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="AdjustmentArb">'Multiple Employers'!$D$24:$G$24</definedName>
     <definedName name="MAKSBELOP">'Multiple Employers'!$C$16</definedName>
+    <definedName name="MAKSBELOP2">'Multiple Employers no rounding'!$C$16</definedName>
     <definedName name="PersonRemainder">'Multiple Employers'!$C$36</definedName>
+    <definedName name="PersonRemainder2">'Multiple Employers no rounding'!$C$36</definedName>
     <definedName name="ScalingFactor">'Multiple Employers'!$C$17</definedName>
     <definedName name="ShortfallIncomeRatioArb">'Multiple Employers'!$D$21:$G$21</definedName>
     <definedName name="ShortfallIncomeRatioPerson">'Multiple Employers'!$D$25:$G$25</definedName>
@@ -41,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="69">
   <si>
     <t>Term</t>
   </si>
@@ -274,13 +277,15 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="_(* #,##0.0000000000_);_(* \(#,##0.0000000000\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="167" formatCode="_(* #,##0.0000000000_);_(* \(#,##0.0000000000\);_(* &quot;-&quot;??????????_);_(@_)"/>
+    <numFmt numFmtId="168" formatCode="0.0000000000%"/>
+    <numFmt numFmtId="169" formatCode="#,##0.0000000000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -326,8 +331,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -356,6 +368,12 @@
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDEBF7"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -388,7 +406,7 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -439,19 +457,25 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="6" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Per cent" xfId="2" builtinId="5"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -765,9 +789,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBE9F233-0C57-4B39-8C81-6D2F9F1844A9}">
   <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -886,7 +910,7 @@
       <c r="H5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="I5" s="36" t="s">
+      <c r="I5" s="34" t="s">
         <v>65</v>
       </c>
     </row>
@@ -969,7 +993,7 @@
       <c r="H8" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="I8" s="36" t="s">
+      <c r="I8" s="34" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1080,7 +1104,7 @@
       <c r="B13" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="37">
+      <c r="C13" s="35">
         <f>ROUND(SUM(D10:G10)/SUM(D7:G7),2)</f>
         <v>0.4</v>
       </c>
@@ -1095,8 +1119,8 @@
       <c r="B14" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="7">
-        <v>93634</v>
+      <c r="C14" s="43">
+        <v>101351</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>2</v>
@@ -1111,12 +1135,12 @@
       </c>
       <c r="C15" s="1">
         <f>ROUND(6*C14/260, 0)</f>
-        <v>2161</v>
+        <v>2339</v>
       </c>
       <c r="H15" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="I15" s="36" t="s">
+      <c r="I15" s="34" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1129,7 +1153,7 @@
       </c>
       <c r="C16" s="1">
         <f>ROUND(C13*C15,0)</f>
-        <v>864</v>
+        <v>936</v>
       </c>
       <c r="H16" s="3" t="s">
         <v>2</v>
@@ -1144,7 +1168,7 @@
       </c>
       <c r="C17" s="24">
         <f>MIN(1, C16/SUM(D10:G10))</f>
-        <v>0.75789473684210529</v>
+        <v>0.82105263157894737</v>
       </c>
       <c r="D17" s="22"/>
       <c r="E17" s="22"/>
@@ -1164,15 +1188,15 @@
       <c r="C18" s="21"/>
       <c r="D18" s="22">
         <f>D10*ScalingFactor</f>
-        <v>367.28744939271257</v>
+        <v>397.89473684210526</v>
       </c>
       <c r="E18" s="22">
         <f>E10*ScalingFactor</f>
-        <v>279.83805668016197</v>
+        <v>303.15789473684214</v>
       </c>
       <c r="F18" s="22">
         <f>F10*ScalingFactor</f>
-        <v>216.87449392712549</v>
+        <v>234.9473684210526</v>
       </c>
       <c r="G18" s="22">
         <f>G10*ScalingFactor</f>
@@ -1192,11 +1216,11 @@
       <c r="C19" s="21"/>
       <c r="D19" s="22">
         <f>MIN(D18,D12)</f>
-        <v>367.28744939271257</v>
+        <v>397.89473684210526</v>
       </c>
       <c r="E19" s="22">
         <f t="shared" ref="E19:G19" si="6">MIN(E18,E12)</f>
-        <v>279.83805668016197</v>
+        <v>303.15789473684214</v>
       </c>
       <c r="F19" s="22">
         <f t="shared" si="6"/>
@@ -1218,11 +1242,11 @@
       <c r="C20" s="21"/>
       <c r="D20" s="22">
         <f>D19-D12</f>
-        <v>-117.32793522267207</v>
+        <v>-86.720647773279381</v>
       </c>
       <c r="E20" s="22">
         <f t="shared" ref="E20:G20" si="7">E19-E12</f>
-        <v>-52.469635627530408</v>
+        <v>-29.149797570850239</v>
       </c>
       <c r="F20" s="22">
         <f t="shared" si="7"/>
@@ -1303,7 +1327,7 @@
       </c>
       <c r="F23" s="22">
         <f>F18-F19</f>
-        <v>145.33603238866397</v>
+        <v>163.40890688259105</v>
       </c>
       <c r="G23" s="22">
         <f>G18-G19</f>
@@ -1323,11 +1347,11 @@
       <c r="C24" s="21"/>
       <c r="D24" s="22">
         <f>MIN(-D20,IF(SUM($D$20:$G$20)&gt;=0, 0, SUM($D$23:$G$23)*D22))</f>
-        <v>98.453441295546554</v>
+        <v>86.720647773279381</v>
       </c>
       <c r="E24" s="22">
         <f t="shared" ref="E24:G24" si="9">MIN(-E20,IF(SUM($D$20:$G$20)&gt;=0, 0, SUM($D$23:$G$23)*E22))</f>
-        <v>46.882591093117405</v>
+        <v>29.149797570850239</v>
       </c>
       <c r="F24" s="22">
         <f t="shared" si="9"/>
@@ -1403,11 +1427,11 @@
       <c r="C27" s="21"/>
       <c r="D27" s="25">
         <f>ROUND(D19+D24,0)</f>
-        <v>466</v>
+        <v>485</v>
       </c>
       <c r="E27" s="25">
         <f t="shared" ref="E27:G27" si="11">ROUND(E19+E24,0)</f>
-        <v>327</v>
+        <v>332</v>
       </c>
       <c r="F27" s="25">
         <f t="shared" si="11"/>
@@ -1439,7 +1463,7 @@
       </c>
       <c r="F28" s="21">
         <f>ROUND(F23-SUM(AdjustmentArb)*F26,0)</f>
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="G28" s="21">
         <f>ROUND(G23-SUM(AdjustmentArb)*G26,0)</f>
@@ -1562,14 +1586,14 @@
       <c r="B34" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="C34" s="34" t="str">
+      <c r="C34" s="36" t="str">
         <f>IF(SUM(D32:G33)&lt;=MAKSBELOP,"Everyone paid",IF(SUM(D32:G32)&lt;=MAKSBELOP,"Arbeidsgivere fully paid; Person partially paid by Person request", "Arbeidsgivere partial payment ratio by Arbeidsgiver request"))</f>
-        <v>Arbeidsgivere partial payment ratio by Arbeidsgiver request</v>
-      </c>
-      <c r="D34" s="34"/>
-      <c r="E34" s="34"/>
-      <c r="F34" s="34"/>
-      <c r="G34" s="34"/>
+        <v>Arbeidsgivere fully paid; Person partially paid by Person request</v>
+      </c>
+      <c r="D34" s="36"/>
+      <c r="E34" s="36"/>
+      <c r="F34" s="36"/>
+      <c r="G34" s="36"/>
       <c r="H34" s="31"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
@@ -1582,15 +1606,15 @@
       <c r="C35" s="29"/>
       <c r="D35" s="28">
         <f>IF(SUM($D$32:$G$33)&lt;=MAKSBELOP,D32,IF(SUM($D$32:$G$32)&lt;=MAKSBELOP,D32,ROUND(D32*MAKSBELOP/SUM($D$32:$G$32),0)))</f>
-        <v>471</v>
+        <v>485</v>
       </c>
       <c r="E35" s="28">
         <f>IF(SUM($D$32:$G$33)&lt;=MAKSBELOP,E32,IF(SUM($D$32:$G$32)&lt;=MAKSBELOP,E32,ROUND(E32*MAKSBELOP/SUM($D$32:$G$32),0)))</f>
-        <v>323</v>
+        <v>332</v>
       </c>
       <c r="F35" s="28">
         <f>IF(SUM($D$32:$G$33)&lt;=MAKSBELOP,F32,IF(SUM($D$32:$G$32)&lt;=MAKSBELOP,F32,ROUND(F32*MAKSBELOP/SUM($D$32:$G$32),0)))</f>
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G35" s="28">
         <f>IF(SUM($D$32:$G$33)&lt;=MAKSBELOP,G32,IF(SUM($D$32:$G$32)&lt;=MAKSBELOP,G32,ROUND(G32*MAKSBELOP/SUM($D$32:$G$32),0)))</f>
@@ -1607,7 +1631,7 @@
       </c>
       <c r="C36" s="29">
         <f>MAKSBELOP-SUM(D35:G35)</f>
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="D36" s="28"/>
       <c r="E36" s="28"/>
@@ -1629,11 +1653,11 @@
       </c>
       <c r="E37" s="28">
         <f>IF(SUM($D$32:$G$33)&lt;=MAKSBELOP,E33,IF(SUM($D$32:$G$32)&lt;=MAKSBELOP,ROUND(PersonRemainder*E33/SUM($D$33:$G$33),0),0))</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F37" s="28">
         <f>IF(SUM($D$32:$G$33)&lt;=MAKSBELOP,F33,IF(SUM($D$32:$G$32)&lt;=MAKSBELOP,ROUND(PersonRemainder*F33/SUM($D$33:$G$33),0),0))</f>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="G37" s="28">
         <f>IF(SUM($D$32:$G$33)&lt;=MAKSBELOP,G33,IF(SUM($D$32:$G$32)&lt;=MAKSBELOP,ROUND(PersonRemainder*G33/SUM($D$33:$G$33),0),0))</f>
@@ -1669,12 +1693,12 @@
       <c r="D40" s="11"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A41" s="35" t="s">
+      <c r="A41" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="B41" s="35"/>
-      <c r="C41" s="35"/>
-      <c r="D41" s="35"/>
+      <c r="B41" s="37"/>
+      <c r="C41" s="37"/>
+      <c r="D41" s="37"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="15" t="s">
@@ -1700,4 +1724,896 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A506B608-BF2F-BB48-9883-32866B0664B3}">
+  <dimension ref="A1:H38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="139" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="35.6640625" customWidth="1"/>
+    <col min="2" max="2" width="42.1640625" customWidth="1"/>
+    <col min="3" max="3" width="21.1640625" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="4"/>
+      <c r="H2" s="3"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="7">
+        <v>21000</v>
+      </c>
+      <c r="E3" s="7">
+        <v>10000</v>
+      </c>
+      <c r="F3" s="7">
+        <v>31000</v>
+      </c>
+      <c r="G3" s="7">
+        <v>0</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="4"/>
+      <c r="B4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="19">
+        <f>D3/SUM($D$3:$G$3)</f>
+        <v>0.33870967741935482</v>
+      </c>
+      <c r="E4" s="19">
+        <f t="shared" ref="E4:G4" si="0">E3/SUM($D$3:$G$3)</f>
+        <v>0.16129032258064516</v>
+      </c>
+      <c r="F4" s="19">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="G4" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="2">
+        <f>D3*12/260</f>
+        <v>969.23076923076928</v>
+      </c>
+      <c r="E5" s="2">
+        <f t="shared" ref="E5:G5" si="1">E3*12/260</f>
+        <v>461.53846153846155</v>
+      </c>
+      <c r="F5" s="2">
+        <f t="shared" si="1"/>
+        <v>1430.7692307692307</v>
+      </c>
+      <c r="G5" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="13">
+        <v>1</v>
+      </c>
+      <c r="E6" s="13">
+        <v>1</v>
+      </c>
+      <c r="F6" s="13">
+        <v>1</v>
+      </c>
+      <c r="G6" s="13">
+        <v>1</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="2">
+        <f>D5*D6</f>
+        <v>969.23076923076928</v>
+      </c>
+      <c r="E7" s="2">
+        <f t="shared" ref="E7:G7" si="2">E5*E6</f>
+        <v>461.53846153846155</v>
+      </c>
+      <c r="F7" s="2">
+        <f t="shared" si="2"/>
+        <v>1430.7692307692307</v>
+      </c>
+      <c r="G7" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B8" t="s">
+        <v>67</v>
+      </c>
+      <c r="D8" s="1">
+        <f>MIN(D7,$C$15)</f>
+        <v>969.23076923076928</v>
+      </c>
+      <c r="E8" s="1">
+        <f t="shared" ref="E8:G8" si="3">MIN(E7,$C$15)</f>
+        <v>461.53846153846155</v>
+      </c>
+      <c r="F8" s="1">
+        <f t="shared" si="3"/>
+        <v>1430.7692307692307</v>
+      </c>
+      <c r="G8" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="E9" s="14">
+        <v>0.8</v>
+      </c>
+      <c r="F9" s="14">
+        <v>0.2</v>
+      </c>
+      <c r="G9" s="14">
+        <v>1</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="2">
+        <f>D7*D9</f>
+        <v>484.61538461538464</v>
+      </c>
+      <c r="E10" s="2">
+        <f t="shared" ref="E10:G10" si="4">E7*E9</f>
+        <v>369.23076923076928</v>
+      </c>
+      <c r="F10" s="2">
+        <f t="shared" si="4"/>
+        <v>286.15384615384613</v>
+      </c>
+      <c r="G10" s="2">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="13">
+        <v>1</v>
+      </c>
+      <c r="E11" s="13">
+        <v>0.9</v>
+      </c>
+      <c r="F11" s="13">
+        <v>0.25</v>
+      </c>
+      <c r="G11" s="13">
+        <v>1</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="12">
+        <f>D10*D11</f>
+        <v>484.61538461538464</v>
+      </c>
+      <c r="E12" s="12">
+        <f t="shared" ref="E12:G12" si="5">E10*E11</f>
+        <v>332.30769230769238</v>
+      </c>
+      <c r="F12" s="12">
+        <f t="shared" si="5"/>
+        <v>71.538461538461533</v>
+      </c>
+      <c r="G12" s="12">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="38">
+        <f>SUM(D10:G10)/SUM(D7:G7)</f>
+        <v>0.39838709677419348</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="7">
+        <v>101351</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="39">
+        <f>6*C14/260</f>
+        <v>2338.8692307692309</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="39">
+        <f>C13*C15</f>
+        <v>931.77532258064502</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="24">
+        <f>MIN(1, C16/SUM(D10:G10))</f>
+        <v>0.81734677419354829</v>
+      </c>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="23" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="21"/>
+      <c r="D18" s="22">
+        <f>D10*ScalingFactor</f>
+        <v>397.89473684210526</v>
+      </c>
+      <c r="E18" s="22">
+        <f>E10*ScalingFactor</f>
+        <v>303.15789473684214</v>
+      </c>
+      <c r="F18" s="22">
+        <f>F10*ScalingFactor</f>
+        <v>234.9473684210526</v>
+      </c>
+      <c r="G18" s="22">
+        <f>G10*ScalingFactor</f>
+        <v>0</v>
+      </c>
+      <c r="H18" s="23" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" s="21"/>
+      <c r="D19" s="22">
+        <f>MIN(D18,D12)</f>
+        <v>397.89473684210526</v>
+      </c>
+      <c r="E19" s="22">
+        <f t="shared" ref="E19:G19" si="6">MIN(E18,E12)</f>
+        <v>303.15789473684214</v>
+      </c>
+      <c r="F19" s="22">
+        <f t="shared" si="6"/>
+        <v>71.538461538461533</v>
+      </c>
+      <c r="G19" s="22">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="H19" s="23" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="20"/>
+      <c r="B20" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" s="21"/>
+      <c r="D20" s="22">
+        <f>D19-D12</f>
+        <v>-86.720647773279381</v>
+      </c>
+      <c r="E20" s="22">
+        <f t="shared" ref="E20:G20" si="7">E19-E12</f>
+        <v>-29.149797570850239</v>
+      </c>
+      <c r="F20" s="22">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="G20" s="22">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="H20" s="23" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="20"/>
+      <c r="B21" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" s="21"/>
+      <c r="D21" s="24">
+        <f>IF(D20 &lt; 0, D4, 0)</f>
+        <v>0.33870967741935482</v>
+      </c>
+      <c r="E21" s="24">
+        <f t="shared" ref="E21:F21" si="8">IF(E20 &lt; 0, E4, 0)</f>
+        <v>0.16129032258064516</v>
+      </c>
+      <c r="F21" s="24">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="G21" s="22"/>
+      <c r="H21" s="23" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="C22" s="21"/>
+      <c r="D22" s="24">
+        <f>IF(SUM(ShortfallIncomeRatioArb)=0,0,D21/SUM(ShortfallIncomeRatioArb))</f>
+        <v>0.67741935483870963</v>
+      </c>
+      <c r="E22" s="24">
+        <f>IF(SUM(ShortfallIncomeRatioArb)=0,0,E21/SUM(ShortfallIncomeRatioArb))</f>
+        <v>0.32258064516129031</v>
+      </c>
+      <c r="F22" s="24">
+        <f>IF(SUM(ShortfallIncomeRatioArb)=0,0,F21/SUM(ShortfallIncomeRatioArb))</f>
+        <v>0</v>
+      </c>
+      <c r="G22" s="24">
+        <f>IF(SUM(ShortfallIncomeRatioArb)=0,0,G21/SUM(ShortfallIncomeRatioArb))</f>
+        <v>0</v>
+      </c>
+      <c r="H22" s="23" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="20"/>
+      <c r="B23" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23" s="21"/>
+      <c r="D23" s="22">
+        <f>D18-D19</f>
+        <v>0</v>
+      </c>
+      <c r="E23" s="22">
+        <f>E18-E19</f>
+        <v>0</v>
+      </c>
+      <c r="F23" s="22">
+        <f>F18-F19</f>
+        <v>163.40890688259105</v>
+      </c>
+      <c r="G23" s="22">
+        <f>G18-G19</f>
+        <v>0</v>
+      </c>
+      <c r="H23" s="23" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C24" s="21"/>
+      <c r="D24" s="22">
+        <f>MIN(-D20,IF(SUM($D$20:$G$20)&gt;=0, 0, SUM($D$23:$G$23)*D22))</f>
+        <v>86.720647773279381</v>
+      </c>
+      <c r="E24" s="22">
+        <f t="shared" ref="E24:G24" si="9">MIN(-E20,IF(SUM($D$20:$G$20)&gt;=0, 0, SUM($D$23:$G$23)*E22))</f>
+        <v>29.149797570850239</v>
+      </c>
+      <c r="F24" s="22">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="G24" s="22">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="H24" s="23" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="20"/>
+      <c r="B25" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="C25" s="21"/>
+      <c r="D25" s="24">
+        <f>IF(D23 = 0, 0, D4)</f>
+        <v>0</v>
+      </c>
+      <c r="E25" s="24">
+        <f t="shared" ref="E25:G25" si="10">IF(E23 = 0, 0, E4)</f>
+        <v>0</v>
+      </c>
+      <c r="F25" s="24">
+        <f t="shared" si="10"/>
+        <v>0.5</v>
+      </c>
+      <c r="G25" s="24">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="H25" s="23" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="20"/>
+      <c r="B26" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="C26" s="21"/>
+      <c r="D26" s="24">
+        <f>IF(SUM(ShortfallIncomeRatioPerson)= 0, 0, D25/SUM(ShortfallIncomeRatioPerson))</f>
+        <v>0</v>
+      </c>
+      <c r="E26" s="24">
+        <f>IF(SUM(ShortfallIncomeRatioPerson)= 0, 0, E25/SUM(ShortfallIncomeRatioPerson))</f>
+        <v>0</v>
+      </c>
+      <c r="F26" s="24">
+        <f>IF(SUM(ShortfallIncomeRatioPerson)= 0, 0, F25/SUM(ShortfallIncomeRatioPerson))</f>
+        <v>1</v>
+      </c>
+      <c r="G26" s="24">
+        <f>IF(SUM(ShortfallIncomeRatioPerson)= 0, 0, G25/SUM(ShortfallIncomeRatioPerson))</f>
+        <v>0</v>
+      </c>
+      <c r="H26" s="23" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" s="21"/>
+      <c r="D27" s="25">
+        <f>ROUND(D19+D24,0)</f>
+        <v>485</v>
+      </c>
+      <c r="E27" s="25">
+        <f t="shared" ref="E27:G27" si="11">ROUND(E19+E24,0)</f>
+        <v>332</v>
+      </c>
+      <c r="F27" s="25">
+        <f t="shared" si="11"/>
+        <v>72</v>
+      </c>
+      <c r="G27" s="22">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="H27" s="23" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B28" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" s="21"/>
+      <c r="D28" s="21">
+        <f>ROUND(D23-SUM(AdjustmentArb)*D26,0)</f>
+        <v>0</v>
+      </c>
+      <c r="E28" s="21">
+        <f>ROUND(E23-SUM(AdjustmentArb)*E26,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F28" s="21">
+        <f>ROUND(F23-SUM(AdjustmentArb)*F26,0)</f>
+        <v>48</v>
+      </c>
+      <c r="G28" s="21">
+        <f>ROUND(G23-SUM(AdjustmentArb)*G26,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H28" s="23" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="20"/>
+      <c r="B29" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29" s="26">
+        <f>C16-SUM(D27:G28)</f>
+        <v>-5.2246774193549754</v>
+      </c>
+      <c r="D29" s="21"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="21"/>
+      <c r="G29" s="21"/>
+      <c r="H29" s="23" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="4"/>
+      <c r="C30" s="17"/>
+      <c r="H30" s="3"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="B31" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="C31" s="29"/>
+      <c r="D31" s="40">
+        <f>D10</f>
+        <v>484.61538461538464</v>
+      </c>
+      <c r="E31" s="40">
+        <f>E10</f>
+        <v>369.23076923076928</v>
+      </c>
+      <c r="F31" s="40">
+        <f>F10</f>
+        <v>286.15384615384613</v>
+      </c>
+      <c r="G31" s="30">
+        <f t="shared" ref="G31" si="12">ROUND(G10,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H31" s="31" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="B32" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="C32" s="29"/>
+      <c r="D32" s="40">
+        <f>D12</f>
+        <v>484.61538461538464</v>
+      </c>
+      <c r="E32" s="40">
+        <f>E12</f>
+        <v>332.30769230769238</v>
+      </c>
+      <c r="F32" s="40">
+        <f>F12</f>
+        <v>71.538461538461533</v>
+      </c>
+      <c r="G32" s="30">
+        <f t="shared" ref="G32" si="13">ROUND(G12,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H32" s="31" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="B33" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="C33" s="29"/>
+      <c r="D33" s="40">
+        <f>D31-D32</f>
+        <v>0</v>
+      </c>
+      <c r="E33" s="40">
+        <f t="shared" ref="E33:G33" si="14">E31-E32</f>
+        <v>36.923076923076906</v>
+      </c>
+      <c r="F33" s="40">
+        <f t="shared" si="14"/>
+        <v>214.61538461538458</v>
+      </c>
+      <c r="G33" s="30">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="H33" s="31" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" s="27"/>
+      <c r="B34" s="32" t="s">
+        <v>61</v>
+      </c>
+      <c r="C34" s="36" t="str">
+        <f>IF(SUM(D32:G33)&lt;=MAKSBELOP,"Everyone paid",IF(SUM(D32:G32)&lt;=MAKSBELOP,"Arbeidsgivere fully paid; Person partially paid by Person request", "Arbeidsgivere partial payment ratio by Arbeidsgiver request"))</f>
+        <v>Arbeidsgivere fully paid; Person partially paid by Person request</v>
+      </c>
+      <c r="D34" s="36"/>
+      <c r="E34" s="36"/>
+      <c r="F34" s="36"/>
+      <c r="G34" s="36"/>
+      <c r="H34" s="31"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B35" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C35" s="29"/>
+      <c r="D35" s="28">
+        <f>IF(SUM($D$32:$G$33)&lt;=MAKSBELOP2,ROUND(D32,0),IF(SUM($D$32:$G$32)&lt;=MAKSBELOP2,ROUND(D32,0),ROUND(D32*MAKSBELOP2/SUM($D$32:$G$32),0)))</f>
+        <v>485</v>
+      </c>
+      <c r="E35" s="28">
+        <f>IF(SUM($D$32:$G$33)&lt;=MAKSBELOP2,ROUND(E32,0),IF(SUM($D$32:$G$32)&lt;=MAKSBELOP2,ROUND(E32,0),ROUND(E32*MAKSBELOP2/SUM($D$32:$G$32),0)))</f>
+        <v>332</v>
+      </c>
+      <c r="F35" s="28">
+        <f>IF(SUM($D$32:$G$33)&lt;=MAKSBELOP2,ROUND(F32,0),IF(SUM($D$32:$G$32)&lt;=MAKSBELOP2,ROUND(F32,0),ROUND(F32*MAKSBELOP2/SUM($D$32:$G$32),0)))</f>
+        <v>72</v>
+      </c>
+      <c r="G35" s="28">
+        <f>IF(SUM($D$32:$G$33)&lt;=MAKSBELOP,G32,IF(SUM($D$32:$G$32)&lt;=MAKSBELOP,G32,ROUND(G32*MAKSBELOP/SUM($D$32:$G$32),0)))</f>
+        <v>0</v>
+      </c>
+      <c r="H35" s="31" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" s="27"/>
+      <c r="B36" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="C36" s="41">
+        <f>MAKSBELOP2-SUM(D35:G35)</f>
+        <v>42.775322580645025</v>
+      </c>
+      <c r="D36" s="28"/>
+      <c r="E36" s="28"/>
+      <c r="F36" s="28"/>
+      <c r="G36" s="28"/>
+      <c r="H36" s="31"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="B37" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="C37" s="28"/>
+      <c r="D37" s="42">
+        <f>IF(SUM($D$32:$G$33)&lt;=MAKSBELOP2,ROUND(D33,0),IF(SUM($D$32:$G$32)&lt;=MAKSBELOP2,ROUND(PersonRemainder2*D33/SUM($D$33:$G$33),0),0))</f>
+        <v>0</v>
+      </c>
+      <c r="E37" s="42">
+        <f>IF(SUM($D$32:$G$33)&lt;=MAKSBELOP2,ROUND(E33,0),IF(SUM($D$32:$G$32)&lt;=MAKSBELOP2,ROUND(PersonRemainder2*E33/SUM($D$33:$G$33),0),0))</f>
+        <v>6</v>
+      </c>
+      <c r="F37" s="42">
+        <f>IF(SUM($D$32:$G$33)&lt;=MAKSBELOP2,ROUND(F33,0),IF(SUM($D$32:$G$32)&lt;=MAKSBELOP2,ROUND(PersonRemainder2*F33/SUM($D$33:$G$33),0),0))</f>
+        <v>36</v>
+      </c>
+      <c r="G37" s="28">
+        <f>IF(SUM($D$32:$G$33)&lt;=MAKSBELOP,G33,IF(SUM($D$32:$G$32)&lt;=MAKSBELOP,ROUND(PersonRemainder*G33/SUM($D$33:$G$33),0),0))</f>
+        <v>0</v>
+      </c>
+      <c r="H37" s="31" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" s="27"/>
+      <c r="B38" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="C38" s="41">
+        <f>MAKSBELOP2-SUM(D35:G37)</f>
+        <v>0.77532258064502457</v>
+      </c>
+      <c r="D38" s="28"/>
+      <c r="E38" s="28"/>
+      <c r="F38" s="28"/>
+      <c r="G38" s="28"/>
+      <c r="H38" s="31" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C34:G34"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Endre beregning av utbetaling ved å avrunde til slutt
Co-authored-by: Kevin Sillerud <kevin.sillerud@gmail.com>
</commit_message>
<xml_diff>
--- a/doc/okonomi/Utbetaling.xlsx
+++ b/doc/okonomi/Utbetaling.xlsx
@@ -1,30 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martetarnes/IdeaProjects/helse-spleis/doc/okonomi/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hegehaavaldsen/Develop/helse-spleis/doc/okonomi/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FFA8C1D-B8E4-9040-B9E3-3F26D03D32BA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0A9B7828-7FFB-364B-80D2-00FBDB51F5D8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="-18160" windowWidth="76800" windowHeight="42700" activeTab="1" xr2:uid="{4751B54A-2E15-734D-9A93-8E38B5748ECD}"/>
+    <workbookView xWindow="35840" yWindow="-20300" windowWidth="38400" windowHeight="42700" xr2:uid="{4751B54A-2E15-734D-9A93-8E38B5748ECD}"/>
   </bookViews>
   <sheets>
-    <sheet name="Multiple Employers" sheetId="2" r:id="rId1"/>
-    <sheet name="Multiple Employers no rounding" sheetId="3" r:id="rId2"/>
+    <sheet name="Flere arbeidsgivere, ny " sheetId="4" r:id="rId1"/>
+    <sheet name="Flere arbeidsgivere, gammel" sheetId="2" r:id="rId2"/>
+    <sheet name="Flere arbeidsgivere, eldre" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="AdjustmentArb">'Multiple Employers'!$D$24:$G$24</definedName>
-    <definedName name="MAKSBELOP">'Multiple Employers'!$C$16</definedName>
-    <definedName name="MAKSBELOP2">'Multiple Employers no rounding'!$C$16</definedName>
-    <definedName name="PersonRemainder">'Multiple Employers'!$C$36</definedName>
-    <definedName name="PersonRemainder2">'Multiple Employers no rounding'!$C$36</definedName>
-    <definedName name="ScalingFactor">'Multiple Employers'!$C$17</definedName>
-    <definedName name="ShortfallIncomeRatioArb">'Multiple Employers'!$D$21:$G$21</definedName>
-    <definedName name="ShortfallIncomeRatioPerson">'Multiple Employers'!$D$25:$G$25</definedName>
+    <definedName name="AdjustmentArb">'Flere arbeidsgivere, gammel'!$D$24:$G$24</definedName>
+    <definedName name="MAKSBELOP">'Flere arbeidsgivere, gammel'!$C$16</definedName>
+    <definedName name="MAKSBELOP2">'Flere arbeidsgivere, eldre'!$C$16</definedName>
+    <definedName name="MAKSBELOP3">'Flere arbeidsgivere, ny '!$B$16</definedName>
+    <definedName name="PersonRemainder">'Flere arbeidsgivere, gammel'!$C$36</definedName>
+    <definedName name="PersonRemainder2">'Flere arbeidsgivere, eldre'!$C$36</definedName>
+    <definedName name="ScalingFactor">'Flere arbeidsgivere, gammel'!$C$17</definedName>
+    <definedName name="ShortfallIncomeRatioArb">'Flere arbeidsgivere, gammel'!$D$21:$G$21</definedName>
+    <definedName name="ShortfallIncomeRatioPerson">'Flere arbeidsgivere, gammel'!$D$25:$G$25</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="120">
   <si>
     <t>Term</t>
   </si>
@@ -272,20 +274,174 @@
   <si>
     <t>New: Fred 26-06</t>
   </si>
+  <si>
+    <t xml:space="preserve">Arbeidsgiverbeløp før avrunding </t>
+  </si>
+  <si>
+    <t>Rest til utbetaling til arbeidsgiver</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total utbetaling til arbeidsgivere </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Totalt utbetalt </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rest til utbetaling til person </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Personutbetalinger </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Personutbetalinger før avrunding </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brukes til å fordele restbeløp </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inkludert restbeløpet i raden over </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Utebetales til arbeidsgivere fordelt etter differansen i rad 25 (høyeste tall får penger først) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avrundingsdifferanse </t>
+  </si>
+  <si>
+    <t>Avrundingsbeløp fordelt</t>
+  </si>
+  <si>
+    <t>Beregnet månedsinntekt etter § 8-28</t>
+  </si>
+  <si>
+    <t>Arbeidsforholdets inntekts andel av den totale inntekten</t>
+  </si>
+  <si>
+    <t>Dagsats beregnet kun ut ifra beregnet månedsinntekt (uten hensyn til andre arbeidsforhold,grad etc)</t>
+  </si>
+  <si>
+    <t>For arbeidstaker er det 100%, for næringsdrivende 80%</t>
+  </si>
+  <si>
+    <t>Maks dagsats før reduksjon til 6G og reduksjon for sykmeldingsgrad</t>
+  </si>
+  <si>
+    <t>Maks dagsats ved en arbeidsgiver og 100% syk</t>
+  </si>
+  <si>
+    <t>Arbeidsuførhetsgrad</t>
+  </si>
+  <si>
+    <t>Maks dagsats redusert for arbeidsuførhetsgrad</t>
+  </si>
+  <si>
+    <t>Hvor mange prosent arbeidsgiver krever i refusjon</t>
+  </si>
+  <si>
+    <t>Det beløpet arbeidsgiver skal ha refundert/forventer å få ut ifra refusjonsgrad</t>
+  </si>
+  <si>
+    <t>Den totale graden av arbeidsuførhet på tvers av alle arbeidsforholdene</t>
+  </si>
+  <si>
+    <t>Grunnbeløpet pr år</t>
+  </si>
+  <si>
+    <t>Maks dagsats etter reduksjon for 6G</t>
+  </si>
+  <si>
+    <t>Maks dagsats bruker kan få ut ifra den totale graden av arbeidsuførhet på tvers av alle arbeidsforholdene, redusert for 6G</t>
+  </si>
+  <si>
+    <t>Maks dagsats redusert for grad av arbeidsuførhet</t>
+  </si>
+  <si>
+    <t>Det beløpet arbeidsgiver krever refundert/forventer å få ut ifra refusjonsgrad</t>
+  </si>
+  <si>
+    <t>Det beløpet arbeidstakeren kan få utbetalt før reduskjon for 6G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Situasjon </t>
+  </si>
+  <si>
+    <t>Fordelt restbeløp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brukes til å fordele restbeløp i B29 på alle arbeidsgiverne  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Utbetaling til arbeidsfivere med avrunding og fordelt restbeløp </t>
+  </si>
+  <si>
+    <t>Avrundet arbeidsgiverbeløp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total utbetaling til arbeidsgivere (inkludert restbeløpet i raden over) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Personutbetaling før avrunding </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avrundingsbeløp fordelt </t>
+  </si>
+  <si>
+    <t>Arbeidsgiverbeløp, inkl. avrunding</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Personbeløp, inkl. avrunding </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Formel: Det arbeidsgiver skal ha i refusjon ganger maks samlet dagsats redusert for 6G, delt på totalt refusjonskrav for alle arbeidsgiverne. </t>
+  </si>
+  <si>
+    <t>Eksempel: 969 x 2150/2629 = 792</t>
+  </si>
+  <si>
+    <t>Utebetales til arbeidstakere fordelt etter differansen i rad 34 (høyest tall får penger først)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Begrep	</t>
+  </si>
+  <si>
+    <t>Arbeidsgiver 1</t>
+  </si>
+  <si>
+    <t>Arbeidsgiver 2</t>
+  </si>
+  <si>
+    <t>Arbeidsgiver 3</t>
+  </si>
+  <si>
+    <t>Arbeidsgiver 4</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Kommentar</t>
+  </si>
+  <si>
+    <t>Desimaltall</t>
+  </si>
+  <si>
+    <t>Heltall</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="6">
+  <numFmts count="7">
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="_(* #,##0.0000000000_);_(* \(#,##0.0000000000\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="167" formatCode="_(* #,##0.0000000000_);_(* \(#,##0.0000000000\);_(* &quot;-&quot;??????????_);_(@_)"/>
     <numFmt numFmtId="168" formatCode="0.0000000000%"/>
     <numFmt numFmtId="169" formatCode="#,##0.0000000000"/>
+    <numFmt numFmtId="170" formatCode="0.0000000000"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -331,13 +487,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -372,12 +521,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFDDEBF7"/>
-        <bgColor rgb="FF000000"/>
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -400,13 +549,59 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -459,23 +654,80 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="6" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="2" builtinId="5"/>
+    <cellStyle name="Per cent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -786,12 +1038,953 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29F2E11B-4534-BF4F-894D-178F9F0F299B}">
+  <dimension ref="A1:H51"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="31.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="107.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="D1" s="27" t="s">
+        <v>113</v>
+      </c>
+      <c r="E1" s="27" t="s">
+        <v>114</v>
+      </c>
+      <c r="F1" s="27" t="s">
+        <v>115</v>
+      </c>
+      <c r="G1" s="52" t="s">
+        <v>116</v>
+      </c>
+      <c r="H1" s="27" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="53"/>
+      <c r="B2" s="54"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="49"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="53" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="54"/>
+      <c r="C3" s="56">
+        <f>499*260/12</f>
+        <v>10811.666666666666</v>
+      </c>
+      <c r="D3" s="56">
+        <v>0</v>
+      </c>
+      <c r="E3" s="56">
+        <v>0</v>
+      </c>
+      <c r="F3" s="56"/>
+      <c r="G3" s="55" t="s">
+        <v>118</v>
+      </c>
+      <c r="H3" s="49" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="53"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="57">
+        <f>C3/SUM($C$3:$F$3)</f>
+        <v>1</v>
+      </c>
+      <c r="D4" s="57">
+        <f t="shared" ref="D4:F4" si="0">D3/SUM($C$3:$F$3)</f>
+        <v>0</v>
+      </c>
+      <c r="E4" s="57">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F4" s="57">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G4" s="55" t="s">
+        <v>118</v>
+      </c>
+      <c r="H4" s="49" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="58" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="54"/>
+      <c r="C5" s="59">
+        <f>C3*12/260</f>
+        <v>499</v>
+      </c>
+      <c r="D5" s="59">
+        <f t="shared" ref="D5:E5" si="1">D3*12/260</f>
+        <v>0</v>
+      </c>
+      <c r="E5" s="59">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F5" s="59">
+        <f>F3*12/260</f>
+        <v>0</v>
+      </c>
+      <c r="G5" s="55" t="s">
+        <v>118</v>
+      </c>
+      <c r="H5" s="49" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="53" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="54"/>
+      <c r="C6" s="60">
+        <v>1</v>
+      </c>
+      <c r="D6" s="60">
+        <v>1</v>
+      </c>
+      <c r="E6" s="60">
+        <v>1</v>
+      </c>
+      <c r="F6" s="60">
+        <v>1</v>
+      </c>
+      <c r="G6" s="55" t="s">
+        <v>119</v>
+      </c>
+      <c r="H6" s="49" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="53" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="54"/>
+      <c r="C7" s="59">
+        <f>C5*C6</f>
+        <v>499</v>
+      </c>
+      <c r="D7" s="59">
+        <f t="shared" ref="D7:F7" si="2">D5*D6</f>
+        <v>0</v>
+      </c>
+      <c r="E7" s="59">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F7" s="59">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G7" s="55" t="s">
+        <v>118</v>
+      </c>
+      <c r="H7" s="49" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="53" t="s">
+        <v>66</v>
+      </c>
+      <c r="B8" s="54"/>
+      <c r="C8" s="61">
+        <f>MIN(C7,$B$16)</f>
+        <v>499</v>
+      </c>
+      <c r="D8" s="61">
+        <f t="shared" ref="D8:F8" si="3">MIN(D7,$B$16)</f>
+        <v>0</v>
+      </c>
+      <c r="E8" s="61">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F8" s="61">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G8" s="55" t="s">
+        <v>119</v>
+      </c>
+      <c r="H8" s="49" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="53" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="54"/>
+      <c r="C9" s="62">
+        <v>1</v>
+      </c>
+      <c r="D9" s="62">
+        <v>0.5</v>
+      </c>
+      <c r="E9" s="62">
+        <v>1</v>
+      </c>
+      <c r="F9" s="62">
+        <v>1</v>
+      </c>
+      <c r="G9" s="55" t="s">
+        <v>118</v>
+      </c>
+      <c r="H9" s="49" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="53" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="54"/>
+      <c r="C10" s="59">
+        <f>C7*C9</f>
+        <v>499</v>
+      </c>
+      <c r="D10" s="59">
+        <f>D7*D9</f>
+        <v>0</v>
+      </c>
+      <c r="E10" s="59">
+        <f>E7*E9</f>
+        <v>0</v>
+      </c>
+      <c r="F10" s="59">
+        <f t="shared" ref="F10" si="4">F7*F9</f>
+        <v>0</v>
+      </c>
+      <c r="G10" s="55" t="s">
+        <v>118</v>
+      </c>
+      <c r="H10" s="49" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="53" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="54"/>
+      <c r="C11" s="60">
+        <v>0.5</v>
+      </c>
+      <c r="D11" s="60">
+        <v>1</v>
+      </c>
+      <c r="E11" s="60">
+        <v>1</v>
+      </c>
+      <c r="F11" s="60">
+        <v>1</v>
+      </c>
+      <c r="G11" s="55" t="s">
+        <v>118</v>
+      </c>
+      <c r="H11" s="49" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="53" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="54"/>
+      <c r="C12" s="63">
+        <f>C10*C11</f>
+        <v>249.5</v>
+      </c>
+      <c r="D12" s="63">
+        <f>D10*D11</f>
+        <v>0</v>
+      </c>
+      <c r="E12" s="63">
+        <f t="shared" ref="E12:F12" si="5">E10*E11</f>
+        <v>0</v>
+      </c>
+      <c r="F12" s="63">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="G12" s="55" t="s">
+        <v>118</v>
+      </c>
+      <c r="H12" s="49" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="53" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" s="64">
+        <f>SUM(C10:F10)/SUM(C7:F7)</f>
+        <v>1</v>
+      </c>
+      <c r="C13" s="54"/>
+      <c r="D13" s="54"/>
+      <c r="E13" s="54"/>
+      <c r="F13" s="54"/>
+      <c r="G13" s="55" t="s">
+        <v>118</v>
+      </c>
+      <c r="H13" s="49" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="53" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="56">
+        <v>93634</v>
+      </c>
+      <c r="C14" s="54"/>
+      <c r="D14" s="54"/>
+      <c r="E14" s="54"/>
+      <c r="F14" s="54"/>
+      <c r="G14" s="55" t="s">
+        <v>119</v>
+      </c>
+      <c r="H14" s="49" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="53" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="59">
+        <f>6*B14/260</f>
+        <v>2160.7846153846153</v>
+      </c>
+      <c r="C15" s="54"/>
+      <c r="D15" s="54"/>
+      <c r="E15" s="54"/>
+      <c r="F15" s="54"/>
+      <c r="G15" s="55" t="s">
+        <v>118</v>
+      </c>
+      <c r="H15" s="49" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="53" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="59">
+        <f>ROUND(B13*B15, 0)</f>
+        <v>2161</v>
+      </c>
+      <c r="C16" s="54"/>
+      <c r="D16" s="54"/>
+      <c r="E16" s="54"/>
+      <c r="F16" s="54"/>
+      <c r="G16" s="55" t="s">
+        <v>118</v>
+      </c>
+      <c r="H16" s="49" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="53"/>
+      <c r="B17" s="65"/>
+      <c r="C17" s="54"/>
+      <c r="D17" s="54"/>
+      <c r="E17" s="54"/>
+      <c r="F17" s="54"/>
+      <c r="G17" s="55"/>
+      <c r="H17" s="49"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="29"/>
+      <c r="C18" s="51">
+        <f>C10</f>
+        <v>499</v>
+      </c>
+      <c r="D18" s="51">
+        <f>D10</f>
+        <v>0</v>
+      </c>
+      <c r="E18" s="51">
+        <f>E10</f>
+        <v>0</v>
+      </c>
+      <c r="F18" s="51">
+        <f>F10</f>
+        <v>0</v>
+      </c>
+      <c r="G18" s="31" t="s">
+        <v>118</v>
+      </c>
+      <c r="H18" s="28" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="B19" s="29"/>
+      <c r="C19" s="51">
+        <f>C12</f>
+        <v>249.5</v>
+      </c>
+      <c r="D19" s="51">
+        <f>D12</f>
+        <v>0</v>
+      </c>
+      <c r="E19" s="51">
+        <f>E12</f>
+        <v>0</v>
+      </c>
+      <c r="F19" s="51">
+        <f>F12</f>
+        <v>0</v>
+      </c>
+      <c r="G19" s="31" t="s">
+        <v>118</v>
+      </c>
+      <c r="H19" s="28" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="B20" s="29"/>
+      <c r="C20" s="51">
+        <f>C18-C19</f>
+        <v>249.5</v>
+      </c>
+      <c r="D20" s="51">
+        <f>D18-D19</f>
+        <v>0</v>
+      </c>
+      <c r="E20" s="51">
+        <f t="shared" ref="E20" si="6">E18-E19</f>
+        <v>0</v>
+      </c>
+      <c r="F20" s="51">
+        <f>F18-F19</f>
+        <v>0</v>
+      </c>
+      <c r="G20" s="31" t="s">
+        <v>118</v>
+      </c>
+      <c r="H20" s="28" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="27" t="s">
+        <v>98</v>
+      </c>
+      <c r="B21" s="76" t="str">
+        <f>IF(SUM(C19:F20)&lt;=MAKSBELOP3,"Arbeidsgiver og person blir refundert hele beløpet",IF(SUM(C19:F19)&lt;=MAKSBELOP3,"Arbeidsgivere blir refundert hele beløpet; Person blir delvis refundert", "Arbeidsgivere blir delvis refundert"))</f>
+        <v>Arbeidsgiver og person blir refundert hele beløpet</v>
+      </c>
+      <c r="C21" s="77"/>
+      <c r="D21" s="77"/>
+      <c r="E21" s="77"/>
+      <c r="F21" s="78"/>
+      <c r="G21" s="31"/>
+      <c r="H21" s="28"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="27"/>
+      <c r="B22" s="41"/>
+      <c r="C22" s="42"/>
+      <c r="D22" s="42"/>
+      <c r="E22" s="42"/>
+      <c r="F22" s="43"/>
+      <c r="G22" s="31"/>
+      <c r="H22" s="28"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="B23" s="41"/>
+      <c r="C23" s="50">
+        <f>IF(SUM($C$19:$F$20)&lt;=MAKSBELOP3,C19,IF(SUM($C$19:$F$19)&lt;=MAKSBELOP3,C19, C19*MAKSBELOP3/SUM($C$19:$F$19)))</f>
+        <v>249.5</v>
+      </c>
+      <c r="D23" s="50">
+        <f>IF(SUM($C$19:$F$20)&lt;=MAKSBELOP3,D19,IF(SUM($C$19:$F$19)&lt;=MAKSBELOP3,D19, D19*MAKSBELOP3/SUM($C$19:$F$19)))</f>
+        <v>0</v>
+      </c>
+      <c r="E23" s="50">
+        <f>IF(SUM($C$19:$F$20)&lt;=MAKSBELOP3,E19,IF(SUM($C$19:$F$19)&lt;=MAKSBELOP3,E19, E19*MAKSBELOP3/SUM($C$19:$F$19)))</f>
+        <v>0</v>
+      </c>
+      <c r="F23" s="50">
+        <f>IF(SUM($C$19:$F$20)&lt;=MAKSBELOP3,F19,IF(SUM($C$19:$F$19)&lt;=MAKSBELOP3,F19, F19*MAKSBELOP3/SUM($C$19:$F$19)))</f>
+        <v>0</v>
+      </c>
+      <c r="G23" s="31" t="s">
+        <v>118</v>
+      </c>
+      <c r="H23" s="28" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" s="29"/>
+      <c r="C24" s="45">
+        <f>FLOOR(C23,1)</f>
+        <v>249</v>
+      </c>
+      <c r="D24" s="45">
+        <f t="shared" ref="D24:F24" si="7">FLOOR(D23,1)</f>
+        <v>0</v>
+      </c>
+      <c r="E24" s="45">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="F24" s="45">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="G24" s="31" t="s">
+        <v>119</v>
+      </c>
+      <c r="H24" s="28" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="B25" s="29"/>
+      <c r="C25" s="50">
+        <f>C23-C24-COLUMN(C25)/10000000</f>
+        <v>0.49999969999999999</v>
+      </c>
+      <c r="D25" s="50">
+        <f>D23-D24-COLUMN(D25)/10000000</f>
+        <v>-3.9999999999999998E-7</v>
+      </c>
+      <c r="E25" s="50">
+        <f t="shared" ref="E25:F25" si="8">E23-E24-COLUMN(E25)/10000000</f>
+        <v>-4.9999999999999998E-7</v>
+      </c>
+      <c r="F25" s="50">
+        <f t="shared" si="8"/>
+        <v>-5.9999999999999997E-7</v>
+      </c>
+      <c r="G25" s="31" t="s">
+        <v>118</v>
+      </c>
+      <c r="H25" s="28" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="B26" s="29"/>
+      <c r="C26" s="40">
+        <f>IF($B$29&gt;0,IF(LARGE($C$25:$F$25,$B$29)&lt;=C$25,1,0), 0)</f>
+        <v>1</v>
+      </c>
+      <c r="D26" s="40">
+        <f t="shared" ref="D26:F26" si="9">IF($B$29&gt;0,IF(LARGE($C$25:$F$25,$B$29)&lt;=D$25,1,0), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="E26" s="40">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="F26" s="40">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="G26" s="31" t="s">
+        <v>119</v>
+      </c>
+      <c r="H26" s="28" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="67" t="s">
+        <v>106</v>
+      </c>
+      <c r="B27" s="71"/>
+      <c r="C27" s="69">
+        <f>C24+C26</f>
+        <v>250</v>
+      </c>
+      <c r="D27" s="69">
+        <f t="shared" ref="D27:F27" si="10">D24+D26</f>
+        <v>0</v>
+      </c>
+      <c r="E27" s="69">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="F27" s="69">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="G27" s="73" t="s">
+        <v>119</v>
+      </c>
+      <c r="H27" s="67" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="27"/>
+      <c r="B28" s="29"/>
+      <c r="C28" s="50"/>
+      <c r="D28" s="50"/>
+      <c r="E28" s="50"/>
+      <c r="F28" s="50"/>
+      <c r="G28" s="31"/>
+      <c r="H28" s="28"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="B29" s="30">
+        <f>B30-SUM(C24:F24)</f>
+        <v>1</v>
+      </c>
+      <c r="C29" s="28"/>
+      <c r="D29" s="28"/>
+      <c r="E29" s="28"/>
+      <c r="F29" s="28"/>
+      <c r="G29" s="31" t="s">
+        <v>119</v>
+      </c>
+      <c r="H29" s="28" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="B30" s="29">
+        <f>ROUND(SUM(C23:F23), 0)</f>
+        <v>250</v>
+      </c>
+      <c r="C30" s="40"/>
+      <c r="D30" s="28"/>
+      <c r="E30" s="28"/>
+      <c r="F30" s="28"/>
+      <c r="G30" s="31"/>
+      <c r="H30" s="28" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="27"/>
+      <c r="B31" s="44"/>
+      <c r="C31" s="28"/>
+      <c r="D31" s="28"/>
+      <c r="E31" s="28"/>
+      <c r="F31" s="28"/>
+      <c r="G31" s="31"/>
+      <c r="H31" s="28"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="B32" s="44"/>
+      <c r="C32" s="51">
+        <f>IF(SUM($C$19:$F$20)&lt;=MAKSBELOP3,C$20,IF(SUM($C$19:$F$19)&lt;=MAKSBELOP3,$B$39*C$20/SUM($C$20:$F$20),0))</f>
+        <v>249.5</v>
+      </c>
+      <c r="D32" s="51">
+        <f>IF(SUM($C$19:$F$20)&lt;=MAKSBELOP3,D$20,IF(SUM($C$19:$F$19)&lt;=MAKSBELOP3,$B$39*D$20/SUM($C$20:$F$20),0))</f>
+        <v>0</v>
+      </c>
+      <c r="E32" s="51">
+        <f>IF(SUM($C$19:$F$20)&lt;=MAKSBELOP3,E$20,IF(SUM($C$19:$F$19)&lt;=MAKSBELOP3,$B$39*E$20/SUM($C$20:$F$20),0))</f>
+        <v>0</v>
+      </c>
+      <c r="F32" s="51">
+        <f>IF(SUM($C$19:$F$20)&lt;=MAKSBELOP3,F$20,IF(SUM($C$19:$F$19)&lt;=MAKSBELOP3,$B$39*F$20/SUM($C$20:$F$20),0))</f>
+        <v>0</v>
+      </c>
+      <c r="G32" s="31" t="s">
+        <v>118</v>
+      </c>
+      <c r="H32" s="28" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="B33" s="28"/>
+      <c r="C33" s="66">
+        <f>FLOOR(C32, 1)</f>
+        <v>249</v>
+      </c>
+      <c r="D33" s="66">
+        <f t="shared" ref="D33:F33" si="11">FLOOR(D32, 1)</f>
+        <v>0</v>
+      </c>
+      <c r="E33" s="66">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="F33" s="66">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="G33" s="31" t="s">
+        <v>119</v>
+      </c>
+      <c r="H33" s="28"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="B34" s="46"/>
+      <c r="C34" s="50">
+        <f>IF(C20=0,0,C$32-C$33-$B$38/10000000)</f>
+        <v>0.5</v>
+      </c>
+      <c r="D34" s="50">
+        <f>IF(D20=0,0,D$32-D$33-$B$38/10000000)</f>
+        <v>0</v>
+      </c>
+      <c r="E34" s="50">
+        <f>IF(E20=0,0,E$32-E$33-$B$38/10000000)</f>
+        <v>0</v>
+      </c>
+      <c r="F34" s="50">
+        <f>IF(F20=0,0,F$32-F$33-$B$38/10000000)</f>
+        <v>0</v>
+      </c>
+      <c r="G34" s="31" t="s">
+        <v>118</v>
+      </c>
+      <c r="H34" s="28" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="B35" s="46"/>
+      <c r="C35" s="40">
+        <f>IF($B$38&gt;0, IF(LARGE($C$34:$F$34,$B$38)&lt;=C$34,1,0), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="D35" s="40">
+        <f>IF($B$38&gt;0, IF(LARGE($C$34:$F$34,$B$38)&lt;=D$34,1,0), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="E35" s="40">
+        <f t="shared" ref="E35:F35" si="12">IF($B$38&gt;0, IF(LARGE($C$34:$F$34,$B$38)&lt;=E$34,1,0), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="F35" s="40">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="G35" s="31" t="s">
+        <v>119</v>
+      </c>
+      <c r="H35" s="28"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" s="67" t="s">
+        <v>107</v>
+      </c>
+      <c r="B36" s="74"/>
+      <c r="C36" s="69">
+        <f>C33+C35</f>
+        <v>249</v>
+      </c>
+      <c r="D36" s="69">
+        <f t="shared" ref="D36:F36" si="13">D33+D35</f>
+        <v>0</v>
+      </c>
+      <c r="E36" s="69">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="F36" s="69">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="G36" s="73" t="s">
+        <v>119</v>
+      </c>
+      <c r="H36" s="68"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" s="27"/>
+      <c r="B37" s="46"/>
+      <c r="C37" s="40"/>
+      <c r="D37" s="40"/>
+      <c r="E37" s="40"/>
+      <c r="F37" s="40"/>
+      <c r="G37" s="31"/>
+      <c r="H37" s="28"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="B38" s="75">
+        <f>B39-SUM(C33:F33)</f>
+        <v>0</v>
+      </c>
+      <c r="C38" s="28"/>
+      <c r="D38" s="28"/>
+      <c r="E38" s="28"/>
+      <c r="F38" s="28"/>
+      <c r="G38" s="31" t="s">
+        <v>119</v>
+      </c>
+      <c r="H38" s="28" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="B39" s="46">
+        <f>MIN(ROUND(MAKSBELOP3-B30,0), ROUND(C18-B30,0))</f>
+        <v>249</v>
+      </c>
+      <c r="C39" s="29"/>
+      <c r="D39" s="28"/>
+      <c r="E39" s="28"/>
+      <c r="F39" s="28"/>
+      <c r="G39" s="31" t="s">
+        <v>119</v>
+      </c>
+      <c r="H39" s="28" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40" s="27"/>
+      <c r="B40" s="46"/>
+      <c r="C40" s="28"/>
+      <c r="D40" s="28"/>
+      <c r="E40" s="28"/>
+      <c r="F40" s="28"/>
+      <c r="G40" s="31"/>
+      <c r="H40" s="28"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" s="67" t="s">
+        <v>72</v>
+      </c>
+      <c r="B41" s="72">
+        <f>B30+B39</f>
+        <v>499</v>
+      </c>
+      <c r="C41" s="68"/>
+      <c r="D41" s="68"/>
+      <c r="E41" s="68"/>
+      <c r="F41" s="68"/>
+      <c r="G41" s="70"/>
+      <c r="H41" s="68"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B43" s="17"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A44" s="47"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A45" s="48"/>
+      <c r="H45" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H46" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B47" s="17"/>
+    </row>
+    <row r="51" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H51" s="54"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B21:F21"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBE9F233-0C57-4B39-8C81-6D2F9F1844A9}">
   <dimension ref="A1:I44"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
+      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1119,8 +2312,8 @@
       <c r="B14" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="43">
-        <v>101351</v>
+      <c r="C14" s="56">
+        <v>93634</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>2</v>
@@ -1135,7 +2328,7 @@
       </c>
       <c r="C15" s="1">
         <f>ROUND(6*C14/260, 0)</f>
-        <v>2339</v>
+        <v>2161</v>
       </c>
       <c r="H15" s="3" t="s">
         <v>2</v>
@@ -1153,13 +2346,13 @@
       </c>
       <c r="C16" s="1">
         <f>ROUND(C13*C15,0)</f>
-        <v>936</v>
+        <v>864</v>
       </c>
       <c r="H16" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="20" t="s">
         <v>50</v>
       </c>
@@ -1168,7 +2361,7 @@
       </c>
       <c r="C17" s="24">
         <f>MIN(1, C16/SUM(D10:G10))</f>
-        <v>0.82105263157894737</v>
+        <v>0.75789473684210529</v>
       </c>
       <c r="D17" s="22"/>
       <c r="E17" s="22"/>
@@ -1178,7 +2371,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="20" t="s">
         <v>24</v>
       </c>
@@ -1188,15 +2381,15 @@
       <c r="C18" s="21"/>
       <c r="D18" s="22">
         <f>D10*ScalingFactor</f>
-        <v>397.89473684210526</v>
+        <v>367.28744939271257</v>
       </c>
       <c r="E18" s="22">
         <f>E10*ScalingFactor</f>
-        <v>303.15789473684214</v>
+        <v>279.83805668016197</v>
       </c>
       <c r="F18" s="22">
         <f>F10*ScalingFactor</f>
-        <v>234.9473684210526</v>
+        <v>216.87449392712549</v>
       </c>
       <c r="G18" s="22">
         <f>G10*ScalingFactor</f>
@@ -1206,7 +2399,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="20" t="s">
         <v>51</v>
       </c>
@@ -1216,11 +2409,11 @@
       <c r="C19" s="21"/>
       <c r="D19" s="22">
         <f>MIN(D18,D12)</f>
-        <v>397.89473684210526</v>
+        <v>367.28744939271257</v>
       </c>
       <c r="E19" s="22">
         <f t="shared" ref="E19:G19" si="6">MIN(E18,E12)</f>
-        <v>303.15789473684214</v>
+        <v>279.83805668016197</v>
       </c>
       <c r="F19" s="22">
         <f t="shared" si="6"/>
@@ -1234,7 +2427,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="20"/>
       <c r="B20" s="21" t="s">
         <v>34</v>
@@ -1242,11 +2435,11 @@
       <c r="C20" s="21"/>
       <c r="D20" s="22">
         <f>D19-D12</f>
-        <v>-86.720647773279381</v>
+        <v>-117.32793522267207</v>
       </c>
       <c r="E20" s="22">
         <f t="shared" ref="E20:G20" si="7">E19-E12</f>
-        <v>-29.149797570850239</v>
+        <v>-52.469635627530408</v>
       </c>
       <c r="F20" s="22">
         <f t="shared" si="7"/>
@@ -1260,7 +2453,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="20"/>
       <c r="B21" s="21" t="s">
         <v>55</v>
@@ -1283,7 +2476,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="20" t="s">
         <v>52</v>
       </c>
@@ -1311,7 +2504,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="20"/>
       <c r="B23" s="21" t="s">
         <v>32</v>
@@ -1327,7 +2520,7 @@
       </c>
       <c r="F23" s="22">
         <f>F18-F19</f>
-        <v>163.40890688259105</v>
+        <v>145.33603238866397</v>
       </c>
       <c r="G23" s="22">
         <f>G18-G19</f>
@@ -1337,7 +2530,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="20" t="s">
         <v>53</v>
       </c>
@@ -1347,11 +2540,11 @@
       <c r="C24" s="21"/>
       <c r="D24" s="22">
         <f>MIN(-D20,IF(SUM($D$20:$G$20)&gt;=0, 0, SUM($D$23:$G$23)*D22))</f>
-        <v>86.720647773279381</v>
+        <v>98.453441295546554</v>
       </c>
       <c r="E24" s="22">
         <f t="shared" ref="E24:G24" si="9">MIN(-E20,IF(SUM($D$20:$G$20)&gt;=0, 0, SUM($D$23:$G$23)*E22))</f>
-        <v>29.149797570850239</v>
+        <v>46.882591093117405</v>
       </c>
       <c r="F24" s="22">
         <f t="shared" si="9"/>
@@ -1365,7 +2558,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="20"/>
       <c r="B25" s="21" t="s">
         <v>54</v>
@@ -1391,7 +2584,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="20"/>
       <c r="B26" s="21" t="s">
         <v>57</v>
@@ -1417,7 +2610,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="20" t="s">
         <v>22</v>
       </c>
@@ -1427,11 +2620,11 @@
       <c r="C27" s="21"/>
       <c r="D27" s="25">
         <f>ROUND(D19+D24,0)</f>
-        <v>485</v>
+        <v>466</v>
       </c>
       <c r="E27" s="25">
         <f t="shared" ref="E27:G27" si="11">ROUND(E19+E24,0)</f>
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="F27" s="25">
         <f t="shared" si="11"/>
@@ -1445,7 +2638,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="20" t="s">
         <v>23</v>
       </c>
@@ -1463,7 +2656,7 @@
       </c>
       <c r="F28" s="21">
         <f>ROUND(F23-SUM(AdjustmentArb)*F26,0)</f>
-        <v>48</v>
+        <v>0</v>
       </c>
       <c r="G28" s="21">
         <f>ROUND(G23-SUM(AdjustmentArb)*G26,0)</f>
@@ -1473,7 +2666,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="20"/>
       <c r="B29" s="21" t="s">
         <v>11</v>
@@ -1586,14 +2779,14 @@
       <c r="B34" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="C34" s="36" t="str">
+      <c r="C34" s="79" t="str">
         <f>IF(SUM(D32:G33)&lt;=MAKSBELOP,"Everyone paid",IF(SUM(D32:G32)&lt;=MAKSBELOP,"Arbeidsgivere fully paid; Person partially paid by Person request", "Arbeidsgivere partial payment ratio by Arbeidsgiver request"))</f>
-        <v>Arbeidsgivere fully paid; Person partially paid by Person request</v>
-      </c>
-      <c r="D34" s="36"/>
-      <c r="E34" s="36"/>
-      <c r="F34" s="36"/>
-      <c r="G34" s="36"/>
+        <v>Arbeidsgivere partial payment ratio by Arbeidsgiver request</v>
+      </c>
+      <c r="D34" s="79"/>
+      <c r="E34" s="79"/>
+      <c r="F34" s="79"/>
+      <c r="G34" s="79"/>
       <c r="H34" s="31"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
@@ -1606,15 +2799,15 @@
       <c r="C35" s="29"/>
       <c r="D35" s="28">
         <f>IF(SUM($D$32:$G$33)&lt;=MAKSBELOP,D32,IF(SUM($D$32:$G$32)&lt;=MAKSBELOP,D32,ROUND(D32*MAKSBELOP/SUM($D$32:$G$32),0)))</f>
-        <v>485</v>
+        <v>471</v>
       </c>
       <c r="E35" s="28">
         <f>IF(SUM($D$32:$G$33)&lt;=MAKSBELOP,E32,IF(SUM($D$32:$G$32)&lt;=MAKSBELOP,E32,ROUND(E32*MAKSBELOP/SUM($D$32:$G$32),0)))</f>
-        <v>332</v>
+        <v>323</v>
       </c>
       <c r="F35" s="28">
         <f>IF(SUM($D$32:$G$33)&lt;=MAKSBELOP,F32,IF(SUM($D$32:$G$32)&lt;=MAKSBELOP,F32,ROUND(F32*MAKSBELOP/SUM($D$32:$G$32),0)))</f>
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G35" s="28">
         <f>IF(SUM($D$32:$G$33)&lt;=MAKSBELOP,G32,IF(SUM($D$32:$G$32)&lt;=MAKSBELOP,G32,ROUND(G32*MAKSBELOP/SUM($D$32:$G$32),0)))</f>
@@ -1631,7 +2824,7 @@
       </c>
       <c r="C36" s="29">
         <f>MAKSBELOP-SUM(D35:G35)</f>
-        <v>47</v>
+        <v>0</v>
       </c>
       <c r="D36" s="28"/>
       <c r="E36" s="28"/>
@@ -1653,11 +2846,11 @@
       </c>
       <c r="E37" s="28">
         <f>IF(SUM($D$32:$G$33)&lt;=MAKSBELOP,E33,IF(SUM($D$32:$G$32)&lt;=MAKSBELOP,ROUND(PersonRemainder*E33/SUM($D$33:$G$33),0),0))</f>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F37" s="28">
         <f>IF(SUM($D$32:$G$33)&lt;=MAKSBELOP,F33,IF(SUM($D$32:$G$32)&lt;=MAKSBELOP,ROUND(PersonRemainder*F33/SUM($D$33:$G$33),0),0))</f>
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="G37" s="28">
         <f>IF(SUM($D$32:$G$33)&lt;=MAKSBELOP,G33,IF(SUM($D$32:$G$32)&lt;=MAKSBELOP,ROUND(PersonRemainder*G33/SUM($D$33:$G$33),0),0))</f>
@@ -1693,12 +2886,12 @@
       <c r="D40" s="11"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A41" s="37" t="s">
+      <c r="A41" s="80" t="s">
         <v>5</v>
       </c>
-      <c r="B41" s="37"/>
-      <c r="C41" s="37"/>
-      <c r="D41" s="37"/>
+      <c r="B41" s="80"/>
+      <c r="C41" s="80"/>
+      <c r="D41" s="80"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="15" t="s">
@@ -1726,12 +2919,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A506B608-BF2F-BB48-9883-32866B0664B3}">
   <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="139" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+    <sheetView zoomScale="228" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2035,7 +3228,7 @@
       <c r="B13" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="38">
+      <c r="C13" s="36">
         <f>SUM(D10:G10)/SUM(D7:G7)</f>
         <v>0.39838709677419348</v>
       </c>
@@ -2064,7 +3257,7 @@
       <c r="B15" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="39">
+      <c r="C15" s="37">
         <f>6*C14/260</f>
         <v>2338.8692307692309</v>
       </c>
@@ -2079,7 +3272,7 @@
       <c r="B16" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="39">
+      <c r="C16" s="37">
         <f>C13*C15</f>
         <v>931.77532258064502</v>
       </c>
@@ -2116,15 +3309,15 @@
       <c r="C18" s="21"/>
       <c r="D18" s="22">
         <f>D10*ScalingFactor</f>
-        <v>397.89473684210526</v>
+        <v>367.28744939271257</v>
       </c>
       <c r="E18" s="22">
         <f>E10*ScalingFactor</f>
-        <v>303.15789473684214</v>
+        <v>279.83805668016197</v>
       </c>
       <c r="F18" s="22">
         <f>F10*ScalingFactor</f>
-        <v>234.9473684210526</v>
+        <v>216.87449392712549</v>
       </c>
       <c r="G18" s="22">
         <f>G10*ScalingFactor</f>
@@ -2144,11 +3337,11 @@
       <c r="C19" s="21"/>
       <c r="D19" s="22">
         <f>MIN(D18,D12)</f>
-        <v>397.89473684210526</v>
+        <v>367.28744939271257</v>
       </c>
       <c r="E19" s="22">
         <f t="shared" ref="E19:G19" si="6">MIN(E18,E12)</f>
-        <v>303.15789473684214</v>
+        <v>279.83805668016197</v>
       </c>
       <c r="F19" s="22">
         <f t="shared" si="6"/>
@@ -2170,11 +3363,11 @@
       <c r="C20" s="21"/>
       <c r="D20" s="22">
         <f>D19-D12</f>
-        <v>-86.720647773279381</v>
+        <v>-117.32793522267207</v>
       </c>
       <c r="E20" s="22">
         <f t="shared" ref="E20:G20" si="7">E19-E12</f>
-        <v>-29.149797570850239</v>
+        <v>-52.469635627530408</v>
       </c>
       <c r="F20" s="22">
         <f t="shared" si="7"/>
@@ -2255,7 +3448,7 @@
       </c>
       <c r="F23" s="22">
         <f>F18-F19</f>
-        <v>163.40890688259105</v>
+        <v>145.33603238866397</v>
       </c>
       <c r="G23" s="22">
         <f>G18-G19</f>
@@ -2275,11 +3468,11 @@
       <c r="C24" s="21"/>
       <c r="D24" s="22">
         <f>MIN(-D20,IF(SUM($D$20:$G$20)&gt;=0, 0, SUM($D$23:$G$23)*D22))</f>
-        <v>86.720647773279381</v>
+        <v>98.453441295546554</v>
       </c>
       <c r="E24" s="22">
         <f t="shared" ref="E24:G24" si="9">MIN(-E20,IF(SUM($D$20:$G$20)&gt;=0, 0, SUM($D$23:$G$23)*E22))</f>
-        <v>29.149797570850239</v>
+        <v>46.882591093117405</v>
       </c>
       <c r="F24" s="22">
         <f t="shared" si="9"/>
@@ -2355,11 +3548,11 @@
       <c r="C27" s="21"/>
       <c r="D27" s="25">
         <f>ROUND(D19+D24,0)</f>
-        <v>485</v>
+        <v>466</v>
       </c>
       <c r="E27" s="25">
         <f t="shared" ref="E27:G27" si="11">ROUND(E19+E24,0)</f>
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="F27" s="25">
         <f t="shared" si="11"/>
@@ -2391,7 +3584,7 @@
       </c>
       <c r="F28" s="21">
         <f>ROUND(F23-SUM(AdjustmentArb)*F26,0)</f>
-        <v>48</v>
+        <v>0</v>
       </c>
       <c r="G28" s="21">
         <f>ROUND(G23-SUM(AdjustmentArb)*G26,0)</f>
@@ -2408,7 +3601,7 @@
       </c>
       <c r="C29" s="26">
         <f>C16-SUM(D27:G28)</f>
-        <v>-5.2246774193549754</v>
+        <v>66.775322580645025</v>
       </c>
       <c r="D29" s="21"/>
       <c r="E29" s="21"/>
@@ -2431,15 +3624,15 @@
         <v>30</v>
       </c>
       <c r="C31" s="29"/>
-      <c r="D31" s="40">
+      <c r="D31" s="38">
         <f>D10</f>
         <v>484.61538461538464</v>
       </c>
-      <c r="E31" s="40">
+      <c r="E31" s="38">
         <f>E10</f>
         <v>369.23076923076928</v>
       </c>
-      <c r="F31" s="40">
+      <c r="F31" s="38">
         <f>F10</f>
         <v>286.15384615384613</v>
       </c>
@@ -2459,15 +3652,15 @@
         <v>59</v>
       </c>
       <c r="C32" s="29"/>
-      <c r="D32" s="40">
+      <c r="D32" s="38">
         <f>D12</f>
         <v>484.61538461538464</v>
       </c>
-      <c r="E32" s="40">
+      <c r="E32" s="38">
         <f>E12</f>
         <v>332.30769230769238</v>
       </c>
-      <c r="F32" s="40">
+      <c r="F32" s="38">
         <f>F12</f>
         <v>71.538461538461533</v>
       </c>
@@ -2487,15 +3680,15 @@
         <v>60</v>
       </c>
       <c r="C33" s="29"/>
-      <c r="D33" s="40">
+      <c r="D33" s="38">
         <f>D31-D32</f>
         <v>0</v>
       </c>
-      <c r="E33" s="40">
+      <c r="E33" s="38">
         <f t="shared" ref="E33:G33" si="14">E31-E32</f>
         <v>36.923076923076906</v>
       </c>
-      <c r="F33" s="40">
+      <c r="F33" s="38">
         <f t="shared" si="14"/>
         <v>214.61538461538458</v>
       </c>
@@ -2512,14 +3705,14 @@
       <c r="B34" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="C34" s="36" t="str">
+      <c r="C34" s="79" t="str">
         <f>IF(SUM(D32:G33)&lt;=MAKSBELOP,"Everyone paid",IF(SUM(D32:G32)&lt;=MAKSBELOP,"Arbeidsgivere fully paid; Person partially paid by Person request", "Arbeidsgivere partial payment ratio by Arbeidsgiver request"))</f>
-        <v>Arbeidsgivere fully paid; Person partially paid by Person request</v>
-      </c>
-      <c r="D34" s="36"/>
-      <c r="E34" s="36"/>
-      <c r="F34" s="36"/>
-      <c r="G34" s="36"/>
+        <v>Arbeidsgivere partial payment ratio by Arbeidsgiver request</v>
+      </c>
+      <c r="D34" s="79"/>
+      <c r="E34" s="79"/>
+      <c r="F34" s="79"/>
+      <c r="G34" s="79"/>
       <c r="H34" s="31"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
@@ -2555,7 +3748,7 @@
       <c r="B36" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="C36" s="41">
+      <c r="C36" s="39">
         <f>MAKSBELOP2-SUM(D35:G35)</f>
         <v>42.775322580645025</v>
       </c>
@@ -2573,15 +3766,15 @@
         <v>10</v>
       </c>
       <c r="C37" s="28"/>
-      <c r="D37" s="42">
+      <c r="D37" s="40">
         <f>IF(SUM($D$32:$G$33)&lt;=MAKSBELOP2,ROUND(D33,0),IF(SUM($D$32:$G$32)&lt;=MAKSBELOP2,ROUND(PersonRemainder2*D33/SUM($D$33:$G$33),0),0))</f>
         <v>0</v>
       </c>
-      <c r="E37" s="42">
+      <c r="E37" s="40">
         <f>IF(SUM($D$32:$G$33)&lt;=MAKSBELOP2,ROUND(E33,0),IF(SUM($D$32:$G$32)&lt;=MAKSBELOP2,ROUND(PersonRemainder2*E33/SUM($D$33:$G$33),0),0))</f>
         <v>6</v>
       </c>
-      <c r="F37" s="42">
+      <c r="F37" s="40">
         <f>IF(SUM($D$32:$G$33)&lt;=MAKSBELOP2,ROUND(F33,0),IF(SUM($D$32:$G$32)&lt;=MAKSBELOP2,ROUND(PersonRemainder2*F33/SUM($D$33:$G$33),0),0))</f>
         <v>36</v>
       </c>
@@ -2598,7 +3791,7 @@
       <c r="B38" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="C38" s="41">
+      <c r="C38" s="39">
         <f>MAKSBELOP2-SUM(D35:G37)</f>
         <v>0.77532258064502457</v>
       </c>

</xml_diff>

<commit_message>
trekker personbeløp-reduseringkvotient ut som eget felt
</commit_message>
<xml_diff>
--- a/doc/okonomi/Utbetaling.xlsx
+++ b/doc/okonomi/Utbetaling.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/david/dev/nav/helse-spleis/doc/okonomi/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D14D593-F0DE-7F4F-B868-90605DF29B42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FE1C50E-CBC3-3845-BBBC-F0F82E1E8F14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="65700" windowHeight="36520" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
     <definedName name="AdjustmentArb">'Flere arbeidsgivere, gammel'!$D$24:$G$24</definedName>
     <definedName name="MAKSBELOP">'Flere arbeidsgivere, gammel'!$C$16</definedName>
     <definedName name="MAKSBELOP2">'Flere arbeidsgivere, eldre'!$C$16</definedName>
-    <definedName name="MAKSBELOP3">'Flere arbeidsgivere, ny '!$B$30</definedName>
+    <definedName name="MAKSBELOP3">'Flere arbeidsgivere, ny '!#REF!</definedName>
     <definedName name="PersonRemainder">'Flere arbeidsgivere, gammel'!$C$36</definedName>
     <definedName name="PersonRemainder2">'Flere arbeidsgivere, eldre'!$C$36</definedName>
     <definedName name="ScalingFactor">'Flere arbeidsgivere, gammel'!$C$17</definedName>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="151">
   <si>
     <t xml:space="preserve">Begrep	</t>
   </si>
@@ -140,9 +140,6 @@
     <t>Maksbeløp</t>
   </si>
   <si>
-    <t>Maks dagsats bruker kan få ut ifra den totale graden av arbeidsuførhet på tvers av alle arbeidsforholdene, redusert for 6G</t>
-  </si>
-  <si>
     <t>Maks dagsats redusert for grad av arbeidsuførhet</t>
   </si>
   <si>
@@ -155,9 +152,6 @@
     <t>Personbeløp før 6g</t>
   </si>
   <si>
-    <t>Det beløpet arbeidstakeren kan få utbetalt før reduskjon for 6G</t>
-  </si>
-  <si>
     <t xml:space="preserve">Situasjon </t>
   </si>
   <si>
@@ -192,9 +186,6 @@
   </si>
   <si>
     <t xml:space="preserve">Total utbetaling til arbeidsgivere </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total utbetaling til arbeidsgivere (inkludert restbeløpet i raden over) </t>
   </si>
   <si>
     <t xml:space="preserve">Personutbetalinger før avrunding </t>
@@ -512,6 +503,24 @@
   </si>
   <si>
     <t xml:space="preserve">Utbetaling til arbeidsgivere med avrunding og fordelt restbeløp </t>
+  </si>
+  <si>
+    <t>Det beløpet arbeidstakeren kan få utbetalt før reduksjon for 6G</t>
+  </si>
+  <si>
+    <t>Total utbetaling til arbeidsgivere , eksl. avrunding</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total utbetaling til arbeidsgivere (ekskludert restbeløpet) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total utbetaling til arbeidsgivere (inkludert restbeløpet) </t>
+  </si>
+  <si>
+    <t>Total utbetaling til arbeidsgivere (inkludert restbeløpet) , som årlig</t>
+  </si>
+  <si>
+    <t>Personbeløp 6g-reduksjonsfaktor</t>
   </si>
 </sst>
 </file>
@@ -568,7 +577,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -603,6 +612,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor rgb="FFE2F0D9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -692,7 +707,7 @@
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -813,6 +828,13 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1198,10 +1220,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H61"/>
+  <dimension ref="A1:H64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="D47" sqref="D47"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1300,7 +1322,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C5" s="39">
         <f>C3*12</f>
@@ -1322,7 +1344,7 @@
         <v>8</v>
       </c>
       <c r="H5" s="70" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -1350,12 +1372,12 @@
         <v>8</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="69" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B7" s="73">
         <f>SUM(C6:F6)*12</f>
@@ -1388,7 +1410,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="69" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B9" s="72">
         <f>SUM(C5:F5)</f>
@@ -1398,7 +1420,7 @@
         <v>8</v>
       </c>
       <c r="H9" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -1427,12 +1449,12 @@
         <v>14</v>
       </c>
       <c r="H11" s="76" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B12" s="9">
         <f>ROUND(B11/260,)</f>
@@ -1442,12 +1464,12 @@
         <v>14</v>
       </c>
       <c r="H12" s="76" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="69" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B13" s="39">
         <f>ROUND(MIN(B9,B11)/260,)*260</f>
@@ -1457,12 +1479,12 @@
         <v>14</v>
       </c>
       <c r="H13" s="76" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="69" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B14" s="68">
         <f>B13/260</f>
@@ -1472,7 +1494,7 @@
         <v>14</v>
       </c>
       <c r="H14" s="76" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
@@ -1552,12 +1574,12 @@
         <v>8</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="74" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C19" s="75">
         <f>C8*C4</f>
@@ -1579,7 +1601,7 @@
         <v>8</v>
       </c>
       <c r="H19" s="76" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
@@ -1612,7 +1634,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="74" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B21" s="68">
         <f>SUM(C20:F20)</f>
@@ -1622,12 +1644,12 @@
         <v>8</v>
       </c>
       <c r="H21" s="76" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="74" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B22" s="73">
         <f>B21*260</f>
@@ -1637,7 +1659,7 @@
         <v>8</v>
       </c>
       <c r="H22" s="76" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
@@ -1665,12 +1687,12 @@
         <v>8</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="74" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B24" s="68">
         <f>SUM(C23:F23)</f>
@@ -1680,12 +1702,12 @@
         <v>8</v>
       </c>
       <c r="H24" s="76" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="74" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B25" s="73">
         <f>B24*260</f>
@@ -1695,12 +1717,12 @@
         <v>8</v>
       </c>
       <c r="H25" s="76" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="74" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B26" s="68">
         <f>B21-B24</f>
@@ -1710,23 +1732,24 @@
         <v>8</v>
       </c>
       <c r="H26" s="76" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="74" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B27" s="73">
         <f>B26*260</f>
         <v>200400</v>
       </c>
       <c r="C27" s="73"/>
+      <c r="D27" s="81"/>
       <c r="G27" s="71" t="s">
         <v>8</v>
       </c>
       <c r="H27" s="76" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
@@ -1750,55 +1773,36 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="74" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B29" s="77">
         <f>ROUND(B13*B28/260,)*260</f>
         <v>490360</v>
       </c>
       <c r="C29" s="4"/>
-      <c r="D29" s="13"/>
+      <c r="D29" s="4"/>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
       <c r="G29" s="71" t="s">
         <v>14</v>
       </c>
       <c r="H29" s="76" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A30" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B30" s="9">
-        <f>B29/260</f>
-        <v>1886</v>
-      </c>
-      <c r="C30" s="4"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H30" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A31" s="74" t="s">
-        <v>135</v>
-      </c>
-      <c r="B31">
+      <c r="A30" s="74" t="s">
+        <v>132</v>
+      </c>
+      <c r="B30">
         <f>MIN(1,B29/B25)</f>
         <v>1</v>
       </c>
-      <c r="G31" s="71" t="s">
+      <c r="G30" s="71" t="s">
         <v>8</v>
       </c>
-      <c r="H31" s="76" t="s">
-        <v>136</v>
+      <c r="H30" s="76" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
@@ -1826,12 +1830,12 @@
         <v>8</v>
       </c>
       <c r="H32" s="24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B33" s="15"/>
       <c r="C33" s="16">
@@ -1854,12 +1858,12 @@
         <v>8</v>
       </c>
       <c r="H33" s="24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B34" s="15"/>
       <c r="C34" s="16">
@@ -1882,16 +1886,16 @@
         <v>8</v>
       </c>
       <c r="H34" s="24" t="s">
-        <v>35</v>
+        <v>145</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B35" s="19" t="str">
-        <f>IF(SUM(C33:F34)&lt;=MAKSBELOP3,"Arbeidsgiver og person blir refundert hele beløpet",IF(SUM(C33:F33)&lt;=MAKSBELOP3,"Arbeidsgivere blir refundert hele beløpet; Person blir delvis refundert", "Arbeidsgivere blir delvis refundert"))</f>
-        <v>Arbeidsgivere blir refundert hele beløpet; Person blir delvis refundert</v>
+        <f>IF(B27&lt;=B29,"Arbeidsgiver og person blir refundert hele beløpet",IF(B25&lt;=B29,"Arbeidsgivere blir refundert hele beløpet; Person blir delvis refundert", "Arbeidsgivere blir delvis refundert"))</f>
+        <v>Arbeidsgiver og person blir refundert hele beløpet</v>
       </c>
       <c r="C35" s="19"/>
       <c r="D35" s="19"/>
@@ -1912,35 +1916,35 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B37" s="20"/>
       <c r="C37" s="23">
-        <f>C33*$B$31</f>
+        <f>C33*$B$30</f>
         <v>120</v>
       </c>
       <c r="D37" s="23">
-        <f>D33*$B$31</f>
+        <f>D33*$B$30</f>
         <v>32.307692307692307</v>
       </c>
       <c r="E37" s="23">
-        <f>E33*$B$31</f>
+        <f>E33*$B$30</f>
         <v>692.30769230769226</v>
       </c>
       <c r="F37" s="23">
-        <f>F33*$B$31</f>
+        <f>F33*$B$30</f>
         <v>600</v>
       </c>
       <c r="G37" s="17" t="s">
         <v>8</v>
       </c>
       <c r="H37" s="24" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B38" s="15"/>
       <c r="C38" s="24">
@@ -1963,18 +1967,18 @@
         <v>14</v>
       </c>
       <c r="H38" s="24" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B39" s="30">
-        <f>B40-SUM(C38:F38)</f>
-        <v>1</v>
-      </c>
-      <c r="C39" s="24"/>
+        <v>146</v>
+      </c>
+      <c r="B39" s="15">
+        <f>SUM(C38:F38)</f>
+        <v>1444</v>
+      </c>
+      <c r="C39" s="25"/>
       <c r="D39" s="24"/>
       <c r="E39" s="24"/>
       <c r="F39" s="24"/>
@@ -1982,270 +1986,268 @@
         <v>14</v>
       </c>
       <c r="H39" s="24" t="s">
-        <v>46</v>
+        <v>147</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B40" s="15">
-        <f>ROUND(SUM(C37:F37), 0)</f>
-        <v>1445</v>
-      </c>
-      <c r="C40" s="25"/>
+        <v>43</v>
+      </c>
+      <c r="B40" s="30">
+        <f>ROUND(SUM(C37:F37)-B39,)</f>
+        <v>1</v>
+      </c>
+      <c r="C40" s="24"/>
       <c r="D40" s="24"/>
       <c r="E40" s="24"/>
       <c r="F40" s="24"/>
-      <c r="G40" s="17"/>
+      <c r="G40" s="17" t="s">
+        <v>14</v>
+      </c>
       <c r="H40" s="24" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B41" s="15"/>
-      <c r="C41" s="23">
+        <v>45</v>
+      </c>
+      <c r="B41" s="15">
+        <f>B39+B40</f>
+        <v>1445</v>
+      </c>
+      <c r="C41" s="25"/>
+      <c r="D41" s="24"/>
+      <c r="E41" s="24"/>
+      <c r="F41" s="24"/>
+      <c r="G41" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="H41" s="24" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B42" s="15">
+        <f>B41*260</f>
+        <v>375700</v>
+      </c>
+      <c r="C42" s="25"/>
+      <c r="D42" s="24"/>
+      <c r="E42" s="24"/>
+      <c r="F42" s="24"/>
+      <c r="G42" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="H42" s="24" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B43" s="15"/>
+      <c r="C43" s="23">
         <f>C37-TRUNC(C37)</f>
         <v>0</v>
       </c>
-      <c r="D41" s="23">
+      <c r="D43" s="23">
         <f>D37-TRUNC(D37)</f>
         <v>0.3076923076923066</v>
       </c>
-      <c r="E41" s="23">
+      <c r="E43" s="23">
         <f>E37-TRUNC(E37)</f>
         <v>0.30769230769226397</v>
       </c>
-      <c r="F41" s="23">
+      <c r="F43" s="23">
         <f>F37-TRUNC(F37)</f>
         <v>0</v>
       </c>
-      <c r="G41" s="17" t="s">
+      <c r="G43" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="H41" s="24" t="s">
+      <c r="H43" s="24" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B44" s="15"/>
+      <c r="C44" s="25">
+        <f>IF($B$40&gt;0,IF(LARGE($C$43:$F$43,$B$40)&lt;=C$43,1,0), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="D44" s="25">
+        <f>IF($B$40&gt;0,IF(LARGE($C$43:$F$43,$B$40)&lt;=D$43,1,0), 0)</f>
+        <v>1</v>
+      </c>
+      <c r="E44" s="25">
+        <f>IF($B$40&gt;0,IF(LARGE($C$43:$F$43,$B$40)&lt;=E$43,1,0), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="F44" s="25">
+        <f>IF($B$40&gt;0,IF(LARGE($C$43:$F$43,$B$40)&lt;=F$43,1,0), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="G44" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="H44" s="24" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A42" s="1" t="s">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A45" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="B42" s="15"/>
-      <c r="C42" s="25">
-        <f>IF($B$39&gt;0,IF(LARGE($C$41:$F$41,$B$39)&lt;=C$41,1,0), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="D42" s="25">
-        <f>IF($B$39&gt;0,IF(LARGE($C$41:$F$41,$B$39)&lt;=D$41,1,0), 0)</f>
-        <v>1</v>
-      </c>
-      <c r="E42" s="25">
-        <f>IF($B$39&gt;0,IF(LARGE($C$41:$F$41,$B$39)&lt;=E$41,1,0), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="F42" s="25">
-        <f>IF($B$39&gt;0,IF(LARGE($C$41:$F$41,$B$39)&lt;=F$41,1,0), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="G42" s="17" t="s">
+      <c r="B45" s="27"/>
+      <c r="C45" s="28">
+        <f>C38+C44</f>
+        <v>120</v>
+      </c>
+      <c r="D45" s="28">
+        <f>D38+D44</f>
+        <v>33</v>
+      </c>
+      <c r="E45" s="28">
+        <f>E38+E44</f>
+        <v>692</v>
+      </c>
+      <c r="F45" s="28">
+        <f>F38+F44</f>
+        <v>600</v>
+      </c>
+      <c r="G45" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="H42" s="24" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A43" s="26" t="s">
-        <v>44</v>
-      </c>
-      <c r="B43" s="27"/>
-      <c r="C43" s="28">
-        <f>C38+C42</f>
-        <v>120</v>
-      </c>
-      <c r="D43" s="28">
-        <f>D38+D42</f>
-        <v>33</v>
-      </c>
-      <c r="E43" s="28">
-        <f>E38+E42</f>
-        <v>692</v>
-      </c>
-      <c r="F43" s="28">
-        <f>F38+F42</f>
-        <v>600</v>
-      </c>
-      <c r="G43" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="H43" s="26" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A44" s="1"/>
-      <c r="B44" s="15"/>
-      <c r="C44" s="23"/>
-      <c r="D44" s="23"/>
-      <c r="E44" s="23"/>
-      <c r="F44" s="23"/>
-      <c r="G44" s="17"/>
-      <c r="H44" s="24"/>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A45" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B45" s="31"/>
-      <c r="C45" s="16">
-        <f>IF($B$22&lt;=$B$29,C$34,IF($B$25&lt;=$B$29,$B$52*C$34/$B$26,0))</f>
-        <v>274.63473053892216</v>
-      </c>
-      <c r="D45" s="16">
-        <f>IF($B$22&lt;=$B$29,D$34,IF($B$25&lt;=$B$29,$B$52*D$34/$B$26,0))</f>
-        <v>166.36526946107784</v>
-      </c>
-      <c r="E45" s="16">
-        <f>IF($B$22&lt;=$B$29,E$34,IF($B$25&lt;=$B$29,$B$52*E$34/$B$26,0))</f>
-        <v>0</v>
-      </c>
-      <c r="F45" s="16">
-        <f>IF($B$22&lt;=$B$29,F$34,IF($B$25&lt;=$B$29,$B$52*F$34/$B$26,0))</f>
-        <v>0</v>
-      </c>
-      <c r="G45" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="H45" s="24" t="s">
-        <v>50</v>
+      <c r="H45" s="26" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A46" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B46" s="24"/>
-      <c r="C46" s="32">
-        <f>FLOOR(C45, 1)</f>
-        <v>274</v>
-      </c>
-      <c r="D46" s="32">
-        <f>FLOOR(D45, 1)</f>
-        <v>166</v>
-      </c>
-      <c r="E46" s="32">
-        <f>FLOOR(E45, 1)</f>
-        <v>0</v>
-      </c>
-      <c r="F46" s="32">
-        <f>FLOOR(F45, 1)</f>
-        <v>0</v>
-      </c>
-      <c r="G46" s="17" t="s">
-        <v>14</v>
-      </c>
+      <c r="A46" s="1"/>
+      <c r="B46" s="15"/>
+      <c r="C46" s="23"/>
+      <c r="D46" s="23"/>
+      <c r="E46" s="23"/>
+      <c r="F46" s="23"/>
+      <c r="G46" s="17"/>
       <c r="H46" s="24"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B47" s="33"/>
-      <c r="C47" s="23">
-        <f>C45-TRUNC(C46)</f>
-        <v>0.63473053892215603</v>
-      </c>
-      <c r="D47" s="23">
-        <f t="shared" ref="D47:F47" si="1">D45-TRUNC(D46)</f>
-        <v>0.36526946107784397</v>
-      </c>
-      <c r="E47" s="23">
+        <v>54</v>
+      </c>
+      <c r="B47" s="33">
+        <f>ROUND(MIN(B29-B42, B22-B42)/260,)</f>
+        <v>441</v>
+      </c>
+      <c r="C47" s="15">
+        <f>IF($B$22&lt;=$B$29,1,IF($B$25&lt;=$B$29,2,0))</f>
+        <v>2</v>
+      </c>
+      <c r="D47" s="15">
+        <f t="shared" ref="D47:F47" si="1">IF($B$22&lt;=$B$29,1,IF($B$25&lt;=$B$29,2,0))</f>
+        <v>2</v>
+      </c>
+      <c r="E47" s="15">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F47" s="23">
+        <v>2</v>
+      </c>
+      <c r="F47" s="15">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G47" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="H47" s="24" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A48" s="82" t="s">
+        <v>150</v>
+      </c>
+      <c r="B48" s="84">
+        <f>IF($B$22&lt;=$B$29,1,IF($B$25&lt;=$B$29,B47/B26,0))</f>
+        <v>0.57215568862275457</v>
+      </c>
+      <c r="C48" s="83"/>
+      <c r="D48" s="83"/>
+      <c r="E48" s="83"/>
+      <c r="F48" s="83"/>
+      <c r="G48" s="85" t="s">
         <v>8</v>
       </c>
-      <c r="H47" s="24" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A48" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B48" s="33"/>
-      <c r="C48" s="25">
-        <f>IF($B$51&gt;0, IF(LARGE($C$47:$F$47,$B$51)&lt;=C$47,1,0), 0)</f>
-        <v>1</v>
-      </c>
-      <c r="D48" s="25">
-        <f>IF($B$51&gt;0, IF(LARGE($C$47:$F$47,$B$51)&lt;=D$47,1,0), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="E48" s="25">
-        <f>IF($B$51&gt;0, IF(LARGE($C$47:$F$47,$B$51)&lt;=E$47,1,0), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="F48" s="25">
-        <f>IF($B$51&gt;0, IF(LARGE($C$47:$F$47,$B$51)&lt;=F$47,1,0), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="G48" s="17" t="s">
+      <c r="H48" s="83"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B49" s="31"/>
+      <c r="C49" s="16">
+        <f>C34*$B$48</f>
+        <v>274.63473053892221</v>
+      </c>
+      <c r="D49" s="16">
+        <f t="shared" ref="D49:F49" si="2">D34*$B$48</f>
+        <v>166.36526946107787</v>
+      </c>
+      <c r="E49" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F49" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G49" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="H49" s="24" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B50" s="24"/>
+      <c r="C50" s="32">
+        <f>FLOOR(C49, 1)</f>
+        <v>274</v>
+      </c>
+      <c r="D50" s="32">
+        <f>FLOOR(D49, 1)</f>
+        <v>166</v>
+      </c>
+      <c r="E50" s="32">
+        <f>FLOOR(E49, 1)</f>
+        <v>0</v>
+      </c>
+      <c r="F50" s="32">
+        <f>FLOOR(F49, 1)</f>
+        <v>0</v>
+      </c>
+      <c r="G50" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="H48" s="24"/>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A49" s="26" t="s">
-        <v>54</v>
-      </c>
-      <c r="B49" s="34"/>
-      <c r="C49" s="28">
-        <f>C46+C48</f>
-        <v>275</v>
-      </c>
-      <c r="D49" s="28">
-        <f>D46+D48</f>
-        <v>166</v>
-      </c>
-      <c r="E49" s="28">
-        <f>E46+E48</f>
-        <v>0</v>
-      </c>
-      <c r="F49" s="28">
-        <f>F46+F48</f>
-        <v>0</v>
-      </c>
-      <c r="G49" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="H49" s="35"/>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A50" s="1"/>
-      <c r="B50" s="33"/>
-      <c r="C50" s="25"/>
-      <c r="D50" s="25"/>
-      <c r="E50" s="25"/>
-      <c r="F50" s="25"/>
-      <c r="G50" s="17"/>
       <c r="H50" s="24"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B51" s="36">
-        <f>B52-SUM(C46:F46)</f>
+        <f>B47-SUM(C50:F50)</f>
         <v>1</v>
       </c>
       <c r="C51" s="24"/>
@@ -2256,102 +2258,173 @@
         <v>14</v>
       </c>
       <c r="H51" s="24" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B52" s="33">
-        <f>MIN(ROUND(MAKSBELOP3-B40,0), ROUND(SUM(C32:F32)-B40,0))</f>
-        <v>441</v>
-      </c>
-      <c r="C52" s="15"/>
-      <c r="D52" s="24"/>
-      <c r="E52" s="24"/>
-      <c r="F52" s="24"/>
+        <v>38</v>
+      </c>
+      <c r="B52" s="33"/>
+      <c r="C52" s="23">
+        <f>C49-TRUNC(C50)</f>
+        <v>0.63473053892221287</v>
+      </c>
+      <c r="D52" s="23">
+        <f>D49-TRUNC(D50)</f>
+        <v>0.36526946107787239</v>
+      </c>
+      <c r="E52" s="23">
+        <f>E49-TRUNC(E50)</f>
+        <v>0</v>
+      </c>
+      <c r="F52" s="23">
+        <f>F49-TRUNC(F50)</f>
+        <v>0</v>
+      </c>
       <c r="G52" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="H52" s="24" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B53" s="33"/>
+      <c r="C53" s="25">
+        <f>IF($B$51&gt;0, IF(LARGE($C$52:$F$52,$B$51)&lt;=C$52,1,0), 0)</f>
+        <v>1</v>
+      </c>
+      <c r="D53" s="25">
+        <f>IF($B$51&gt;0, IF(LARGE($C$52:$F$52,$B$51)&lt;=D$52,1,0), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="E53" s="25">
+        <f>IF($B$51&gt;0, IF(LARGE($C$52:$F$52,$B$51)&lt;=E$52,1,0), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="F53" s="25">
+        <f>IF($B$51&gt;0, IF(LARGE($C$52:$F$52,$B$51)&lt;=F$52,1,0), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="G53" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="H52" s="24" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A53" s="1"/>
-      <c r="B53" s="33"/>
-      <c r="C53" s="24"/>
-      <c r="D53" s="24"/>
-      <c r="E53" s="24"/>
-      <c r="F53" s="24"/>
-      <c r="G53" s="17"/>
       <c r="H53" s="24"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="26" t="s">
-        <v>59</v>
-      </c>
-      <c r="B54" s="37">
-        <f>B40+B52</f>
+        <v>51</v>
+      </c>
+      <c r="B54" s="34"/>
+      <c r="C54" s="28">
+        <f>C50+C53</f>
+        <v>275</v>
+      </c>
+      <c r="D54" s="28">
+        <f>D50+D53</f>
+        <v>166</v>
+      </c>
+      <c r="E54" s="28">
+        <f>E50+E53</f>
+        <v>0</v>
+      </c>
+      <c r="F54" s="28">
+        <f>F50+F53</f>
+        <v>0</v>
+      </c>
+      <c r="G54" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="H54" s="35"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A55" s="1"/>
+      <c r="B55" s="33"/>
+      <c r="C55" s="25"/>
+      <c r="D55" s="25"/>
+      <c r="E55" s="25"/>
+      <c r="F55" s="25"/>
+      <c r="G55" s="17"/>
+      <c r="H55" s="24"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A56" s="1"/>
+      <c r="B56" s="33"/>
+      <c r="C56" s="24"/>
+      <c r="D56" s="24"/>
+      <c r="E56" s="24"/>
+      <c r="F56" s="24"/>
+      <c r="G56" s="17"/>
+      <c r="H56" s="24"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A57" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="B57" s="37">
+        <f>B41+B47</f>
         <v>1886</v>
       </c>
-      <c r="C54" s="35"/>
-      <c r="D54" s="35"/>
-      <c r="E54" s="35"/>
-      <c r="F54" s="35"/>
-      <c r="G54" s="38"/>
-      <c r="H54" s="35"/>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A56" s="40"/>
-      <c r="B56" s="68"/>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A57" s="44"/>
-      <c r="B57" t="s">
-        <v>120</v>
-      </c>
-      <c r="C57">
+      <c r="C57" s="35"/>
+      <c r="D57" s="35"/>
+      <c r="E57" s="35"/>
+      <c r="F57" s="35"/>
+      <c r="G57" s="38"/>
+      <c r="H57" s="35"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A59" s="40"/>
+      <c r="B59" s="68"/>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A60" s="44"/>
+      <c r="B60" t="s">
+        <v>117</v>
+      </c>
+      <c r="C60">
         <v>1895</v>
       </c>
-      <c r="H57" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B58" t="s">
-        <v>121</v>
-      </c>
-      <c r="C58">
-        <v>298</v>
-      </c>
-      <c r="H58" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B59" t="s">
-        <v>122</v>
-      </c>
-      <c r="C59">
-        <v>307</v>
-      </c>
-      <c r="H59" s="4"/>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B60" t="s">
-        <v>123</v>
-      </c>
-      <c r="C60">
-        <v>635</v>
+      <c r="H60" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B61" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="C61">
+        <v>298</v>
+      </c>
+      <c r="H61" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B62" t="s">
+        <v>119</v>
+      </c>
+      <c r="C62">
+        <v>307</v>
+      </c>
+      <c r="H62" s="4"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B63" t="s">
+        <v>120</v>
+      </c>
+      <c r="C63">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B64" t="s">
+        <v>121</v>
+      </c>
+      <c r="C64">
         <v>655</v>
       </c>
     </row>
@@ -2385,28 +2458,28 @@
   <sheetData>
     <row r="1" spans="1:9" s="44" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="42" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" s="42" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="E1" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="42" t="s">
+      <c r="F1" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="D1" s="43" t="s">
+      <c r="G1" s="43" t="s">
         <v>65</v>
       </c>
-      <c r="E1" s="43" t="s">
+      <c r="H1" s="43" t="s">
         <v>66</v>
-      </c>
-      <c r="F1" s="43" t="s">
-        <v>67</v>
-      </c>
-      <c r="G1" s="43" t="s">
-        <v>68</v>
-      </c>
-      <c r="H1" s="43" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -2417,7 +2490,7 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D3" s="7">
         <v>21000</v>
@@ -2432,13 +2505,13 @@
         <v>0</v>
       </c>
       <c r="H3" s="41" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="44"/>
       <c r="B4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D4" s="8">
         <f>D3/SUM($D$3:$G$3)</f>
@@ -2457,7 +2530,7 @@
         <v>0</v>
       </c>
       <c r="H4" s="41" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -2465,7 +2538,7 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D5" s="45">
         <f>D3*12/260</f>
@@ -2484,10 +2557,10 @@
         <v>0</v>
       </c>
       <c r="H5" s="41" t="s">
+        <v>68</v>
+      </c>
+      <c r="I5" s="46" t="s">
         <v>71</v>
-      </c>
-      <c r="I5" s="46" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -2495,7 +2568,7 @@
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D6" s="10">
         <v>1</v>
@@ -2510,7 +2583,7 @@
         <v>1</v>
       </c>
       <c r="H6" s="41" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -2518,7 +2591,7 @@
         <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D7" s="45">
         <f>D5*D6</f>
@@ -2537,10 +2610,10 @@
         <v>0</v>
       </c>
       <c r="H7" s="41" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="I7" s="47" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -2548,7 +2621,7 @@
         <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D8" s="11">
         <f>MIN(D7,$C$15)</f>
@@ -2567,10 +2640,10 @@
         <v>0</v>
       </c>
       <c r="H8" s="41" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="I8" s="46" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -2578,7 +2651,7 @@
         <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D9" s="12">
         <v>0.5</v>
@@ -2593,7 +2666,7 @@
         <v>1</v>
       </c>
       <c r="H9" s="41" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -2601,7 +2674,7 @@
         <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D10" s="45">
         <f>D7*D9</f>
@@ -2620,7 +2693,7 @@
         <v>0</v>
       </c>
       <c r="H10" s="41" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -2628,7 +2701,7 @@
         <v>22</v>
       </c>
       <c r="B11" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D11" s="10">
         <v>1</v>
@@ -2643,7 +2716,7 @@
         <v>1</v>
       </c>
       <c r="H11" s="41" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -2651,7 +2724,7 @@
         <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D12" s="48">
         <f>D10*D11</f>
@@ -2670,7 +2743,7 @@
         <v>0</v>
       </c>
       <c r="H12" s="41" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -2678,14 +2751,14 @@
         <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C13" s="49">
         <f>ROUND(SUM(D10:G10)/SUM(D7:G7),2)</f>
         <v>0.4</v>
       </c>
       <c r="H13" s="41" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -2693,13 +2766,13 @@
         <v>26</v>
       </c>
       <c r="B14" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C14" s="7">
         <v>93634</v>
       </c>
       <c r="H14" s="41" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -2707,17 +2780,17 @@
         <v>28</v>
       </c>
       <c r="B15" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C15" s="11">
         <f>ROUND(6*C14/260, 0)</f>
         <v>2161</v>
       </c>
       <c r="H15" s="41" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="I15" s="46" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
@@ -2725,22 +2798,22 @@
         <v>29</v>
       </c>
       <c r="B16" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C16" s="11">
         <f>ROUND(C13*C15,0)</f>
         <v>864</v>
       </c>
       <c r="H16" s="41" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="50" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B17" s="51" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C17" s="52">
         <f>MIN(1, C16/SUM(D10:G10))</f>
@@ -2751,15 +2824,15 @@
       <c r="F17" s="53"/>
       <c r="G17" s="53"/>
       <c r="H17" s="54" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="50" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B18" s="51" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C18" s="51"/>
       <c r="D18" s="53">
@@ -2779,15 +2852,15 @@
         <v>0</v>
       </c>
       <c r="H18" s="54" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="50" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B19" s="51" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C19" s="51"/>
       <c r="D19" s="53">
@@ -2807,13 +2880,13 @@
         <v>0</v>
       </c>
       <c r="H19" s="54" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="50"/>
       <c r="B20" s="51" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C20" s="51"/>
       <c r="D20" s="53">
@@ -2833,13 +2906,13 @@
         <v>0</v>
       </c>
       <c r="H20" s="54" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="50"/>
       <c r="B21" s="51" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C21" s="51"/>
       <c r="D21" s="52">
@@ -2856,15 +2929,15 @@
       </c>
       <c r="G21" s="53"/>
       <c r="H21" s="54" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="22" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="50" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B22" s="51" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C22" s="51"/>
       <c r="D22" s="52">
@@ -2884,13 +2957,13 @@
         <v>0</v>
       </c>
       <c r="H22" s="54" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="23" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="50"/>
       <c r="B23" s="51" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C23" s="51"/>
       <c r="D23" s="53">
@@ -2910,15 +2983,15 @@
         <v>0</v>
       </c>
       <c r="H23" s="54" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="50" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B24" s="51" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C24" s="51"/>
       <c r="D24" s="53">
@@ -2938,13 +3011,13 @@
         <v>0</v>
       </c>
       <c r="H24" s="54" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="25" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="50"/>
       <c r="B25" s="51" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C25" s="51"/>
       <c r="D25" s="52">
@@ -2964,13 +3037,13 @@
         <v>0</v>
       </c>
       <c r="H25" s="54" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="26" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="50"/>
       <c r="B26" s="51" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C26" s="51"/>
       <c r="D26" s="52">
@@ -2990,15 +3063,15 @@
         <v>0</v>
       </c>
       <c r="H26" s="54" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="27" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="50" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B27" s="51" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C27" s="51"/>
       <c r="D27" s="55">
@@ -3018,15 +3091,15 @@
         <v>0</v>
       </c>
       <c r="H27" s="54" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="28" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="50" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B28" s="51" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C28" s="51"/>
       <c r="D28" s="51">
@@ -3046,13 +3119,13 @@
         <v>0</v>
       </c>
       <c r="H28" s="54" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="29" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="50"/>
       <c r="B29" s="51" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C29" s="56">
         <f>C16-SUM(D27:G28)</f>
@@ -3063,7 +3136,7 @@
       <c r="F29" s="51"/>
       <c r="G29" s="51"/>
       <c r="H29" s="54" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
@@ -3075,7 +3148,7 @@
         <v>20</v>
       </c>
       <c r="B31" s="18" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C31" s="15"/>
       <c r="D31" s="30">
@@ -3095,18 +3168,18 @@
         <v>0</v>
       </c>
       <c r="H31" s="17" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="I31" s="47" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B32" s="18" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C32" s="15"/>
       <c r="D32" s="30">
@@ -3126,15 +3199,15 @@
         <v>0</v>
       </c>
       <c r="H32" s="17" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B33" s="18" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C33" s="15"/>
       <c r="D33" s="30">
@@ -3154,13 +3227,13 @@
         <v>0</v>
       </c>
       <c r="H33" s="17" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="1"/>
       <c r="B34" s="57" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C34" s="79" t="str">
         <f>IF(SUM(D32:G33)&lt;=MAKSBELOP,"Everyone paid",IF(SUM(D32:G32)&lt;=MAKSBELOP,"Arbeidsgivere fully paid; Person partially paid by Person request", "Arbeidsgivere partial payment ratio by Arbeidsgiver request"))</f>
@@ -3174,10 +3247,10 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B35" s="18" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C35" s="15"/>
       <c r="D35" s="18">
@@ -3197,13 +3270,13 @@
         <v>0</v>
       </c>
       <c r="H35" s="17" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="36" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="1"/>
       <c r="B36" s="18" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C36" s="15">
         <f>MAKSBELOP-SUM(D35:G35)</f>
@@ -3217,10 +3290,10 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B37" s="18" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C37" s="18"/>
       <c r="D37" s="18">
@@ -3240,13 +3313,13 @@
         <v>0</v>
       </c>
       <c r="H37" s="17" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="1"/>
       <c r="B38" s="18" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C38" s="15">
         <f>MAKSBELOP-SUM(D35:G37)</f>
@@ -3257,12 +3330,12 @@
       <c r="F38" s="18"/>
       <c r="G38" s="18"/>
       <c r="H38" s="17" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="58" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B40" s="59"/>
       <c r="C40" s="60"/>
@@ -3270,7 +3343,7 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="80" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B41" s="80"/>
       <c r="C41" s="80"/>
@@ -3278,7 +3351,7 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="62" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B43" s="63">
         <v>1430.76</v>
@@ -3286,7 +3359,7 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="62" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B44" s="63">
         <f>ROUND(B43*260/12,0)</f>
@@ -3325,28 +3398,28 @@
   <sheetData>
     <row r="1" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="42" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" s="42" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="E1" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="42" t="s">
+      <c r="F1" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="D1" s="43" t="s">
+      <c r="G1" s="43" t="s">
         <v>65</v>
       </c>
-      <c r="E1" s="43" t="s">
+      <c r="H1" s="43" t="s">
         <v>66</v>
-      </c>
-      <c r="F1" s="43" t="s">
-        <v>67</v>
-      </c>
-      <c r="G1" s="43" t="s">
-        <v>68</v>
-      </c>
-      <c r="H1" s="43" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -3358,7 +3431,7 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D3" s="7">
         <v>21000</v>
@@ -3373,13 +3446,13 @@
         <v>0</v>
       </c>
       <c r="H3" s="41" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="44"/>
       <c r="B4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D4" s="8">
         <f>D3/SUM($D$3:$G$3)</f>
@@ -3398,7 +3471,7 @@
         <v>0</v>
       </c>
       <c r="H4" s="41" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -3406,7 +3479,7 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D5" s="45">
         <f>D3*12/260</f>
@@ -3425,7 +3498,7 @@
         <v>0</v>
       </c>
       <c r="H5" s="41" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -3433,7 +3506,7 @@
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D6" s="10">
         <v>1</v>
@@ -3448,7 +3521,7 @@
         <v>1</v>
       </c>
       <c r="H6" s="41" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -3456,7 +3529,7 @@
         <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D7" s="45">
         <f>D5*D6</f>
@@ -3475,7 +3548,7 @@
         <v>0</v>
       </c>
       <c r="H7" s="41" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -3483,7 +3556,7 @@
         <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D8" s="11">
         <f>MIN(D7,$C$15)</f>
@@ -3502,7 +3575,7 @@
         <v>0</v>
       </c>
       <c r="H8" s="41" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -3510,7 +3583,7 @@
         <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D9" s="12">
         <v>0.5</v>
@@ -3525,7 +3598,7 @@
         <v>1</v>
       </c>
       <c r="H9" s="41" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -3533,7 +3606,7 @@
         <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D10" s="45">
         <f>D7*D9</f>
@@ -3552,7 +3625,7 @@
         <v>0</v>
       </c>
       <c r="H10" s="41" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -3560,7 +3633,7 @@
         <v>22</v>
       </c>
       <c r="B11" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D11" s="10">
         <v>1</v>
@@ -3575,7 +3648,7 @@
         <v>1</v>
       </c>
       <c r="H11" s="41" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -3583,7 +3656,7 @@
         <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D12" s="48">
         <f>D10*D11</f>
@@ -3602,7 +3675,7 @@
         <v>0</v>
       </c>
       <c r="H12" s="41" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -3610,14 +3683,14 @@
         <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C13" s="64">
         <f>SUM(D10:G10)/SUM(D7:G7)</f>
         <v>0.39838709677419348</v>
       </c>
       <c r="H13" s="41" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
@@ -3625,13 +3698,13 @@
         <v>26</v>
       </c>
       <c r="B14" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C14" s="7">
         <v>101351</v>
       </c>
       <c r="H14" s="41" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
@@ -3639,14 +3712,14 @@
         <v>28</v>
       </c>
       <c r="B15" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C15" s="65">
         <f>6*C14/260</f>
         <v>2338.8692307692309</v>
       </c>
       <c r="H15" s="41" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
@@ -3654,22 +3727,22 @@
         <v>29</v>
       </c>
       <c r="B16" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C16" s="65">
         <f>C13*C15</f>
         <v>931.77532258064502</v>
       </c>
       <c r="H16" s="41" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="50" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B17" s="51" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C17" s="52">
         <f>MIN(1, C16/SUM(D10:G10))</f>
@@ -3680,15 +3753,15 @@
       <c r="F17" s="53"/>
       <c r="G17" s="53"/>
       <c r="H17" s="54" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="50" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B18" s="51" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C18" s="51"/>
       <c r="D18" s="53">
@@ -3708,15 +3781,15 @@
         <v>0</v>
       </c>
       <c r="H18" s="54" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="50" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B19" s="51" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C19" s="51"/>
       <c r="D19" s="53">
@@ -3736,13 +3809,13 @@
         <v>0</v>
       </c>
       <c r="H19" s="54" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="50"/>
       <c r="B20" s="51" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C20" s="51"/>
       <c r="D20" s="53">
@@ -3762,13 +3835,13 @@
         <v>0</v>
       </c>
       <c r="H20" s="54" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="21" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="50"/>
       <c r="B21" s="51" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C21" s="51"/>
       <c r="D21" s="52">
@@ -3785,15 +3858,15 @@
       </c>
       <c r="G21" s="53"/>
       <c r="H21" s="54" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="22" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="50" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B22" s="51" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C22" s="51"/>
       <c r="D22" s="52">
@@ -3813,13 +3886,13 @@
         <v>0</v>
       </c>
       <c r="H22" s="54" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="50"/>
       <c r="B23" s="51" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C23" s="51"/>
       <c r="D23" s="53">
@@ -3839,15 +3912,15 @@
         <v>0</v>
       </c>
       <c r="H23" s="54" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="50" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B24" s="51" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C24" s="51"/>
       <c r="D24" s="53">
@@ -3867,13 +3940,13 @@
         <v>0</v>
       </c>
       <c r="H24" s="54" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="25" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="50"/>
       <c r="B25" s="51" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C25" s="51"/>
       <c r="D25" s="52">
@@ -3893,13 +3966,13 @@
         <v>0</v>
       </c>
       <c r="H25" s="54" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="26" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="50"/>
       <c r="B26" s="51" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C26" s="51"/>
       <c r="D26" s="52">
@@ -3919,15 +3992,15 @@
         <v>0</v>
       </c>
       <c r="H26" s="54" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="50" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B27" s="51" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C27" s="51"/>
       <c r="D27" s="55">
@@ -3947,15 +4020,15 @@
         <v>0</v>
       </c>
       <c r="H27" s="54" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="28" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="50" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B28" s="51" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C28" s="51"/>
       <c r="D28" s="51">
@@ -3975,13 +4048,13 @@
         <v>0</v>
       </c>
       <c r="H28" s="54" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="29" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="50"/>
       <c r="B29" s="51" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C29" s="56">
         <f>C16-SUM(D27:G28)</f>
@@ -3992,7 +4065,7 @@
       <c r="F29" s="51"/>
       <c r="G29" s="51"/>
       <c r="H29" s="54" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
@@ -4005,7 +4078,7 @@
         <v>20</v>
       </c>
       <c r="B31" s="18" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C31" s="15"/>
       <c r="D31" s="66">
@@ -4025,15 +4098,15 @@
         <v>0</v>
       </c>
       <c r="H31" s="17" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B32" s="18" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C32" s="15"/>
       <c r="D32" s="66">
@@ -4053,15 +4126,15 @@
         <v>0</v>
       </c>
       <c r="H32" s="17" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B33" s="18" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C33" s="15"/>
       <c r="D33" s="66">
@@ -4081,13 +4154,13 @@
         <v>0</v>
       </c>
       <c r="H33" s="17" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="1"/>
       <c r="B34" s="57" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C34" s="79" t="str">
         <f>IF(SUM(D32:G33)&lt;=MAKSBELOP,"Everyone paid",IF(SUM(D32:G32)&lt;=MAKSBELOP,"Arbeidsgivere fully paid; Person partially paid by Person request", "Arbeidsgivere partial payment ratio by Arbeidsgiver request"))</f>
@@ -4101,10 +4174,10 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B35" s="18" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C35" s="15"/>
       <c r="D35" s="18">
@@ -4124,13 +4197,13 @@
         <v>0</v>
       </c>
       <c r="H35" s="17" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="1"/>
       <c r="B36" s="18" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C36" s="67">
         <f>MAKSBELOP2-SUM(D35:G35)</f>
@@ -4144,10 +4217,10 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B37" s="18" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C37" s="18"/>
       <c r="D37" s="25">
@@ -4167,13 +4240,13 @@
         <v>0</v>
       </c>
       <c r="H37" s="17" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="1"/>
       <c r="B38" s="18" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C38" s="67">
         <f>MAKSBELOP2-SUM(D35:G37)</f>
@@ -4184,7 +4257,7 @@
       <c r="F38" s="18"/>
       <c r="G38" s="18"/>
       <c r="H38" s="17" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fikser tilfeller hvor nevner er 0
</commit_message>
<xml_diff>
--- a/doc/okonomi/Utbetaling.xlsx
+++ b/doc/okonomi/Utbetaling.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/david/dev/nav/helse-spleis/doc/okonomi/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C33B8B89-FAF3-844D-9564-79DACC236F23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F6F2FCD-5FE2-564C-B953-AB4C4B0984AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="65700" windowHeight="36520" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -527,7 +527,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="9">
+  <numFmts count="11">
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* \-??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* \-??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="0.0000000000"/>
@@ -537,6 +537,8 @@
     <numFmt numFmtId="170" formatCode="#,##0.0000000000"/>
     <numFmt numFmtId="171" formatCode="_(* #,##0.000000000_);_(* \(#,##0.000000000\);_(* \-??_);_(@_)"/>
     <numFmt numFmtId="172" formatCode="_-* #,##0.000000_-;\-* #,##0.000000_-;_-* &quot;-&quot;??????????_-;_-@_-"/>
+    <numFmt numFmtId="173" formatCode="_-* #,##0.000000_-;\-* #,##0.000000_-;_-* &quot;-&quot;??????_-;_-@_-"/>
+    <numFmt numFmtId="174" formatCode="_-* #,##0.0000000000_-;\-* #,##0.0000000000_-;_-* &quot;-&quot;??????????_-;_-@_-"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -707,7 +709,7 @@
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -836,6 +838,9 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1222,8 +1227,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1279,7 +1284,7 @@
         <v>13000</v>
       </c>
       <c r="D3" s="7">
-        <v>14000</v>
+        <v>5000</v>
       </c>
       <c r="E3" s="7">
         <v>15000</v>
@@ -1299,19 +1304,19 @@
       <c r="B4" s="4"/>
       <c r="C4" s="8">
         <f>C3/SUM($C$3:$F$3)</f>
-        <v>0.23636363636363636</v>
+        <v>0.28260869565217389</v>
       </c>
       <c r="D4" s="8">
         <f>D3/SUM($C$3:$F$3)</f>
-        <v>0.25454545454545452</v>
+        <v>0.10869565217391304</v>
       </c>
       <c r="E4" s="8">
         <f>E3/SUM($C$3:$F$3)</f>
-        <v>0.27272727272727271</v>
+        <v>0.32608695652173914</v>
       </c>
       <c r="F4" s="8">
         <f>F3/SUM($C$3:$F$3)</f>
-        <v>0.23636363636363636</v>
+        <v>0.28260869565217389</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>8</v>
@@ -1330,7 +1335,7 @@
       </c>
       <c r="D5" s="39">
         <f t="shared" ref="D5:F5" si="0">D3*12</f>
-        <v>168000</v>
+        <v>60000</v>
       </c>
       <c r="E5" s="39">
         <f t="shared" si="0"/>
@@ -1352,22 +1357,10 @@
         <v>23</v>
       </c>
       <c r="B6" s="4"/>
-      <c r="C6" s="13">
-        <f>C3*0.2</f>
-        <v>2600</v>
-      </c>
-      <c r="D6" s="13">
-        <f>D3*0.1</f>
-        <v>1400</v>
-      </c>
-      <c r="E6" s="13">
-        <f>E3</f>
-        <v>15000</v>
-      </c>
-      <c r="F6" s="13">
-        <f>F3</f>
-        <v>13000</v>
-      </c>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
       <c r="G6" s="5" t="s">
         <v>8</v>
       </c>
@@ -1381,7 +1374,7 @@
       </c>
       <c r="B7" s="73">
         <f>SUM(C6:F6)*12</f>
-        <v>384000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -1414,7 +1407,7 @@
       </c>
       <c r="B9" s="72">
         <f>SUM(C5:F5)</f>
-        <v>660000</v>
+        <v>552000</v>
       </c>
       <c r="G9" s="71" t="s">
         <v>8</v>
@@ -1473,7 +1466,7 @@
       </c>
       <c r="B13" s="39">
         <f>ROUND(MIN(B9,B11)/260,)*260</f>
-        <v>561860</v>
+        <v>551980</v>
       </c>
       <c r="G13" s="71" t="s">
         <v>14</v>
@@ -1488,7 +1481,7 @@
       </c>
       <c r="B14" s="68">
         <f>B13/260</f>
-        <v>2161</v>
+        <v>2123</v>
       </c>
       <c r="G14" s="71" t="s">
         <v>14</v>
@@ -1508,7 +1501,7 @@
       </c>
       <c r="D16" s="9">
         <f>D5/260</f>
-        <v>646.15384615384619</v>
+        <v>230.76923076923077</v>
       </c>
       <c r="E16" s="9">
         <f>E5/260</f>
@@ -1560,7 +1553,7 @@
       </c>
       <c r="D18" s="9">
         <f>D16*D17</f>
-        <v>646.15384615384619</v>
+        <v>230.76923076923077</v>
       </c>
       <c r="E18" s="9">
         <f>E16*E17</f>
@@ -1583,19 +1576,19 @@
       </c>
       <c r="C19" s="75">
         <f>C8*C4</f>
-        <v>0.23636363636363636</v>
+        <v>0.28260869565217389</v>
       </c>
       <c r="D19" s="75">
         <f>D8*D4</f>
-        <v>0.12727272727272726</v>
+        <v>5.434782608695652E-2</v>
       </c>
       <c r="E19" s="75">
         <f>E8*E4</f>
-        <v>0.27272727272727271</v>
+        <v>0.32608695652173914</v>
       </c>
       <c r="F19" s="75">
         <f>F8*F4</f>
-        <v>0.23636363636363636</v>
+        <v>0.28260869565217389</v>
       </c>
       <c r="G19" s="71" t="s">
         <v>8</v>
@@ -1615,7 +1608,7 @@
       </c>
       <c r="D20" s="9">
         <f>D18*D8</f>
-        <v>323.07692307692309</v>
+        <v>115.38461538461539</v>
       </c>
       <c r="E20" s="9">
         <f>E18*E8</f>
@@ -1638,7 +1631,7 @@
       </c>
       <c r="B21" s="68">
         <f>SUM(C20:F20)</f>
-        <v>2215.3846153846152</v>
+        <v>2007.6923076923076</v>
       </c>
       <c r="G21" s="71" t="s">
         <v>8</v>
@@ -1653,7 +1646,7 @@
       </c>
       <c r="B22" s="73">
         <f>B21*260</f>
-        <v>576000</v>
+        <v>522000</v>
       </c>
       <c r="G22" s="71" t="s">
         <v>8</v>
@@ -1669,19 +1662,19 @@
       <c r="B23" s="4"/>
       <c r="C23" s="13">
         <f>MIN(C20,C6*C8*12/260)</f>
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="D23" s="13">
         <f>MIN(D20,D6*D8*12/260)</f>
-        <v>32.307692307692307</v>
+        <v>0</v>
       </c>
       <c r="E23" s="13">
         <f>MIN(E20,E6*E8*12/260)</f>
-        <v>692.30769230769226</v>
+        <v>0</v>
       </c>
       <c r="F23" s="13">
         <f>MIN(F20,F6*F8*12/260)</f>
-        <v>600</v>
+        <v>0</v>
       </c>
       <c r="G23" s="5" t="s">
         <v>8</v>
@@ -1696,7 +1689,7 @@
       </c>
       <c r="B24" s="68">
         <f>SUM(C23:F23)</f>
-        <v>1444.6153846153845</v>
+        <v>0</v>
       </c>
       <c r="G24" s="71" t="s">
         <v>8</v>
@@ -1711,7 +1704,7 @@
       </c>
       <c r="B25" s="73">
         <f>B24*260</f>
-        <v>375600</v>
+        <v>0</v>
       </c>
       <c r="G25" s="71" t="s">
         <v>8</v>
@@ -1726,8 +1719,10 @@
       </c>
       <c r="B26" s="68">
         <f>B21-B24</f>
-        <v>770.76923076923072</v>
-      </c>
+        <v>2007.6923076923076</v>
+      </c>
+      <c r="D26" s="86"/>
+      <c r="E26" s="87"/>
       <c r="G26" s="71" t="s">
         <v>8</v>
       </c>
@@ -1741,10 +1736,11 @@
       </c>
       <c r="B27" s="73">
         <f>B26*260</f>
-        <v>200400</v>
+        <v>522000</v>
       </c>
       <c r="C27" s="73"/>
       <c r="D27" s="79"/>
+      <c r="E27" s="87"/>
       <c r="G27" s="71" t="s">
         <v>8</v>
       </c>
@@ -1758,7 +1754,7 @@
       </c>
       <c r="B28" s="14">
         <f>SUM(C19:F19)</f>
-        <v>0.87272727272727268</v>
+        <v>0.94565217391304346</v>
       </c>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
@@ -1777,7 +1773,7 @@
       </c>
       <c r="B29" s="77">
         <f>ROUND(B13*B28/260,)*260</f>
-        <v>490360</v>
+        <v>522080</v>
       </c>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
@@ -1794,8 +1790,8 @@
       <c r="A30" s="74" t="s">
         <v>132</v>
       </c>
-      <c r="B30">
-        <f>MIN(1,B29/B25)</f>
+      <c r="B30" s="86">
+        <f>B29/MAX(B29,B25)</f>
         <v>1</v>
       </c>
       <c r="G30" s="71" t="s">
@@ -1816,7 +1812,7 @@
       </c>
       <c r="D32" s="16">
         <f>D20</f>
-        <v>323.07692307692309</v>
+        <v>115.38461538461539</v>
       </c>
       <c r="E32" s="16">
         <f>E20</f>
@@ -1840,19 +1836,19 @@
       <c r="B33" s="15"/>
       <c r="C33" s="16">
         <f>C23</f>
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="D33" s="16">
         <f>D23</f>
-        <v>32.307692307692307</v>
+        <v>0</v>
       </c>
       <c r="E33" s="16">
         <f>E23</f>
-        <v>692.30769230769226</v>
+        <v>0</v>
       </c>
       <c r="F33" s="16">
         <f>F23</f>
-        <v>600</v>
+        <v>0</v>
       </c>
       <c r="G33" s="17" t="s">
         <v>8</v>
@@ -1868,19 +1864,19 @@
       <c r="B34" s="15"/>
       <c r="C34" s="16">
         <f>C32-C33</f>
-        <v>480</v>
+        <v>600</v>
       </c>
       <c r="D34" s="16">
         <f>D32-D33</f>
-        <v>290.76923076923077</v>
+        <v>115.38461538461539</v>
       </c>
       <c r="E34" s="16">
         <f>E32-E33</f>
-        <v>0</v>
+        <v>692.30769230769226</v>
       </c>
       <c r="F34" s="16">
         <f>F32-F33</f>
-        <v>0</v>
+        <v>600</v>
       </c>
       <c r="G34" s="17" t="s">
         <v>8</v>
@@ -1921,19 +1917,19 @@
       <c r="B37" s="20"/>
       <c r="C37" s="23">
         <f>C33*$B$30</f>
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="D37" s="23">
         <f>D33*$B$30</f>
-        <v>32.307692307692307</v>
+        <v>0</v>
       </c>
       <c r="E37" s="23">
         <f>E33*$B$30</f>
-        <v>692.30769230769226</v>
+        <v>0</v>
       </c>
       <c r="F37" s="23">
         <f>F33*$B$30</f>
-        <v>600</v>
+        <v>0</v>
       </c>
       <c r="G37" s="17" t="s">
         <v>8</v>
@@ -1949,19 +1945,19 @@
       <c r="B38" s="15"/>
       <c r="C38" s="24">
         <f>FLOOR(C37,1)</f>
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="D38" s="24">
         <f>FLOOR(D37,1)</f>
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="E38" s="24">
         <f>FLOOR(E37,1)</f>
-        <v>692</v>
+        <v>0</v>
       </c>
       <c r="F38" s="24">
         <f>FLOOR(F37,1)</f>
-        <v>600</v>
+        <v>0</v>
       </c>
       <c r="G38" s="17" t="s">
         <v>14</v>
@@ -1976,7 +1972,7 @@
       </c>
       <c r="B39" s="15">
         <f>SUM(C38:F38)</f>
-        <v>1444</v>
+        <v>0</v>
       </c>
       <c r="C39" s="25"/>
       <c r="D39" s="24"/>
@@ -1995,7 +1991,7 @@
       </c>
       <c r="B40" s="30">
         <f>ROUND(SUM(C37:F37)-B39,)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C40" s="24"/>
       <c r="D40" s="24"/>
@@ -2014,7 +2010,7 @@
       </c>
       <c r="B41" s="15">
         <f>B39+B40</f>
-        <v>1445</v>
+        <v>0</v>
       </c>
       <c r="C41" s="25"/>
       <c r="D41" s="24"/>
@@ -2033,7 +2029,7 @@
       </c>
       <c r="B42" s="15">
         <f>B41*260</f>
-        <v>375700</v>
+        <v>0</v>
       </c>
       <c r="C42" s="25"/>
       <c r="D42" s="24"/>
@@ -2057,11 +2053,11 @@
       </c>
       <c r="D43" s="23">
         <f>D37-TRUNC(D37)</f>
-        <v>0.3076923076923066</v>
+        <v>0</v>
       </c>
       <c r="E43" s="23">
         <f>E37-TRUNC(E37)</f>
-        <v>0.30769230769226397</v>
+        <v>0</v>
       </c>
       <c r="F43" s="23">
         <f>F37-TRUNC(F37)</f>
@@ -2085,7 +2081,7 @@
       </c>
       <c r="D44" s="25">
         <f>IF($B$40&gt;0,IF(LARGE($C$43:$F$43,$B$40)&lt;=D$43,1,0), 0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E44" s="25">
         <f>IF($B$40&gt;0,IF(LARGE($C$43:$F$43,$B$40)&lt;=E$43,1,0), 0)</f>
@@ -2109,19 +2105,19 @@
       <c r="B45" s="27"/>
       <c r="C45" s="28">
         <f>C38+C44</f>
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="D45" s="28">
         <f>D38+D44</f>
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="E45" s="28">
         <f>E38+E44</f>
-        <v>692</v>
+        <v>0</v>
       </c>
       <c r="F45" s="28">
         <f>F38+F44</f>
-        <v>600</v>
+        <v>0</v>
       </c>
       <c r="G45" s="29" t="s">
         <v>14</v>
@@ -2146,23 +2142,23 @@
       </c>
       <c r="B47" s="33">
         <f>ROUND(MIN(B29-B42, B22-B42)/260,)</f>
-        <v>441</v>
+        <v>2008</v>
       </c>
       <c r="C47" s="15">
         <f>IF($B$22&lt;=$B$29,1,IF($B$25&lt;=$B$29,2,0))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D47" s="15">
         <f t="shared" ref="D47:F47" si="1">IF($B$22&lt;=$B$29,1,IF($B$25&lt;=$B$29,2,0))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E47" s="15">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F47" s="15">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G47" s="17" t="s">
         <v>14</v>
@@ -2175,11 +2171,11 @@
       <c r="A48" s="80" t="s">
         <v>150</v>
       </c>
-      <c r="B48" s="82">
-        <f>IF($B$22&lt;=$B$29,1,B47/B26)</f>
-        <v>0.57215568862275457</v>
-      </c>
-      <c r="C48" s="81"/>
+      <c r="B48" s="88">
+        <f>IF(B26 &gt; 0, MIN(1,B47/B26), 0)</f>
+        <v>1</v>
+      </c>
+      <c r="C48" s="82"/>
       <c r="D48" s="81"/>
       <c r="E48" s="81"/>
       <c r="F48" s="81"/>
@@ -2195,19 +2191,19 @@
       <c r="B49" s="31"/>
       <c r="C49" s="16">
         <f>C34*$B$48</f>
-        <v>274.63473053892221</v>
+        <v>600</v>
       </c>
       <c r="D49" s="16">
         <f t="shared" ref="D49:F49" si="2">D34*$B$48</f>
-        <v>166.36526946107787</v>
+        <v>115.38461538461539</v>
       </c>
       <c r="E49" s="16">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>692.30769230769226</v>
       </c>
       <c r="F49" s="16">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>600</v>
       </c>
       <c r="G49" s="17" t="s">
         <v>8</v>
@@ -2223,19 +2219,19 @@
       <c r="B50" s="24"/>
       <c r="C50" s="32">
         <f>FLOOR(C49, 1)</f>
-        <v>274</v>
+        <v>600</v>
       </c>
       <c r="D50" s="32">
         <f>FLOOR(D49, 1)</f>
-        <v>166</v>
+        <v>115</v>
       </c>
       <c r="E50" s="32">
         <f>FLOOR(E49, 1)</f>
-        <v>0</v>
+        <v>692</v>
       </c>
       <c r="F50" s="32">
         <f>FLOOR(F49, 1)</f>
-        <v>0</v>
+        <v>600</v>
       </c>
       <c r="G50" s="17" t="s">
         <v>14</v>
@@ -2268,15 +2264,15 @@
       <c r="B52" s="33"/>
       <c r="C52" s="23">
         <f>C49-TRUNC(C50)</f>
-        <v>0.63473053892221287</v>
+        <v>0</v>
       </c>
       <c r="D52" s="23">
         <f>D49-TRUNC(D50)</f>
-        <v>0.36526946107787239</v>
+        <v>0.3846153846153868</v>
       </c>
       <c r="E52" s="23">
         <f>E49-TRUNC(E50)</f>
-        <v>0</v>
+        <v>0.30769230769226397</v>
       </c>
       <c r="F52" s="23">
         <f>F49-TRUNC(F50)</f>
@@ -2296,11 +2292,11 @@
       <c r="B53" s="33"/>
       <c r="C53" s="25">
         <f>IF($B$51&gt;0, IF(LARGE($C$52:$F$52,$B$51)&lt;=C$52,1,0), 0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D53" s="25">
         <f>IF($B$51&gt;0, IF(LARGE($C$52:$F$52,$B$51)&lt;=D$52,1,0), 0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E53" s="25">
         <f>IF($B$51&gt;0, IF(LARGE($C$52:$F$52,$B$51)&lt;=E$52,1,0), 0)</f>
@@ -2322,19 +2318,19 @@
       <c r="B54" s="34"/>
       <c r="C54" s="28">
         <f>C50+C53</f>
-        <v>275</v>
+        <v>600</v>
       </c>
       <c r="D54" s="28">
         <f>D50+D53</f>
-        <v>166</v>
+        <v>116</v>
       </c>
       <c r="E54" s="28">
         <f>E50+E53</f>
-        <v>0</v>
+        <v>692</v>
       </c>
       <c r="F54" s="28">
         <f>F50+F53</f>
-        <v>0</v>
+        <v>600</v>
       </c>
       <c r="G54" s="29" t="s">
         <v>14</v>
@@ -2367,7 +2363,7 @@
       </c>
       <c r="B57" s="37">
         <f>B41+B47</f>
-        <v>1886</v>
+        <v>2008</v>
       </c>
       <c r="C57" s="35"/>
       <c r="D57" s="35"/>

</xml_diff>

<commit_message>
forenkler utregning av personbeløp
hvordan personbeløpet ble regnet ut samsvarte ikke med koden
</commit_message>
<xml_diff>
--- a/doc/okonomi/Utbetaling.xlsx
+++ b/doc/okonomi/Utbetaling.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/david/dev/nav/helse-spleis/doc/okonomi/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F6F2FCD-5FE2-564C-B953-AB4C4B0984AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17A49876-B427-0F45-B010-4D44E8D18CE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="65700" windowHeight="36520" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3980" yWindow="1440" windowWidth="65700" windowHeight="36520" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Flere arbeidsgivere, ny " sheetId="1" r:id="rId1"/>
@@ -709,7 +709,7 @@
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -832,15 +832,16 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1227,8 +1228,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1281,17 +1282,11 @@
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="7">
-        <v>13000</v>
-      </c>
-      <c r="D3" s="7">
         <v>5000</v>
       </c>
-      <c r="E3" s="7">
-        <v>15000</v>
-      </c>
-      <c r="F3" s="7">
-        <v>13000</v>
-      </c>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
       <c r="G3" s="5" t="s">
         <v>8</v>
       </c>
@@ -1304,19 +1299,19 @@
       <c r="B4" s="4"/>
       <c r="C4" s="8">
         <f>C3/SUM($C$3:$F$3)</f>
-        <v>0.28260869565217389</v>
+        <v>1</v>
       </c>
       <c r="D4" s="8">
         <f>D3/SUM($C$3:$F$3)</f>
-        <v>0.10869565217391304</v>
+        <v>0</v>
       </c>
       <c r="E4" s="8">
         <f>E3/SUM($C$3:$F$3)</f>
-        <v>0.32608695652173914</v>
+        <v>0</v>
       </c>
       <c r="F4" s="8">
         <f>F3/SUM($C$3:$F$3)</f>
-        <v>0.28260869565217389</v>
+        <v>0</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>8</v>
@@ -1331,19 +1326,19 @@
       </c>
       <c r="C5" s="39">
         <f>C3*12</f>
-        <v>156000</v>
+        <v>60000</v>
       </c>
       <c r="D5" s="39">
         <f t="shared" ref="D5:F5" si="0">D3*12</f>
-        <v>60000</v>
+        <v>0</v>
       </c>
       <c r="E5" s="39">
         <f t="shared" si="0"/>
-        <v>180000</v>
+        <v>0</v>
       </c>
       <c r="F5" s="39">
         <f t="shared" si="0"/>
-        <v>156000</v>
+        <v>0</v>
       </c>
       <c r="G5" s="71" t="s">
         <v>8</v>
@@ -1357,7 +1352,10 @@
         <v>23</v>
       </c>
       <c r="B6" s="4"/>
-      <c r="C6" s="13"/>
+      <c r="C6" s="13">
+        <f>C3*1</f>
+        <v>5000</v>
+      </c>
       <c r="D6" s="13"/>
       <c r="E6" s="13"/>
       <c r="F6" s="13"/>
@@ -1374,7 +1372,7 @@
       </c>
       <c r="B7" s="73">
         <f>SUM(C6:F6)*12</f>
-        <v>0</v>
+        <v>60000</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -1407,7 +1405,7 @@
       </c>
       <c r="B9" s="72">
         <f>SUM(C5:F5)</f>
-        <v>552000</v>
+        <v>60000</v>
       </c>
       <c r="G9" s="71" t="s">
         <v>8</v>
@@ -1466,7 +1464,7 @@
       </c>
       <c r="B13" s="39">
         <f>ROUND(MIN(B9,B11)/260,)*260</f>
-        <v>551980</v>
+        <v>60060</v>
       </c>
       <c r="G13" s="71" t="s">
         <v>14</v>
@@ -1481,7 +1479,7 @@
       </c>
       <c r="B14" s="68">
         <f>B13/260</f>
-        <v>2123</v>
+        <v>231</v>
       </c>
       <c r="G14" s="71" t="s">
         <v>14</v>
@@ -1497,19 +1495,19 @@
       <c r="B16" s="4"/>
       <c r="C16" s="9">
         <f>C5/260</f>
-        <v>600</v>
+        <v>230.76923076923077</v>
       </c>
       <c r="D16" s="9">
         <f>D5/260</f>
-        <v>230.76923076923077</v>
+        <v>0</v>
       </c>
       <c r="E16" s="9">
         <f>E5/260</f>
-        <v>692.30769230769226</v>
+        <v>0</v>
       </c>
       <c r="F16" s="9">
         <f>F5/260</f>
-        <v>600</v>
+        <v>0</v>
       </c>
       <c r="G16" s="5" t="s">
         <v>8</v>
@@ -1549,19 +1547,19 @@
       <c r="B18" s="4"/>
       <c r="C18" s="9">
         <f>C16*C17</f>
-        <v>600</v>
+        <v>230.76923076923077</v>
       </c>
       <c r="D18" s="9">
         <f>D16*D17</f>
-        <v>230.76923076923077</v>
+        <v>0</v>
       </c>
       <c r="E18" s="9">
         <f>E16*E17</f>
-        <v>692.30769230769226</v>
+        <v>0</v>
       </c>
       <c r="F18" s="9">
         <f>F16*F17</f>
-        <v>600</v>
+        <v>0</v>
       </c>
       <c r="G18" s="5" t="s">
         <v>8</v>
@@ -1576,19 +1574,19 @@
       </c>
       <c r="C19" s="75">
         <f>C8*C4</f>
-        <v>0.28260869565217389</v>
+        <v>1</v>
       </c>
       <c r="D19" s="75">
         <f>D8*D4</f>
-        <v>5.434782608695652E-2</v>
+        <v>0</v>
       </c>
       <c r="E19" s="75">
         <f>E8*E4</f>
-        <v>0.32608695652173914</v>
+        <v>0</v>
       </c>
       <c r="F19" s="75">
         <f>F8*F4</f>
-        <v>0.28260869565217389</v>
+        <v>0</v>
       </c>
       <c r="G19" s="71" t="s">
         <v>8</v>
@@ -1604,19 +1602,19 @@
       <c r="B20" s="4"/>
       <c r="C20" s="9">
         <f>C18*C8</f>
-        <v>600</v>
+        <v>230.76923076923077</v>
       </c>
       <c r="D20" s="9">
         <f>D18*D8</f>
-        <v>115.38461538461539</v>
+        <v>0</v>
       </c>
       <c r="E20" s="9">
         <f>E18*E8</f>
-        <v>692.30769230769226</v>
+        <v>0</v>
       </c>
       <c r="F20" s="9">
         <f>F18*F8</f>
-        <v>600</v>
+        <v>0</v>
       </c>
       <c r="G20" s="5" t="s">
         <v>8</v>
@@ -1631,7 +1629,7 @@
       </c>
       <c r="B21" s="68">
         <f>SUM(C20:F20)</f>
-        <v>2007.6923076923076</v>
+        <v>230.76923076923077</v>
       </c>
       <c r="G21" s="71" t="s">
         <v>8</v>
@@ -1646,7 +1644,7 @@
       </c>
       <c r="B22" s="73">
         <f>B21*260</f>
-        <v>522000</v>
+        <v>60000</v>
       </c>
       <c r="G22" s="71" t="s">
         <v>8</v>
@@ -1662,7 +1660,7 @@
       <c r="B23" s="4"/>
       <c r="C23" s="13">
         <f>MIN(C20,C6*C8*12/260)</f>
-        <v>0</v>
+        <v>230.76923076923077</v>
       </c>
       <c r="D23" s="13">
         <f>MIN(D20,D6*D8*12/260)</f>
@@ -1689,7 +1687,7 @@
       </c>
       <c r="B24" s="68">
         <f>SUM(C23:F23)</f>
-        <v>0</v>
+        <v>230.76923076923077</v>
       </c>
       <c r="G24" s="71" t="s">
         <v>8</v>
@@ -1704,7 +1702,7 @@
       </c>
       <c r="B25" s="73">
         <f>B24*260</f>
-        <v>0</v>
+        <v>60000</v>
       </c>
       <c r="G25" s="71" t="s">
         <v>8</v>
@@ -1719,10 +1717,10 @@
       </c>
       <c r="B26" s="68">
         <f>B21-B24</f>
-        <v>2007.6923076923076</v>
-      </c>
-      <c r="D26" s="86"/>
-      <c r="E26" s="87"/>
+        <v>0</v>
+      </c>
+      <c r="D26" s="84"/>
+      <c r="E26" s="85"/>
       <c r="G26" s="71" t="s">
         <v>8</v>
       </c>
@@ -1736,11 +1734,11 @@
       </c>
       <c r="B27" s="73">
         <f>B26*260</f>
-        <v>522000</v>
+        <v>0</v>
       </c>
       <c r="C27" s="73"/>
       <c r="D27" s="79"/>
-      <c r="E27" s="87"/>
+      <c r="E27" s="85"/>
       <c r="G27" s="71" t="s">
         <v>8</v>
       </c>
@@ -1754,7 +1752,7 @@
       </c>
       <c r="B28" s="14">
         <f>SUM(C19:F19)</f>
-        <v>0.94565217391304346</v>
+        <v>1</v>
       </c>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
@@ -1773,10 +1771,9 @@
       </c>
       <c r="B29" s="77">
         <f>ROUND(B13*B28/260,)*260</f>
-        <v>522080</v>
+        <v>60060</v>
       </c>
       <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
       <c r="G29" s="71" t="s">
@@ -1790,16 +1787,20 @@
       <c r="A30" s="74" t="s">
         <v>132</v>
       </c>
-      <c r="B30" s="86">
+      <c r="B30" s="84">
         <f>B29/MAX(B29,B25)</f>
         <v>1</v>
       </c>
+      <c r="C30" s="84"/>
       <c r="G30" s="71" t="s">
         <v>8</v>
       </c>
       <c r="H30" s="76" t="s">
         <v>133</v>
       </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D31" s="84"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
@@ -1808,19 +1809,19 @@
       <c r="B32" s="15"/>
       <c r="C32" s="16">
         <f>C20</f>
-        <v>600</v>
+        <v>230.76923076923077</v>
       </c>
       <c r="D32" s="16">
         <f>D20</f>
-        <v>115.38461538461539</v>
+        <v>0</v>
       </c>
       <c r="E32" s="16">
         <f>E20</f>
-        <v>692.30769230769226</v>
+        <v>0</v>
       </c>
       <c r="F32" s="16">
         <f>F20</f>
-        <v>600</v>
+        <v>0</v>
       </c>
       <c r="G32" s="17" t="s">
         <v>8</v>
@@ -1836,7 +1837,7 @@
       <c r="B33" s="15"/>
       <c r="C33" s="16">
         <f>C23</f>
-        <v>0</v>
+        <v>230.76923076923077</v>
       </c>
       <c r="D33" s="16">
         <f>D23</f>
@@ -1864,19 +1865,19 @@
       <c r="B34" s="15"/>
       <c r="C34" s="16">
         <f>C32-C33</f>
-        <v>600</v>
+        <v>0</v>
       </c>
       <c r="D34" s="16">
         <f>D32-D33</f>
-        <v>115.38461538461539</v>
+        <v>0</v>
       </c>
       <c r="E34" s="16">
         <f>E32-E33</f>
-        <v>692.30769230769226</v>
+        <v>0</v>
       </c>
       <c r="F34" s="16">
         <f>F32-F33</f>
-        <v>600</v>
+        <v>0</v>
       </c>
       <c r="G34" s="17" t="s">
         <v>8</v>
@@ -1917,7 +1918,7 @@
       <c r="B37" s="20"/>
       <c r="C37" s="23">
         <f>C33*$B$30</f>
-        <v>0</v>
+        <v>230.76923076923077</v>
       </c>
       <c r="D37" s="23">
         <f>D33*$B$30</f>
@@ -1945,7 +1946,7 @@
       <c r="B38" s="15"/>
       <c r="C38" s="24">
         <f>FLOOR(C37,1)</f>
-        <v>0</v>
+        <v>230</v>
       </c>
       <c r="D38" s="24">
         <f>FLOOR(D37,1)</f>
@@ -1972,7 +1973,7 @@
       </c>
       <c r="B39" s="15">
         <f>SUM(C38:F38)</f>
-        <v>0</v>
+        <v>230</v>
       </c>
       <c r="C39" s="25"/>
       <c r="D39" s="24"/>
@@ -1991,7 +1992,7 @@
       </c>
       <c r="B40" s="30">
         <f>ROUND(SUM(C37:F37)-B39,)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C40" s="24"/>
       <c r="D40" s="24"/>
@@ -2010,7 +2011,7 @@
       </c>
       <c r="B41" s="15">
         <f>B39+B40</f>
-        <v>0</v>
+        <v>231</v>
       </c>
       <c r="C41" s="25"/>
       <c r="D41" s="24"/>
@@ -2029,7 +2030,7 @@
       </c>
       <c r="B42" s="15">
         <f>B41*260</f>
-        <v>0</v>
+        <v>60060</v>
       </c>
       <c r="C42" s="25"/>
       <c r="D42" s="24"/>
@@ -2049,7 +2050,7 @@
       <c r="B43" s="15"/>
       <c r="C43" s="23">
         <f>C37-TRUNC(C37)</f>
-        <v>0</v>
+        <v>0.7692307692307736</v>
       </c>
       <c r="D43" s="23">
         <f>D37-TRUNC(D37)</f>
@@ -2077,7 +2078,7 @@
       <c r="B44" s="15"/>
       <c r="C44" s="25">
         <f>IF($B$40&gt;0,IF(LARGE($C$43:$F$43,$B$40)&lt;=C$43,1,0), 0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D44" s="25">
         <f>IF($B$40&gt;0,IF(LARGE($C$43:$F$43,$B$40)&lt;=D$43,1,0), 0)</f>
@@ -2105,7 +2106,7 @@
       <c r="B45" s="27"/>
       <c r="C45" s="28">
         <f>C38+C44</f>
-        <v>0</v>
+        <v>231</v>
       </c>
       <c r="D45" s="28">
         <f>D38+D44</f>
@@ -2128,7 +2129,7 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="1"/>
-      <c r="B46" s="15"/>
+      <c r="B46" s="89"/>
       <c r="C46" s="23"/>
       <c r="D46" s="23"/>
       <c r="E46" s="23"/>
@@ -2141,25 +2142,13 @@
         <v>54</v>
       </c>
       <c r="B47" s="33">
-        <f>ROUND(MIN(B29-B42, B22-B42)/260,)</f>
-        <v>2008</v>
-      </c>
-      <c r="C47" s="15">
-        <f>IF($B$22&lt;=$B$29,1,IF($B$25&lt;=$B$29,2,0))</f>
-        <v>1</v>
-      </c>
-      <c r="D47" s="15">
-        <f t="shared" ref="D47:F47" si="1">IF($B$22&lt;=$B$29,1,IF($B$25&lt;=$B$29,2,0))</f>
-        <v>1</v>
-      </c>
-      <c r="E47" s="15">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="F47" s="15">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
+        <f>ROUND((B29-B42)/260,)</f>
+        <v>0</v>
+      </c>
+      <c r="C47" s="15"/>
+      <c r="D47" s="15"/>
+      <c r="E47" s="15"/>
+      <c r="F47" s="15"/>
       <c r="G47" s="17" t="s">
         <v>14</v>
       </c>
@@ -2171,9 +2160,9 @@
       <c r="A48" s="80" t="s">
         <v>150</v>
       </c>
-      <c r="B48" s="88">
+      <c r="B48" s="86">
         <f>IF(B26 &gt; 0, MIN(1,B47/B26), 0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C48" s="82"/>
       <c r="D48" s="81"/>
@@ -2191,19 +2180,19 @@
       <c r="B49" s="31"/>
       <c r="C49" s="16">
         <f>C34*$B$48</f>
-        <v>600</v>
+        <v>0</v>
       </c>
       <c r="D49" s="16">
-        <f t="shared" ref="D49:F49" si="2">D34*$B$48</f>
-        <v>115.38461538461539</v>
+        <f t="shared" ref="D49:F49" si="1">D34*$B$48</f>
+        <v>0</v>
       </c>
       <c r="E49" s="16">
-        <f t="shared" si="2"/>
-        <v>692.30769230769226</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="F49" s="16">
-        <f t="shared" si="2"/>
-        <v>600</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="G49" s="17" t="s">
         <v>8</v>
@@ -2219,19 +2208,19 @@
       <c r="B50" s="24"/>
       <c r="C50" s="32">
         <f>FLOOR(C49, 1)</f>
-        <v>600</v>
+        <v>0</v>
       </c>
       <c r="D50" s="32">
         <f>FLOOR(D49, 1)</f>
-        <v>115</v>
+        <v>0</v>
       </c>
       <c r="E50" s="32">
         <f>FLOOR(E49, 1)</f>
-        <v>692</v>
+        <v>0</v>
       </c>
       <c r="F50" s="32">
         <f>FLOOR(F49, 1)</f>
-        <v>600</v>
+        <v>0</v>
       </c>
       <c r="G50" s="17" t="s">
         <v>14</v>
@@ -2244,7 +2233,7 @@
       </c>
       <c r="B51" s="36">
         <f>B47-SUM(C50:F50)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C51" s="24"/>
       <c r="D51" s="24"/>
@@ -2268,11 +2257,11 @@
       </c>
       <c r="D52" s="23">
         <f>D49-TRUNC(D50)</f>
-        <v>0.3846153846153868</v>
+        <v>0</v>
       </c>
       <c r="E52" s="23">
         <f>E49-TRUNC(E50)</f>
-        <v>0.30769230769226397</v>
+        <v>0</v>
       </c>
       <c r="F52" s="23">
         <f>F49-TRUNC(F50)</f>
@@ -2296,7 +2285,7 @@
       </c>
       <c r="D53" s="25">
         <f>IF($B$51&gt;0, IF(LARGE($C$52:$F$52,$B$51)&lt;=D$52,1,0), 0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E53" s="25">
         <f>IF($B$51&gt;0, IF(LARGE($C$52:$F$52,$B$51)&lt;=E$52,1,0), 0)</f>
@@ -2318,19 +2307,19 @@
       <c r="B54" s="34"/>
       <c r="C54" s="28">
         <f>C50+C53</f>
-        <v>600</v>
+        <v>0</v>
       </c>
       <c r="D54" s="28">
         <f>D50+D53</f>
-        <v>116</v>
+        <v>0</v>
       </c>
       <c r="E54" s="28">
         <f>E50+E53</f>
-        <v>692</v>
+        <v>0</v>
       </c>
       <c r="F54" s="28">
         <f>F50+F53</f>
-        <v>600</v>
+        <v>0</v>
       </c>
       <c r="G54" s="29" t="s">
         <v>14</v>
@@ -2363,7 +2352,7 @@
       </c>
       <c r="B57" s="37">
         <f>B41+B47</f>
-        <v>2008</v>
+        <v>231</v>
       </c>
       <c r="C57" s="35"/>
       <c r="D57" s="35"/>
@@ -3231,14 +3220,14 @@
       <c r="B34" s="57" t="s">
         <v>105</v>
       </c>
-      <c r="C34" s="84" t="str">
+      <c r="C34" s="87" t="str">
         <f>IF(SUM(D32:G33)&lt;=MAKSBELOP,"Everyone paid",IF(SUM(D32:G32)&lt;=MAKSBELOP,"Arbeidsgivere fully paid; Person partially paid by Person request", "Arbeidsgivere partial payment ratio by Arbeidsgiver request"))</f>
         <v>Arbeidsgivere partial payment ratio by Arbeidsgiver request</v>
       </c>
-      <c r="D34" s="84"/>
-      <c r="E34" s="84"/>
-      <c r="F34" s="84"/>
-      <c r="G34" s="84"/>
+      <c r="D34" s="87"/>
+      <c r="E34" s="87"/>
+      <c r="F34" s="87"/>
+      <c r="G34" s="87"/>
       <c r="H34" s="17"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
@@ -3338,12 +3327,12 @@
       <c r="D40" s="61"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A41" s="85" t="s">
+      <c r="A41" s="88" t="s">
         <v>108</v>
       </c>
-      <c r="B41" s="85"/>
-      <c r="C41" s="85"/>
-      <c r="D41" s="85"/>
+      <c r="B41" s="88"/>
+      <c r="C41" s="88"/>
+      <c r="D41" s="88"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="62" t="s">
@@ -4158,14 +4147,14 @@
       <c r="B34" s="57" t="s">
         <v>105</v>
       </c>
-      <c r="C34" s="84" t="str">
+      <c r="C34" s="87" t="str">
         <f>IF(SUM(D32:G33)&lt;=MAKSBELOP,"Everyone paid",IF(SUM(D32:G32)&lt;=MAKSBELOP,"Arbeidsgivere fully paid; Person partially paid by Person request", "Arbeidsgivere partial payment ratio by Arbeidsgiver request"))</f>
         <v>Arbeidsgivere partial payment ratio by Arbeidsgiver request</v>
       </c>
-      <c r="D34" s="84"/>
-      <c r="E34" s="84"/>
-      <c r="F34" s="84"/>
-      <c r="G34" s="84"/>
+      <c r="D34" s="87"/>
+      <c r="E34" s="87"/>
+      <c r="F34" s="87"/>
+      <c r="G34" s="87"/>
       <c r="H34" s="17"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
viser gradert refusjon (som daglig og årlig)
</commit_message>
<xml_diff>
--- a/doc/okonomi/Utbetaling.xlsx
+++ b/doc/okonomi/Utbetaling.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/david/dev/nav/helse-spleis/doc/okonomi/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1055867-02D2-FA42-946C-9A06A12783FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{404D211C-EDB5-3747-824B-9BEE2A007DD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-51200" yWindow="500" windowWidth="51200" windowHeight="28300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="76800" windowHeight="41000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Flere arbeidsgivere, ny " sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="147">
   <si>
     <t xml:space="preserve">Begrep	</t>
   </si>
@@ -501,6 +501,15 @@
   <si>
     <t>Personbeløp 6g-reduksjonsfaktor</t>
   </si>
+  <si>
+    <t>Gradert refusjon</t>
+  </si>
+  <si>
+    <t>Maks refusjon før redusering for dekningsgrunnlag</t>
+  </si>
+  <si>
+    <t>Totalt refusjon</t>
+  </si>
 </sst>
 </file>
 
@@ -519,7 +528,7 @@
     <numFmt numFmtId="172" formatCode="_-* #,##0.000000_-;\-* #,##0.000000_-;_-* &quot;-&quot;??????????_-;_-@_-"/>
     <numFmt numFmtId="173" formatCode="_-* #,##0.000000_-;\-* #,##0.000000_-;_-* &quot;-&quot;??????_-;_-@_-"/>
     <numFmt numFmtId="174" formatCode="_-* #,##0.0000000000_-;\-* #,##0.0000000000_-;_-* &quot;-&quot;??????????_-;_-@_-"/>
-    <numFmt numFmtId="176" formatCode="_-* #,##0.00000000_-;\-* #,##0.00000000_-;_-* &quot;-&quot;??????????_-;_-@_-"/>
+    <numFmt numFmtId="175" formatCode="_-* #,##0.00000000_-;\-* #,##0.00000000_-;_-* &quot;-&quot;??????????_-;_-@_-"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -749,7 +758,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -817,15 +825,16 @@
     <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1213,7 +1222,7 @@
   <dimension ref="A1:H62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1268,9 +1277,15 @@
       <c r="C3" s="7">
         <v>26016.25</v>
       </c>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
+      <c r="D3" s="7">
+        <v>5000</v>
+      </c>
+      <c r="E3" s="7">
+        <v>10000</v>
+      </c>
+      <c r="F3" s="7">
+        <v>35000</v>
+      </c>
       <c r="G3" s="5" t="s">
         <v>8</v>
       </c>
@@ -1283,19 +1298,19 @@
       <c r="B4" s="4"/>
       <c r="C4" s="8">
         <f>C3/SUM($C$3:$F$3)</f>
-        <v>1</v>
+        <v>0.3422459013697729</v>
       </c>
       <c r="D4" s="8">
         <f>D3/SUM($C$3:$F$3)</f>
-        <v>0</v>
+        <v>6.5775409863022716E-2</v>
       </c>
       <c r="E4" s="8">
         <f>E3/SUM($C$3:$F$3)</f>
-        <v>0</v>
+        <v>0.13155081972604543</v>
       </c>
       <c r="F4" s="8">
         <f>F3/SUM($C$3:$F$3)</f>
-        <v>0</v>
+        <v>0.46042786904115895</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>8</v>
@@ -1314,20 +1329,20 @@
       </c>
       <c r="D5" s="39">
         <f t="shared" ref="D5:F5" si="0">D3*12</f>
-        <v>0</v>
+        <v>60000</v>
       </c>
       <c r="E5" s="39">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>120000</v>
       </c>
       <c r="F5" s="39">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G5" s="71" t="s">
+        <v>420000</v>
+      </c>
+      <c r="G5" s="70" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="70" t="s">
+      <c r="H5" s="69" t="s">
         <v>111</v>
       </c>
     </row>
@@ -1342,10 +1357,16 @@
       </c>
       <c r="D6" s="13">
         <f>D3</f>
-        <v>0</v>
-      </c>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
+        <v>5000</v>
+      </c>
+      <c r="E6" s="13">
+        <f>E3</f>
+        <v>10000</v>
+      </c>
+      <c r="F6" s="13">
+        <f>F3*0.3</f>
+        <v>10500</v>
+      </c>
       <c r="G6" s="5" t="s">
         <v>8</v>
       </c>
@@ -1354,12 +1375,12 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="69" t="s">
+      <c r="A7" s="68" t="s">
         <v>127</v>
       </c>
-      <c r="B7" s="73">
+      <c r="B7" s="72">
         <f>SUM(C6:F6)*12</f>
-        <v>312195</v>
+        <v>618195</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -1387,14 +1408,14 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="69" t="s">
+      <c r="A9" s="68" t="s">
         <v>114</v>
       </c>
-      <c r="B9" s="72">
+      <c r="B9" s="71">
         <f>SUM(C5:F5)</f>
-        <v>312195</v>
-      </c>
-      <c r="G9" s="71" t="s">
+        <v>912195</v>
+      </c>
+      <c r="G9" s="70" t="s">
         <v>8</v>
       </c>
       <c r="H9" t="s">
@@ -1416,17 +1437,17 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="69" t="s">
+      <c r="A11" s="68" t="s">
         <v>28</v>
       </c>
       <c r="B11" s="39">
         <f>B10*6</f>
         <v>561804</v>
       </c>
-      <c r="G11" s="71" t="s">
+      <c r="G11" s="70" t="s">
         <v>14</v>
       </c>
-      <c r="H11" s="76" t="s">
+      <c r="H11" s="75" t="s">
         <v>119</v>
       </c>
     </row>
@@ -1438,40 +1459,40 @@
         <f>ROUND(B11/260,)</f>
         <v>2161</v>
       </c>
-      <c r="G12" s="71" t="s">
+      <c r="G12" s="70" t="s">
         <v>14</v>
       </c>
-      <c r="H12" s="76" t="s">
+      <c r="H12" s="75" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="69" t="s">
+      <c r="A13" s="68" t="s">
         <v>110</v>
       </c>
       <c r="B13" s="39">
         <f>ROUND(MIN(B9,B11)/260,)*260</f>
-        <v>312260</v>
-      </c>
-      <c r="G13" s="71" t="s">
+        <v>561860</v>
+      </c>
+      <c r="G13" s="70" t="s">
         <v>14</v>
       </c>
-      <c r="H13" s="76" t="s">
+      <c r="H13" s="75" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="69" t="s">
+      <c r="A14" s="68" t="s">
         <v>113</v>
       </c>
-      <c r="B14" s="68">
+      <c r="B14" s="67">
         <f>B13/260</f>
-        <v>1201</v>
-      </c>
-      <c r="G14" s="71" t="s">
+        <v>2161</v>
+      </c>
+      <c r="G14" s="70" t="s">
         <v>14</v>
       </c>
-      <c r="H14" s="76" t="s">
+      <c r="H14" s="75" t="s">
         <v>122</v>
       </c>
     </row>
@@ -1486,15 +1507,15 @@
       </c>
       <c r="D16" s="9">
         <f>D5/260</f>
-        <v>0</v>
+        <v>230.76923076923077</v>
       </c>
       <c r="E16" s="9">
         <f>E5/260</f>
-        <v>0</v>
+        <v>461.53846153846155</v>
       </c>
       <c r="F16" s="9">
         <f>F5/260</f>
-        <v>0</v>
+        <v>1615.3846153846155</v>
       </c>
       <c r="G16" s="5" t="s">
         <v>8</v>
@@ -1538,15 +1559,15 @@
       </c>
       <c r="D18" s="9">
         <f>D16*D17</f>
-        <v>0</v>
+        <v>230.76923076923077</v>
       </c>
       <c r="E18" s="9">
         <f>E16*E17</f>
-        <v>0</v>
+        <v>461.53846153846155</v>
       </c>
       <c r="F18" s="9">
         <f>F16*F17</f>
-        <v>0</v>
+        <v>1615.3846153846155</v>
       </c>
       <c r="G18" s="5" t="s">
         <v>8</v>
@@ -1556,29 +1577,29 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" s="74" t="s">
+      <c r="A19" s="73" t="s">
         <v>115</v>
       </c>
-      <c r="C19" s="75">
+      <c r="C19" s="74">
         <f>C8*C4</f>
-        <v>0.5</v>
-      </c>
-      <c r="D19" s="75">
+        <v>0.17112295068488645</v>
+      </c>
+      <c r="D19" s="74">
         <f>D8*D4</f>
-        <v>0</v>
-      </c>
-      <c r="E19" s="75">
+        <v>6.5775409863022716E-2</v>
+      </c>
+      <c r="E19" s="74">
         <f>E8*E4</f>
         <v>0</v>
       </c>
-      <c r="F19" s="75">
+      <c r="F19" s="74">
         <f>F8*F4</f>
-        <v>0</v>
-      </c>
-      <c r="G19" s="71" t="s">
+        <v>0.46042786904115895</v>
+      </c>
+      <c r="G19" s="70" t="s">
         <v>8</v>
       </c>
-      <c r="H19" s="76" t="s">
+      <c r="H19" s="75" t="s">
         <v>117</v>
       </c>
     </row>
@@ -1593,7 +1614,7 @@
       </c>
       <c r="D20" s="9">
         <f>D18*D8</f>
-        <v>0</v>
+        <v>230.76923076923077</v>
       </c>
       <c r="E20" s="9">
         <f>E18*E8</f>
@@ -1601,7 +1622,7 @@
       </c>
       <c r="F20" s="9">
         <f>F18*F8</f>
-        <v>0</v>
+        <v>1615.3846153846155</v>
       </c>
       <c r="G20" s="5" t="s">
         <v>8</v>
@@ -1611,415 +1632,412 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" s="74" t="s">
+      <c r="A21" s="73" t="s">
+        <v>144</v>
+      </c>
+      <c r="C21" s="67">
+        <f>C6*C8*12/260</f>
+        <v>600.375</v>
+      </c>
+      <c r="D21" s="67">
+        <f t="shared" ref="D21:F21" si="1">D6*D8*12/260</f>
+        <v>230.76923076923077</v>
+      </c>
+      <c r="E21" s="67">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F21" s="67">
+        <f t="shared" si="1"/>
+        <v>484.61538461538464</v>
+      </c>
+      <c r="G21" s="70" t="s">
+        <v>8</v>
+      </c>
+      <c r="H21" s="75" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="73" t="s">
         <v>132</v>
       </c>
-      <c r="B21" s="68">
+      <c r="B22" s="72">
         <f>SUM(C20:F20)</f>
-        <v>600.375</v>
-      </c>
-      <c r="G21" s="71" t="s">
+        <v>2446.5288461538462</v>
+      </c>
+      <c r="G22" s="70" t="s">
         <v>8</v>
       </c>
-      <c r="H21" s="76" t="s">
+      <c r="H22" s="75" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" s="74" t="s">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="73" t="s">
         <v>127</v>
       </c>
-      <c r="B22" s="73">
-        <f>B21*260</f>
-        <v>156097.5</v>
-      </c>
-      <c r="G22" s="71" t="s">
+      <c r="B23" s="72">
+        <f>B22*260</f>
+        <v>636097.5</v>
+      </c>
+      <c r="G23" s="70" t="s">
         <v>8</v>
       </c>
-      <c r="H22" s="76" t="s">
+      <c r="H23" s="75" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="73" t="s">
+        <v>146</v>
+      </c>
+      <c r="B24" s="72">
+        <f>SUM(C21:F21)</f>
+        <v>1315.7596153846152</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" s="73" t="s">
+        <v>127</v>
+      </c>
+      <c r="B25" s="72">
+        <f>B24*260</f>
+        <v>342097.49999999994</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="4"/>
-      <c r="C23" s="13">
+      <c r="B26" s="4"/>
+      <c r="C26" s="13">
         <f>MIN(C20,C6*C8*12/260)</f>
         <v>600.375</v>
       </c>
-      <c r="D23" s="13">
+      <c r="D26" s="13">
         <f>MIN(D20,D6*D8*12/260)</f>
-        <v>0</v>
-      </c>
-      <c r="E23" s="13">
+        <v>230.76923076923077</v>
+      </c>
+      <c r="E26" s="13">
         <f>MIN(E20,E6*E8*12/260)</f>
         <v>0</v>
       </c>
-      <c r="F23" s="13">
+      <c r="F26" s="13">
         <f>MIN(F20,F6*F8*12/260)</f>
-        <v>0</v>
-      </c>
-      <c r="G23" s="5" t="s">
+        <v>484.61538461538464</v>
+      </c>
+      <c r="G26" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="H23" s="6" t="s">
+      <c r="H26" s="6" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" s="74" t="s">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="73" t="s">
         <v>124</v>
       </c>
-      <c r="B24" s="68">
-        <f>SUM(C23:F23)</f>
+      <c r="B27" s="67">
+        <f>SUM(C26:F26)</f>
+        <v>1315.7596153846152</v>
+      </c>
+      <c r="G27" s="70" t="s">
+        <v>8</v>
+      </c>
+      <c r="H27" s="75" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="73" t="s">
+        <v>127</v>
+      </c>
+      <c r="B28" s="72">
+        <f>B27*260</f>
+        <v>342097.49999999994</v>
+      </c>
+      <c r="G28" s="70" t="s">
+        <v>8</v>
+      </c>
+      <c r="H28" s="75" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="73" t="s">
+        <v>134</v>
+      </c>
+      <c r="B29" s="67">
+        <f>B22-B27</f>
+        <v>1130.7692307692309</v>
+      </c>
+      <c r="D29" s="83"/>
+      <c r="E29" s="84"/>
+      <c r="G29" s="70" t="s">
+        <v>8</v>
+      </c>
+      <c r="H29" s="75" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="73" t="s">
+        <v>127</v>
+      </c>
+      <c r="B30" s="72">
+        <f>B29*260</f>
+        <v>294000.00000000006</v>
+      </c>
+      <c r="C30" s="72"/>
+      <c r="D30" s="78"/>
+      <c r="E30" s="84"/>
+      <c r="G30" s="70" t="s">
+        <v>8</v>
+      </c>
+      <c r="H30" s="75" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B31" s="14">
+        <f>SUM(C19:F19)</f>
+        <v>0.69732622958906809</v>
+      </c>
+      <c r="C31" s="89"/>
+      <c r="D31" s="92">
+        <f>C5*C17*C8/260</f>
         <v>600.375</v>
       </c>
-      <c r="G24" s="71" t="s">
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="H24" s="76" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" s="74" t="s">
-        <v>127</v>
-      </c>
-      <c r="B25" s="73">
-        <f>B24*260</f>
-        <v>156097.5</v>
-      </c>
-      <c r="G25" s="71" t="s">
+      <c r="H31" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="73" t="s">
+        <v>118</v>
+      </c>
+      <c r="B32" s="76">
+        <f>ROUND(B13*B31/260,)*260</f>
+        <v>391820</v>
+      </c>
+      <c r="C32" s="87">
+        <f>B32/B23</f>
+        <v>0.61597475229819332</v>
+      </c>
+      <c r="D32" s="83">
+        <f>C20*C32</f>
+        <v>369.8158419110278</v>
+      </c>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="70" t="s">
+        <v>14</v>
+      </c>
+      <c r="H32" s="75" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" s="73" t="s">
+        <v>125</v>
+      </c>
+      <c r="B33" s="83">
+        <f>B32/MAX(B32,B28)</f>
+        <v>1</v>
+      </c>
+      <c r="C33" s="83"/>
+      <c r="D33" s="88"/>
+      <c r="G33" s="70" t="s">
         <v>8</v>
       </c>
-      <c r="H25" s="76" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" s="74" t="s">
-        <v>134</v>
-      </c>
-      <c r="B26" s="68">
-        <f>B21-B24</f>
-        <v>0</v>
-      </c>
-      <c r="D26" s="84"/>
-      <c r="E26" s="85"/>
-      <c r="G26" s="71" t="s">
-        <v>8</v>
-      </c>
-      <c r="H26" s="76" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" s="74" t="s">
-        <v>127</v>
-      </c>
-      <c r="B27" s="73">
-        <f>B26*260</f>
-        <v>0</v>
-      </c>
-      <c r="C27" s="73"/>
-      <c r="D27" s="79"/>
-      <c r="E27" s="85"/>
-      <c r="G27" s="71" t="s">
-        <v>8</v>
-      </c>
-      <c r="H27" s="76" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B28" s="14">
-        <f>SUM(C19:F19)</f>
-        <v>0.5</v>
-      </c>
-      <c r="C28" s="92"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="H28" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" s="74" t="s">
-        <v>118</v>
-      </c>
-      <c r="B29" s="77">
-        <f>ROUND(B13*B28/260,)*260</f>
-        <v>156260</v>
-      </c>
-      <c r="C29" s="90"/>
-      <c r="D29" s="84"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="71" t="s">
-        <v>14</v>
-      </c>
-      <c r="H29" s="76" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A30" s="74" t="s">
-        <v>125</v>
-      </c>
-      <c r="B30" s="84">
-        <f>B29/MAX(B29,B25)</f>
-        <v>1</v>
-      </c>
-      <c r="C30" s="84"/>
-      <c r="D30" s="91"/>
-      <c r="G30" s="71" t="s">
-        <v>8</v>
-      </c>
-      <c r="H30" s="76" t="s">
+      <c r="H33" s="75" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D31" s="84"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D34" s="83"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B32" s="15"/>
-      <c r="C32" s="16">
+      <c r="B35" s="15"/>
+      <c r="C35" s="16">
         <f>C20</f>
         <v>600.375</v>
       </c>
-      <c r="D32" s="16">
+      <c r="D35" s="16">
         <f>D20</f>
-        <v>0</v>
-      </c>
-      <c r="E32" s="16">
+        <v>230.76923076923077</v>
+      </c>
+      <c r="E35" s="16">
         <f>E20</f>
         <v>0</v>
       </c>
-      <c r="F32" s="16">
+      <c r="F35" s="16">
         <f>F20</f>
-        <v>0</v>
-      </c>
-      <c r="G32" s="17" t="s">
+        <v>1615.3846153846155</v>
+      </c>
+      <c r="G35" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="H32" s="24" t="s">
+      <c r="H35" s="24" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="s">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B33" s="15"/>
-      <c r="C33" s="16">
-        <f>C23</f>
+      <c r="B36" s="15"/>
+      <c r="C36" s="16">
+        <f>C26</f>
         <v>600.375</v>
       </c>
-      <c r="D33" s="16">
-        <f>D23</f>
-        <v>0</v>
-      </c>
-      <c r="E33" s="16">
-        <f>E23</f>
-        <v>0</v>
-      </c>
-      <c r="F33" s="16">
-        <f>F23</f>
-        <v>0</v>
-      </c>
-      <c r="G33" s="17" t="s">
+      <c r="D36" s="16">
+        <f>D26</f>
+        <v>230.76923076923077</v>
+      </c>
+      <c r="E36" s="16">
+        <f>E26</f>
+        <v>0</v>
+      </c>
+      <c r="F36" s="16">
+        <f>F26</f>
+        <v>484.61538461538464</v>
+      </c>
+      <c r="G36" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="H33" s="24" t="s">
+      <c r="H36" s="24" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B34" s="15"/>
-      <c r="C34" s="16">
-        <f>C32-C33</f>
-        <v>0</v>
-      </c>
-      <c r="D34" s="16">
-        <f>D32-D33</f>
-        <v>0</v>
-      </c>
-      <c r="E34" s="16">
-        <f>E32-E33</f>
-        <v>0</v>
-      </c>
-      <c r="F34" s="16">
-        <f>F32-F33</f>
-        <v>0</v>
-      </c>
-      <c r="G34" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="H34" s="24" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B35" s="19" t="str">
-        <f>IF(B27&lt;=B29,"Arbeidsgiver og person blir refundert hele beløpet",IF(B25&lt;=B29,"Arbeidsgivere blir refundert hele beløpet; Person blir delvis refundert", "Arbeidsgivere blir delvis refundert"))</f>
-        <v>Arbeidsgiver og person blir refundert hele beløpet</v>
-      </c>
-      <c r="C35" s="19"/>
-      <c r="D35" s="19"/>
-      <c r="E35" s="19"/>
-      <c r="F35" s="19"/>
-      <c r="G35" s="17"/>
-      <c r="H35" s="24"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A36" s="1"/>
-      <c r="B36" s="20"/>
-      <c r="C36" s="78"/>
-      <c r="D36" s="21"/>
-      <c r="E36" s="21"/>
-      <c r="F36" s="22"/>
-      <c r="G36" s="17"/>
-      <c r="H36" s="24"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B37" s="20"/>
-      <c r="C37" s="23">
-        <f>C33*$B$30</f>
-        <v>600.375</v>
-      </c>
-      <c r="D37" s="23">
-        <f>D33*$B$30</f>
-        <v>0</v>
-      </c>
-      <c r="E37" s="23">
-        <f>E33*$B$30</f>
-        <v>0</v>
-      </c>
-      <c r="F37" s="23">
-        <f>F33*$B$30</f>
-        <v>0</v>
+        <v>33</v>
+      </c>
+      <c r="B37" s="15"/>
+      <c r="C37" s="16">
+        <f>C35-C36</f>
+        <v>0</v>
+      </c>
+      <c r="D37" s="16">
+        <f>D35-D36</f>
+        <v>0</v>
+      </c>
+      <c r="E37" s="16">
+        <f>E35-E36</f>
+        <v>0</v>
+      </c>
+      <c r="F37" s="16">
+        <f>F35-F36</f>
+        <v>1130.7692307692309</v>
       </c>
       <c r="G37" s="17" t="s">
         <v>8</v>
       </c>
       <c r="H37" s="24" t="s">
-        <v>35</v>
+        <v>138</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B38" s="15"/>
-      <c r="C38" s="24">
-        <f>FLOOR(C37,1)</f>
-        <v>600</v>
-      </c>
-      <c r="D38" s="24">
-        <f>FLOOR(D37,1)</f>
-        <v>0</v>
-      </c>
-      <c r="E38" s="24">
-        <f>FLOOR(E37,1)</f>
-        <v>0</v>
-      </c>
-      <c r="F38" s="24">
-        <f>FLOOR(F37,1)</f>
-        <v>0</v>
-      </c>
-      <c r="G38" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="H38" s="24" t="s">
-        <v>37</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="B38" s="19" t="str">
+        <f>IF(B30&lt;=B32,"Arbeidsgiver og person blir refundert hele beløpet",IF(B28&lt;=B32,"Arbeidsgivere blir refundert hele beløpet; Person blir delvis refundert", "Arbeidsgivere blir delvis refundert"))</f>
+        <v>Arbeidsgiver og person blir refundert hele beløpet</v>
+      </c>
+      <c r="C38" s="19"/>
+      <c r="D38" s="19"/>
+      <c r="E38" s="19"/>
+      <c r="F38" s="19"/>
+      <c r="G38" s="17"/>
+      <c r="H38" s="24"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A39" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="B39" s="15">
-        <f>SUM(C38:F38)</f>
-        <v>600</v>
-      </c>
-      <c r="C39" s="25"/>
-      <c r="D39" s="24"/>
-      <c r="E39" s="24"/>
-      <c r="F39" s="24"/>
-      <c r="G39" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="H39" s="24" t="s">
-        <v>140</v>
-      </c>
+      <c r="A39" s="1"/>
+      <c r="B39" s="20"/>
+      <c r="C39" s="77"/>
+      <c r="D39" s="21"/>
+      <c r="E39" s="21"/>
+      <c r="F39" s="22"/>
+      <c r="G39" s="17"/>
+      <c r="H39" s="24"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B40" s="30">
-        <f>ROUND(SUM(C37:F37)-B39,)</f>
-        <v>0</v>
-      </c>
-      <c r="C40" s="24"/>
-      <c r="D40" s="24"/>
-      <c r="E40" s="24"/>
-      <c r="F40" s="24"/>
+        <v>35</v>
+      </c>
+      <c r="B40" s="20"/>
+      <c r="C40" s="23">
+        <f>C36*$B$33</f>
+        <v>600.375</v>
+      </c>
+      <c r="D40" s="23">
+        <f>D36*$B$33</f>
+        <v>230.76923076923077</v>
+      </c>
+      <c r="E40" s="23">
+        <f>E36*$B$33</f>
+        <v>0</v>
+      </c>
+      <c r="F40" s="23">
+        <f>F36*$B$33</f>
+        <v>484.61538461538464</v>
+      </c>
       <c r="G40" s="17" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="H40" s="24" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B41" s="15">
-        <f>B39+B40</f>
+        <v>36</v>
+      </c>
+      <c r="B41" s="15"/>
+      <c r="C41" s="24">
+        <f>FLOOR(C40,1)</f>
         <v>600</v>
       </c>
-      <c r="C41" s="25"/>
-      <c r="D41" s="24"/>
-      <c r="E41" s="24"/>
-      <c r="F41" s="24"/>
+      <c r="D41" s="24">
+        <f>FLOOR(D40,1)</f>
+        <v>230</v>
+      </c>
+      <c r="E41" s="24">
+        <f>FLOOR(E40,1)</f>
+        <v>0</v>
+      </c>
+      <c r="F41" s="24">
+        <f>FLOOR(F40,1)</f>
+        <v>484</v>
+      </c>
       <c r="G41" s="17" t="s">
         <v>14</v>
       </c>
       <c r="H41" s="24" t="s">
-        <v>141</v>
+        <v>37</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>127</v>
+        <v>139</v>
       </c>
       <c r="B42" s="15">
-        <f>B41*260</f>
-        <v>156000</v>
+        <f>SUM(C41:F41)</f>
+        <v>1314</v>
       </c>
       <c r="C42" s="25"/>
       <c r="D42" s="24"/>
@@ -2029,260 +2047,244 @@
         <v>14</v>
       </c>
       <c r="H42" s="24" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B43" s="15"/>
-      <c r="C43" s="23">
-        <f>C37-TRUNC(C37)</f>
-        <v>0.375</v>
-      </c>
-      <c r="D43" s="23">
-        <f>D37-TRUNC(D37)</f>
-        <v>0</v>
-      </c>
-      <c r="E43" s="23">
-        <f>E37-TRUNC(E37)</f>
-        <v>0</v>
-      </c>
-      <c r="F43" s="23">
-        <f>F37-TRUNC(F37)</f>
-        <v>0</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="B43" s="30">
+        <f>ROUND(SUM(C40:F40)-B42,)</f>
+        <v>2</v>
+      </c>
+      <c r="C43" s="24"/>
+      <c r="D43" s="24"/>
+      <c r="E43" s="24"/>
+      <c r="F43" s="24"/>
       <c r="G43" s="17" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="H43" s="24" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B44" s="15"/>
-      <c r="C44" s="25">
-        <f>IF($B$40&gt;0,IF(LARGE($C$43:$F$43,$B$40)&lt;=C$43,1,0), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="D44" s="25">
-        <f>IF($B$40&gt;0,IF(LARGE($C$43:$F$43,$B$40)&lt;=D$43,1,0), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="E44" s="25">
-        <f>IF($B$40&gt;0,IF(LARGE($C$43:$F$43,$B$40)&lt;=E$43,1,0), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="F44" s="25">
-        <f>IF($B$40&gt;0,IF(LARGE($C$43:$F$43,$B$40)&lt;=F$43,1,0), 0)</f>
-        <v>0</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="B44" s="15">
+        <f>B42+B43</f>
+        <v>1316</v>
+      </c>
+      <c r="C44" s="25"/>
+      <c r="D44" s="24"/>
+      <c r="E44" s="24"/>
+      <c r="F44" s="24"/>
       <c r="G44" s="17" t="s">
         <v>14</v>
       </c>
       <c r="H44" s="24" t="s">
-        <v>41</v>
+        <v>141</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A45" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="B45" s="27"/>
-      <c r="C45" s="28">
-        <f>C38+C44</f>
-        <v>600</v>
-      </c>
-      <c r="D45" s="28">
-        <f>D38+D44</f>
-        <v>0</v>
-      </c>
-      <c r="E45" s="28">
-        <f>E38+E44</f>
-        <v>0</v>
-      </c>
-      <c r="F45" s="28">
-        <f>F38+F44</f>
-        <v>0</v>
-      </c>
-      <c r="G45" s="29" t="s">
+      <c r="A45" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B45" s="15">
+        <f>B44*260</f>
+        <v>342160</v>
+      </c>
+      <c r="C45" s="25"/>
+      <c r="D45" s="24"/>
+      <c r="E45" s="24"/>
+      <c r="F45" s="24"/>
+      <c r="G45" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="H45" s="26" t="s">
-        <v>137</v>
+      <c r="H45" s="24" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A46" s="1"/>
-      <c r="B46" s="87"/>
-      <c r="C46" s="23"/>
-      <c r="D46" s="23"/>
-      <c r="E46" s="23"/>
-      <c r="F46" s="23"/>
-      <c r="G46" s="17"/>
-      <c r="H46" s="24"/>
+      <c r="A46" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B46" s="15"/>
+      <c r="C46" s="23">
+        <f>C40-TRUNC(C40)</f>
+        <v>0.375</v>
+      </c>
+      <c r="D46" s="23">
+        <f>D40-TRUNC(D40)</f>
+        <v>0.7692307692307736</v>
+      </c>
+      <c r="E46" s="23">
+        <f>E40-TRUNC(E40)</f>
+        <v>0</v>
+      </c>
+      <c r="F46" s="23">
+        <f>F40-TRUNC(F40)</f>
+        <v>0.61538461538464162</v>
+      </c>
+      <c r="G46" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="H46" s="24" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B47" s="33">
-        <f>ROUND((B29-B42)/260,)</f>
+        <v>40</v>
+      </c>
+      <c r="B47" s="15"/>
+      <c r="C47" s="25">
+        <f>IF($B$43&gt;0,IF(LARGE($C$46:$F$46,$B$43)&lt;=C$46,1,0), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="D47" s="25">
+        <f>IF($B$43&gt;0,IF(LARGE($C$46:$F$46,$B$43)&lt;=D$46,1,0), 0)</f>
         <v>1</v>
       </c>
-      <c r="C47" s="15"/>
-      <c r="D47" s="15"/>
-      <c r="E47" s="15"/>
-      <c r="F47" s="15"/>
+      <c r="E47" s="25">
+        <f>IF($B$43&gt;0,IF(LARGE($C$46:$F$46,$B$43)&lt;=E$46,1,0), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="F47" s="25">
+        <f>IF($B$43&gt;0,IF(LARGE($C$46:$F$46,$B$43)&lt;=F$46,1,0), 0)</f>
+        <v>1</v>
+      </c>
       <c r="G47" s="17" t="s">
         <v>14</v>
       </c>
       <c r="H47" s="24" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A48" s="80" t="s">
-        <v>143</v>
-      </c>
-      <c r="B48" s="86">
-        <f>IF(B26 &gt; 0, MIN(1,B47/B26), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="C48" s="82"/>
-      <c r="D48" s="81"/>
-      <c r="E48" s="81"/>
-      <c r="F48" s="81"/>
-      <c r="G48" s="83" t="s">
-        <v>8</v>
-      </c>
-      <c r="H48" s="81"/>
+      <c r="A48" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="B48" s="27"/>
+      <c r="C48" s="28">
+        <f>C41+C47</f>
+        <v>600</v>
+      </c>
+      <c r="D48" s="28">
+        <f>D41+D47</f>
+        <v>231</v>
+      </c>
+      <c r="E48" s="28">
+        <f>E41+E47</f>
+        <v>0</v>
+      </c>
+      <c r="F48" s="28">
+        <f>F41+F47</f>
+        <v>485</v>
+      </c>
+      <c r="G48" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="H48" s="26" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A49" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B49" s="31"/>
-      <c r="C49" s="16">
-        <f>C34*$B$48</f>
-        <v>0</v>
-      </c>
-      <c r="D49" s="16">
-        <f t="shared" ref="D49:F49" si="1">D34*$B$48</f>
-        <v>0</v>
-      </c>
-      <c r="E49" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F49" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G49" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="H49" s="24" t="s">
-        <v>47</v>
-      </c>
+      <c r="A49" s="1"/>
+      <c r="B49" s="86"/>
+      <c r="C49" s="23"/>
+      <c r="D49" s="23"/>
+      <c r="E49" s="23"/>
+      <c r="F49" s="23"/>
+      <c r="G49" s="17"/>
+      <c r="H49" s="24"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B50" s="24"/>
-      <c r="C50" s="32">
-        <f>FLOOR(C49, 1)</f>
-        <v>0</v>
-      </c>
-      <c r="D50" s="32">
-        <f>FLOOR(D49, 1)</f>
-        <v>0</v>
-      </c>
-      <c r="E50" s="32">
-        <f>FLOOR(E49, 1)</f>
-        <v>0</v>
-      </c>
-      <c r="F50" s="32">
-        <f>FLOOR(F49, 1)</f>
-        <v>0</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="B50" s="33">
+        <f>ROUND((B32-B45)/260,)</f>
+        <v>191</v>
+      </c>
+      <c r="C50" s="15"/>
+      <c r="D50" s="15"/>
+      <c r="E50" s="15"/>
+      <c r="F50" s="15"/>
       <c r="G50" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="H50" s="24"/>
+      <c r="H50" s="24" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A51" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B51" s="36">
-        <f>B47-SUM(C50:F50)</f>
-        <v>1</v>
-      </c>
-      <c r="C51" s="24"/>
-      <c r="D51" s="24"/>
-      <c r="E51" s="24"/>
-      <c r="F51" s="24"/>
-      <c r="G51" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="H51" s="24" t="s">
-        <v>53</v>
-      </c>
+      <c r="A51" s="79" t="s">
+        <v>143</v>
+      </c>
+      <c r="B51" s="85">
+        <f>IF(B29 &gt; 0, MIN(1,B50/B29), 0)</f>
+        <v>0.1689115646258503</v>
+      </c>
+      <c r="C51" s="81"/>
+      <c r="D51" s="80"/>
+      <c r="E51" s="80"/>
+      <c r="F51" s="80"/>
+      <c r="G51" s="82" t="s">
+        <v>8</v>
+      </c>
+      <c r="H51" s="80"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B52" s="33"/>
-      <c r="C52" s="23">
-        <f>C49-TRUNC(C50)</f>
-        <v>0</v>
-      </c>
-      <c r="D52" s="23">
-        <f>D49-TRUNC(D50)</f>
-        <v>0</v>
-      </c>
-      <c r="E52" s="23">
-        <f>E49-TRUNC(E50)</f>
-        <v>0</v>
-      </c>
-      <c r="F52" s="23">
-        <f>F49-TRUNC(F50)</f>
-        <v>0</v>
+        <v>46</v>
+      </c>
+      <c r="B52" s="31"/>
+      <c r="C52" s="16">
+        <f>C37*$B$51</f>
+        <v>0</v>
+      </c>
+      <c r="D52" s="16">
+        <f>D37*$B$51</f>
+        <v>0</v>
+      </c>
+      <c r="E52" s="16">
+        <f>E37*$B$51</f>
+        <v>0</v>
+      </c>
+      <c r="F52" s="16">
+        <f>F37*$B$51</f>
+        <v>191</v>
       </c>
       <c r="G52" s="17" t="s">
         <v>8</v>
       </c>
       <c r="H52" s="24" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B53" s="33"/>
-      <c r="C53" s="25">
-        <f>IF($B$51&gt;0, IF(LARGE($C$52:$F$52,$B$51)&lt;=C$52,1,0), 0)</f>
-        <v>1</v>
-      </c>
-      <c r="D53" s="25">
-        <f>IF($B$51&gt;0, IF(LARGE($C$52:$F$52,$B$51)&lt;=D$52,1,0), 0)</f>
-        <v>1</v>
-      </c>
-      <c r="E53" s="25">
-        <f>IF($B$51&gt;0, IF(LARGE($C$52:$F$52,$B$51)&lt;=E$52,1,0), 0)</f>
-        <v>1</v>
-      </c>
-      <c r="F53" s="25">
-        <f>IF($B$51&gt;0, IF(LARGE($C$52:$F$52,$B$51)&lt;=F$52,1,0), 0)</f>
-        <v>1</v>
+        <v>48</v>
+      </c>
+      <c r="B53" s="24"/>
+      <c r="C53" s="32">
+        <f>FLOOR(C52, 1)</f>
+        <v>0</v>
+      </c>
+      <c r="D53" s="32">
+        <f>FLOOR(D52, 1)</f>
+        <v>0</v>
+      </c>
+      <c r="E53" s="32">
+        <f>FLOOR(E52, 1)</f>
+        <v>0</v>
+      </c>
+      <c r="F53" s="32">
+        <f>FLOOR(F52, 1)</f>
+        <v>191</v>
       </c>
       <c r="G53" s="17" t="s">
         <v>14</v>
@@ -2290,72 +2292,138 @@
       <c r="H53" s="24"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A54" s="26" t="s">
-        <v>51</v>
-      </c>
-      <c r="B54" s="34"/>
-      <c r="C54" s="28">
-        <f>C50+C53</f>
-        <v>1</v>
-      </c>
-      <c r="D54" s="28">
-        <f>D50+D53</f>
-        <v>1</v>
-      </c>
-      <c r="E54" s="28">
-        <f>E50+E53</f>
-        <v>1</v>
-      </c>
-      <c r="F54" s="28">
-        <f>F50+F53</f>
-        <v>1</v>
-      </c>
-      <c r="G54" s="29" t="s">
+      <c r="A54" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B54" s="36">
+        <f>B50-SUM(C53:F53)</f>
+        <v>0</v>
+      </c>
+      <c r="C54" s="24"/>
+      <c r="D54" s="24"/>
+      <c r="E54" s="24"/>
+      <c r="F54" s="24"/>
+      <c r="G54" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="H54" s="35"/>
+      <c r="H54" s="24" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A55" s="1"/>
+      <c r="A55" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="B55" s="33"/>
-      <c r="C55" s="25"/>
-      <c r="D55" s="25"/>
-      <c r="E55" s="25"/>
-      <c r="F55" s="25"/>
-      <c r="G55" s="17"/>
-      <c r="H55" s="24"/>
+      <c r="C55" s="23">
+        <f>C52-TRUNC(C53)</f>
+        <v>0</v>
+      </c>
+      <c r="D55" s="23">
+        <f>D52-TRUNC(D53)</f>
+        <v>0</v>
+      </c>
+      <c r="E55" s="23">
+        <f>E52-TRUNC(E53)</f>
+        <v>0</v>
+      </c>
+      <c r="F55" s="23">
+        <f>F52-TRUNC(F53)</f>
+        <v>0</v>
+      </c>
+      <c r="G55" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="H55" s="24" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A56" s="1"/>
+      <c r="A56" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="B56" s="33"/>
-      <c r="C56" s="24"/>
-      <c r="D56" s="24"/>
-      <c r="E56" s="24"/>
-      <c r="F56" s="24"/>
-      <c r="G56" s="17"/>
+      <c r="C56" s="25">
+        <f>IF($B$54&gt;0, IF(LARGE($C$55:$F$55,$B$54)&lt;=C$55,1,0), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="D56" s="25">
+        <f>IF($B$54&gt;0, IF(LARGE($C$55:$F$55,$B$54)&lt;=D$55,1,0), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="E56" s="25">
+        <f>IF($B$54&gt;0, IF(LARGE($C$55:$F$55,$B$54)&lt;=E$55,1,0), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="F56" s="25">
+        <f>IF($B$54&gt;0, IF(LARGE($C$55:$F$55,$B$54)&lt;=F$55,1,0), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="G56" s="17" t="s">
+        <v>14</v>
+      </c>
       <c r="H56" s="24"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="B57" s="34"/>
+      <c r="C57" s="28">
+        <f>C53+C56</f>
+        <v>0</v>
+      </c>
+      <c r="D57" s="28">
+        <f>D53+D56</f>
+        <v>0</v>
+      </c>
+      <c r="E57" s="28">
+        <f>E53+E56</f>
+        <v>0</v>
+      </c>
+      <c r="F57" s="28">
+        <f>F53+F56</f>
+        <v>191</v>
+      </c>
+      <c r="G57" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="H57" s="35"/>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A58" s="1"/>
+      <c r="B58" s="33"/>
+      <c r="C58" s="25"/>
+      <c r="D58" s="25"/>
+      <c r="E58" s="25"/>
+      <c r="F58" s="25"/>
+      <c r="G58" s="17"/>
+      <c r="H58" s="24"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A59" s="1"/>
+      <c r="B59" s="33"/>
+      <c r="C59" s="24"/>
+      <c r="D59" s="24"/>
+      <c r="E59" s="24"/>
+      <c r="F59" s="24"/>
+      <c r="G59" s="17"/>
+      <c r="H59" s="24"/>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A60" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="B57" s="37">
-        <f>B41+B47</f>
-        <v>601</v>
-      </c>
-      <c r="C57" s="35"/>
-      <c r="D57" s="35"/>
-      <c r="E57" s="35"/>
-      <c r="F57" s="35"/>
-      <c r="G57" s="38"/>
-      <c r="H57" s="35"/>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A59" s="40"/>
-      <c r="B59" s="68"/>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A60" s="44"/>
+      <c r="B60" s="37">
+        <f>B44+B50</f>
+        <v>1507</v>
+      </c>
+      <c r="C60" s="35"/>
+      <c r="D60" s="35"/>
+      <c r="E60" s="35"/>
+      <c r="F60" s="35"/>
+      <c r="G60" s="38"/>
+      <c r="H60" s="35"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="H62" s="4"/>
@@ -2384,41 +2452,41 @@
     <col min="5" max="5" width="16.33203125" customWidth="1"/>
     <col min="6" max="6" width="17.33203125" customWidth="1"/>
     <col min="7" max="7" width="15.6640625" customWidth="1"/>
-    <col min="8" max="8" width="8.6640625" style="41" customWidth="1"/>
+    <col min="8" max="8" width="8.6640625" style="40" customWidth="1"/>
     <col min="9" max="9" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="44" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="42" t="s">
+    <row r="1" spans="1:9" s="43" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="41" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="41" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="42" t="s">
+      <c r="C1" s="41" t="s">
         <v>59</v>
       </c>
-      <c r="D1" s="43" t="s">
+      <c r="D1" s="42" t="s">
         <v>60</v>
       </c>
-      <c r="E1" s="43" t="s">
+      <c r="E1" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="F1" s="43" t="s">
+      <c r="F1" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="G1" s="43" t="s">
+      <c r="G1" s="42" t="s">
         <v>63</v>
       </c>
-      <c r="H1" s="43" t="s">
+      <c r="H1" s="42" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="44"/>
+      <c r="A2" s="43"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="43" t="s">
         <v>7</v>
       </c>
       <c r="B3" t="s">
@@ -2436,12 +2504,12 @@
       <c r="G3" s="7">
         <v>0</v>
       </c>
-      <c r="H3" s="41" t="s">
+      <c r="H3" s="40" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="44"/>
+      <c r="A4" s="43"/>
       <c r="B4" t="s">
         <v>67</v>
       </c>
@@ -2461,42 +2529,42 @@
         <f>G3/SUM($D$3:$G$3)</f>
         <v>0</v>
       </c>
-      <c r="H4" s="41" t="s">
+      <c r="H4" s="40" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="44" t="s">
+      <c r="A5" s="43" t="s">
         <v>11</v>
       </c>
       <c r="B5" t="s">
         <v>68</v>
       </c>
-      <c r="D5" s="45">
+      <c r="D5" s="44">
         <f>D3*12/260</f>
         <v>969.23076923076928</v>
       </c>
-      <c r="E5" s="45">
+      <c r="E5" s="44">
         <f>E3*12/260</f>
         <v>461.53846153846155</v>
       </c>
-      <c r="F5" s="45">
+      <c r="F5" s="44">
         <f>F3*12/260</f>
         <v>1430.7692307692307</v>
       </c>
-      <c r="G5" s="45">
+      <c r="G5" s="44">
         <f>G3*12/260</f>
         <v>0</v>
       </c>
-      <c r="H5" s="41" t="s">
+      <c r="H5" s="40" t="s">
         <v>66</v>
       </c>
-      <c r="I5" s="46" t="s">
+      <c r="I5" s="45" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="44" t="s">
+      <c r="A6" s="43" t="s">
         <v>13</v>
       </c>
       <c r="B6" t="s">
@@ -2514,42 +2582,42 @@
       <c r="G6" s="10">
         <v>1</v>
       </c>
-      <c r="H6" s="41" t="s">
+      <c r="H6" s="40" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="44" t="s">
+      <c r="A7" s="43" t="s">
         <v>16</v>
       </c>
       <c r="B7" t="s">
         <v>72</v>
       </c>
-      <c r="D7" s="45">
+      <c r="D7" s="44">
         <f>D5*D6</f>
         <v>969.23076923076928</v>
       </c>
-      <c r="E7" s="45">
+      <c r="E7" s="44">
         <f>E5*E6</f>
         <v>461.53846153846155</v>
       </c>
-      <c r="F7" s="45">
+      <c r="F7" s="44">
         <f>F5*F6</f>
         <v>1430.7692307692307</v>
       </c>
-      <c r="G7" s="45">
+      <c r="G7" s="44">
         <f>G5*G6</f>
         <v>0</v>
       </c>
-      <c r="H7" s="41" t="s">
+      <c r="H7" s="40" t="s">
         <v>66</v>
       </c>
-      <c r="I7" s="47" t="s">
+      <c r="I7" s="46" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="44" t="s">
+      <c r="A8" s="43" t="s">
         <v>17</v>
       </c>
       <c r="B8" t="s">
@@ -2571,15 +2639,15 @@
         <f>MIN(G7,$C$15)</f>
         <v>0</v>
       </c>
-      <c r="H8" s="41" t="s">
+      <c r="H8" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="I8" s="46" t="s">
+      <c r="I8" s="45" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="44" t="s">
+      <c r="A9" s="43" t="s">
         <v>18</v>
       </c>
       <c r="B9" t="s">
@@ -2597,39 +2665,39 @@
       <c r="G9" s="12">
         <v>1</v>
       </c>
-      <c r="H9" s="41" t="s">
+      <c r="H9" s="40" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="44" t="s">
+      <c r="A10" s="43" t="s">
         <v>20</v>
       </c>
       <c r="B10" t="s">
         <v>76</v>
       </c>
-      <c r="D10" s="45">
+      <c r="D10" s="44">
         <f>D7*D9</f>
         <v>484.61538461538464</v>
       </c>
-      <c r="E10" s="45">
+      <c r="E10" s="44">
         <f>E7*E9</f>
         <v>369.23076923076928</v>
       </c>
-      <c r="F10" s="45">
+      <c r="F10" s="44">
         <f>F7*F9</f>
         <v>286.15384615384613</v>
       </c>
-      <c r="G10" s="45">
+      <c r="G10" s="44">
         <f>G7*G9</f>
         <v>0</v>
       </c>
-      <c r="H10" s="41" t="s">
+      <c r="H10" s="40" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="44" t="s">
+      <c r="A11" s="43" t="s">
         <v>22</v>
       </c>
       <c r="B11" t="s">
@@ -2647,54 +2715,54 @@
       <c r="G11" s="10">
         <v>1</v>
       </c>
-      <c r="H11" s="41" t="s">
+      <c r="H11" s="40" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="44" t="s">
+      <c r="A12" s="43" t="s">
         <v>23</v>
       </c>
       <c r="B12" t="s">
         <v>78</v>
       </c>
-      <c r="D12" s="48">
+      <c r="D12" s="47">
         <f>D10*D11</f>
         <v>484.61538461538464</v>
       </c>
-      <c r="E12" s="48">
+      <c r="E12" s="47">
         <f>E10*E11</f>
         <v>332.30769230769238</v>
       </c>
-      <c r="F12" s="48">
+      <c r="F12" s="47">
         <f>F10*F11</f>
         <v>71.538461538461533</v>
       </c>
-      <c r="G12" s="48">
+      <c r="G12" s="47">
         <f>G10*G11</f>
         <v>0</v>
       </c>
-      <c r="H12" s="41" t="s">
+      <c r="H12" s="40" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="44" t="s">
+      <c r="A13" s="43" t="s">
         <v>24</v>
       </c>
       <c r="B13" t="s">
         <v>79</v>
       </c>
-      <c r="C13" s="49">
+      <c r="C13" s="48">
         <f>ROUND(SUM(D10:G10)/SUM(D7:G7),2)</f>
         <v>0.4</v>
       </c>
-      <c r="H13" s="41" t="s">
+      <c r="H13" s="40" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="44" t="s">
+      <c r="A14" s="43" t="s">
         <v>26</v>
       </c>
       <c r="B14" t="s">
@@ -2703,12 +2771,12 @@
       <c r="C14" s="7">
         <v>93634</v>
       </c>
-      <c r="H14" s="41" t="s">
+      <c r="H14" s="40" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="44" t="s">
+      <c r="A15" s="43" t="s">
         <v>28</v>
       </c>
       <c r="B15" t="s">
@@ -2718,15 +2786,15 @@
         <f>ROUND(6*C14/260, 0)</f>
         <v>2161</v>
       </c>
-      <c r="H15" s="41" t="s">
+      <c r="H15" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="I15" s="46" t="s">
+      <c r="I15" s="45" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="44" t="s">
+      <c r="A16" s="43" t="s">
         <v>29</v>
       </c>
       <c r="B16" t="s">
@@ -2736,343 +2804,343 @@
         <f>ROUND(C13*C15,0)</f>
         <v>864</v>
       </c>
-      <c r="H16" s="41" t="s">
+      <c r="H16" s="40" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="50" t="s">
+      <c r="A17" s="49" t="s">
         <v>83</v>
       </c>
-      <c r="B17" s="51" t="s">
+      <c r="B17" s="50" t="s">
         <v>84</v>
       </c>
-      <c r="C17" s="52">
+      <c r="C17" s="51">
         <f>MIN(1, C16/SUM(D10:G10))</f>
         <v>0.75789473684210529</v>
       </c>
-      <c r="D17" s="53"/>
-      <c r="E17" s="53"/>
-      <c r="F17" s="53"/>
-      <c r="G17" s="53"/>
-      <c r="H17" s="54" t="s">
+      <c r="D17" s="52"/>
+      <c r="E17" s="52"/>
+      <c r="F17" s="52"/>
+      <c r="G17" s="52"/>
+      <c r="H17" s="53" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="50" t="s">
+      <c r="A18" s="49" t="s">
         <v>85</v>
       </c>
-      <c r="B18" s="51" t="s">
+      <c r="B18" s="50" t="s">
         <v>86</v>
       </c>
-      <c r="C18" s="51"/>
-      <c r="D18" s="53">
+      <c r="C18" s="50"/>
+      <c r="D18" s="52">
         <f>D10*ScalingFactor</f>
         <v>367.28744939271257</v>
       </c>
-      <c r="E18" s="53">
+      <c r="E18" s="52">
         <f>E10*ScalingFactor</f>
         <v>279.83805668016197</v>
       </c>
-      <c r="F18" s="53">
+      <c r="F18" s="52">
         <f>F10*ScalingFactor</f>
         <v>216.87449392712549</v>
       </c>
-      <c r="G18" s="53">
+      <c r="G18" s="52">
         <f>G10*ScalingFactor</f>
         <v>0</v>
       </c>
-      <c r="H18" s="54" t="s">
+      <c r="H18" s="53" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="50" t="s">
+      <c r="A19" s="49" t="s">
         <v>87</v>
       </c>
-      <c r="B19" s="51" t="s">
+      <c r="B19" s="50" t="s">
         <v>88</v>
       </c>
-      <c r="C19" s="51"/>
-      <c r="D19" s="53">
+      <c r="C19" s="50"/>
+      <c r="D19" s="52">
         <f>MIN(D18,D12)</f>
         <v>367.28744939271257</v>
       </c>
-      <c r="E19" s="53">
+      <c r="E19" s="52">
         <f>MIN(E18,E12)</f>
         <v>279.83805668016197</v>
       </c>
-      <c r="F19" s="53">
+      <c r="F19" s="52">
         <f>MIN(F18,F12)</f>
         <v>71.538461538461533</v>
       </c>
-      <c r="G19" s="53">
+      <c r="G19" s="52">
         <f>MIN(G18,G12)</f>
         <v>0</v>
       </c>
-      <c r="H19" s="54" t="s">
+      <c r="H19" s="53" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="50"/>
-      <c r="B20" s="51" t="s">
+      <c r="A20" s="49"/>
+      <c r="B20" s="50" t="s">
         <v>89</v>
       </c>
-      <c r="C20" s="51"/>
-      <c r="D20" s="53">
+      <c r="C20" s="50"/>
+      <c r="D20" s="52">
         <f>D19-D12</f>
         <v>-117.32793522267207</v>
       </c>
-      <c r="E20" s="53">
+      <c r="E20" s="52">
         <f>E19-E12</f>
         <v>-52.469635627530408</v>
       </c>
-      <c r="F20" s="53">
+      <c r="F20" s="52">
         <f>F19-F12</f>
         <v>0</v>
       </c>
-      <c r="G20" s="53">
+      <c r="G20" s="52">
         <f>G19-G12</f>
         <v>0</v>
       </c>
-      <c r="H20" s="54" t="s">
+      <c r="H20" s="53" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="50"/>
-      <c r="B21" s="51" t="s">
+      <c r="A21" s="49"/>
+      <c r="B21" s="50" t="s">
         <v>90</v>
       </c>
-      <c r="C21" s="51"/>
-      <c r="D21" s="52">
+      <c r="C21" s="50"/>
+      <c r="D21" s="51">
         <f>IF(D20 &lt; 0, D4, 0)</f>
         <v>0.33870967741935482</v>
       </c>
-      <c r="E21" s="52">
+      <c r="E21" s="51">
         <f>IF(E20 &lt; 0, E4, 0)</f>
         <v>0.16129032258064516</v>
       </c>
-      <c r="F21" s="52">
+      <c r="F21" s="51">
         <f>IF(F20 &lt; 0, F4, 0)</f>
         <v>0</v>
       </c>
-      <c r="G21" s="53"/>
-      <c r="H21" s="54" t="s">
+      <c r="G21" s="52"/>
+      <c r="H21" s="53" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="50" t="s">
+      <c r="A22" s="49" t="s">
         <v>91</v>
       </c>
-      <c r="B22" s="51" t="s">
+      <c r="B22" s="50" t="s">
         <v>92</v>
       </c>
-      <c r="C22" s="51"/>
-      <c r="D22" s="52">
+      <c r="C22" s="50"/>
+      <c r="D22" s="51">
         <f>IF(SUM(ShortfallIncomeRatioArb)=0,0,D21/SUM(ShortfallIncomeRatioArb))</f>
         <v>0.67741935483870963</v>
       </c>
-      <c r="E22" s="52">
+      <c r="E22" s="51">
         <f>IF(SUM(ShortfallIncomeRatioArb)=0,0,E21/SUM(ShortfallIncomeRatioArb))</f>
         <v>0.32258064516129031</v>
       </c>
-      <c r="F22" s="52">
+      <c r="F22" s="51">
         <f>IF(SUM(ShortfallIncomeRatioArb)=0,0,F21/SUM(ShortfallIncomeRatioArb))</f>
         <v>0</v>
       </c>
-      <c r="G22" s="52">
+      <c r="G22" s="51">
         <f>IF(SUM(ShortfallIncomeRatioArb)=0,0,G21/SUM(ShortfallIncomeRatioArb))</f>
         <v>0</v>
       </c>
-      <c r="H22" s="54" t="s">
+      <c r="H22" s="53" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="23" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="50"/>
-      <c r="B23" s="51" t="s">
+      <c r="A23" s="49"/>
+      <c r="B23" s="50" t="s">
         <v>93</v>
       </c>
-      <c r="C23" s="51"/>
-      <c r="D23" s="53">
+      <c r="C23" s="50"/>
+      <c r="D23" s="52">
         <f>D18-D19</f>
         <v>0</v>
       </c>
-      <c r="E23" s="53">
+      <c r="E23" s="52">
         <f>E18-E19</f>
         <v>0</v>
       </c>
-      <c r="F23" s="53">
+      <c r="F23" s="52">
         <f>F18-F19</f>
         <v>145.33603238866397</v>
       </c>
-      <c r="G23" s="53">
+      <c r="G23" s="52">
         <f>G18-G19</f>
         <v>0</v>
       </c>
-      <c r="H23" s="54" t="s">
+      <c r="H23" s="53" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="50" t="s">
+      <c r="A24" s="49" t="s">
         <v>94</v>
       </c>
-      <c r="B24" s="51" t="s">
+      <c r="B24" s="50" t="s">
         <v>95</v>
       </c>
-      <c r="C24" s="51"/>
-      <c r="D24" s="53">
+      <c r="C24" s="50"/>
+      <c r="D24" s="52">
         <f>MIN(-D20,IF(SUM($D$20:$G$20)&gt;=0, 0, SUM($D$23:$G$23)*D22))</f>
         <v>98.453441295546554</v>
       </c>
-      <c r="E24" s="53">
+      <c r="E24" s="52">
         <f>MIN(-E20,IF(SUM($D$20:$G$20)&gt;=0, 0, SUM($D$23:$G$23)*E22))</f>
         <v>46.882591093117405</v>
       </c>
-      <c r="F24" s="53">
+      <c r="F24" s="52">
         <f>MIN(-F20,IF(SUM($D$20:$G$20)&gt;=0, 0, SUM($D$23:$G$23)*F22))</f>
         <v>0</v>
       </c>
-      <c r="G24" s="53">
+      <c r="G24" s="52">
         <f>MIN(-G20,IF(SUM($D$20:$G$20)&gt;=0, 0, SUM($D$23:$G$23)*G22))</f>
         <v>0</v>
       </c>
-      <c r="H24" s="54" t="s">
+      <c r="H24" s="53" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="25" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="50"/>
-      <c r="B25" s="51" t="s">
+      <c r="A25" s="49"/>
+      <c r="B25" s="50" t="s">
         <v>96</v>
       </c>
-      <c r="C25" s="51"/>
-      <c r="D25" s="52">
+      <c r="C25" s="50"/>
+      <c r="D25" s="51">
         <f>IF(D23 = 0, 0, D4)</f>
         <v>0</v>
       </c>
-      <c r="E25" s="52">
+      <c r="E25" s="51">
         <f>IF(E23 = 0, 0, E4)</f>
         <v>0</v>
       </c>
-      <c r="F25" s="52">
+      <c r="F25" s="51">
         <f>IF(F23 = 0, 0, F4)</f>
         <v>0.5</v>
       </c>
-      <c r="G25" s="52">
+      <c r="G25" s="51">
         <f>IF(G23 = 0, 0, G4)</f>
         <v>0</v>
       </c>
-      <c r="H25" s="54" t="s">
+      <c r="H25" s="53" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="26" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="50"/>
-      <c r="B26" s="51" t="s">
+      <c r="A26" s="49"/>
+      <c r="B26" s="50" t="s">
         <v>97</v>
       </c>
-      <c r="C26" s="51"/>
-      <c r="D26" s="52">
+      <c r="C26" s="50"/>
+      <c r="D26" s="51">
         <f>IF(SUM(ShortfallIncomeRatioPerson)= 0, 0, D25/SUM(ShortfallIncomeRatioPerson))</f>
         <v>0</v>
       </c>
-      <c r="E26" s="52">
+      <c r="E26" s="51">
         <f>IF(SUM(ShortfallIncomeRatioPerson)= 0, 0, E25/SUM(ShortfallIncomeRatioPerson))</f>
         <v>0</v>
       </c>
-      <c r="F26" s="52">
+      <c r="F26" s="51">
         <f>IF(SUM(ShortfallIncomeRatioPerson)= 0, 0, F25/SUM(ShortfallIncomeRatioPerson))</f>
         <v>1</v>
       </c>
-      <c r="G26" s="52">
+      <c r="G26" s="51">
         <f>IF(SUM(ShortfallIncomeRatioPerson)= 0, 0, G25/SUM(ShortfallIncomeRatioPerson))</f>
         <v>0</v>
       </c>
-      <c r="H26" s="54" t="s">
+      <c r="H26" s="53" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="27" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="50" t="s">
+      <c r="A27" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="B27" s="51" t="s">
+      <c r="B27" s="50" t="s">
         <v>98</v>
       </c>
-      <c r="C27" s="51"/>
-      <c r="D27" s="55">
+      <c r="C27" s="50"/>
+      <c r="D27" s="54">
         <f>ROUND(D19+D24,0)</f>
         <v>466</v>
       </c>
-      <c r="E27" s="55">
+      <c r="E27" s="54">
         <f>ROUND(E19+E24,0)</f>
         <v>327</v>
       </c>
-      <c r="F27" s="55">
+      <c r="F27" s="54">
         <f>ROUND(F19+F24,0)</f>
         <v>72</v>
       </c>
-      <c r="G27" s="53">
+      <c r="G27" s="52">
         <f>ROUND(G19+G24,0)</f>
         <v>0</v>
       </c>
-      <c r="H27" s="54" t="s">
+      <c r="H27" s="53" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="28" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="50" t="s">
+      <c r="A28" s="49" t="s">
         <v>54</v>
       </c>
-      <c r="B28" s="51" t="s">
+      <c r="B28" s="50" t="s">
         <v>99</v>
       </c>
-      <c r="C28" s="51"/>
-      <c r="D28" s="51">
+      <c r="C28" s="50"/>
+      <c r="D28" s="50">
         <f>ROUND(D23-SUM(AdjustmentArb)*D26,0)</f>
         <v>0</v>
       </c>
-      <c r="E28" s="51">
+      <c r="E28" s="50">
         <f>ROUND(E23-SUM(AdjustmentArb)*E26,0)</f>
         <v>0</v>
       </c>
-      <c r="F28" s="51">
+      <c r="F28" s="50">
         <f>ROUND(F23-SUM(AdjustmentArb)*F26,0)</f>
         <v>0</v>
       </c>
-      <c r="G28" s="51">
+      <c r="G28" s="50">
         <f>ROUND(G23-SUM(AdjustmentArb)*G26,0)</f>
         <v>0</v>
       </c>
-      <c r="H28" s="54" t="s">
+      <c r="H28" s="53" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="29" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="50"/>
-      <c r="B29" s="51" t="s">
+      <c r="A29" s="49"/>
+      <c r="B29" s="50" t="s">
         <v>100</v>
       </c>
-      <c r="C29" s="56">
+      <c r="C29" s="55">
         <f>C16-SUM(D27:G28)</f>
         <v>-1</v>
       </c>
-      <c r="D29" s="51"/>
-      <c r="E29" s="51"/>
-      <c r="F29" s="51"/>
-      <c r="G29" s="51"/>
-      <c r="H29" s="54" t="s">
+      <c r="D29" s="50"/>
+      <c r="E29" s="50"/>
+      <c r="F29" s="50"/>
+      <c r="G29" s="50"/>
+      <c r="H29" s="53" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A30" s="44"/>
+      <c r="A30" s="43"/>
       <c r="C30" s="39"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
@@ -3102,7 +3170,7 @@
       <c r="H31" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="I31" s="47" t="s">
+      <c r="I31" s="46" t="s">
         <v>73</v>
       </c>
     </row>
@@ -3164,17 +3232,17 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="1"/>
-      <c r="B34" s="57" t="s">
+      <c r="B34" s="56" t="s">
         <v>103</v>
       </c>
-      <c r="C34" s="88" t="str">
+      <c r="C34" s="90" t="str">
         <f>IF(SUM(D32:G33)&lt;=MAKSBELOP,"Everyone paid",IF(SUM(D32:G32)&lt;=MAKSBELOP,"Arbeidsgivere fully paid; Person partially paid by Person request", "Arbeidsgivere partial payment ratio by Arbeidsgiver request"))</f>
         <v>Arbeidsgivere partial payment ratio by Arbeidsgiver request</v>
       </c>
-      <c r="D34" s="88"/>
-      <c r="E34" s="88"/>
-      <c r="F34" s="88"/>
-      <c r="G34" s="88"/>
+      <c r="D34" s="90"/>
+      <c r="E34" s="90"/>
+      <c r="F34" s="90"/>
+      <c r="G34" s="90"/>
       <c r="H34" s="17"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
@@ -3266,34 +3334,34 @@
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A40" s="58" t="s">
+      <c r="A40" s="57" t="s">
         <v>105</v>
       </c>
-      <c r="B40" s="59"/>
-      <c r="C40" s="60"/>
-      <c r="D40" s="61"/>
+      <c r="B40" s="58"/>
+      <c r="C40" s="59"/>
+      <c r="D40" s="60"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A41" s="89" t="s">
+      <c r="A41" s="91" t="s">
         <v>106</v>
       </c>
-      <c r="B41" s="89"/>
-      <c r="C41" s="89"/>
-      <c r="D41" s="89"/>
+      <c r="B41" s="91"/>
+      <c r="C41" s="91"/>
+      <c r="D41" s="91"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A43" s="62" t="s">
+      <c r="A43" s="61" t="s">
         <v>107</v>
       </c>
-      <c r="B43" s="63">
+      <c r="B43" s="62">
         <v>1430.76</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A44" s="62" t="s">
+      <c r="A44" s="61" t="s">
         <v>108</v>
       </c>
-      <c r="B44" s="63">
+      <c r="B44" s="62">
         <f>ROUND(B43*260/12,0)</f>
         <v>31000</v>
       </c>
@@ -3329,37 +3397,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="41" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="41" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="42" t="s">
+      <c r="C1" s="41" t="s">
         <v>59</v>
       </c>
-      <c r="D1" s="43" t="s">
+      <c r="D1" s="42" t="s">
         <v>60</v>
       </c>
-      <c r="E1" s="43" t="s">
+      <c r="E1" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="F1" s="43" t="s">
+      <c r="F1" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="G1" s="43" t="s">
+      <c r="G1" s="42" t="s">
         <v>63</v>
       </c>
-      <c r="H1" s="43" t="s">
+      <c r="H1" s="42" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="44"/>
-      <c r="H2" s="41"/>
+      <c r="A2" s="43"/>
+      <c r="H2" s="40"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="43" t="s">
         <v>7</v>
       </c>
       <c r="B3" t="s">
@@ -3377,12 +3445,12 @@
       <c r="G3" s="7">
         <v>0</v>
       </c>
-      <c r="H3" s="41" t="s">
+      <c r="H3" s="40" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="44"/>
+      <c r="A4" s="43"/>
       <c r="B4" t="s">
         <v>67</v>
       </c>
@@ -3402,39 +3470,39 @@
         <f>G3/SUM($D$3:$G$3)</f>
         <v>0</v>
       </c>
-      <c r="H4" s="41" t="s">
+      <c r="H4" s="40" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="44" t="s">
+      <c r="A5" s="43" t="s">
         <v>11</v>
       </c>
       <c r="B5" t="s">
         <v>68</v>
       </c>
-      <c r="D5" s="45">
+      <c r="D5" s="44">
         <f>D3*12/260</f>
         <v>969.23076923076928</v>
       </c>
-      <c r="E5" s="45">
+      <c r="E5" s="44">
         <f>E3*12/260</f>
         <v>461.53846153846155</v>
       </c>
-      <c r="F5" s="45">
+      <c r="F5" s="44">
         <f>F3*12/260</f>
         <v>1430.7692307692307</v>
       </c>
-      <c r="G5" s="45">
+      <c r="G5" s="44">
         <f>G3*12/260</f>
         <v>0</v>
       </c>
-      <c r="H5" s="41" t="s">
+      <c r="H5" s="40" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="44" t="s">
+      <c r="A6" s="43" t="s">
         <v>13</v>
       </c>
       <c r="B6" t="s">
@@ -3452,39 +3520,39 @@
       <c r="G6" s="10">
         <v>1</v>
       </c>
-      <c r="H6" s="41" t="s">
+      <c r="H6" s="40" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="44" t="s">
+      <c r="A7" s="43" t="s">
         <v>16</v>
       </c>
       <c r="B7" t="s">
         <v>72</v>
       </c>
-      <c r="D7" s="45">
+      <c r="D7" s="44">
         <f>D5*D6</f>
         <v>969.23076923076928</v>
       </c>
-      <c r="E7" s="45">
+      <c r="E7" s="44">
         <f>E5*E6</f>
         <v>461.53846153846155</v>
       </c>
-      <c r="F7" s="45">
+      <c r="F7" s="44">
         <f>F5*F6</f>
         <v>1430.7692307692307</v>
       </c>
-      <c r="G7" s="45">
+      <c r="G7" s="44">
         <f>G5*G6</f>
         <v>0</v>
       </c>
-      <c r="H7" s="41" t="s">
+      <c r="H7" s="40" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="44" t="s">
+      <c r="A8" s="43" t="s">
         <v>17</v>
       </c>
       <c r="B8" t="s">
@@ -3506,12 +3574,12 @@
         <f>MIN(G7,$C$15)</f>
         <v>0</v>
       </c>
-      <c r="H8" s="41" t="s">
+      <c r="H8" s="40" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="44" t="s">
+      <c r="A9" s="43" t="s">
         <v>18</v>
       </c>
       <c r="B9" t="s">
@@ -3529,39 +3597,39 @@
       <c r="G9" s="12">
         <v>1</v>
       </c>
-      <c r="H9" s="41" t="s">
+      <c r="H9" s="40" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="44" t="s">
+      <c r="A10" s="43" t="s">
         <v>20</v>
       </c>
       <c r="B10" t="s">
         <v>76</v>
       </c>
-      <c r="D10" s="45">
+      <c r="D10" s="44">
         <f>D7*D9</f>
         <v>484.61538461538464</v>
       </c>
-      <c r="E10" s="45">
+      <c r="E10" s="44">
         <f>E7*E9</f>
         <v>369.23076923076928</v>
       </c>
-      <c r="F10" s="45">
+      <c r="F10" s="44">
         <f>F7*F9</f>
         <v>286.15384615384613</v>
       </c>
-      <c r="G10" s="45">
+      <c r="G10" s="44">
         <f>G7*G9</f>
         <v>0</v>
       </c>
-      <c r="H10" s="41" t="s">
+      <c r="H10" s="40" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="44" t="s">
+      <c r="A11" s="43" t="s">
         <v>22</v>
       </c>
       <c r="B11" t="s">
@@ -3579,54 +3647,54 @@
       <c r="G11" s="10">
         <v>1</v>
       </c>
-      <c r="H11" s="41" t="s">
+      <c r="H11" s="40" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="44" t="s">
+      <c r="A12" s="43" t="s">
         <v>23</v>
       </c>
       <c r="B12" t="s">
         <v>78</v>
       </c>
-      <c r="D12" s="48">
+      <c r="D12" s="47">
         <f>D10*D11</f>
         <v>484.61538461538464</v>
       </c>
-      <c r="E12" s="48">
+      <c r="E12" s="47">
         <f>E10*E11</f>
         <v>332.30769230769238</v>
       </c>
-      <c r="F12" s="48">
+      <c r="F12" s="47">
         <f>F10*F11</f>
         <v>71.538461538461533</v>
       </c>
-      <c r="G12" s="48">
+      <c r="G12" s="47">
         <f>G10*G11</f>
         <v>0</v>
       </c>
-      <c r="H12" s="41" t="s">
+      <c r="H12" s="40" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="44" t="s">
+      <c r="A13" s="43" t="s">
         <v>24</v>
       </c>
       <c r="B13" t="s">
         <v>79</v>
       </c>
-      <c r="C13" s="64">
+      <c r="C13" s="63">
         <f>SUM(D10:G10)/SUM(D7:G7)</f>
         <v>0.39838709677419348</v>
       </c>
-      <c r="H13" s="41" t="s">
+      <c r="H13" s="40" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="44" t="s">
+      <c r="A14" s="43" t="s">
         <v>26</v>
       </c>
       <c r="B14" t="s">
@@ -3635,375 +3703,375 @@
       <c r="C14" s="7">
         <v>101351</v>
       </c>
-      <c r="H14" s="41" t="s">
+      <c r="H14" s="40" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="44" t="s">
+      <c r="A15" s="43" t="s">
         <v>28</v>
       </c>
       <c r="B15" t="s">
         <v>81</v>
       </c>
-      <c r="C15" s="65">
+      <c r="C15" s="64">
         <f>6*C14/260</f>
         <v>2338.8692307692309</v>
       </c>
-      <c r="H15" s="41" t="s">
+      <c r="H15" s="40" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="44" t="s">
+      <c r="A16" s="43" t="s">
         <v>29</v>
       </c>
       <c r="B16" t="s">
         <v>82</v>
       </c>
-      <c r="C16" s="65">
+      <c r="C16" s="64">
         <f>C13*C15</f>
         <v>931.77532258064502</v>
       </c>
-      <c r="H16" s="41" t="s">
+      <c r="H16" s="40" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="50" t="s">
+      <c r="A17" s="49" t="s">
         <v>83</v>
       </c>
-      <c r="B17" s="51" t="s">
+      <c r="B17" s="50" t="s">
         <v>84</v>
       </c>
-      <c r="C17" s="52">
+      <c r="C17" s="51">
         <f>MIN(1, C16/SUM(D10:G10))</f>
         <v>0.81734677419354829</v>
       </c>
-      <c r="D17" s="53"/>
-      <c r="E17" s="53"/>
-      <c r="F17" s="53"/>
-      <c r="G17" s="53"/>
-      <c r="H17" s="54" t="s">
+      <c r="D17" s="52"/>
+      <c r="E17" s="52"/>
+      <c r="F17" s="52"/>
+      <c r="G17" s="52"/>
+      <c r="H17" s="53" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="50" t="s">
+      <c r="A18" s="49" t="s">
         <v>85</v>
       </c>
-      <c r="B18" s="51" t="s">
+      <c r="B18" s="50" t="s">
         <v>86</v>
       </c>
-      <c r="C18" s="51"/>
-      <c r="D18" s="53">
+      <c r="C18" s="50"/>
+      <c r="D18" s="52">
         <f>D10*ScalingFactor</f>
         <v>367.28744939271257</v>
       </c>
-      <c r="E18" s="53">
+      <c r="E18" s="52">
         <f>E10*ScalingFactor</f>
         <v>279.83805668016197</v>
       </c>
-      <c r="F18" s="53">
+      <c r="F18" s="52">
         <f>F10*ScalingFactor</f>
         <v>216.87449392712549</v>
       </c>
-      <c r="G18" s="53">
+      <c r="G18" s="52">
         <f>G10*ScalingFactor</f>
         <v>0</v>
       </c>
-      <c r="H18" s="54" t="s">
+      <c r="H18" s="53" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="50" t="s">
+      <c r="A19" s="49" t="s">
         <v>87</v>
       </c>
-      <c r="B19" s="51" t="s">
+      <c r="B19" s="50" t="s">
         <v>88</v>
       </c>
-      <c r="C19" s="51"/>
-      <c r="D19" s="53">
+      <c r="C19" s="50"/>
+      <c r="D19" s="52">
         <f>MIN(D18,D12)</f>
         <v>367.28744939271257</v>
       </c>
-      <c r="E19" s="53">
+      <c r="E19" s="52">
         <f>MIN(E18,E12)</f>
         <v>279.83805668016197</v>
       </c>
-      <c r="F19" s="53">
+      <c r="F19" s="52">
         <f>MIN(F18,F12)</f>
         <v>71.538461538461533</v>
       </c>
-      <c r="G19" s="53">
+      <c r="G19" s="52">
         <f>MIN(G18,G12)</f>
         <v>0</v>
       </c>
-      <c r="H19" s="54" t="s">
+      <c r="H19" s="53" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="50"/>
-      <c r="B20" s="51" t="s">
+      <c r="A20" s="49"/>
+      <c r="B20" s="50" t="s">
         <v>89</v>
       </c>
-      <c r="C20" s="51"/>
-      <c r="D20" s="53">
+      <c r="C20" s="50"/>
+      <c r="D20" s="52">
         <f>D19-D12</f>
         <v>-117.32793522267207</v>
       </c>
-      <c r="E20" s="53">
+      <c r="E20" s="52">
         <f>E19-E12</f>
         <v>-52.469635627530408</v>
       </c>
-      <c r="F20" s="53">
+      <c r="F20" s="52">
         <f>F19-F12</f>
         <v>0</v>
       </c>
-      <c r="G20" s="53">
+      <c r="G20" s="52">
         <f>G19-G12</f>
         <v>0</v>
       </c>
-      <c r="H20" s="54" t="s">
+      <c r="H20" s="53" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="21" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="50"/>
-      <c r="B21" s="51" t="s">
+      <c r="A21" s="49"/>
+      <c r="B21" s="50" t="s">
         <v>90</v>
       </c>
-      <c r="C21" s="51"/>
-      <c r="D21" s="52">
+      <c r="C21" s="50"/>
+      <c r="D21" s="51">
         <f>IF(D20 &lt; 0, D4, 0)</f>
         <v>0.33870967741935482</v>
       </c>
-      <c r="E21" s="52">
+      <c r="E21" s="51">
         <f>IF(E20 &lt; 0, E4, 0)</f>
         <v>0.16129032258064516</v>
       </c>
-      <c r="F21" s="52">
+      <c r="F21" s="51">
         <f>IF(F20 &lt; 0, F4, 0)</f>
         <v>0</v>
       </c>
-      <c r="G21" s="53"/>
-      <c r="H21" s="54" t="s">
+      <c r="G21" s="52"/>
+      <c r="H21" s="53" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="50" t="s">
+      <c r="A22" s="49" t="s">
         <v>91</v>
       </c>
-      <c r="B22" s="51" t="s">
+      <c r="B22" s="50" t="s">
         <v>92</v>
       </c>
-      <c r="C22" s="51"/>
-      <c r="D22" s="52">
+      <c r="C22" s="50"/>
+      <c r="D22" s="51">
         <f>IF(SUM(ShortfallIncomeRatioArb)=0,0,D21/SUM(ShortfallIncomeRatioArb))</f>
         <v>0.67741935483870963</v>
       </c>
-      <c r="E22" s="52">
+      <c r="E22" s="51">
         <f>IF(SUM(ShortfallIncomeRatioArb)=0,0,E21/SUM(ShortfallIncomeRatioArb))</f>
         <v>0.32258064516129031</v>
       </c>
-      <c r="F22" s="52">
+      <c r="F22" s="51">
         <f>IF(SUM(ShortfallIncomeRatioArb)=0,0,F21/SUM(ShortfallIncomeRatioArb))</f>
         <v>0</v>
       </c>
-      <c r="G22" s="52">
+      <c r="G22" s="51">
         <f>IF(SUM(ShortfallIncomeRatioArb)=0,0,G21/SUM(ShortfallIncomeRatioArb))</f>
         <v>0</v>
       </c>
-      <c r="H22" s="54" t="s">
+      <c r="H22" s="53" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="50"/>
-      <c r="B23" s="51" t="s">
+      <c r="A23" s="49"/>
+      <c r="B23" s="50" t="s">
         <v>93</v>
       </c>
-      <c r="C23" s="51"/>
-      <c r="D23" s="53">
+      <c r="C23" s="50"/>
+      <c r="D23" s="52">
         <f>D18-D19</f>
         <v>0</v>
       </c>
-      <c r="E23" s="53">
+      <c r="E23" s="52">
         <f>E18-E19</f>
         <v>0</v>
       </c>
-      <c r="F23" s="53">
+      <c r="F23" s="52">
         <f>F18-F19</f>
         <v>145.33603238866397</v>
       </c>
-      <c r="G23" s="53">
+      <c r="G23" s="52">
         <f>G18-G19</f>
         <v>0</v>
       </c>
-      <c r="H23" s="54" t="s">
+      <c r="H23" s="53" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="50" t="s">
+      <c r="A24" s="49" t="s">
         <v>94</v>
       </c>
-      <c r="B24" s="51" t="s">
+      <c r="B24" s="50" t="s">
         <v>95</v>
       </c>
-      <c r="C24" s="51"/>
-      <c r="D24" s="53">
+      <c r="C24" s="50"/>
+      <c r="D24" s="52">
         <f>MIN(-D20,IF(SUM($D$20:$G$20)&gt;=0, 0, SUM($D$23:$G$23)*D22))</f>
         <v>98.453441295546554</v>
       </c>
-      <c r="E24" s="53">
+      <c r="E24" s="52">
         <f>MIN(-E20,IF(SUM($D$20:$G$20)&gt;=0, 0, SUM($D$23:$G$23)*E22))</f>
         <v>46.882591093117405</v>
       </c>
-      <c r="F24" s="53">
+      <c r="F24" s="52">
         <f>MIN(-F20,IF(SUM($D$20:$G$20)&gt;=0, 0, SUM($D$23:$G$23)*F22))</f>
         <v>0</v>
       </c>
-      <c r="G24" s="53">
+      <c r="G24" s="52">
         <f>MIN(-G20,IF(SUM($D$20:$G$20)&gt;=0, 0, SUM($D$23:$G$23)*G22))</f>
         <v>0</v>
       </c>
-      <c r="H24" s="54" t="s">
+      <c r="H24" s="53" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="25" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="50"/>
-      <c r="B25" s="51" t="s">
+      <c r="A25" s="49"/>
+      <c r="B25" s="50" t="s">
         <v>96</v>
       </c>
-      <c r="C25" s="51"/>
-      <c r="D25" s="52">
+      <c r="C25" s="50"/>
+      <c r="D25" s="51">
         <f>IF(D23 = 0, 0, D4)</f>
         <v>0</v>
       </c>
-      <c r="E25" s="52">
+      <c r="E25" s="51">
         <f>IF(E23 = 0, 0, E4)</f>
         <v>0</v>
       </c>
-      <c r="F25" s="52">
+      <c r="F25" s="51">
         <f>IF(F23 = 0, 0, F4)</f>
         <v>0.5</v>
       </c>
-      <c r="G25" s="52">
+      <c r="G25" s="51">
         <f>IF(G23 = 0, 0, G4)</f>
         <v>0</v>
       </c>
-      <c r="H25" s="54" t="s">
+      <c r="H25" s="53" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="26" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="50"/>
-      <c r="B26" s="51" t="s">
+      <c r="A26" s="49"/>
+      <c r="B26" s="50" t="s">
         <v>97</v>
       </c>
-      <c r="C26" s="51"/>
-      <c r="D26" s="52">
+      <c r="C26" s="50"/>
+      <c r="D26" s="51">
         <f>IF(SUM(ShortfallIncomeRatioPerson)= 0, 0, D25/SUM(ShortfallIncomeRatioPerson))</f>
         <v>0</v>
       </c>
-      <c r="E26" s="52">
+      <c r="E26" s="51">
         <f>IF(SUM(ShortfallIncomeRatioPerson)= 0, 0, E25/SUM(ShortfallIncomeRatioPerson))</f>
         <v>0</v>
       </c>
-      <c r="F26" s="52">
+      <c r="F26" s="51">
         <f>IF(SUM(ShortfallIncomeRatioPerson)= 0, 0, F25/SUM(ShortfallIncomeRatioPerson))</f>
         <v>1</v>
       </c>
-      <c r="G26" s="52">
+      <c r="G26" s="51">
         <f>IF(SUM(ShortfallIncomeRatioPerson)= 0, 0, G25/SUM(ShortfallIncomeRatioPerson))</f>
         <v>0</v>
       </c>
-      <c r="H26" s="54" t="s">
+      <c r="H26" s="53" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="50" t="s">
+      <c r="A27" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="B27" s="51" t="s">
+      <c r="B27" s="50" t="s">
         <v>98</v>
       </c>
-      <c r="C27" s="51"/>
-      <c r="D27" s="55">
+      <c r="C27" s="50"/>
+      <c r="D27" s="54">
         <f>ROUND(D19+D24,0)</f>
         <v>466</v>
       </c>
-      <c r="E27" s="55">
+      <c r="E27" s="54">
         <f>ROUND(E19+E24,0)</f>
         <v>327</v>
       </c>
-      <c r="F27" s="55">
+      <c r="F27" s="54">
         <f>ROUND(F19+F24,0)</f>
         <v>72</v>
       </c>
-      <c r="G27" s="53">
+      <c r="G27" s="52">
         <f>ROUND(G19+G24,0)</f>
         <v>0</v>
       </c>
-      <c r="H27" s="54" t="s">
+      <c r="H27" s="53" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="28" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="50" t="s">
+      <c r="A28" s="49" t="s">
         <v>54</v>
       </c>
-      <c r="B28" s="51" t="s">
+      <c r="B28" s="50" t="s">
         <v>99</v>
       </c>
-      <c r="C28" s="51"/>
-      <c r="D28" s="51">
+      <c r="C28" s="50"/>
+      <c r="D28" s="50">
         <f>ROUND(D23-SUM(AdjustmentArb)*D26,0)</f>
         <v>0</v>
       </c>
-      <c r="E28" s="51">
+      <c r="E28" s="50">
         <f>ROUND(E23-SUM(AdjustmentArb)*E26,0)</f>
         <v>0</v>
       </c>
-      <c r="F28" s="51">
+      <c r="F28" s="50">
         <f>ROUND(F23-SUM(AdjustmentArb)*F26,0)</f>
         <v>0</v>
       </c>
-      <c r="G28" s="51">
+      <c r="G28" s="50">
         <f>ROUND(G23-SUM(AdjustmentArb)*G26,0)</f>
         <v>0</v>
       </c>
-      <c r="H28" s="54" t="s">
+      <c r="H28" s="53" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="29" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="50"/>
-      <c r="B29" s="51" t="s">
+      <c r="A29" s="49"/>
+      <c r="B29" s="50" t="s">
         <v>100</v>
       </c>
-      <c r="C29" s="56">
+      <c r="C29" s="55">
         <f>C16-SUM(D27:G28)</f>
         <v>66.775322580645025</v>
       </c>
-      <c r="D29" s="51"/>
-      <c r="E29" s="51"/>
-      <c r="F29" s="51"/>
-      <c r="G29" s="51"/>
-      <c r="H29" s="54" t="s">
+      <c r="D29" s="50"/>
+      <c r="E29" s="50"/>
+      <c r="F29" s="50"/>
+      <c r="G29" s="50"/>
+      <c r="H29" s="53" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A30" s="44"/>
+      <c r="A30" s="43"/>
       <c r="C30" s="39"/>
-      <c r="H30" s="41"/>
+      <c r="H30" s="40"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
@@ -4013,15 +4081,15 @@
         <v>76</v>
       </c>
       <c r="C31" s="15"/>
-      <c r="D31" s="66">
+      <c r="D31" s="65">
         <f>D10</f>
         <v>484.61538461538464</v>
       </c>
-      <c r="E31" s="66">
+      <c r="E31" s="65">
         <f>E10</f>
         <v>369.23076923076928</v>
       </c>
-      <c r="F31" s="66">
+      <c r="F31" s="65">
         <f>F10</f>
         <v>286.15384615384613</v>
       </c>
@@ -4041,15 +4109,15 @@
         <v>101</v>
       </c>
       <c r="C32" s="15"/>
-      <c r="D32" s="66">
+      <c r="D32" s="65">
         <f>D12</f>
         <v>484.61538461538464</v>
       </c>
-      <c r="E32" s="66">
+      <c r="E32" s="65">
         <f>E12</f>
         <v>332.30769230769238</v>
       </c>
-      <c r="F32" s="66">
+      <c r="F32" s="65">
         <f>F12</f>
         <v>71.538461538461533</v>
       </c>
@@ -4069,15 +4137,15 @@
         <v>102</v>
       </c>
       <c r="C33" s="15"/>
-      <c r="D33" s="66">
+      <c r="D33" s="65">
         <f>D31-D32</f>
         <v>0</v>
       </c>
-      <c r="E33" s="66">
+      <c r="E33" s="65">
         <f>E31-E32</f>
         <v>36.923076923076906</v>
       </c>
-      <c r="F33" s="66">
+      <c r="F33" s="65">
         <f>F31-F32</f>
         <v>214.61538461538458</v>
       </c>
@@ -4091,17 +4159,17 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="1"/>
-      <c r="B34" s="57" t="s">
+      <c r="B34" s="56" t="s">
         <v>103</v>
       </c>
-      <c r="C34" s="88" t="str">
+      <c r="C34" s="90" t="str">
         <f>IF(SUM(D32:G33)&lt;=MAKSBELOP,"Everyone paid",IF(SUM(D32:G32)&lt;=MAKSBELOP,"Arbeidsgivere fully paid; Person partially paid by Person request", "Arbeidsgivere partial payment ratio by Arbeidsgiver request"))</f>
         <v>Arbeidsgivere partial payment ratio by Arbeidsgiver request</v>
       </c>
-      <c r="D34" s="88"/>
-      <c r="E34" s="88"/>
-      <c r="F34" s="88"/>
-      <c r="G34" s="88"/>
+      <c r="D34" s="90"/>
+      <c r="E34" s="90"/>
+      <c r="F34" s="90"/>
+      <c r="G34" s="90"/>
       <c r="H34" s="17"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
@@ -4137,7 +4205,7 @@
       <c r="B36" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="C36" s="67">
+      <c r="C36" s="66">
         <f>MAKSBELOP2-SUM(D35:G35)</f>
         <v>42.775322580645025</v>
       </c>
@@ -4180,7 +4248,7 @@
       <c r="B38" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="C38" s="67">
+      <c r="C38" s="66">
         <f>MAKSBELOP2-SUM(D35:G37)</f>
         <v>0.77532258064502457</v>
       </c>

</xml_diff>

<commit_message>
runder av refusjon og dekningsgrunnlag
det er avklart juridisk at vi følger samme avrundningsregler for dekningsgrunnlaget og refusjon
som vi gjør med sykepengegrunnlaget.

Dette gjør vi for å unngå 1 kr-differanser mellom sykepengegrunnlaget
og totalt refusjonsbeløp, sånn at vi ikke lager personutbetalinger pga. avrundningsdifferanser.
</commit_message>
<xml_diff>
--- a/doc/okonomi/Utbetaling.xlsx
+++ b/doc/okonomi/Utbetaling.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/david/dev/nav/helse-spleis/doc/okonomi/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EEC8836-80EF-134A-A235-35642D87C5EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63F84AC2-5FB4-E44B-AD80-B779A52633AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="47620" windowHeight="41000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="151">
   <si>
     <t xml:space="preserve">Begrep	</t>
   </si>
@@ -111,9 +111,6 @@
   </si>
   <si>
     <t>Gradert dekningsgrunnlag</t>
-  </si>
-  <si>
-    <t>Maks dagsats redusert for arbeidsuførhetsgrad</t>
   </si>
   <si>
     <t>Refusjonsgrad</t>
@@ -460,9 +457,6 @@
     <t>Den totale mengden refusjon arbeidsgiverne ønsker, per dag</t>
   </si>
   <si>
-    <t>Maks dagsats før reduksjon til 6G og reduksjon for total sykdomsgrad</t>
-  </si>
-  <si>
     <t>Totalt dekningsgrunnlag for alle arbeidsgiverne</t>
   </si>
   <si>
@@ -505,20 +499,35 @@
     <t>Gradert refusjon</t>
   </si>
   <si>
-    <t>Maks refusjon før redusering for dekningsgrunnlag</t>
-  </si>
-  <si>
     <t>Totalt refusjon</t>
   </si>
   <si>
     <t>Det som skal betales per dag, totalt</t>
+  </si>
+  <si>
+    <t>Maks dagsats før reduksjon til 6G og reduksjon for total sykdomsgrad. Rundet av på dagsats etter gradering</t>
+  </si>
+  <si>
+    <t>Maks dagsats redusert for arbeidsuførhetsgrad. Rundet av på dagsats etter gradering</t>
+  </si>
+  <si>
+    <t>Maks refusjon før redusering for dekningsgrunnlag. Rundet av på dagsats før og etter gradering</t>
+  </si>
+  <si>
+    <t>Vektet refusjonssgrad</t>
+  </si>
+  <si>
+    <t>Hvor stor andel av total refusjon hver arbeidsgiver vil ha</t>
+  </si>
+  <si>
+    <t>Rest til utbetaling før avrunding</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="14">
+  <numFmts count="16">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* \-??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* \-??_);_(@_)"/>
@@ -532,7 +541,9 @@
     <numFmt numFmtId="173" formatCode="_-* #,##0.000000_-;\-* #,##0.000000_-;_-* &quot;-&quot;??????_-;_-@_-"/>
     <numFmt numFmtId="174" formatCode="_-* #,##0.0000000000_-;\-* #,##0.0000000000_-;_-* &quot;-&quot;??????????_-;_-@_-"/>
     <numFmt numFmtId="175" formatCode="_-* #,##0.00000000_-;\-* #,##0.00000000_-;_-* &quot;-&quot;??????????_-;_-@_-"/>
-    <numFmt numFmtId="184" formatCode="_-* #,##0.000000000_-;\-* #,##0.000000000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-* #,##0.000000000_-;\-* #,##0.000000000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="182" formatCode="_(* #,##0.00000_);_(* \(#,##0.00000\);_(* \-??_);_(@_)"/>
+    <numFmt numFmtId="190" formatCode="0.0"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -703,7 +714,7 @@
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -833,13 +844,23 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="184" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="190" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1224,10 +1245,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H62"/>
+  <dimension ref="A1:H63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1326,7 +1347,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C5" s="39">
         <f>C3*12</f>
@@ -1348,17 +1369,17 @@
         <v>8</v>
       </c>
       <c r="H5" s="69" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="13">
-        <f>C3*0.5</f>
-        <v>22500</v>
+        <f>C3*1</f>
+        <v>45000</v>
       </c>
       <c r="D6" s="13">
         <f>D3</f>
@@ -1376,16 +1397,16 @@
         <v>8</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="68" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B7" s="72">
         <f>SUM(C6:F6)*12</f>
-        <v>576000</v>
+        <v>846000</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -1403,7 +1424,7 @@
         <v>0</v>
       </c>
       <c r="F8" s="12">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="G8" s="5" t="s">
         <v>8</v>
@@ -1414,7 +1435,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="68" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B9" s="71">
         <f>SUM(C5:F5)</f>
@@ -1424,12 +1445,12 @@
         <v>8</v>
       </c>
       <c r="H9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B10" s="7">
         <v>93634</v>
@@ -1438,12 +1459,12 @@
         <v>14</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="68" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B11" s="39">
         <f>B10*6</f>
@@ -1453,12 +1474,12 @@
         <v>14</v>
       </c>
       <c r="H11" s="75" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B12" s="9">
         <f>ROUND(B11/260,)</f>
@@ -1468,12 +1489,12 @@
         <v>14</v>
       </c>
       <c r="H12" s="75" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="68" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B13" s="39">
         <f>ROUND(MIN(B9,B11)/260,)*260</f>
@@ -1483,12 +1504,12 @@
         <v>14</v>
       </c>
       <c r="H13" s="75" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="68" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B14" s="67">
         <f>B13/260</f>
@@ -1498,7 +1519,7 @@
         <v>14</v>
       </c>
       <c r="H14" s="75" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
@@ -1558,32 +1579,32 @@
         <v>16</v>
       </c>
       <c r="B18" s="4"/>
-      <c r="C18" s="9">
-        <f>C16*C17</f>
-        <v>2076.9230769230771</v>
-      </c>
-      <c r="D18" s="9">
-        <f>D16*D17</f>
-        <v>230.76923076923077</v>
-      </c>
-      <c r="E18" s="9">
-        <f>E16*E17</f>
-        <v>461.53846153846155</v>
-      </c>
-      <c r="F18" s="9">
-        <f>F16*F17</f>
-        <v>1615.3846153846155</v>
+      <c r="C18" s="99">
+        <f>ROUND(C16*C17,0)</f>
+        <v>2077</v>
+      </c>
+      <c r="D18" s="99">
+        <f t="shared" ref="D18:F18" si="1">ROUND(D16*D17,0)</f>
+        <v>231</v>
+      </c>
+      <c r="E18" s="99">
+        <f t="shared" si="1"/>
+        <v>462</v>
+      </c>
+      <c r="F18" s="99">
+        <f t="shared" si="1"/>
+        <v>1615</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>130</v>
+        <v>145</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="73" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C19" s="74">
         <f>C8*C4</f>
@@ -1599,13 +1620,13 @@
       </c>
       <c r="F19" s="74">
         <f>F8*F4</f>
-        <v>0.36842105263157893</v>
+        <v>0.29473684210526313</v>
       </c>
       <c r="G19" s="70" t="s">
         <v>8</v>
       </c>
       <c r="H19" s="75" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
@@ -1613,166 +1634,174 @@
         <v>20</v>
       </c>
       <c r="B20" s="4"/>
-      <c r="C20" s="9">
-        <f>C18*C8</f>
-        <v>1038.4615384615386</v>
-      </c>
-      <c r="D20" s="9">
-        <f>D18*D8</f>
-        <v>230.76923076923077</v>
-      </c>
-      <c r="E20" s="9">
-        <f>E18*E8</f>
-        <v>0</v>
-      </c>
-      <c r="F20" s="9">
-        <f>F18*F8</f>
-        <v>1615.3846153846155</v>
+      <c r="C20" s="99">
+        <f>ROUND(C18*C8,0)</f>
+        <v>1039</v>
+      </c>
+      <c r="D20" s="99">
+        <f t="shared" ref="D20:F20" si="2">ROUND(D18*D8,0)</f>
+        <v>231</v>
+      </c>
+      <c r="E20" s="99">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F20" s="99">
+        <f t="shared" si="2"/>
+        <v>1292</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>21</v>
+        <v>146</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="73" t="s">
-        <v>144</v>
-      </c>
-      <c r="C21" s="67">
-        <f>C6*C8*12/260</f>
-        <v>519.23076923076928</v>
-      </c>
-      <c r="D21" s="67">
-        <f t="shared" ref="D21:F21" si="1">D6*D8*12/260</f>
-        <v>230.76923076923077</v>
-      </c>
-      <c r="E21" s="67">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F21" s="67">
-        <f t="shared" si="1"/>
-        <v>484.61538461538464</v>
+        <v>142</v>
+      </c>
+      <c r="C21" s="100">
+        <f>ROUND(ROUND(C6*12/260,0)*C8,0)</f>
+        <v>1039</v>
+      </c>
+      <c r="D21" s="100">
+        <f t="shared" ref="D21:F21" si="3">ROUND(ROUND(D6*12/260,0)*D8,0)</f>
+        <v>231</v>
+      </c>
+      <c r="E21" s="100">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F21" s="100">
+        <f t="shared" si="3"/>
+        <v>388</v>
       </c>
       <c r="G21" s="70" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="H21" s="75" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="73" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B22" s="72">
         <f>SUM(C20:F20)</f>
-        <v>2884.6153846153848</v>
+        <v>2562</v>
       </c>
       <c r="G22" s="70" t="s">
         <v>8</v>
       </c>
       <c r="H22" s="75" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="73" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B23" s="72">
         <f>B22*260</f>
-        <v>750000</v>
+        <v>666120</v>
       </c>
       <c r="G23" s="70" t="s">
         <v>8</v>
       </c>
       <c r="H23" s="75" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="73" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B24" s="72">
         <f>SUM(C21:F21)</f>
-        <v>1234.6153846153848</v>
+        <v>1658</v>
       </c>
       <c r="C24" s="67"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="73" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B25" s="72">
         <f>B24*260</f>
-        <v>321000.00000000006</v>
+        <v>431080</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B26" s="4"/>
-      <c r="C26" s="13">
-        <f>MIN(C20,C6*C8*12/260)</f>
-        <v>519.23076923076928</v>
-      </c>
-      <c r="D26" s="13">
-        <f>MIN(D20,D6*D8*12/260)</f>
-        <v>230.76923076923077</v>
-      </c>
-      <c r="E26" s="13">
-        <f>MIN(E20,E6*E8*12/260)</f>
-        <v>0</v>
-      </c>
-      <c r="F26" s="13">
-        <f>MIN(F20,F6*F8*12/260)</f>
-        <v>484.61538461538464</v>
+      <c r="C26" s="101">
+        <f>MIN(C20,C21)</f>
+        <v>1039</v>
+      </c>
+      <c r="D26" s="101">
+        <f t="shared" ref="D26:F26" si="4">MIN(D20,D21)</f>
+        <v>231</v>
+      </c>
+      <c r="E26" s="101">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F26" s="101">
+        <f t="shared" si="4"/>
+        <v>388</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="73" t="s">
-        <v>124</v>
-      </c>
-      <c r="B27" s="67">
-        <f>SUM(C26:F26)</f>
-        <v>1234.6153846153848</v>
-      </c>
-      <c r="C27" s="93"/>
-      <c r="D27" s="93"/>
-      <c r="E27" s="93"/>
-      <c r="F27" s="93"/>
+        <v>148</v>
+      </c>
+      <c r="C27" s="97">
+        <f>C26/$B$24</f>
+        <v>0.62665862484921597</v>
+      </c>
+      <c r="D27" s="97">
+        <f t="shared" ref="D27:F27" si="5">D26/$B$24</f>
+        <v>0.13932448733413752</v>
+      </c>
+      <c r="E27" s="97">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="F27" s="97">
+        <f t="shared" si="5"/>
+        <v>0.23401688781664656</v>
+      </c>
       <c r="G27" s="70" t="s">
         <v>8</v>
       </c>
       <c r="H27" s="75" t="s">
-        <v>129</v>
+        <v>149</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="73" t="s">
-        <v>127</v>
-      </c>
-      <c r="B28" s="72">
-        <f>B27*260</f>
-        <v>321000.00000000006</v>
-      </c>
-      <c r="C28" s="67"/>
-      <c r="D28" s="67"/>
-      <c r="E28" s="67"/>
-      <c r="F28" s="67"/>
+        <v>123</v>
+      </c>
+      <c r="B28" s="98">
+        <f>SUM(C26:F26)</f>
+        <v>1658</v>
+      </c>
+      <c r="C28" s="91"/>
+      <c r="D28" s="91"/>
+      <c r="E28" s="91"/>
+      <c r="F28" s="91"/>
       <c r="G28" s="70" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="H28" s="75" t="s">
         <v>128</v>
@@ -1780,303 +1809,303 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="73" t="s">
-        <v>134</v>
-      </c>
-      <c r="B29" s="67">
-        <f>B22-B27</f>
-        <v>1650</v>
-      </c>
-      <c r="D29" s="83"/>
-      <c r="E29" s="84"/>
+        <v>126</v>
+      </c>
+      <c r="B29" s="72">
+        <f>B28*260</f>
+        <v>431080</v>
+      </c>
+      <c r="C29" s="67"/>
+      <c r="D29" s="67"/>
+      <c r="E29" s="67"/>
+      <c r="F29" s="67"/>
       <c r="G29" s="70" t="s">
         <v>8</v>
       </c>
       <c r="H29" s="75" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="73" t="s">
-        <v>127</v>
-      </c>
-      <c r="B30" s="72">
-        <f>B29*260</f>
-        <v>429000</v>
-      </c>
-      <c r="C30" s="67"/>
-      <c r="D30" s="78"/>
+        <v>132</v>
+      </c>
+      <c r="B30" s="67">
+        <f>B22-B28</f>
+        <v>904</v>
+      </c>
+      <c r="D30" s="83"/>
       <c r="E30" s="84"/>
       <c r="G30" s="70" t="s">
         <v>8</v>
       </c>
       <c r="H30" s="75" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A31" s="3" t="s">
+      <c r="A31" s="73" t="s">
+        <v>126</v>
+      </c>
+      <c r="B31" s="72">
+        <f>B30*260</f>
+        <v>235040</v>
+      </c>
+      <c r="C31" s="67"/>
+      <c r="D31" s="78"/>
+      <c r="E31" s="84"/>
+      <c r="G31" s="70" t="s">
+        <v>8</v>
+      </c>
+      <c r="H31" s="75" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B32" s="14">
+        <f>SUM(C19:F19)</f>
+        <v>0.58421052631578951</v>
+      </c>
+      <c r="C32" s="89"/>
+      <c r="D32" s="90"/>
+      <c r="E32" s="90"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H32" s="6" t="s">
         <v>24</v>
-      </c>
-      <c r="B31" s="14">
-        <f>SUM(C19:F19)</f>
-        <v>0.65789473684210531</v>
-      </c>
-      <c r="C31" s="89"/>
-      <c r="D31" s="90"/>
-      <c r="E31" s="90"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="H31" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A32" s="73" t="s">
-        <v>118</v>
-      </c>
-      <c r="B32" s="76">
-        <f>ROUND(B13*B31/260,)*260</f>
-        <v>369720</v>
-      </c>
-      <c r="C32" s="87"/>
-      <c r="D32" s="83"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
-      <c r="G32" s="70" t="s">
-        <v>14</v>
-      </c>
-      <c r="H32" s="75" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="73" t="s">
-        <v>113</v>
-      </c>
-      <c r="B33" s="83">
-        <f>B32/260</f>
-        <v>1422</v>
-      </c>
-      <c r="C33" s="83"/>
-      <c r="D33" s="88"/>
+        <v>117</v>
+      </c>
+      <c r="B33" s="76">
+        <f>ROUND(B13*B32/260,)*260</f>
+        <v>328120</v>
+      </c>
+      <c r="C33" s="87"/>
+      <c r="D33" s="83"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
       <c r="G33" s="70" t="s">
         <v>14</v>
       </c>
       <c r="H33" s="75" t="s">
-        <v>147</v>
+        <v>122</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="73" t="s">
+        <v>112</v>
+      </c>
+      <c r="B34" s="83">
+        <f>B33/260</f>
+        <v>1262</v>
+      </c>
+      <c r="C34" s="83"/>
+      <c r="D34" s="88"/>
+      <c r="G34" s="70" t="s">
+        <v>14</v>
+      </c>
+      <c r="H34" s="75" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" s="73" t="s">
+        <v>124</v>
+      </c>
+      <c r="B35" s="83">
+        <f>B33/MAX(B33,B29)</f>
+        <v>0.76115802171290714</v>
+      </c>
+      <c r="D35" s="83"/>
+      <c r="G35" s="70" t="s">
+        <v>8</v>
+      </c>
+      <c r="H35" s="75" t="s">
         <v>125</v>
-      </c>
-      <c r="B34" s="83">
-        <f>B32/MAX(B32,B28)</f>
-        <v>1</v>
-      </c>
-      <c r="D34" s="83"/>
-      <c r="G34" s="70" t="s">
-        <v>8</v>
-      </c>
-      <c r="H34" s="75" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B35" s="15"/>
-      <c r="C35" s="16">
-        <f>C20</f>
-        <v>1038.4615384615386</v>
-      </c>
-      <c r="D35" s="16">
-        <f>D20</f>
-        <v>230.76923076923077</v>
-      </c>
-      <c r="E35" s="16">
-        <f>E20</f>
-        <v>0</v>
-      </c>
-      <c r="F35" s="16">
-        <f>F20</f>
-        <v>1615.3846153846155</v>
-      </c>
-      <c r="G35" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="H35" s="24" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="B36" s="15"/>
       <c r="C36" s="16">
-        <f>C26</f>
-        <v>519.23076923076928</v>
+        <f>C20</f>
+        <v>1039</v>
       </c>
       <c r="D36" s="16">
-        <f>D26</f>
-        <v>230.76923076923077</v>
+        <f>D20</f>
+        <v>231</v>
       </c>
       <c r="E36" s="16">
-        <f>E26</f>
+        <f>E20</f>
         <v>0</v>
       </c>
       <c r="F36" s="16">
-        <f>F26</f>
-        <v>484.61538461538464</v>
+        <f>F20</f>
+        <v>1292</v>
       </c>
       <c r="G36" s="17" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="H36" s="24" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B37" s="15"/>
       <c r="C37" s="16">
-        <f>C35-C36</f>
-        <v>519.23076923076928</v>
+        <f>C26</f>
+        <v>1039</v>
       </c>
       <c r="D37" s="16">
-        <f>D35-D36</f>
-        <v>0</v>
+        <f>D26</f>
+        <v>231</v>
       </c>
       <c r="E37" s="16">
-        <f>E35-E36</f>
+        <f>E26</f>
         <v>0</v>
       </c>
       <c r="F37" s="16">
-        <f>F35-F36</f>
-        <v>1130.7692307692309</v>
+        <f>F26</f>
+        <v>388</v>
       </c>
       <c r="G37" s="17" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="H37" s="24" t="s">
-        <v>138</v>
+        <v>31</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B38" s="19" t="str">
-        <f>IF(B30&lt;=B32,"Arbeidsgiver og person blir refundert hele beløpet",IF(B28&lt;=B32,"Arbeidsgivere blir refundert hele beløpet; Person blir delvis refundert", "Arbeidsgivere blir delvis refundert"))</f>
-        <v>Arbeidsgivere blir refundert hele beløpet; Person blir delvis refundert</v>
-      </c>
-      <c r="C38" s="19"/>
-      <c r="D38" s="19"/>
-      <c r="E38" s="19"/>
-      <c r="F38" s="19"/>
-      <c r="G38" s="17"/>
-      <c r="H38" s="24"/>
+        <v>32</v>
+      </c>
+      <c r="B38" s="15"/>
+      <c r="C38" s="16">
+        <f>C36-C37</f>
+        <v>0</v>
+      </c>
+      <c r="D38" s="16">
+        <f>D36-D37</f>
+        <v>0</v>
+      </c>
+      <c r="E38" s="16">
+        <f>E36-E37</f>
+        <v>0</v>
+      </c>
+      <c r="F38" s="16">
+        <f>F36-F37</f>
+        <v>904</v>
+      </c>
+      <c r="G38" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="H38" s="24" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A39" s="1"/>
-      <c r="B39" s="20"/>
-      <c r="C39" s="77"/>
-      <c r="D39" s="21"/>
-      <c r="E39" s="21"/>
-      <c r="F39" s="22"/>
+      <c r="A39" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B39" s="19" t="str">
+        <f>IF(B31&lt;=B33,"Arbeidsgiver og person blir refundert hele beløpet",IF(B29&lt;=B33,"Arbeidsgivere blir refundert hele beløpet; Person blir delvis refundert", "Arbeidsgivere blir delvis refundert"))</f>
+        <v>Arbeidsgiver og person blir refundert hele beløpet</v>
+      </c>
+      <c r="C39" s="19"/>
+      <c r="D39" s="19"/>
+      <c r="E39" s="19"/>
+      <c r="F39" s="19"/>
       <c r="G39" s="17"/>
       <c r="H39" s="24"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A40" s="1" t="s">
-        <v>35</v>
-      </c>
+      <c r="A40" s="1"/>
       <c r="B40" s="20"/>
-      <c r="C40" s="23">
-        <f>C36*$B$34</f>
-        <v>519.23076923076928</v>
-      </c>
-      <c r="D40" s="23">
-        <f>D36*$B$34</f>
-        <v>230.76923076923077</v>
-      </c>
-      <c r="E40" s="23">
-        <f>E36*$B$34</f>
-        <v>0</v>
-      </c>
-      <c r="F40" s="23">
-        <f>F36*$B$34</f>
-        <v>484.61538461538464</v>
-      </c>
-      <c r="G40" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="H40" s="24" t="s">
-        <v>35</v>
-      </c>
+      <c r="C40" s="77"/>
+      <c r="D40" s="21"/>
+      <c r="E40" s="21"/>
+      <c r="F40" s="22"/>
+      <c r="G40" s="17"/>
+      <c r="H40" s="24"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B41" s="15"/>
-      <c r="C41" s="24">
-        <f>FLOOR(C40,1)</f>
-        <v>519</v>
-      </c>
-      <c r="D41" s="24">
-        <f>FLOOR(D40,1)</f>
-        <v>230</v>
-      </c>
-      <c r="E41" s="24">
-        <f>FLOOR(E40,1)</f>
-        <v>0</v>
-      </c>
-      <c r="F41" s="24">
-        <f>FLOOR(F40,1)</f>
-        <v>484</v>
+        <v>34</v>
+      </c>
+      <c r="B41" s="20"/>
+      <c r="C41" s="23">
+        <f>C37*$B$35</f>
+        <v>790.84318455971049</v>
+      </c>
+      <c r="D41" s="23">
+        <f>D37*$B$35</f>
+        <v>175.82750301568154</v>
+      </c>
+      <c r="E41" s="23">
+        <f>E37*$B$35</f>
+        <v>0</v>
+      </c>
+      <c r="F41" s="23">
+        <f>F37*$B$35</f>
+        <v>295.32931242460796</v>
       </c>
       <c r="G41" s="17" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="H41" s="24" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="B42" s="15">
-        <f>SUM(C41:F41)</f>
-        <v>1233</v>
-      </c>
-      <c r="C42" s="25"/>
-      <c r="D42" s="24"/>
-      <c r="E42" s="24"/>
-      <c r="F42" s="24"/>
+        <v>35</v>
+      </c>
+      <c r="B42" s="15"/>
+      <c r="C42" s="24">
+        <f>FLOOR(C41,1)</f>
+        <v>790</v>
+      </c>
+      <c r="D42" s="24">
+        <f>FLOOR(D41,1)</f>
+        <v>175</v>
+      </c>
+      <c r="E42" s="24">
+        <f>FLOOR(E41,1)</f>
+        <v>0</v>
+      </c>
+      <c r="F42" s="24">
+        <f>FLOOR(F41,1)</f>
+        <v>295</v>
+      </c>
       <c r="G42" s="17" t="s">
         <v>14</v>
       </c>
       <c r="H42" s="24" t="s">
-        <v>140</v>
+        <v>36</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B43" s="30">
-        <f>ROUND(SUM(C40:F40)-B42,)</f>
-        <v>2</v>
-      </c>
-      <c r="C43" s="24"/>
+        <v>137</v>
+      </c>
+      <c r="B43" s="15">
+        <f>SUM(C42:F42)</f>
+        <v>1260</v>
+      </c>
+      <c r="C43" s="25"/>
       <c r="D43" s="24"/>
       <c r="E43" s="24"/>
       <c r="F43" s="24"/>
@@ -2084,37 +2113,37 @@
         <v>14</v>
       </c>
       <c r="H43" s="24" t="s">
-        <v>44</v>
+        <v>138</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B44" s="15">
-        <f>B42+B43</f>
-        <v>1235</v>
-      </c>
-      <c r="C44" s="25"/>
-      <c r="D44" s="24"/>
-      <c r="E44" s="24"/>
-      <c r="F44" s="24"/>
-      <c r="G44" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="H44" s="24" t="s">
-        <v>141</v>
+        <v>150</v>
+      </c>
+      <c r="B44" s="96">
+        <f>SUM(C41:F41)-B43</f>
+        <v>2</v>
+      </c>
+      <c r="C44" s="94"/>
+      <c r="D44" s="94"/>
+      <c r="E44" s="94"/>
+      <c r="F44" s="94"/>
+      <c r="G44" s="95" t="s">
+        <v>8</v>
+      </c>
+      <c r="H44" s="94" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="B45" s="15">
-        <f>B44*260</f>
-        <v>321100</v>
-      </c>
-      <c r="C45" s="25"/>
+        <v>42</v>
+      </c>
+      <c r="B45" s="30">
+        <f>ROUND(B44,)</f>
+        <v>2</v>
+      </c>
+      <c r="C45" s="24"/>
       <c r="D45" s="24"/>
       <c r="E45" s="24"/>
       <c r="F45" s="24"/>
@@ -2122,335 +2151,373 @@
         <v>14</v>
       </c>
       <c r="H45" s="24" t="s">
-        <v>142</v>
+        <v>43</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B46" s="15"/>
-      <c r="C46" s="23">
-        <f>C40-TRUNC(C40)</f>
-        <v>0.23076923076928324</v>
-      </c>
-      <c r="D46" s="23">
-        <f>D40-TRUNC(D40)</f>
-        <v>0.7692307692307736</v>
-      </c>
-      <c r="E46" s="23">
-        <f>E40-TRUNC(E40)</f>
-        <v>0</v>
-      </c>
-      <c r="F46" s="23">
-        <f>F40-TRUNC(F40)</f>
-        <v>0.61538461538464162</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="B46" s="15">
+        <f>B43+B45</f>
+        <v>1262</v>
+      </c>
+      <c r="C46" s="25"/>
+      <c r="D46" s="24"/>
+      <c r="E46" s="24"/>
+      <c r="F46" s="24"/>
       <c r="G46" s="17" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="H46" s="24" t="s">
-        <v>39</v>
+        <v>139</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B47" s="15"/>
-      <c r="C47" s="25">
-        <f>IF($B$43&gt;0,IF(LARGE($C$46:$F$46,$B$43)&lt;=C$46,1,0), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="D47" s="25">
-        <f>IF($B$43&gt;0,IF(LARGE($C$46:$F$46,$B$43)&lt;=D$46,1,0), 0)</f>
-        <v>1</v>
-      </c>
-      <c r="E47" s="25">
-        <f>IF($B$43&gt;0,IF(LARGE($C$46:$F$46,$B$43)&lt;=E$46,1,0), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="F47" s="25">
-        <f>IF($B$43&gt;0,IF(LARGE($C$46:$F$46,$B$43)&lt;=F$46,1,0), 0)</f>
-        <v>1</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="B47" s="15">
+        <f>B46*260</f>
+        <v>328120</v>
+      </c>
+      <c r="C47" s="25"/>
+      <c r="D47" s="24"/>
+      <c r="E47" s="24"/>
+      <c r="F47" s="24"/>
       <c r="G47" s="17" t="s">
         <v>14</v>
       </c>
       <c r="H47" s="24" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B48" s="15"/>
+      <c r="C48" s="23">
+        <f>C41-TRUNC(C41)</f>
+        <v>0.84318455971049389</v>
+      </c>
+      <c r="D48" s="23">
+        <f>D41-TRUNC(D41)</f>
+        <v>0.82750301568154327</v>
+      </c>
+      <c r="E48" s="23">
+        <f>E41-TRUNC(E41)</f>
+        <v>0</v>
+      </c>
+      <c r="F48" s="23">
+        <f>F41-TRUNC(F41)</f>
+        <v>0.32931242460796284</v>
+      </c>
+      <c r="G48" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="H48" s="24" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B49" s="15"/>
+      <c r="C49" s="25">
+        <f>IF($B$45&gt;0,IF(LARGE($C$48:$F$48,$B$45)&lt;=C$48,1,0), 0)</f>
+        <v>1</v>
+      </c>
+      <c r="D49" s="25">
+        <f>IF($B$45&gt;0,IF(LARGE($C$48:$F$48,$B$45)&lt;=D$48,1,0), 0)</f>
+        <v>1</v>
+      </c>
+      <c r="E49" s="25">
+        <f>IF($B$45&gt;0,IF(LARGE($C$48:$F$48,$B$45)&lt;=E$48,1,0), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="F49" s="25">
+        <f>IF($B$45&gt;0,IF(LARGE($C$48:$F$48,$B$45)&lt;=F$48,1,0), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="G49" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="H49" s="24" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A50" s="26" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A48" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="B48" s="27"/>
-      <c r="C48" s="28">
-        <f>C41+C47</f>
-        <v>519</v>
-      </c>
-      <c r="D48" s="28">
-        <f>D41+D47</f>
-        <v>231</v>
-      </c>
-      <c r="E48" s="28">
-        <f>E41+E47</f>
-        <v>0</v>
-      </c>
-      <c r="F48" s="28">
-        <f>F41+F47</f>
-        <v>485</v>
-      </c>
-      <c r="G48" s="29" t="s">
+      <c r="B50" s="27"/>
+      <c r="C50" s="28">
+        <f>C42+C49</f>
+        <v>791</v>
+      </c>
+      <c r="D50" s="28">
+        <f>D42+D49</f>
+        <v>176</v>
+      </c>
+      <c r="E50" s="28">
+        <f>E42+E49</f>
+        <v>0</v>
+      </c>
+      <c r="F50" s="28">
+        <f>F42+F49</f>
+        <v>295</v>
+      </c>
+      <c r="G50" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="H48" s="26" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A49" s="1"/>
-      <c r="B49" s="86"/>
-      <c r="C49" s="23"/>
-      <c r="D49" s="23"/>
-      <c r="E49" s="23"/>
-      <c r="F49" s="23"/>
-      <c r="G49" s="17"/>
-      <c r="H49" s="24"/>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A50" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B50" s="33">
-        <f>ROUND((B32-B45)/260,)</f>
-        <v>187</v>
-      </c>
-      <c r="C50" s="15"/>
-      <c r="D50" s="15"/>
-      <c r="E50" s="15"/>
-      <c r="F50" s="15"/>
-      <c r="G50" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="H50" s="24" t="s">
-        <v>55</v>
+      <c r="H50" s="26" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A51" s="79" t="s">
-        <v>143</v>
-      </c>
-      <c r="B51" s="85">
-        <f>IF(B29 &gt; 0, MIN(1,B50/B29), 0)</f>
-        <v>0.11333333333333333</v>
-      </c>
-      <c r="C51" s="81"/>
-      <c r="D51" s="80"/>
-      <c r="E51" s="80"/>
-      <c r="F51" s="80"/>
-      <c r="G51" s="82" t="s">
-        <v>8</v>
-      </c>
-      <c r="H51" s="80"/>
+      <c r="A51" s="1"/>
+      <c r="B51" s="86"/>
+      <c r="C51" s="23"/>
+      <c r="D51" s="23"/>
+      <c r="E51" s="23"/>
+      <c r="F51" s="23"/>
+      <c r="G51" s="17"/>
+      <c r="H51" s="24"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B52" s="31"/>
-      <c r="C52" s="16">
-        <f>C37*$B$51</f>
-        <v>58.846153846153847</v>
-      </c>
-      <c r="D52" s="16">
-        <f>D37*$B$51</f>
-        <v>0</v>
-      </c>
-      <c r="E52" s="16">
-        <f>E37*$B$51</f>
-        <v>0</v>
-      </c>
-      <c r="F52" s="16">
-        <f>F37*$B$51</f>
-        <v>128.15384615384616</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="B52" s="33">
+        <f>ROUND((B33-B47)/260,)</f>
+        <v>0</v>
+      </c>
+      <c r="C52" s="15"/>
+      <c r="D52" s="15"/>
+      <c r="E52" s="15"/>
+      <c r="F52" s="15"/>
       <c r="G52" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="H52" s="24" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A53" s="79" t="s">
+        <v>141</v>
+      </c>
+      <c r="B53" s="85">
+        <f>IF(B30 &gt; 0, MIN(1,B52/B30), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="C53" s="81"/>
+      <c r="D53" s="80"/>
+      <c r="E53" s="80"/>
+      <c r="F53" s="80"/>
+      <c r="G53" s="82" t="s">
         <v>8</v>
       </c>
-      <c r="H52" s="24" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A53" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B53" s="24"/>
-      <c r="C53" s="32">
-        <f>FLOOR(C52, 1)</f>
-        <v>58</v>
-      </c>
-      <c r="D53" s="32">
-        <f>FLOOR(D52, 1)</f>
-        <v>0</v>
-      </c>
-      <c r="E53" s="32">
-        <f>FLOOR(E52, 1)</f>
-        <v>0</v>
-      </c>
-      <c r="F53" s="32">
-        <f>FLOOR(F52, 1)</f>
-        <v>128</v>
-      </c>
-      <c r="G53" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="H53" s="24"/>
+      <c r="H53" s="80"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B54" s="36">
-        <f>B50-SUM(C53:F53)</f>
-        <v>1</v>
-      </c>
-      <c r="C54" s="24"/>
-      <c r="D54" s="24"/>
-      <c r="E54" s="24"/>
-      <c r="F54" s="24"/>
+        <v>45</v>
+      </c>
+      <c r="B54" s="31"/>
+      <c r="C54" s="16">
+        <f>C38*$B$53</f>
+        <v>0</v>
+      </c>
+      <c r="D54" s="16">
+        <f>D38*$B$53</f>
+        <v>0</v>
+      </c>
+      <c r="E54" s="16">
+        <f>E38*$B$53</f>
+        <v>0</v>
+      </c>
+      <c r="F54" s="16">
+        <f>F38*$B$53</f>
+        <v>0</v>
+      </c>
       <c r="G54" s="17" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="H54" s="24" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B55" s="33"/>
-      <c r="C55" s="23">
-        <f>C52-TRUNC(C53)</f>
-        <v>0.8461538461538467</v>
-      </c>
-      <c r="D55" s="23">
-        <f>D52-TRUNC(D53)</f>
-        <v>0</v>
-      </c>
-      <c r="E55" s="23">
-        <f>E52-TRUNC(E53)</f>
-        <v>0</v>
-      </c>
-      <c r="F55" s="23">
-        <f>F52-TRUNC(F53)</f>
-        <v>0.15384615384616041</v>
+        <v>47</v>
+      </c>
+      <c r="B55" s="24"/>
+      <c r="C55" s="32">
+        <f>FLOOR(C54, 1)</f>
+        <v>0</v>
+      </c>
+      <c r="D55" s="32">
+        <f>FLOOR(D54, 1)</f>
+        <v>0</v>
+      </c>
+      <c r="E55" s="32">
+        <f>FLOOR(E54, 1)</f>
+        <v>0</v>
+      </c>
+      <c r="F55" s="32">
+        <f>FLOOR(F54, 1)</f>
+        <v>0</v>
       </c>
       <c r="G55" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="H55" s="24" t="s">
-        <v>49</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="H55" s="24"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B56" s="33"/>
-      <c r="C56" s="25">
-        <f>IF($B$54&gt;0, IF(LARGE($C$55:$F$55,$B$54)&lt;=C$55,1,0), 0)</f>
-        <v>1</v>
-      </c>
-      <c r="D56" s="25">
-        <f>IF($B$54&gt;0, IF(LARGE($C$55:$F$55,$B$54)&lt;=D$55,1,0), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="E56" s="25">
-        <f>IF($B$54&gt;0, IF(LARGE($C$55:$F$55,$B$54)&lt;=E$55,1,0), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="F56" s="25">
-        <f>IF($B$54&gt;0, IF(LARGE($C$55:$F$55,$B$54)&lt;=F$55,1,0), 0)</f>
-        <v>0</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="B56" s="36">
+        <f>B52-SUM(C55:F55)</f>
+        <v>0</v>
+      </c>
+      <c r="C56" s="24"/>
+      <c r="D56" s="24"/>
+      <c r="E56" s="24"/>
+      <c r="F56" s="24"/>
       <c r="G56" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="H56" s="24"/>
+      <c r="H56" s="24" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A57" s="26" t="s">
-        <v>51</v>
-      </c>
-      <c r="B57" s="34"/>
-      <c r="C57" s="28">
-        <f>C53+C56</f>
-        <v>59</v>
-      </c>
-      <c r="D57" s="28">
-        <f>D53+D56</f>
-        <v>0</v>
-      </c>
-      <c r="E57" s="28">
-        <f>E53+E56</f>
-        <v>0</v>
-      </c>
-      <c r="F57" s="28">
-        <f>F53+F56</f>
-        <v>128</v>
-      </c>
-      <c r="G57" s="29" t="s">
+      <c r="A57" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B57" s="33"/>
+      <c r="C57" s="23">
+        <f>C54-TRUNC(C55)</f>
+        <v>0</v>
+      </c>
+      <c r="D57" s="23">
+        <f>D54-TRUNC(D55)</f>
+        <v>0</v>
+      </c>
+      <c r="E57" s="23">
+        <f>E54-TRUNC(E55)</f>
+        <v>0</v>
+      </c>
+      <c r="F57" s="23">
+        <f>F54-TRUNC(F55)</f>
+        <v>0</v>
+      </c>
+      <c r="G57" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="H57" s="24" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A58" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B58" s="33"/>
+      <c r="C58" s="25">
+        <f>IF($B$56&gt;0, IF(LARGE($C$57:$F$57,$B$56)&lt;=C$57,1,0), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="D58" s="25">
+        <f>IF($B$56&gt;0, IF(LARGE($C$57:$F$57,$B$56)&lt;=D$57,1,0), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="E58" s="25">
+        <f>IF($B$56&gt;0, IF(LARGE($C$57:$F$57,$B$56)&lt;=E$57,1,0), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="F58" s="25">
+        <f>IF($B$56&gt;0, IF(LARGE($C$57:$F$57,$B$56)&lt;=F$57,1,0), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="G58" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="H57" s="35"/>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A58" s="1"/>
-      <c r="B58" s="33"/>
-      <c r="C58" s="25"/>
-      <c r="D58" s="25"/>
-      <c r="E58" s="25"/>
-      <c r="F58" s="25"/>
-      <c r="G58" s="17"/>
       <c r="H58" s="24"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A59" s="1"/>
-      <c r="B59" s="33"/>
-      <c r="C59" s="24"/>
-      <c r="D59" s="24"/>
-      <c r="E59" s="24"/>
-      <c r="F59" s="24"/>
-      <c r="G59" s="17"/>
-      <c r="H59" s="24"/>
+      <c r="A59" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="B59" s="34"/>
+      <c r="C59" s="28">
+        <f>C55+C58</f>
+        <v>0</v>
+      </c>
+      <c r="D59" s="28">
+        <f>D55+D58</f>
+        <v>0</v>
+      </c>
+      <c r="E59" s="28">
+        <f>E55+E58</f>
+        <v>0</v>
+      </c>
+      <c r="F59" s="28">
+        <f>F55+F58</f>
+        <v>0</v>
+      </c>
+      <c r="G59" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="H59" s="35"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A60" s="26" t="s">
-        <v>56</v>
-      </c>
-      <c r="B60" s="37">
-        <f>B44+B50</f>
-        <v>1422</v>
-      </c>
-      <c r="C60" s="35"/>
-      <c r="D60" s="35"/>
-      <c r="E60" s="35"/>
-      <c r="F60" s="35"/>
-      <c r="G60" s="38"/>
-      <c r="H60" s="35"/>
+      <c r="A60" s="1"/>
+      <c r="B60" s="33"/>
+      <c r="C60" s="25"/>
+      <c r="D60" s="25"/>
+      <c r="E60" s="25"/>
+      <c r="F60" s="25"/>
+      <c r="G60" s="17"/>
+      <c r="H60" s="24"/>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A61" s="1"/>
+      <c r="B61" s="33"/>
+      <c r="C61" s="24"/>
+      <c r="D61" s="24"/>
+      <c r="E61" s="24"/>
+      <c r="F61" s="24"/>
+      <c r="G61" s="17"/>
+      <c r="H61" s="24"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="H62" s="4"/>
+      <c r="A62" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="B62" s="37">
+        <f>B46+B52</f>
+        <v>1262</v>
+      </c>
+      <c r="C62" s="35"/>
+      <c r="D62" s="35"/>
+      <c r="E62" s="35"/>
+      <c r="F62" s="35"/>
+      <c r="G62" s="38"/>
+      <c r="H62" s="35"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H63" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <ignoredErrors>
-    <ignoredError sqref="B24 B29" formula="1"/>
+    <ignoredError sqref="B30 B24" formula="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -2479,28 +2546,28 @@
   <sheetData>
     <row r="1" spans="1:9" s="43" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="41" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="41" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="C1" s="41" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="41" t="s">
+      <c r="D1" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="D1" s="42" t="s">
+      <c r="E1" s="42" t="s">
         <v>60</v>
       </c>
-      <c r="E1" s="42" t="s">
+      <c r="F1" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="F1" s="42" t="s">
+      <c r="G1" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="G1" s="42" t="s">
+      <c r="H1" s="42" t="s">
         <v>63</v>
-      </c>
-      <c r="H1" s="42" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -2511,7 +2578,7 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D3" s="7">
         <v>21000</v>
@@ -2526,13 +2593,13 @@
         <v>0</v>
       </c>
       <c r="H3" s="40" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="43"/>
       <c r="B4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D4" s="8">
         <f>D3/SUM($D$3:$G$3)</f>
@@ -2551,7 +2618,7 @@
         <v>0</v>
       </c>
       <c r="H4" s="40" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -2559,7 +2626,7 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D5" s="44">
         <f>D3*12/260</f>
@@ -2578,10 +2645,10 @@
         <v>0</v>
       </c>
       <c r="H5" s="40" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I5" s="45" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -2589,7 +2656,7 @@
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D6" s="10">
         <v>1</v>
@@ -2604,7 +2671,7 @@
         <v>1</v>
       </c>
       <c r="H6" s="40" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -2612,7 +2679,7 @@
         <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D7" s="44">
         <f>D5*D6</f>
@@ -2631,10 +2698,10 @@
         <v>0</v>
       </c>
       <c r="H7" s="40" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I7" s="46" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -2642,7 +2709,7 @@
         <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D8" s="11">
         <f>MIN(D7,$C$15)</f>
@@ -2661,10 +2728,10 @@
         <v>0</v>
       </c>
       <c r="H8" s="40" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I8" s="45" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -2672,7 +2739,7 @@
         <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D9" s="12">
         <v>0.5</v>
@@ -2687,7 +2754,7 @@
         <v>1</v>
       </c>
       <c r="H9" s="40" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -2695,7 +2762,7 @@
         <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D10" s="44">
         <f>D7*D9</f>
@@ -2714,15 +2781,15 @@
         <v>0</v>
       </c>
       <c r="H10" s="40" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="43" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D11" s="10">
         <v>1</v>
@@ -2737,15 +2804,15 @@
         <v>1</v>
       </c>
       <c r="H11" s="40" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="43" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D12" s="47">
         <f>D10*D11</f>
@@ -2764,77 +2831,77 @@
         <v>0</v>
       </c>
       <c r="H12" s="40" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="43" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C13" s="48">
         <f>ROUND(SUM(D10:G10)/SUM(D7:G7),2)</f>
         <v>0.4</v>
       </c>
       <c r="H13" s="40" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="43" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C14" s="7">
         <v>93634</v>
       </c>
       <c r="H14" s="40" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="43" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C15" s="11">
         <f>ROUND(6*C14/260, 0)</f>
         <v>2161</v>
       </c>
       <c r="H15" s="40" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I15" s="45" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="43" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C16" s="11">
         <f>ROUND(C13*C15,0)</f>
         <v>864</v>
       </c>
       <c r="H16" s="40" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="49" t="s">
+        <v>82</v>
+      </c>
+      <c r="B17" s="50" t="s">
         <v>83</v>
-      </c>
-      <c r="B17" s="50" t="s">
-        <v>84</v>
       </c>
       <c r="C17" s="51">
         <f>MIN(1, C16/SUM(D10:G10))</f>
@@ -2845,15 +2912,15 @@
       <c r="F17" s="52"/>
       <c r="G17" s="52"/>
       <c r="H17" s="53" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="49" t="s">
+        <v>84</v>
+      </c>
+      <c r="B18" s="50" t="s">
         <v>85</v>
-      </c>
-      <c r="B18" s="50" t="s">
-        <v>86</v>
       </c>
       <c r="C18" s="50"/>
       <c r="D18" s="52">
@@ -2873,15 +2940,15 @@
         <v>0</v>
       </c>
       <c r="H18" s="53" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="49" t="s">
+        <v>86</v>
+      </c>
+      <c r="B19" s="50" t="s">
         <v>87</v>
-      </c>
-      <c r="B19" s="50" t="s">
-        <v>88</v>
       </c>
       <c r="C19" s="50"/>
       <c r="D19" s="52">
@@ -2901,13 +2968,13 @@
         <v>0</v>
       </c>
       <c r="H19" s="53" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="49"/>
       <c r="B20" s="50" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C20" s="50"/>
       <c r="D20" s="52">
@@ -2927,13 +2994,13 @@
         <v>0</v>
       </c>
       <c r="H20" s="53" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="49"/>
       <c r="B21" s="50" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C21" s="50"/>
       <c r="D21" s="51">
@@ -2950,15 +3017,15 @@
       </c>
       <c r="G21" s="52"/>
       <c r="H21" s="53" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="22" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="49" t="s">
+        <v>90</v>
+      </c>
+      <c r="B22" s="50" t="s">
         <v>91</v>
-      </c>
-      <c r="B22" s="50" t="s">
-        <v>92</v>
       </c>
       <c r="C22" s="50"/>
       <c r="D22" s="51">
@@ -2978,13 +3045,13 @@
         <v>0</v>
       </c>
       <c r="H22" s="53" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="23" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="49"/>
       <c r="B23" s="50" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C23" s="50"/>
       <c r="D23" s="52">
@@ -3004,15 +3071,15 @@
         <v>0</v>
       </c>
       <c r="H23" s="53" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="49" t="s">
+        <v>93</v>
+      </c>
+      <c r="B24" s="50" t="s">
         <v>94</v>
-      </c>
-      <c r="B24" s="50" t="s">
-        <v>95</v>
       </c>
       <c r="C24" s="50"/>
       <c r="D24" s="52">
@@ -3032,13 +3099,13 @@
         <v>0</v>
       </c>
       <c r="H24" s="53" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="25" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="49"/>
       <c r="B25" s="50" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C25" s="50"/>
       <c r="D25" s="51">
@@ -3058,13 +3125,13 @@
         <v>0</v>
       </c>
       <c r="H25" s="53" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="26" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="49"/>
       <c r="B26" s="50" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C26" s="50"/>
       <c r="D26" s="51">
@@ -3084,15 +3151,15 @@
         <v>0</v>
       </c>
       <c r="H26" s="53" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="27" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="49" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B27" s="50" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C27" s="50"/>
       <c r="D27" s="54">
@@ -3112,15 +3179,15 @@
         <v>0</v>
       </c>
       <c r="H27" s="53" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="28" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="49" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B28" s="50" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C28" s="50"/>
       <c r="D28" s="50">
@@ -3140,13 +3207,13 @@
         <v>0</v>
       </c>
       <c r="H28" s="53" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="29" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="49"/>
       <c r="B29" s="50" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C29" s="55">
         <f>C16-SUM(D27:G28)</f>
@@ -3157,7 +3224,7 @@
       <c r="F29" s="50"/>
       <c r="G29" s="50"/>
       <c r="H29" s="53" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
@@ -3169,7 +3236,7 @@
         <v>20</v>
       </c>
       <c r="B31" s="18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C31" s="15"/>
       <c r="D31" s="30">
@@ -3189,18 +3256,18 @@
         <v>0</v>
       </c>
       <c r="H31" s="17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I31" s="46" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B32" s="18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C32" s="15"/>
       <c r="D32" s="30">
@@ -3220,15 +3287,15 @@
         <v>0</v>
       </c>
       <c r="H32" s="17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B33" s="18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C33" s="15"/>
       <c r="D33" s="30">
@@ -3248,30 +3315,30 @@
         <v>0</v>
       </c>
       <c r="H33" s="17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="1"/>
       <c r="B34" s="56" t="s">
-        <v>103</v>
-      </c>
-      <c r="C34" s="91" t="str">
+        <v>102</v>
+      </c>
+      <c r="C34" s="92" t="str">
         <f>IF(SUM(D32:G33)&lt;=MAKSBELOP,"Everyone paid",IF(SUM(D32:G32)&lt;=MAKSBELOP,"Arbeidsgivere fully paid; Person partially paid by Person request", "Arbeidsgivere partial payment ratio by Arbeidsgiver request"))</f>
         <v>Arbeidsgivere partial payment ratio by Arbeidsgiver request</v>
       </c>
-      <c r="D34" s="91"/>
-      <c r="E34" s="91"/>
-      <c r="F34" s="91"/>
-      <c r="G34" s="91"/>
+      <c r="D34" s="92"/>
+      <c r="E34" s="92"/>
+      <c r="F34" s="92"/>
+      <c r="G34" s="92"/>
       <c r="H34" s="17"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B35" s="18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C35" s="15"/>
       <c r="D35" s="18">
@@ -3291,13 +3358,13 @@
         <v>0</v>
       </c>
       <c r="H35" s="17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="36" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="1"/>
       <c r="B36" s="18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C36" s="15">
         <f>MAKSBELOP-SUM(D35:G35)</f>
@@ -3311,10 +3378,10 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B37" s="18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C37" s="18"/>
       <c r="D37" s="18">
@@ -3334,13 +3401,13 @@
         <v>0</v>
       </c>
       <c r="H37" s="17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="1"/>
       <c r="B38" s="18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C38" s="15">
         <f>MAKSBELOP-SUM(D35:G37)</f>
@@ -3351,28 +3418,28 @@
       <c r="F38" s="18"/>
       <c r="G38" s="18"/>
       <c r="H38" s="17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="57" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B40" s="58"/>
       <c r="C40" s="59"/>
       <c r="D40" s="60"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A41" s="92" t="s">
-        <v>106</v>
-      </c>
-      <c r="B41" s="92"/>
-      <c r="C41" s="92"/>
-      <c r="D41" s="92"/>
+      <c r="A41" s="93" t="s">
+        <v>105</v>
+      </c>
+      <c r="B41" s="93"/>
+      <c r="C41" s="93"/>
+      <c r="D41" s="93"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="61" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B43" s="62">
         <v>1430.76</v>
@@ -3380,7 +3447,7 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="61" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B44" s="62">
         <f>ROUND(B43*260/12,0)</f>
@@ -3419,28 +3486,28 @@
   <sheetData>
     <row r="1" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="41" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="41" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="C1" s="41" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="41" t="s">
+      <c r="D1" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="D1" s="42" t="s">
+      <c r="E1" s="42" t="s">
         <v>60</v>
       </c>
-      <c r="E1" s="42" t="s">
+      <c r="F1" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="F1" s="42" t="s">
+      <c r="G1" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="G1" s="42" t="s">
+      <c r="H1" s="42" t="s">
         <v>63</v>
-      </c>
-      <c r="H1" s="42" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -3452,7 +3519,7 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D3" s="7">
         <v>21000</v>
@@ -3467,13 +3534,13 @@
         <v>0</v>
       </c>
       <c r="H3" s="40" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="43"/>
       <c r="B4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D4" s="8">
         <f>D3/SUM($D$3:$G$3)</f>
@@ -3492,7 +3559,7 @@
         <v>0</v>
       </c>
       <c r="H4" s="40" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -3500,7 +3567,7 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D5" s="44">
         <f>D3*12/260</f>
@@ -3519,7 +3586,7 @@
         <v>0</v>
       </c>
       <c r="H5" s="40" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -3527,7 +3594,7 @@
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D6" s="10">
         <v>1</v>
@@ -3542,7 +3609,7 @@
         <v>1</v>
       </c>
       <c r="H6" s="40" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -3550,7 +3617,7 @@
         <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D7" s="44">
         <f>D5*D6</f>
@@ -3569,7 +3636,7 @@
         <v>0</v>
       </c>
       <c r="H7" s="40" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -3577,7 +3644,7 @@
         <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D8" s="11">
         <f>MIN(D7,$C$15)</f>
@@ -3596,7 +3663,7 @@
         <v>0</v>
       </c>
       <c r="H8" s="40" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -3604,7 +3671,7 @@
         <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D9" s="12">
         <v>0.5</v>
@@ -3619,7 +3686,7 @@
         <v>1</v>
       </c>
       <c r="H9" s="40" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -3627,7 +3694,7 @@
         <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D10" s="44">
         <f>D7*D9</f>
@@ -3646,15 +3713,15 @@
         <v>0</v>
       </c>
       <c r="H10" s="40" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="43" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D11" s="10">
         <v>1</v>
@@ -3669,15 +3736,15 @@
         <v>1</v>
       </c>
       <c r="H11" s="40" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="43" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D12" s="47">
         <f>D10*D11</f>
@@ -3696,74 +3763,74 @@
         <v>0</v>
       </c>
       <c r="H12" s="40" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="43" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C13" s="63">
         <f>SUM(D10:G10)/SUM(D7:G7)</f>
         <v>0.39838709677419348</v>
       </c>
       <c r="H13" s="40" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="43" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C14" s="7">
         <v>101351</v>
       </c>
       <c r="H14" s="40" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="43" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C15" s="64">
         <f>6*C14/260</f>
         <v>2338.8692307692309</v>
       </c>
       <c r="H15" s="40" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="43" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C16" s="64">
         <f>C13*C15</f>
         <v>931.77532258064502</v>
       </c>
       <c r="H16" s="40" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="49" t="s">
+        <v>82</v>
+      </c>
+      <c r="B17" s="50" t="s">
         <v>83</v>
-      </c>
-      <c r="B17" s="50" t="s">
-        <v>84</v>
       </c>
       <c r="C17" s="51">
         <f>MIN(1, C16/SUM(D10:G10))</f>
@@ -3774,15 +3841,15 @@
       <c r="F17" s="52"/>
       <c r="G17" s="52"/>
       <c r="H17" s="53" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="49" t="s">
+        <v>84</v>
+      </c>
+      <c r="B18" s="50" t="s">
         <v>85</v>
-      </c>
-      <c r="B18" s="50" t="s">
-        <v>86</v>
       </c>
       <c r="C18" s="50"/>
       <c r="D18" s="52">
@@ -3802,15 +3869,15 @@
         <v>0</v>
       </c>
       <c r="H18" s="53" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="49" t="s">
+        <v>86</v>
+      </c>
+      <c r="B19" s="50" t="s">
         <v>87</v>
-      </c>
-      <c r="B19" s="50" t="s">
-        <v>88</v>
       </c>
       <c r="C19" s="50"/>
       <c r="D19" s="52">
@@ -3830,13 +3897,13 @@
         <v>0</v>
       </c>
       <c r="H19" s="53" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="49"/>
       <c r="B20" s="50" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C20" s="50"/>
       <c r="D20" s="52">
@@ -3856,13 +3923,13 @@
         <v>0</v>
       </c>
       <c r="H20" s="53" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="49"/>
       <c r="B21" s="50" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C21" s="50"/>
       <c r="D21" s="51">
@@ -3879,15 +3946,15 @@
       </c>
       <c r="G21" s="52"/>
       <c r="H21" s="53" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="22" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="49" t="s">
+        <v>90</v>
+      </c>
+      <c r="B22" s="50" t="s">
         <v>91</v>
-      </c>
-      <c r="B22" s="50" t="s">
-        <v>92</v>
       </c>
       <c r="C22" s="50"/>
       <c r="D22" s="51">
@@ -3907,13 +3974,13 @@
         <v>0</v>
       </c>
       <c r="H22" s="53" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="49"/>
       <c r="B23" s="50" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C23" s="50"/>
       <c r="D23" s="52">
@@ -3933,15 +4000,15 @@
         <v>0</v>
       </c>
       <c r="H23" s="53" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="49" t="s">
+        <v>93</v>
+      </c>
+      <c r="B24" s="50" t="s">
         <v>94</v>
-      </c>
-      <c r="B24" s="50" t="s">
-        <v>95</v>
       </c>
       <c r="C24" s="50"/>
       <c r="D24" s="52">
@@ -3961,13 +4028,13 @@
         <v>0</v>
       </c>
       <c r="H24" s="53" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="25" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="49"/>
       <c r="B25" s="50" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C25" s="50"/>
       <c r="D25" s="51">
@@ -3987,13 +4054,13 @@
         <v>0</v>
       </c>
       <c r="H25" s="53" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="26" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="49"/>
       <c r="B26" s="50" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C26" s="50"/>
       <c r="D26" s="51">
@@ -4013,15 +4080,15 @@
         <v>0</v>
       </c>
       <c r="H26" s="53" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="49" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B27" s="50" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C27" s="50"/>
       <c r="D27" s="54">
@@ -4041,15 +4108,15 @@
         <v>0</v>
       </c>
       <c r="H27" s="53" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="28" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="49" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B28" s="50" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C28" s="50"/>
       <c r="D28" s="50">
@@ -4069,13 +4136,13 @@
         <v>0</v>
       </c>
       <c r="H28" s="53" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="29" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="49"/>
       <c r="B29" s="50" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C29" s="55">
         <f>C16-SUM(D27:G28)</f>
@@ -4086,7 +4153,7 @@
       <c r="F29" s="50"/>
       <c r="G29" s="50"/>
       <c r="H29" s="53" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
@@ -4099,7 +4166,7 @@
         <v>20</v>
       </c>
       <c r="B31" s="18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C31" s="15"/>
       <c r="D31" s="65">
@@ -4119,15 +4186,15 @@
         <v>0</v>
       </c>
       <c r="H31" s="17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B32" s="18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C32" s="15"/>
       <c r="D32" s="65">
@@ -4147,15 +4214,15 @@
         <v>0</v>
       </c>
       <c r="H32" s="17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B33" s="18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C33" s="15"/>
       <c r="D33" s="65">
@@ -4175,30 +4242,30 @@
         <v>0</v>
       </c>
       <c r="H33" s="17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="1"/>
       <c r="B34" s="56" t="s">
-        <v>103</v>
-      </c>
-      <c r="C34" s="91" t="str">
+        <v>102</v>
+      </c>
+      <c r="C34" s="92" t="str">
         <f>IF(SUM(D32:G33)&lt;=MAKSBELOP,"Everyone paid",IF(SUM(D32:G32)&lt;=MAKSBELOP,"Arbeidsgivere fully paid; Person partially paid by Person request", "Arbeidsgivere partial payment ratio by Arbeidsgiver request"))</f>
         <v>Arbeidsgivere partial payment ratio by Arbeidsgiver request</v>
       </c>
-      <c r="D34" s="91"/>
-      <c r="E34" s="91"/>
-      <c r="F34" s="91"/>
-      <c r="G34" s="91"/>
+      <c r="D34" s="92"/>
+      <c r="E34" s="92"/>
+      <c r="F34" s="92"/>
+      <c r="G34" s="92"/>
       <c r="H34" s="17"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B35" s="18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C35" s="15"/>
       <c r="D35" s="18">
@@ -4218,13 +4285,13 @@
         <v>0</v>
       </c>
       <c r="H35" s="17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="1"/>
       <c r="B36" s="18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C36" s="66">
         <f>MAKSBELOP2-SUM(D35:G35)</f>
@@ -4238,10 +4305,10 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B37" s="18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C37" s="18"/>
       <c r="D37" s="25">
@@ -4261,13 +4328,13 @@
         <v>0</v>
       </c>
       <c r="H37" s="17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="1"/>
       <c r="B38" s="18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C38" s="66">
         <f>MAKSBELOP2-SUM(D35:G37)</f>
@@ -4278,7 +4345,7 @@
       <c r="F38" s="18"/>
       <c r="G38" s="18"/>
       <c r="H38" s="17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
legger til rad for refusjon ut fra vektet refusjon
</commit_message>
<xml_diff>
--- a/doc/okonomi/Utbetaling.xlsx
+++ b/doc/okonomi/Utbetaling.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/david/dev/nav/helse-spleis/doc/okonomi/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63F84AC2-5FB4-E44B-AD80-B779A52633AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59F3D9CD-72EE-7A47-82BC-291881548269}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="47620" windowHeight="41000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="153">
   <si>
     <t xml:space="preserve">Begrep	</t>
   </si>
@@ -522,6 +522,12 @@
   <si>
     <t>Rest til utbetaling før avrunding</t>
   </si>
+  <si>
+    <t>Arbeidsgiverrefusjon som følge av andel av dagsats vektet refusjon utgjør</t>
+  </si>
+  <si>
+    <t>Utregnet refusjon før avrunding</t>
+  </si>
 </sst>
 </file>
 
@@ -542,8 +548,8 @@
     <numFmt numFmtId="174" formatCode="_-* #,##0.0000000000_-;\-* #,##0.0000000000_-;_-* &quot;-&quot;??????????_-;_-@_-"/>
     <numFmt numFmtId="175" formatCode="_-* #,##0.00000000_-;\-* #,##0.00000000_-;_-* &quot;-&quot;??????????_-;_-@_-"/>
     <numFmt numFmtId="176" formatCode="_-* #,##0.000000000_-;\-* #,##0.000000000_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="182" formatCode="_(* #,##0.00000_);_(* \(#,##0.00000\);_(* \-??_);_(@_)"/>
-    <numFmt numFmtId="190" formatCode="0.0"/>
+    <numFmt numFmtId="177" formatCode="_(* #,##0.00000_);_(* \(#,##0.00000\);_(* \-??_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="0.0"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -714,7 +720,7 @@
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -829,7 +835,6 @@
     <xf numFmtId="171" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -845,22 +850,22 @@
     <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="190" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1245,10 +1250,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H63"/>
+  <dimension ref="A1:H64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1579,19 +1584,19 @@
         <v>16</v>
       </c>
       <c r="B18" s="4"/>
-      <c r="C18" s="99">
+      <c r="C18" s="96">
         <f>ROUND(C16*C17,0)</f>
         <v>2077</v>
       </c>
-      <c r="D18" s="99">
+      <c r="D18" s="96">
         <f t="shared" ref="D18:F18" si="1">ROUND(D16*D17,0)</f>
         <v>231</v>
       </c>
-      <c r="E18" s="99">
+      <c r="E18" s="96">
         <f t="shared" si="1"/>
         <v>462</v>
       </c>
-      <c r="F18" s="99">
+      <c r="F18" s="96">
         <f t="shared" si="1"/>
         <v>1615</v>
       </c>
@@ -1634,19 +1639,19 @@
         <v>20</v>
       </c>
       <c r="B20" s="4"/>
-      <c r="C20" s="99">
+      <c r="C20" s="96">
         <f>ROUND(C18*C8,0)</f>
         <v>1039</v>
       </c>
-      <c r="D20" s="99">
+      <c r="D20" s="96">
         <f t="shared" ref="D20:F20" si="2">ROUND(D18*D8,0)</f>
         <v>231</v>
       </c>
-      <c r="E20" s="99">
+      <c r="E20" s="96">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F20" s="99">
+      <c r="F20" s="96">
         <f t="shared" si="2"/>
         <v>1292</v>
       </c>
@@ -1661,19 +1666,19 @@
       <c r="A21" s="73" t="s">
         <v>142</v>
       </c>
-      <c r="C21" s="100">
+      <c r="C21" s="97">
         <f>ROUND(ROUND(C6*12/260,0)*C8,0)</f>
         <v>1039</v>
       </c>
-      <c r="D21" s="100">
+      <c r="D21" s="97">
         <f t="shared" ref="D21:F21" si="3">ROUND(ROUND(D6*12/260,0)*D8,0)</f>
         <v>231</v>
       </c>
-      <c r="E21" s="100">
+      <c r="E21" s="97">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="F21" s="100">
+      <c r="F21" s="97">
         <f t="shared" si="3"/>
         <v>388</v>
       </c>
@@ -1738,19 +1743,19 @@
         <v>22</v>
       </c>
       <c r="B26" s="4"/>
-      <c r="C26" s="101">
+      <c r="C26" s="98">
         <f>MIN(C20,C21)</f>
         <v>1039</v>
       </c>
-      <c r="D26" s="101">
+      <c r="D26" s="98">
         <f t="shared" ref="D26:F26" si="4">MIN(D20,D21)</f>
         <v>231</v>
       </c>
-      <c r="E26" s="101">
+      <c r="E26" s="98">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="F26" s="101">
+      <c r="F26" s="98">
         <f t="shared" si="4"/>
         <v>388</v>
       </c>
@@ -1765,19 +1770,19 @@
       <c r="A27" s="73" t="s">
         <v>148</v>
       </c>
-      <c r="C27" s="97">
+      <c r="C27" s="94">
         <f>C26/$B$24</f>
         <v>0.62665862484921597</v>
       </c>
-      <c r="D27" s="97">
+      <c r="D27" s="94">
         <f t="shared" ref="D27:F27" si="5">D26/$B$24</f>
         <v>0.13932448733413752</v>
       </c>
-      <c r="E27" s="97">
+      <c r="E27" s="94">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="F27" s="97">
+      <c r="F27" s="94">
         <f t="shared" si="5"/>
         <v>0.23401688781664656</v>
       </c>
@@ -1790,379 +1795,381 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="73" t="s">
+        <v>152</v>
+      </c>
+      <c r="C28" s="67">
+        <f>$B$35*C27</f>
+        <v>790.84318455971061</v>
+      </c>
+      <c r="D28" s="67">
+        <f>$B$35*D27</f>
+        <v>175.82750301568154</v>
+      </c>
+      <c r="E28" s="67">
+        <f>$B$35*E27</f>
+        <v>0</v>
+      </c>
+      <c r="F28" s="67">
+        <f>$B$35*F27</f>
+        <v>295.32931242460796</v>
+      </c>
+      <c r="H28" s="75" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="73" t="s">
         <v>123</v>
       </c>
-      <c r="B28" s="98">
+      <c r="B29" s="95">
         <f>SUM(C26:F26)</f>
         <v>1658</v>
       </c>
-      <c r="C28" s="91"/>
-      <c r="D28" s="91"/>
-      <c r="E28" s="91"/>
-      <c r="F28" s="91"/>
-      <c r="G28" s="70" t="s">
+      <c r="C29" s="90"/>
+      <c r="D29" s="90"/>
+      <c r="E29" s="90"/>
+      <c r="F29" s="90"/>
+      <c r="G29" s="70" t="s">
         <v>14</v>
       </c>
-      <c r="H28" s="75" t="s">
+      <c r="H29" s="75" t="s">
         <v>128</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" s="73" t="s">
-        <v>126</v>
-      </c>
-      <c r="B29" s="72">
-        <f>B28*260</f>
-        <v>431080</v>
-      </c>
-      <c r="C29" s="67"/>
-      <c r="D29" s="67"/>
-      <c r="E29" s="67"/>
-      <c r="F29" s="67"/>
-      <c r="G29" s="70" t="s">
-        <v>8</v>
-      </c>
-      <c r="H29" s="75" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="73" t="s">
-        <v>132</v>
-      </c>
-      <c r="B30" s="67">
-        <f>B22-B28</f>
-        <v>904</v>
-      </c>
-      <c r="D30" s="83"/>
-      <c r="E30" s="84"/>
+        <v>126</v>
+      </c>
+      <c r="B30" s="72">
+        <f>B29*260</f>
+        <v>431080</v>
+      </c>
+      <c r="C30" s="67"/>
+      <c r="D30" s="67"/>
+      <c r="E30" s="67"/>
+      <c r="F30" s="67"/>
       <c r="G30" s="70" t="s">
         <v>8</v>
       </c>
       <c r="H30" s="75" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="73" t="s">
-        <v>126</v>
-      </c>
-      <c r="B31" s="72">
-        <f>B30*260</f>
-        <v>235040</v>
-      </c>
-      <c r="C31" s="67"/>
-      <c r="D31" s="78"/>
-      <c r="E31" s="84"/>
+        <v>132</v>
+      </c>
+      <c r="B31" s="67">
+        <f>B22-B29</f>
+        <v>904</v>
+      </c>
+      <c r="D31" s="82"/>
+      <c r="E31" s="83"/>
       <c r="G31" s="70" t="s">
         <v>8</v>
       </c>
       <c r="H31" s="75" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="73" t="s">
+        <v>126</v>
+      </c>
+      <c r="B32" s="72">
+        <f>B31*260</f>
+        <v>235040</v>
+      </c>
+      <c r="G32" s="70" t="s">
+        <v>8</v>
+      </c>
+      <c r="H32" s="75" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A32" s="3" t="s">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B32" s="14">
+      <c r="B33" s="14">
         <f>SUM(C19:F19)</f>
         <v>0.58421052631578951</v>
       </c>
-      <c r="C32" s="89"/>
-      <c r="D32" s="90"/>
-      <c r="E32" s="90"/>
-      <c r="F32" s="4"/>
-      <c r="G32" s="5" t="s">
+      <c r="C33" s="88"/>
+      <c r="D33" s="89"/>
+      <c r="E33" s="89"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="H32" s="6" t="s">
+      <c r="H33" s="6" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A33" s="73" t="s">
-        <v>117</v>
-      </c>
-      <c r="B33" s="76">
-        <f>ROUND(B13*B32/260,)*260</f>
-        <v>328120</v>
-      </c>
-      <c r="C33" s="87"/>
-      <c r="D33" s="83"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
-      <c r="G33" s="70" t="s">
-        <v>14</v>
-      </c>
-      <c r="H33" s="75" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="73" t="s">
-        <v>112</v>
-      </c>
-      <c r="B34" s="83">
-        <f>B33/260</f>
-        <v>1262</v>
-      </c>
-      <c r="C34" s="83"/>
-      <c r="D34" s="88"/>
+        <v>117</v>
+      </c>
+      <c r="B34" s="76">
+        <f>ROUND(B13*B33/260,)*260</f>
+        <v>328120</v>
+      </c>
+      <c r="C34" s="86"/>
+      <c r="D34" s="82"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
       <c r="G34" s="70" t="s">
         <v>14</v>
       </c>
       <c r="H34" s="75" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="73" t="s">
+        <v>112</v>
+      </c>
+      <c r="B35" s="82">
+        <f>B34/260</f>
+        <v>1262</v>
+      </c>
+      <c r="C35" s="82"/>
+      <c r="D35" s="87"/>
+      <c r="G35" s="70" t="s">
+        <v>14</v>
+      </c>
+      <c r="H35" s="75" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" s="73" t="s">
         <v>124</v>
       </c>
-      <c r="B35" s="83">
-        <f>B33/MAX(B33,B29)</f>
+      <c r="B36" s="82">
+        <f>B34/MAX(B34,B30)</f>
         <v>0.76115802171290714</v>
       </c>
-      <c r="D35" s="83"/>
-      <c r="G35" s="70" t="s">
+      <c r="D36" s="82"/>
+      <c r="G36" s="70" t="s">
         <v>8</v>
       </c>
-      <c r="H35" s="75" t="s">
+      <c r="H36" s="75" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="s">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B36" s="15"/>
-      <c r="C36" s="16">
+      <c r="B37" s="15"/>
+      <c r="C37" s="16">
         <f>C20</f>
         <v>1039</v>
       </c>
-      <c r="D36" s="16">
+      <c r="D37" s="16">
         <f>D20</f>
         <v>231</v>
       </c>
-      <c r="E36" s="16">
+      <c r="E37" s="16">
         <f>E20</f>
         <v>0</v>
       </c>
-      <c r="F36" s="16">
+      <c r="F37" s="16">
         <f>F20</f>
         <v>1292</v>
       </c>
-      <c r="G36" s="17" t="s">
+      <c r="G37" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="H36" s="24" t="s">
+      <c r="H37" s="24" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B37" s="15"/>
-      <c r="C37" s="16">
+      <c r="B38" s="15"/>
+      <c r="C38" s="16">
         <f>C26</f>
         <v>1039</v>
       </c>
-      <c r="D37" s="16">
+      <c r="D38" s="16">
         <f>D26</f>
         <v>231</v>
       </c>
-      <c r="E37" s="16">
+      <c r="E38" s="16">
         <f>E26</f>
         <v>0</v>
       </c>
-      <c r="F37" s="16">
+      <c r="F38" s="16">
         <f>F26</f>
         <v>388</v>
       </c>
-      <c r="G37" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="H37" s="24" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B38" s="15"/>
-      <c r="C38" s="16">
-        <f>C36-C37</f>
-        <v>0</v>
-      </c>
-      <c r="D38" s="16">
-        <f>D36-D37</f>
-        <v>0</v>
-      </c>
-      <c r="E38" s="16">
-        <f>E36-E37</f>
-        <v>0</v>
-      </c>
-      <c r="F38" s="16">
-        <f>F36-F37</f>
-        <v>904</v>
-      </c>
       <c r="G38" s="17" t="s">
         <v>14</v>
       </c>
       <c r="H38" s="24" t="s">
-        <v>136</v>
+        <v>31</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B39" s="15"/>
+      <c r="C39" s="16">
+        <f>C37-C38</f>
+        <v>0</v>
+      </c>
+      <c r="D39" s="16">
+        <f>D37-D38</f>
+        <v>0</v>
+      </c>
+      <c r="E39" s="16">
+        <f>E37-E38</f>
+        <v>0</v>
+      </c>
+      <c r="F39" s="16">
+        <f>F37-F38</f>
+        <v>904</v>
+      </c>
+      <c r="G39" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="H39" s="24" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B39" s="19" t="str">
-        <f>IF(B31&lt;=B33,"Arbeidsgiver og person blir refundert hele beløpet",IF(B29&lt;=B33,"Arbeidsgivere blir refundert hele beløpet; Person blir delvis refundert", "Arbeidsgivere blir delvis refundert"))</f>
+      <c r="B40" s="19" t="str">
+        <f>IF(B32&lt;=B34,"Arbeidsgiver og person blir refundert hele beløpet",IF(B30&lt;=B34,"Arbeidsgivere blir refundert hele beløpet; Person blir delvis refundert", "Arbeidsgivere blir delvis refundert"))</f>
         <v>Arbeidsgiver og person blir refundert hele beløpet</v>
       </c>
-      <c r="C39" s="19"/>
-      <c r="D39" s="19"/>
-      <c r="E39" s="19"/>
-      <c r="F39" s="19"/>
-      <c r="G39" s="17"/>
-      <c r="H39" s="24"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A40" s="1"/>
-      <c r="B40" s="20"/>
-      <c r="C40" s="77"/>
-      <c r="D40" s="21"/>
-      <c r="E40" s="21"/>
-      <c r="F40" s="22"/>
+      <c r="C40" s="19"/>
+      <c r="D40" s="19"/>
+      <c r="E40" s="19"/>
+      <c r="F40" s="19"/>
       <c r="G40" s="17"/>
       <c r="H40" s="24"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A41" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="A41" s="1"/>
       <c r="B41" s="20"/>
-      <c r="C41" s="23">
-        <f>C37*$B$35</f>
-        <v>790.84318455971049</v>
-      </c>
-      <c r="D41" s="23">
-        <f>D37*$B$35</f>
-        <v>175.82750301568154</v>
-      </c>
-      <c r="E41" s="23">
-        <f>E37*$B$35</f>
-        <v>0</v>
-      </c>
-      <c r="F41" s="23">
-        <f>F37*$B$35</f>
-        <v>295.32931242460796</v>
-      </c>
-      <c r="G41" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="H41" s="24" t="s">
-        <v>34</v>
-      </c>
+      <c r="C41" s="77"/>
+      <c r="D41" s="21"/>
+      <c r="E41" s="21"/>
+      <c r="F41" s="22"/>
+      <c r="G41" s="17"/>
+      <c r="H41" s="24"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B42" s="15"/>
-      <c r="C42" s="24">
-        <f>FLOOR(C41,1)</f>
-        <v>790</v>
-      </c>
-      <c r="D42" s="24">
-        <f>FLOOR(D41,1)</f>
-        <v>175</v>
-      </c>
-      <c r="E42" s="24">
-        <f>FLOOR(E41,1)</f>
-        <v>0</v>
-      </c>
-      <c r="F42" s="24">
-        <f>FLOOR(F41,1)</f>
-        <v>295</v>
+        <v>34</v>
+      </c>
+      <c r="B42" s="20"/>
+      <c r="C42" s="23">
+        <f>C38*$B$36</f>
+        <v>790.84318455971049</v>
+      </c>
+      <c r="D42" s="23">
+        <f>D38*$B$36</f>
+        <v>175.82750301568154</v>
+      </c>
+      <c r="E42" s="23">
+        <f>E38*$B$36</f>
+        <v>0</v>
+      </c>
+      <c r="F42" s="23">
+        <f>F38*$B$36</f>
+        <v>295.32931242460796</v>
       </c>
       <c r="G42" s="17" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="H42" s="24" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="B43" s="15">
-        <f>SUM(C42:F42)</f>
-        <v>1260</v>
-      </c>
-      <c r="C43" s="25"/>
-      <c r="D43" s="24"/>
-      <c r="E43" s="24"/>
-      <c r="F43" s="24"/>
+        <v>35</v>
+      </c>
+      <c r="B43" s="15"/>
+      <c r="C43" s="24">
+        <f>FLOOR(C42,1)</f>
+        <v>790</v>
+      </c>
+      <c r="D43" s="24">
+        <f>FLOOR(D42,1)</f>
+        <v>175</v>
+      </c>
+      <c r="E43" s="24">
+        <f>FLOOR(E42,1)</f>
+        <v>0</v>
+      </c>
+      <c r="F43" s="24">
+        <f>FLOOR(F42,1)</f>
+        <v>295</v>
+      </c>
       <c r="G43" s="17" t="s">
         <v>14</v>
       </c>
       <c r="H43" s="24" t="s">
-        <v>138</v>
+        <v>36</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="B44" s="96">
-        <f>SUM(C41:F41)-B43</f>
-        <v>2</v>
-      </c>
-      <c r="C44" s="94"/>
-      <c r="D44" s="94"/>
-      <c r="E44" s="94"/>
-      <c r="F44" s="94"/>
-      <c r="G44" s="95" t="s">
-        <v>8</v>
-      </c>
-      <c r="H44" s="94" t="s">
-        <v>43</v>
+        <v>137</v>
+      </c>
+      <c r="B44" s="15">
+        <f>SUM(C43:F43)</f>
+        <v>1260</v>
+      </c>
+      <c r="C44" s="25"/>
+      <c r="D44" s="24"/>
+      <c r="E44" s="24"/>
+      <c r="F44" s="24"/>
+      <c r="G44" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="H44" s="24" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B45" s="30">
-        <f>ROUND(B44,)</f>
+        <v>150</v>
+      </c>
+      <c r="B45" s="93">
+        <f>SUM(C42:F42)-B44</f>
         <v>2</v>
       </c>
-      <c r="C45" s="24"/>
-      <c r="D45" s="24"/>
-      <c r="E45" s="24"/>
-      <c r="F45" s="24"/>
-      <c r="G45" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="H45" s="24" t="s">
+      <c r="C45" s="91"/>
+      <c r="D45" s="91"/>
+      <c r="E45" s="91"/>
+      <c r="F45" s="91"/>
+      <c r="G45" s="92" t="s">
+        <v>8</v>
+      </c>
+      <c r="H45" s="91" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B46" s="15">
-        <f>B43+B45</f>
-        <v>1262</v>
-      </c>
-      <c r="C46" s="25"/>
+        <v>42</v>
+      </c>
+      <c r="B46" s="30">
+        <f>ROUND(B45,)</f>
+        <v>2</v>
+      </c>
+      <c r="C46" s="24"/>
       <c r="D46" s="24"/>
       <c r="E46" s="24"/>
       <c r="F46" s="24"/>
@@ -2170,16 +2177,16 @@
         <v>14</v>
       </c>
       <c r="H46" s="24" t="s">
-        <v>139</v>
+        <v>43</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>126</v>
+        <v>44</v>
       </c>
       <c r="B47" s="15">
-        <f>B46*260</f>
-        <v>328120</v>
+        <f>B44+B46</f>
+        <v>1262</v>
       </c>
       <c r="C47" s="25"/>
       <c r="D47" s="24"/>
@@ -2189,335 +2196,354 @@
         <v>14</v>
       </c>
       <c r="H47" s="24" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B48" s="15"/>
-      <c r="C48" s="23">
-        <f>C41-TRUNC(C41)</f>
-        <v>0.84318455971049389</v>
-      </c>
-      <c r="D48" s="23">
-        <f>D41-TRUNC(D41)</f>
-        <v>0.82750301568154327</v>
-      </c>
-      <c r="E48" s="23">
-        <f>E41-TRUNC(E41)</f>
-        <v>0</v>
-      </c>
-      <c r="F48" s="23">
-        <f>F41-TRUNC(F41)</f>
-        <v>0.32931242460796284</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="B48" s="15">
+        <f>B47*260</f>
+        <v>328120</v>
+      </c>
+      <c r="C48" s="25"/>
+      <c r="D48" s="24"/>
+      <c r="E48" s="24"/>
+      <c r="F48" s="24"/>
       <c r="G48" s="17" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="H48" s="24" t="s">
-        <v>38</v>
+        <v>140</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B49" s="15"/>
+      <c r="C49" s="23">
+        <f>C42-TRUNC(C42)</f>
+        <v>0.84318455971049389</v>
+      </c>
+      <c r="D49" s="23">
+        <f>D42-TRUNC(D42)</f>
+        <v>0.82750301568154327</v>
+      </c>
+      <c r="E49" s="23">
+        <f>E42-TRUNC(E42)</f>
+        <v>0</v>
+      </c>
+      <c r="F49" s="23">
+        <f>F42-TRUNC(F42)</f>
+        <v>0.32931242460796284</v>
+      </c>
+      <c r="G49" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="H49" s="24" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B49" s="15"/>
-      <c r="C49" s="25">
-        <f>IF($B$45&gt;0,IF(LARGE($C$48:$F$48,$B$45)&lt;=C$48,1,0), 0)</f>
+      <c r="B50" s="15"/>
+      <c r="C50" s="25">
+        <f>IF($B$46&gt;0,IF(LARGE($C$49:$F$49,$B$46)&lt;=C$49,1,0), 0)</f>
         <v>1</v>
       </c>
-      <c r="D49" s="25">
-        <f>IF($B$45&gt;0,IF(LARGE($C$48:$F$48,$B$45)&lt;=D$48,1,0), 0)</f>
+      <c r="D50" s="25">
+        <f>IF($B$46&gt;0,IF(LARGE($C$49:$F$49,$B$46)&lt;=D$49,1,0), 0)</f>
         <v>1</v>
       </c>
-      <c r="E49" s="25">
-        <f>IF($B$45&gt;0,IF(LARGE($C$48:$F$48,$B$45)&lt;=E$48,1,0), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="F49" s="25">
-        <f>IF($B$45&gt;0,IF(LARGE($C$48:$F$48,$B$45)&lt;=F$48,1,0), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="G49" s="17" t="s">
+      <c r="E50" s="25">
+        <f>IF($B$46&gt;0,IF(LARGE($C$49:$F$49,$B$46)&lt;=E$49,1,0), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="F50" s="25">
+        <f>IF($B$46&gt;0,IF(LARGE($C$49:$F$49,$B$46)&lt;=F$49,1,0), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="G50" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="H49" s="24" t="s">
+      <c r="H50" s="24" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A50" s="26" t="s">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A51" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="B50" s="27"/>
-      <c r="C50" s="28">
-        <f>C42+C49</f>
+      <c r="B51" s="27"/>
+      <c r="C51" s="28">
+        <f>C43+C50</f>
         <v>791</v>
       </c>
-      <c r="D50" s="28">
-        <f>D42+D49</f>
+      <c r="D51" s="28">
+        <f>D43+D50</f>
         <v>176</v>
       </c>
-      <c r="E50" s="28">
-        <f>E42+E49</f>
-        <v>0</v>
-      </c>
-      <c r="F50" s="28">
-        <f>F42+F49</f>
+      <c r="E51" s="28">
+        <f>E43+E50</f>
+        <v>0</v>
+      </c>
+      <c r="F51" s="28">
+        <f>F43+F50</f>
         <v>295</v>
       </c>
-      <c r="G50" s="29" t="s">
+      <c r="G51" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="H50" s="26" t="s">
+      <c r="H51" s="26" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A51" s="1"/>
-      <c r="B51" s="86"/>
-      <c r="C51" s="23"/>
-      <c r="D51" s="23"/>
-      <c r="E51" s="23"/>
-      <c r="F51" s="23"/>
-      <c r="G51" s="17"/>
-      <c r="H51" s="24"/>
-    </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A52" s="1" t="s">
+      <c r="A52" s="1"/>
+      <c r="B52" s="85"/>
+      <c r="C52" s="23"/>
+      <c r="D52" s="23"/>
+      <c r="E52" s="23"/>
+      <c r="F52" s="23"/>
+      <c r="G52" s="17"/>
+      <c r="H52" s="24"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B52" s="33">
-        <f>ROUND((B33-B47)/260,)</f>
-        <v>0</v>
-      </c>
-      <c r="C52" s="15"/>
-      <c r="D52" s="15"/>
-      <c r="E52" s="15"/>
-      <c r="F52" s="15"/>
-      <c r="G52" s="17" t="s">
+      <c r="B53" s="33">
+        <f>ROUND((B34-B48)/260,)</f>
+        <v>0</v>
+      </c>
+      <c r="C53" s="15"/>
+      <c r="D53" s="15"/>
+      <c r="E53" s="15"/>
+      <c r="F53" s="15"/>
+      <c r="G53" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="H52" s="24" t="s">
+      <c r="H53" s="24" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A53" s="79" t="s">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A54" s="78" t="s">
         <v>141</v>
       </c>
-      <c r="B53" s="85">
-        <f>IF(B30 &gt; 0, MIN(1,B52/B30), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="C53" s="81"/>
-      <c r="D53" s="80"/>
-      <c r="E53" s="80"/>
-      <c r="F53" s="80"/>
-      <c r="G53" s="82" t="s">
+      <c r="B54" s="84">
+        <f>IF(B31 &gt; 0, MIN(1,B53/B31), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="C54" s="80"/>
+      <c r="D54" s="79"/>
+      <c r="E54" s="79"/>
+      <c r="F54" s="79"/>
+      <c r="G54" s="81" t="s">
         <v>8</v>
       </c>
-      <c r="H53" s="80"/>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A54" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B54" s="31"/>
-      <c r="C54" s="16">
-        <f>C38*$B$53</f>
-        <v>0</v>
-      </c>
-      <c r="D54" s="16">
-        <f>D38*$B$53</f>
-        <v>0</v>
-      </c>
-      <c r="E54" s="16">
-        <f>E38*$B$53</f>
-        <v>0</v>
-      </c>
-      <c r="F54" s="16">
-        <f>F38*$B$53</f>
-        <v>0</v>
-      </c>
-      <c r="G54" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="H54" s="24" t="s">
-        <v>46</v>
-      </c>
+      <c r="H54" s="79"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B55" s="24"/>
-      <c r="C55" s="32">
-        <f>FLOOR(C54, 1)</f>
-        <v>0</v>
-      </c>
-      <c r="D55" s="32">
-        <f>FLOOR(D54, 1)</f>
-        <v>0</v>
-      </c>
-      <c r="E55" s="32">
-        <f>FLOOR(E54, 1)</f>
-        <v>0</v>
-      </c>
-      <c r="F55" s="32">
-        <f>FLOOR(F54, 1)</f>
+        <v>45</v>
+      </c>
+      <c r="B55" s="31"/>
+      <c r="C55" s="16">
+        <f>C39*$B$54</f>
+        <v>0</v>
+      </c>
+      <c r="D55" s="16">
+        <f>D39*$B$54</f>
+        <v>0</v>
+      </c>
+      <c r="E55" s="16">
+        <f>E39*$B$54</f>
+        <v>0</v>
+      </c>
+      <c r="F55" s="16">
+        <f>F39*$B$54</f>
         <v>0</v>
       </c>
       <c r="G55" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="H55" s="24"/>
+        <v>8</v>
+      </c>
+      <c r="H55" s="24" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B56" s="36">
-        <f>B52-SUM(C55:F55)</f>
-        <v>0</v>
-      </c>
-      <c r="C56" s="24"/>
-      <c r="D56" s="24"/>
-      <c r="E56" s="24"/>
-      <c r="F56" s="24"/>
+        <v>47</v>
+      </c>
+      <c r="B56" s="24"/>
+      <c r="C56" s="32">
+        <f>FLOOR(C55, 1)</f>
+        <v>0</v>
+      </c>
+      <c r="D56" s="32">
+        <f>FLOOR(D55, 1)</f>
+        <v>0</v>
+      </c>
+      <c r="E56" s="32">
+        <f>FLOOR(E55, 1)</f>
+        <v>0</v>
+      </c>
+      <c r="F56" s="32">
+        <f>FLOOR(F55, 1)</f>
+        <v>0</v>
+      </c>
       <c r="G56" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="H56" s="24" t="s">
-        <v>52</v>
-      </c>
+      <c r="H56" s="24"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B57" s="33"/>
-      <c r="C57" s="23">
-        <f>C54-TRUNC(C55)</f>
-        <v>0</v>
-      </c>
-      <c r="D57" s="23">
-        <f>D54-TRUNC(D55)</f>
-        <v>0</v>
-      </c>
-      <c r="E57" s="23">
-        <f>E54-TRUNC(E55)</f>
-        <v>0</v>
-      </c>
-      <c r="F57" s="23">
-        <f>F54-TRUNC(F55)</f>
-        <v>0</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="B57" s="36">
+        <f>B53-SUM(C56:F56)</f>
+        <v>0</v>
+      </c>
+      <c r="C57" s="24"/>
+      <c r="D57" s="24"/>
+      <c r="E57" s="24"/>
+      <c r="F57" s="24"/>
       <c r="G57" s="17" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="H57" s="24" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B58" s="33"/>
+      <c r="C58" s="23">
+        <f>C55-TRUNC(C56)</f>
+        <v>0</v>
+      </c>
+      <c r="D58" s="23">
+        <f>D55-TRUNC(D56)</f>
+        <v>0</v>
+      </c>
+      <c r="E58" s="23">
+        <f>E55-TRUNC(E56)</f>
+        <v>0</v>
+      </c>
+      <c r="F58" s="23">
+        <f>F55-TRUNC(F56)</f>
+        <v>0</v>
+      </c>
+      <c r="G58" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="H58" s="24" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A59" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B58" s="33"/>
-      <c r="C58" s="25">
-        <f>IF($B$56&gt;0, IF(LARGE($C$57:$F$57,$B$56)&lt;=C$57,1,0), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="D58" s="25">
-        <f>IF($B$56&gt;0, IF(LARGE($C$57:$F$57,$B$56)&lt;=D$57,1,0), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="E58" s="25">
-        <f>IF($B$56&gt;0, IF(LARGE($C$57:$F$57,$B$56)&lt;=E$57,1,0), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="F58" s="25">
-        <f>IF($B$56&gt;0, IF(LARGE($C$57:$F$57,$B$56)&lt;=F$57,1,0), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="G58" s="17" t="s">
+      <c r="B59" s="33"/>
+      <c r="C59" s="25">
+        <f>IF($B$57&gt;0, IF(LARGE($C$58:$F$58,$B$57)&lt;=C$58,1,0), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="D59" s="25">
+        <f>IF($B$57&gt;0, IF(LARGE($C$58:$F$58,$B$57)&lt;=D$58,1,0), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="E59" s="25">
+        <f>IF($B$57&gt;0, IF(LARGE($C$58:$F$58,$B$57)&lt;=E$58,1,0), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="F59" s="25">
+        <f>IF($B$57&gt;0, IF(LARGE($C$58:$F$58,$B$57)&lt;=F$58,1,0), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="G59" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="H58" s="24"/>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A59" s="26" t="s">
+      <c r="H59" s="24"/>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A60" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="B59" s="34"/>
-      <c r="C59" s="28">
-        <f>C55+C58</f>
-        <v>0</v>
-      </c>
-      <c r="D59" s="28">
-        <f>D55+D58</f>
-        <v>0</v>
-      </c>
-      <c r="E59" s="28">
-        <f>E55+E58</f>
-        <v>0</v>
-      </c>
-      <c r="F59" s="28">
-        <f>F55+F58</f>
-        <v>0</v>
-      </c>
-      <c r="G59" s="29" t="s">
+      <c r="B60" s="34"/>
+      <c r="C60" s="28">
+        <f>C56+C59</f>
+        <v>0</v>
+      </c>
+      <c r="D60" s="28">
+        <f>D56+D59</f>
+        <v>0</v>
+      </c>
+      <c r="E60" s="28">
+        <f>E56+E59</f>
+        <v>0</v>
+      </c>
+      <c r="F60" s="28">
+        <f>F56+F59</f>
+        <v>0</v>
+      </c>
+      <c r="G60" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="H59" s="35"/>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A60" s="1"/>
-      <c r="B60" s="33"/>
-      <c r="C60" s="25"/>
-      <c r="D60" s="25"/>
-      <c r="E60" s="25"/>
-      <c r="F60" s="25"/>
-      <c r="G60" s="17"/>
-      <c r="H60" s="24"/>
+      <c r="H60" s="35"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" s="1"/>
       <c r="B61" s="33"/>
-      <c r="C61" s="24"/>
-      <c r="D61" s="24"/>
-      <c r="E61" s="24"/>
-      <c r="F61" s="24"/>
+      <c r="C61" s="25"/>
+      <c r="D61" s="25"/>
+      <c r="E61" s="25"/>
+      <c r="F61" s="25"/>
       <c r="G61" s="17"/>
       <c r="H61" s="24"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A62" s="26" t="s">
+      <c r="A62" s="1"/>
+      <c r="B62" s="33"/>
+      <c r="C62" s="24"/>
+      <c r="D62" s="24"/>
+      <c r="E62" s="24"/>
+      <c r="F62" s="24"/>
+      <c r="G62" s="17"/>
+      <c r="H62" s="24"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A63" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="B62" s="37">
-        <f>B46+B52</f>
+      <c r="B63" s="37">
+        <f>B47+B53</f>
         <v>1262</v>
       </c>
-      <c r="C62" s="35"/>
-      <c r="D62" s="35"/>
-      <c r="E62" s="35"/>
-      <c r="F62" s="35"/>
-      <c r="G62" s="38"/>
-      <c r="H62" s="35"/>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="H63" s="4"/>
+      <c r="C63" s="35"/>
+      <c r="D63" s="35"/>
+      <c r="E63" s="35"/>
+      <c r="F63" s="35"/>
+      <c r="G63" s="38"/>
+      <c r="H63" s="35"/>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H64" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <ignoredErrors>
-    <ignoredError sqref="B30 B24" formula="1"/>
+    <ignoredError sqref="B24" formula="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -3323,14 +3349,14 @@
       <c r="B34" s="56" t="s">
         <v>102</v>
       </c>
-      <c r="C34" s="92" t="str">
+      <c r="C34" s="99" t="str">
         <f>IF(SUM(D32:G33)&lt;=MAKSBELOP,"Everyone paid",IF(SUM(D32:G32)&lt;=MAKSBELOP,"Arbeidsgivere fully paid; Person partially paid by Person request", "Arbeidsgivere partial payment ratio by Arbeidsgiver request"))</f>
         <v>Arbeidsgivere partial payment ratio by Arbeidsgiver request</v>
       </c>
-      <c r="D34" s="92"/>
-      <c r="E34" s="92"/>
-      <c r="F34" s="92"/>
-      <c r="G34" s="92"/>
+      <c r="D34" s="99"/>
+      <c r="E34" s="99"/>
+      <c r="F34" s="99"/>
+      <c r="G34" s="99"/>
       <c r="H34" s="17"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
@@ -3430,12 +3456,12 @@
       <c r="D40" s="60"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A41" s="93" t="s">
+      <c r="A41" s="100" t="s">
         <v>105</v>
       </c>
-      <c r="B41" s="93"/>
-      <c r="C41" s="93"/>
-      <c r="D41" s="93"/>
+      <c r="B41" s="100"/>
+      <c r="C41" s="100"/>
+      <c r="D41" s="100"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="61" t="s">
@@ -4250,14 +4276,14 @@
       <c r="B34" s="56" t="s">
         <v>102</v>
       </c>
-      <c r="C34" s="92" t="str">
+      <c r="C34" s="99" t="str">
         <f>IF(SUM(D32:G33)&lt;=MAKSBELOP,"Everyone paid",IF(SUM(D32:G32)&lt;=MAKSBELOP,"Arbeidsgivere fully paid; Person partially paid by Person request", "Arbeidsgivere partial payment ratio by Arbeidsgiver request"))</f>
         <v>Arbeidsgivere partial payment ratio by Arbeidsgiver request</v>
       </c>
-      <c r="D34" s="92"/>
-      <c r="E34" s="92"/>
-      <c r="F34" s="92"/>
-      <c r="G34" s="92"/>
+      <c r="D34" s="99"/>
+      <c r="E34" s="99"/>
+      <c r="F34" s="99"/>
+      <c r="G34" s="99"/>
       <c r="H34" s="17"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
går tilbake på avrunding; ikke lengre runde av før gradering
Vi hadde ulik praksis i forhold til Infotrygd, og da må vi endre praksis tilbake.

Co-authored-by: Hege Haavaldsen <hege.haavaldsen@nav.no>
</commit_message>
<xml_diff>
--- a/doc/okonomi/Utbetaling.xlsx
+++ b/doc/okonomi/Utbetaling.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/david/dev/nav/helse-spleis/doc/okonomi/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59F3D9CD-72EE-7A47-82BC-291881548269}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C181A854-8498-814C-85F5-F53B923251CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="47620" windowHeight="41000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8200" yWindow="5940" windowWidth="52940" windowHeight="32740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Flere arbeidsgivere, ny " sheetId="1" r:id="rId1"/>
@@ -430,9 +430,6 @@
     <t>Dagsbeløpet (1/260) avrundet</t>
   </si>
   <si>
-    <t>Sykepengegrunnlaget begrenset til 6G. Redusert til dagsats (1/260), rundet av, så ganget opp igjen til årsinntekt</t>
-  </si>
-  <si>
     <t>Sykepengegrunnlaget begrenset til 6G som dagsats</t>
   </si>
   <si>
@@ -505,9 +502,6 @@
     <t>Det som skal betales per dag, totalt</t>
   </si>
   <si>
-    <t>Maks dagsats før reduksjon til 6G og reduksjon for total sykdomsgrad. Rundet av på dagsats etter gradering</t>
-  </si>
-  <si>
     <t>Maks dagsats redusert for arbeidsuførhetsgrad. Rundet av på dagsats etter gradering</t>
   </si>
   <si>
@@ -527,13 +521,19 @@
   </si>
   <si>
     <t>Utregnet refusjon før avrunding</t>
+  </si>
+  <si>
+    <t>Sykepengegrunnlaget begrenset til 6G.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maks dagsats før reduksjon til 6G og reduksjon for total sykdomsgrad. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="16">
+  <numFmts count="20">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* \-??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* \-??_);_(@_)"/>
@@ -550,6 +550,10 @@
     <numFmt numFmtId="176" formatCode="_-* #,##0.000000000_-;\-* #,##0.000000000_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="177" formatCode="_(* #,##0.00000_);_(* \(#,##0.00000\);_(* \-??_);_(@_)"/>
     <numFmt numFmtId="178" formatCode="0.0"/>
+    <numFmt numFmtId="183" formatCode="0.000000%"/>
+    <numFmt numFmtId="184" formatCode="0.0000000%"/>
+    <numFmt numFmtId="186" formatCode="_-* #,##0.0000000_-;\-* #,##0.0000000_-;_-* &quot;-&quot;???????_-;_-@_-"/>
+    <numFmt numFmtId="191" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -590,7 +594,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -630,6 +634,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -720,7 +730,7 @@
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -738,7 +748,6 @@
     <xf numFmtId="9" fontId="0" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="10" fontId="0" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -846,7 +855,6 @@
     <xf numFmtId="166" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -866,6 +874,18 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="183" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="184" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="184" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="173" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="191" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="186" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1252,15 +1272,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="31.1640625" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="4" width="15.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" customWidth="1"/>
+    <col min="4" max="4" width="24.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.1640625" customWidth="1"/>
     <col min="6" max="6" width="15.6640625" customWidth="1"/>
     <col min="8" max="8" width="107.6640625" customWidth="1"/>
@@ -1306,17 +1327,13 @@
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="7">
-        <v>45000</v>
+        <v>31000</v>
       </c>
       <c r="D3" s="7">
-        <v>5000</v>
-      </c>
-      <c r="E3" s="7">
-        <v>10000</v>
-      </c>
-      <c r="F3" s="7">
-        <v>35000</v>
-      </c>
+        <v>31000</v>
+      </c>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
       <c r="G3" s="5" t="s">
         <v>8</v>
       </c>
@@ -1329,19 +1346,19 @@
       <c r="B4" s="4"/>
       <c r="C4" s="8">
         <f>C3/SUM($C$3:$F$3)</f>
-        <v>0.47368421052631576</v>
+        <v>0.5</v>
       </c>
       <c r="D4" s="8">
         <f>D3/SUM($C$3:$F$3)</f>
-        <v>5.2631578947368418E-2</v>
+        <v>0.5</v>
       </c>
       <c r="E4" s="8">
         <f>E3/SUM($C$3:$F$3)</f>
-        <v>0.10526315789473684</v>
+        <v>0</v>
       </c>
       <c r="F4" s="8">
         <f>F3/SUM($C$3:$F$3)</f>
-        <v>0.36842105263157893</v>
+        <v>0</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>8</v>
@@ -1354,26 +1371,26 @@
       <c r="A5" t="s">
         <v>108</v>
       </c>
-      <c r="C5" s="39">
+      <c r="C5" s="38">
         <f>C3*12</f>
-        <v>540000</v>
-      </c>
-      <c r="D5" s="39">
+        <v>372000</v>
+      </c>
+      <c r="D5" s="38">
         <f t="shared" ref="D5:F5" si="0">D3*12</f>
-        <v>60000</v>
-      </c>
-      <c r="E5" s="39">
+        <v>372000</v>
+      </c>
+      <c r="E5" s="38">
         <f t="shared" si="0"/>
-        <v>120000</v>
-      </c>
-      <c r="F5" s="39">
+        <v>0</v>
+      </c>
+      <c r="F5" s="38">
         <f t="shared" si="0"/>
-        <v>420000</v>
-      </c>
-      <c r="G5" s="70" t="s">
+        <v>0</v>
+      </c>
+      <c r="G5" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="69" t="s">
+      <c r="H5" s="68" t="s">
         <v>110</v>
       </c>
     </row>
@@ -1382,21 +1399,21 @@
         <v>22</v>
       </c>
       <c r="B6" s="4"/>
-      <c r="C6" s="13">
+      <c r="C6" s="109">
         <f>C3*1</f>
-        <v>45000</v>
-      </c>
-      <c r="D6" s="13">
-        <f>D3</f>
-        <v>5000</v>
-      </c>
-      <c r="E6" s="13">
-        <f>E3</f>
-        <v>10000</v>
-      </c>
-      <c r="F6" s="13">
+        <v>31000</v>
+      </c>
+      <c r="D6" s="109">
+        <f>D3*1</f>
+        <v>31000</v>
+      </c>
+      <c r="E6" s="109">
+        <f>E3*0.25</f>
+        <v>0</v>
+      </c>
+      <c r="F6" s="109">
         <f>F3*0.3</f>
-        <v>10500</v>
+        <v>0</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>8</v>
@@ -1406,12 +1423,12 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="68" t="s">
-        <v>126</v>
-      </c>
-      <c r="B7" s="72">
+      <c r="A7" s="67" t="s">
+        <v>125</v>
+      </c>
+      <c r="B7" s="71">
         <f>SUM(C6:F6)*12</f>
-        <v>846000</v>
+        <v>744000</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -1420,16 +1437,16 @@
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="12">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D8" s="12">
         <v>1</v>
       </c>
       <c r="E8" s="12">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="F8" s="12">
-        <v>0.8</v>
+        <v>0.5</v>
       </c>
       <c r="G8" s="5" t="s">
         <v>8</v>
@@ -1439,14 +1456,14 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="68" t="s">
+      <c r="A9" s="67" t="s">
         <v>113</v>
       </c>
-      <c r="B9" s="71">
+      <c r="B9" s="70">
         <f>SUM(C5:F5)</f>
-        <v>1140000</v>
-      </c>
-      <c r="G9" s="70" t="s">
+        <v>744000</v>
+      </c>
+      <c r="G9" s="69" t="s">
         <v>8</v>
       </c>
       <c r="H9" t="s">
@@ -1468,17 +1485,17 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="68" t="s">
+      <c r="A11" s="67" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="39">
+      <c r="B11" s="38">
         <f>B10*6</f>
         <v>561804</v>
       </c>
-      <c r="G11" s="70" t="s">
+      <c r="G11" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="H11" s="75" t="s">
+      <c r="H11" s="74" t="s">
         <v>118</v>
       </c>
     </row>
@@ -1486,45 +1503,45 @@
       <c r="A12" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="B12" s="9">
+      <c r="B12" s="110">
         <f>ROUND(B11/260,)</f>
         <v>2161</v>
       </c>
-      <c r="G12" s="70" t="s">
+      <c r="G12" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="H12" s="75" t="s">
+      <c r="H12" s="74" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="68" t="s">
+      <c r="A13" s="67" t="s">
         <v>109</v>
       </c>
-      <c r="B13" s="39">
-        <f>ROUND(MIN(B9,B11)/260,)*260</f>
-        <v>561860</v>
-      </c>
-      <c r="G13" s="70" t="s">
+      <c r="B13" s="70">
+        <f>MIN(B9,B11)</f>
+        <v>561804</v>
+      </c>
+      <c r="G13" s="69" t="s">
+        <v>8</v>
+      </c>
+      <c r="H13" s="74" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="67" t="s">
+        <v>112</v>
+      </c>
+      <c r="B14" s="71">
+        <f>ROUND(B13/260,0)</f>
+        <v>2161</v>
+      </c>
+      <c r="G14" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="H13" s="75" t="s">
+      <c r="H14" s="74" t="s">
         <v>120</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="68" t="s">
-        <v>112</v>
-      </c>
-      <c r="B14" s="67">
-        <f>B13/260</f>
-        <v>2161</v>
-      </c>
-      <c r="G14" s="70" t="s">
-        <v>14</v>
-      </c>
-      <c r="H14" s="75" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
@@ -1534,19 +1551,19 @@
       <c r="B16" s="4"/>
       <c r="C16" s="9">
         <f>C5/260</f>
-        <v>2076.9230769230771</v>
+        <v>1430.7692307692307</v>
       </c>
       <c r="D16" s="9">
         <f>D5/260</f>
-        <v>230.76923076923077</v>
+        <v>1430.7692307692307</v>
       </c>
       <c r="E16" s="9">
         <f>E5/260</f>
-        <v>461.53846153846155</v>
+        <v>0</v>
       </c>
       <c r="F16" s="9">
         <f>F5/260</f>
-        <v>1615.3846153846155</v>
+        <v>0</v>
       </c>
       <c r="G16" s="5" t="s">
         <v>8</v>
@@ -1584,53 +1601,53 @@
         <v>16</v>
       </c>
       <c r="B18" s="4"/>
-      <c r="C18" s="96">
-        <f>ROUND(C16*C17,0)</f>
-        <v>2077</v>
-      </c>
-      <c r="D18" s="96">
-        <f t="shared" ref="D18:F18" si="1">ROUND(D16*D17,0)</f>
-        <v>231</v>
-      </c>
-      <c r="E18" s="96">
+      <c r="C18" s="110">
+        <f>C16*C17</f>
+        <v>1430.7692307692307</v>
+      </c>
+      <c r="D18" s="110">
+        <f t="shared" ref="D18:F18" si="1">D16*D17</f>
+        <v>1430.7692307692307</v>
+      </c>
+      <c r="E18" s="110">
         <f t="shared" si="1"/>
-        <v>462</v>
-      </c>
-      <c r="F18" s="96">
+        <v>0</v>
+      </c>
+      <c r="F18" s="94">
         <f t="shared" si="1"/>
-        <v>1615</v>
+        <v>0</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" s="73" t="s">
+      <c r="A19" s="72" t="s">
         <v>114</v>
       </c>
-      <c r="C19" s="74">
+      <c r="C19" s="73">
         <f>C8*C4</f>
-        <v>0.23684210526315788</v>
-      </c>
-      <c r="D19" s="74">
+        <v>0.5</v>
+      </c>
+      <c r="D19" s="73">
         <f>D8*D4</f>
-        <v>5.2631578947368418E-2</v>
-      </c>
-      <c r="E19" s="74">
+        <v>0.5</v>
+      </c>
+      <c r="E19" s="73">
         <f>E8*E4</f>
         <v>0</v>
       </c>
-      <c r="F19" s="74">
+      <c r="F19" s="73">
         <f>F8*F4</f>
-        <v>0.29473684210526313</v>
-      </c>
-      <c r="G19" s="70" t="s">
+        <v>0</v>
+      </c>
+      <c r="G19" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="H19" s="75" t="s">
+      <c r="H19" s="74" t="s">
         <v>116</v>
       </c>
     </row>
@@ -1639,103 +1656,103 @@
         <v>20</v>
       </c>
       <c r="B20" s="4"/>
-      <c r="C20" s="96">
+      <c r="C20" s="94">
         <f>ROUND(C18*C8,0)</f>
-        <v>1039</v>
-      </c>
-      <c r="D20" s="96">
+        <v>1431</v>
+      </c>
+      <c r="D20" s="94">
         <f t="shared" ref="D20:F20" si="2">ROUND(D18*D8,0)</f>
-        <v>231</v>
-      </c>
-      <c r="E20" s="96">
+        <v>1431</v>
+      </c>
+      <c r="E20" s="94">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F20" s="96">
+      <c r="F20" s="94">
         <f t="shared" si="2"/>
-        <v>1292</v>
+        <v>0</v>
       </c>
       <c r="G20" s="5" t="s">
         <v>14</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" s="73" t="s">
+      <c r="A21" s="72" t="s">
+        <v>141</v>
+      </c>
+      <c r="C21" s="95">
+        <f>ROUND(C6*12/260*C8,0)</f>
+        <v>1431</v>
+      </c>
+      <c r="D21" s="95">
+        <f t="shared" ref="D21:F21" si="3">ROUND(D6*12/260*D8,0)</f>
+        <v>1431</v>
+      </c>
+      <c r="E21" s="95">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F21" s="95">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G21" s="69" t="s">
+        <v>14</v>
+      </c>
+      <c r="H21" s="74" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="72" t="s">
+        <v>129</v>
+      </c>
+      <c r="B22" s="71">
+        <f>SUM(C20:F20)</f>
+        <v>2862</v>
+      </c>
+      <c r="G22" s="69" t="s">
+        <v>8</v>
+      </c>
+      <c r="H22" s="74" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="72" t="s">
+        <v>125</v>
+      </c>
+      <c r="B23" s="71">
+        <f>B22*260</f>
+        <v>744120</v>
+      </c>
+      <c r="G23" s="69" t="s">
+        <v>8</v>
+      </c>
+      <c r="H23" s="74" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="72" t="s">
         <v>142</v>
       </c>
-      <c r="C21" s="97">
-        <f>ROUND(ROUND(C6*12/260,0)*C8,0)</f>
-        <v>1039</v>
-      </c>
-      <c r="D21" s="97">
-        <f t="shared" ref="D21:F21" si="3">ROUND(ROUND(D6*12/260,0)*D8,0)</f>
-        <v>231</v>
-      </c>
-      <c r="E21" s="97">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="F21" s="97">
-        <f t="shared" si="3"/>
-        <v>388</v>
-      </c>
-      <c r="G21" s="70" t="s">
-        <v>14</v>
-      </c>
-      <c r="H21" s="75" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" s="73" t="s">
-        <v>130</v>
-      </c>
-      <c r="B22" s="72">
-        <f>SUM(C20:F20)</f>
-        <v>2562</v>
-      </c>
-      <c r="G22" s="70" t="s">
-        <v>8</v>
-      </c>
-      <c r="H22" s="75" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" s="73" t="s">
-        <v>126</v>
-      </c>
-      <c r="B23" s="72">
-        <f>B22*260</f>
-        <v>666120</v>
-      </c>
-      <c r="G23" s="70" t="s">
-        <v>8</v>
-      </c>
-      <c r="H23" s="75" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" s="73" t="s">
-        <v>143</v>
-      </c>
-      <c r="B24" s="72">
+      <c r="B24" s="71">
         <f>SUM(C21:F21)</f>
-        <v>1658</v>
-      </c>
-      <c r="C24" s="67"/>
+        <v>2862</v>
+      </c>
+      <c r="C24" s="66"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" s="73" t="s">
-        <v>126</v>
-      </c>
-      <c r="B25" s="72">
+      <c r="A25" s="72" t="s">
+        <v>125</v>
+      </c>
+      <c r="B25" s="71">
         <f>B24*260</f>
-        <v>431080</v>
+        <v>744120</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
@@ -1743,21 +1760,21 @@
         <v>22</v>
       </c>
       <c r="B26" s="4"/>
-      <c r="C26" s="98">
+      <c r="C26" s="96">
         <f>MIN(C20,C21)</f>
-        <v>1039</v>
-      </c>
-      <c r="D26" s="98">
+        <v>1431</v>
+      </c>
+      <c r="D26" s="96">
         <f t="shared" ref="D26:F26" si="4">MIN(D20,D21)</f>
-        <v>231</v>
-      </c>
-      <c r="E26" s="98">
+        <v>1431</v>
+      </c>
+      <c r="E26" s="96">
+        <f>MIN(E20,E21)</f>
+        <v>0</v>
+      </c>
+      <c r="F26" s="96">
         <f t="shared" si="4"/>
         <v>0</v>
-      </c>
-      <c r="F26" s="98">
-        <f t="shared" si="4"/>
-        <v>388</v>
       </c>
       <c r="G26" s="5" t="s">
         <v>14</v>
@@ -1767,138 +1784,165 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" s="73" t="s">
-        <v>148</v>
-      </c>
-      <c r="C27" s="94">
+      <c r="A27" s="72" t="s">
+        <v>146</v>
+      </c>
+      <c r="C27" s="103">
         <f>C26/$B$24</f>
-        <v>0.62665862484921597</v>
-      </c>
-      <c r="D27" s="94">
+        <v>0.5</v>
+      </c>
+      <c r="D27" s="99">
         <f t="shared" ref="D27:F27" si="5">D26/$B$24</f>
-        <v>0.13932448733413752</v>
-      </c>
-      <c r="E27" s="94">
+        <v>0.5</v>
+      </c>
+      <c r="E27" s="100">
+        <f>E26/$B$24</f>
+        <v>0</v>
+      </c>
+      <c r="F27" s="92">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="F27" s="94">
-        <f t="shared" si="5"/>
-        <v>0.23401688781664656</v>
-      </c>
-      <c r="G27" s="70" t="s">
+      <c r="G27" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="H27" s="75" t="s">
+      <c r="H27" s="74" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="72" t="s">
+        <v>150</v>
+      </c>
+      <c r="C28" s="102">
+        <f>$B$35*C27</f>
+        <v>1080.5</v>
+      </c>
+      <c r="D28" s="66">
+        <f>$B$35*D27</f>
+        <v>1080.5</v>
+      </c>
+      <c r="E28" s="66">
+        <f>$B$35*E27</f>
+        <v>0</v>
+      </c>
+      <c r="F28" s="66">
+        <f>$B$35*F27</f>
+        <v>0</v>
+      </c>
+      <c r="H28" s="74" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" s="73" t="s">
-        <v>152</v>
-      </c>
-      <c r="C28" s="67">
-        <f>$B$35*C27</f>
-        <v>790.84318455971061</v>
-      </c>
-      <c r="D28" s="67">
-        <f>$B$35*D27</f>
-        <v>175.82750301568154</v>
-      </c>
-      <c r="E28" s="67">
-        <f>$B$35*E27</f>
-        <v>0</v>
-      </c>
-      <c r="F28" s="67">
-        <f>$B$35*F27</f>
-        <v>295.32931242460796</v>
-      </c>
-      <c r="H28" s="75" t="s">
-        <v>151</v>
-      </c>
-    </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" s="73" t="s">
-        <v>123</v>
-      </c>
-      <c r="B29" s="95">
+      <c r="A29" s="72" t="s">
+        <v>122</v>
+      </c>
+      <c r="B29" s="93">
         <f>SUM(C26:F26)</f>
-        <v>1658</v>
-      </c>
-      <c r="C29" s="90"/>
-      <c r="D29" s="90"/>
-      <c r="E29" s="90"/>
-      <c r="F29" s="90"/>
-      <c r="G29" s="70" t="s">
+        <v>2862</v>
+      </c>
+      <c r="C29" s="107">
+        <f>1/C27</f>
+        <v>2</v>
+      </c>
+      <c r="D29" s="88"/>
+      <c r="E29" s="88"/>
+      <c r="F29" s="88"/>
+      <c r="G29" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="H29" s="75" t="s">
-        <v>128</v>
+      <c r="H29" s="74" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A30" s="73" t="s">
+      <c r="A30" s="72" t="s">
+        <v>125</v>
+      </c>
+      <c r="B30" s="71">
+        <f>B29*260</f>
+        <v>744120</v>
+      </c>
+      <c r="C30" s="66">
+        <f>FLOOR(C27*$D$36,1)</f>
+        <v>500</v>
+      </c>
+      <c r="D30" s="66">
+        <f t="shared" ref="D30:F30" si="6">FLOOR(D27*$D$36,1)</f>
+        <v>500</v>
+      </c>
+      <c r="E30" s="66">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F30" s="66">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="G30" s="69" t="s">
+        <v>8</v>
+      </c>
+      <c r="H30" s="74" t="s">
         <v>126</v>
       </c>
-      <c r="B30" s="72">
-        <f>B29*260</f>
-        <v>431080</v>
-      </c>
-      <c r="C30" s="67"/>
-      <c r="D30" s="67"/>
-      <c r="E30" s="67"/>
-      <c r="F30" s="67"/>
-      <c r="G30" s="70" t="s">
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="72" t="s">
+        <v>131</v>
+      </c>
+      <c r="B31" s="66">
+        <f>B22-B29</f>
+        <v>0</v>
+      </c>
+      <c r="C31" s="106"/>
+      <c r="D31" s="81">
+        <f>(B35*D36)/FLOOR((1/C27*D36),1)</f>
+        <v>1080.5</v>
+      </c>
+      <c r="F31" s="101"/>
+      <c r="G31" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="H30" s="75" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A31" s="73" t="s">
+      <c r="H31" s="74" t="s">
         <v>132</v>
       </c>
-      <c r="B31" s="67">
-        <f>B22-B29</f>
-        <v>904</v>
-      </c>
-      <c r="D31" s="82"/>
-      <c r="E31" s="83"/>
-      <c r="G31" s="70" t="s">
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="72" t="s">
+        <v>125</v>
+      </c>
+      <c r="B32" s="71">
+        <f>B31*260</f>
+        <v>0</v>
+      </c>
+      <c r="C32" s="82">
+        <f>1/(FLOOR(C28,1)/B35)</f>
+        <v>2.0009259259259258</v>
+      </c>
+      <c r="D32" s="81"/>
+      <c r="G32" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="H31" s="75" t="s">
+      <c r="H32" s="74" t="s">
         <v>133</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A32" s="73" t="s">
-        <v>126</v>
-      </c>
-      <c r="B32" s="72">
-        <f>B31*260</f>
-        <v>235040</v>
-      </c>
-      <c r="G32" s="70" t="s">
-        <v>8</v>
-      </c>
-      <c r="H32" s="75" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B33" s="14">
+      <c r="B33" s="13">
         <f>SUM(C19:F19)</f>
-        <v>0.58421052631578951</v>
-      </c>
-      <c r="C33" s="88"/>
-      <c r="D33" s="89"/>
-      <c r="E33" s="89"/>
-      <c r="F33" s="4"/>
+        <v>1</v>
+      </c>
+      <c r="C33" s="86"/>
+      <c r="D33" s="108">
+        <f>1*D36-SUM(C30:F30)</f>
+        <v>0</v>
+      </c>
+      <c r="E33" s="87"/>
+      <c r="F33" s="85"/>
       <c r="G33" s="5" t="s">
         <v>8</v>
       </c>
@@ -1907,82 +1951,88 @@
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A34" s="73" t="s">
+      <c r="A34" s="72" t="s">
         <v>117</v>
       </c>
-      <c r="B34" s="76">
+      <c r="B34" s="75">
         <f>ROUND(B13*B33/260,)*260</f>
-        <v>328120</v>
-      </c>
-      <c r="C34" s="86"/>
-      <c r="D34" s="82"/>
-      <c r="E34" s="4"/>
+        <v>561860</v>
+      </c>
+      <c r="C34" s="85"/>
+      <c r="D34" s="81">
+        <f>B35*D33/100</f>
+        <v>0</v>
+      </c>
+      <c r="E34" s="85"/>
       <c r="F34" s="4"/>
-      <c r="G34" s="70" t="s">
+      <c r="G34" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="H34" s="75" t="s">
-        <v>122</v>
+      <c r="H34" s="74" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A35" s="73" t="s">
+      <c r="A35" s="72" t="s">
         <v>112</v>
       </c>
-      <c r="B35" s="82">
+      <c r="B35" s="104">
         <f>B34/260</f>
-        <v>1262</v>
-      </c>
-      <c r="C35" s="82"/>
-      <c r="D35" s="87"/>
-      <c r="G35" s="70" t="s">
+        <v>2161</v>
+      </c>
+      <c r="C35" s="81"/>
+      <c r="D35" s="105"/>
+      <c r="G35" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="H35" s="75" t="s">
-        <v>144</v>
+      <c r="H35" s="74" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A36" s="73" t="s">
+      <c r="A36" s="72" t="s">
+        <v>123</v>
+      </c>
+      <c r="B36" s="81">
+        <f>B34/MAX(B34,B30)</f>
+        <v>0.75506638714185881</v>
+      </c>
+      <c r="D36" s="101">
+        <f>1000</f>
+        <v>1000</v>
+      </c>
+      <c r="G36" s="69" t="s">
+        <v>8</v>
+      </c>
+      <c r="H36" s="74" t="s">
         <v>124</v>
-      </c>
-      <c r="B36" s="82">
-        <f>B34/MAX(B34,B30)</f>
-        <v>0.76115802171290714</v>
-      </c>
-      <c r="D36" s="82"/>
-      <c r="G36" s="70" t="s">
-        <v>8</v>
-      </c>
-      <c r="H36" s="75" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B37" s="15"/>
-      <c r="C37" s="16">
+      <c r="B37" s="14"/>
+      <c r="C37" s="15">
         <f>C20</f>
-        <v>1039</v>
-      </c>
-      <c r="D37" s="16">
+        <v>1431</v>
+      </c>
+      <c r="D37" s="15">
         <f>D20</f>
-        <v>231</v>
-      </c>
-      <c r="E37" s="16">
+        <v>1431</v>
+      </c>
+      <c r="E37" s="15">
         <f>E20</f>
         <v>0</v>
       </c>
-      <c r="F37" s="16">
+      <c r="F37" s="15">
         <f>F20</f>
-        <v>1292</v>
-      </c>
-      <c r="G37" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="G37" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="H37" s="24" t="s">
+      <c r="H37" s="23" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1990,27 +2040,27 @@
       <c r="A38" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B38" s="15"/>
-      <c r="C38" s="16">
+      <c r="B38" s="14"/>
+      <c r="C38" s="15">
         <f>C26</f>
-        <v>1039</v>
-      </c>
-      <c r="D38" s="16">
+        <v>1431</v>
+      </c>
+      <c r="D38" s="15">
         <f>D26</f>
-        <v>231</v>
-      </c>
-      <c r="E38" s="16">
+        <v>1431</v>
+      </c>
+      <c r="E38" s="15">
         <f>E26</f>
         <v>0</v>
       </c>
-      <c r="F38" s="16">
+      <c r="F38" s="15">
         <f>F26</f>
-        <v>388</v>
-      </c>
-      <c r="G38" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="G38" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="H38" s="24" t="s">
+      <c r="H38" s="23" t="s">
         <v>31</v>
       </c>
     </row>
@@ -2018,80 +2068,80 @@
       <c r="A39" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B39" s="15"/>
-      <c r="C39" s="16">
+      <c r="B39" s="14"/>
+      <c r="C39" s="15">
         <f>C37-C38</f>
         <v>0</v>
       </c>
-      <c r="D39" s="16">
+      <c r="D39" s="15">
         <f>D37-D38</f>
         <v>0</v>
       </c>
-      <c r="E39" s="16">
+      <c r="E39" s="15">
         <f>E37-E38</f>
         <v>0</v>
       </c>
-      <c r="F39" s="16">
+      <c r="F39" s="15">
         <f>F37-F38</f>
-        <v>904</v>
-      </c>
-      <c r="G39" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="G39" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="H39" s="24" t="s">
-        <v>136</v>
+      <c r="H39" s="23" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B40" s="19" t="str">
+      <c r="B40" s="18" t="str">
         <f>IF(B32&lt;=B34,"Arbeidsgiver og person blir refundert hele beløpet",IF(B30&lt;=B34,"Arbeidsgivere blir refundert hele beløpet; Person blir delvis refundert", "Arbeidsgivere blir delvis refundert"))</f>
         <v>Arbeidsgiver og person blir refundert hele beløpet</v>
       </c>
-      <c r="C40" s="19"/>
-      <c r="D40" s="19"/>
-      <c r="E40" s="19"/>
-      <c r="F40" s="19"/>
-      <c r="G40" s="17"/>
-      <c r="H40" s="24"/>
+      <c r="C40" s="18"/>
+      <c r="D40" s="18"/>
+      <c r="E40" s="18"/>
+      <c r="F40" s="18"/>
+      <c r="G40" s="16"/>
+      <c r="H40" s="23"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="1"/>
-      <c r="B41" s="20"/>
-      <c r="C41" s="77"/>
-      <c r="D41" s="21"/>
-      <c r="E41" s="21"/>
-      <c r="F41" s="22"/>
-      <c r="G41" s="17"/>
-      <c r="H41" s="24"/>
+      <c r="B41" s="19"/>
+      <c r="C41" s="76"/>
+      <c r="D41" s="20"/>
+      <c r="E41" s="20"/>
+      <c r="F41" s="21"/>
+      <c r="G41" s="16"/>
+      <c r="H41" s="23"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B42" s="20"/>
-      <c r="C42" s="23">
+      <c r="B42" s="19"/>
+      <c r="C42" s="22">
         <f>C38*$B$36</f>
-        <v>790.84318455971049</v>
-      </c>
-      <c r="D42" s="23">
+        <v>1080.5</v>
+      </c>
+      <c r="D42" s="22">
         <f>D38*$B$36</f>
-        <v>175.82750301568154</v>
-      </c>
-      <c r="E42" s="23">
+        <v>1080.5</v>
+      </c>
+      <c r="E42" s="22">
         <f>E38*$B$36</f>
         <v>0</v>
       </c>
-      <c r="F42" s="23">
+      <c r="F42" s="22">
         <f>F38*$B$36</f>
-        <v>295.32931242460796</v>
-      </c>
-      <c r="G42" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="G42" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="H42" s="24" t="s">
+      <c r="H42" s="23" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2099,65 +2149,65 @@
       <c r="A43" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B43" s="15"/>
-      <c r="C43" s="24">
+      <c r="B43" s="14"/>
+      <c r="C43" s="23">
         <f>FLOOR(C42,1)</f>
-        <v>790</v>
-      </c>
-      <c r="D43" s="24">
+        <v>1080</v>
+      </c>
+      <c r="D43" s="23">
         <f>FLOOR(D42,1)</f>
-        <v>175</v>
-      </c>
-      <c r="E43" s="24">
+        <v>1080</v>
+      </c>
+      <c r="E43" s="23">
         <f>FLOOR(E42,1)</f>
         <v>0</v>
       </c>
-      <c r="F43" s="24">
+      <c r="F43" s="23">
         <f>FLOOR(F42,1)</f>
-        <v>295</v>
-      </c>
-      <c r="G43" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="G43" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="H43" s="24" t="s">
+      <c r="H43" s="23" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B44" s="14">
+        <f>SUM(C43:F43)</f>
+        <v>2160</v>
+      </c>
+      <c r="C44" s="24"/>
+      <c r="D44" s="23"/>
+      <c r="E44" s="23"/>
+      <c r="F44" s="23"/>
+      <c r="G44" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="H44" s="23" t="s">
         <v>137</v>
-      </c>
-      <c r="B44" s="15">
-        <f>SUM(C43:F43)</f>
-        <v>1260</v>
-      </c>
-      <c r="C44" s="25"/>
-      <c r="D44" s="24"/>
-      <c r="E44" s="24"/>
-      <c r="F44" s="24"/>
-      <c r="G44" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="H44" s="24" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="B45" s="93">
+        <v>148</v>
+      </c>
+      <c r="B45" s="91">
         <f>SUM(C42:F42)-B44</f>
-        <v>2</v>
-      </c>
-      <c r="C45" s="91"/>
-      <c r="D45" s="91"/>
-      <c r="E45" s="91"/>
-      <c r="F45" s="91"/>
-      <c r="G45" s="92" t="s">
+        <v>1</v>
+      </c>
+      <c r="C45" s="89"/>
+      <c r="D45" s="89"/>
+      <c r="E45" s="89"/>
+      <c r="F45" s="89"/>
+      <c r="G45" s="90" t="s">
         <v>8</v>
       </c>
-      <c r="H45" s="91" t="s">
+      <c r="H45" s="89" t="s">
         <v>43</v>
       </c>
     </row>
@@ -2165,18 +2215,18 @@
       <c r="A46" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B46" s="30">
+      <c r="B46" s="29">
         <f>ROUND(B45,)</f>
-        <v>2</v>
-      </c>
-      <c r="C46" s="24"/>
-      <c r="D46" s="24"/>
-      <c r="E46" s="24"/>
-      <c r="F46" s="24"/>
-      <c r="G46" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C46" s="23"/>
+      <c r="D46" s="23"/>
+      <c r="E46" s="23"/>
+      <c r="F46" s="23"/>
+      <c r="G46" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="H46" s="24" t="s">
+      <c r="H46" s="23" t="s">
         <v>43</v>
       </c>
     </row>
@@ -2184,65 +2234,65 @@
       <c r="A47" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B47" s="15">
+      <c r="B47" s="14">
         <f>B44+B46</f>
-        <v>1262</v>
-      </c>
-      <c r="C47" s="25"/>
-      <c r="D47" s="24"/>
-      <c r="E47" s="24"/>
-      <c r="F47" s="24"/>
-      <c r="G47" s="17" t="s">
+        <v>2161</v>
+      </c>
+      <c r="C47" s="24"/>
+      <c r="D47" s="23"/>
+      <c r="E47" s="23"/>
+      <c r="F47" s="23"/>
+      <c r="G47" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="H47" s="24" t="s">
-        <v>139</v>
+      <c r="H47" s="23" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="B48" s="15">
+        <v>125</v>
+      </c>
+      <c r="B48" s="14">
         <f>B47*260</f>
-        <v>328120</v>
-      </c>
-      <c r="C48" s="25"/>
-      <c r="D48" s="24"/>
-      <c r="E48" s="24"/>
-      <c r="F48" s="24"/>
-      <c r="G48" s="17" t="s">
+        <v>561860</v>
+      </c>
+      <c r="C48" s="24"/>
+      <c r="D48" s="23"/>
+      <c r="E48" s="23"/>
+      <c r="F48" s="23"/>
+      <c r="G48" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="H48" s="24" t="s">
-        <v>140</v>
+      <c r="H48" s="23" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B49" s="15"/>
-      <c r="C49" s="23">
+      <c r="B49" s="14"/>
+      <c r="C49" s="22">
         <f>C42-TRUNC(C42)</f>
-        <v>0.84318455971049389</v>
-      </c>
-      <c r="D49" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="D49" s="22">
         <f>D42-TRUNC(D42)</f>
-        <v>0.82750301568154327</v>
-      </c>
-      <c r="E49" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="E49" s="22">
         <f>E42-TRUNC(E42)</f>
         <v>0</v>
       </c>
-      <c r="F49" s="23">
+      <c r="F49" s="22">
         <f>F42-TRUNC(F42)</f>
-        <v>0.32931242460796284</v>
-      </c>
-      <c r="G49" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="G49" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="H49" s="24" t="s">
+      <c r="H49" s="23" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2250,129 +2300,129 @@
       <c r="A50" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B50" s="15"/>
-      <c r="C50" s="25">
+      <c r="B50" s="14"/>
+      <c r="C50" s="24">
         <f>IF($B$46&gt;0,IF(LARGE($C$49:$F$49,$B$46)&lt;=C$49,1,0), 0)</f>
         <v>1</v>
       </c>
-      <c r="D50" s="25">
-        <f>IF($B$46&gt;0,IF(LARGE($C$49:$F$49,$B$46)&lt;=D$49,1,0), 0)</f>
-        <v>1</v>
-      </c>
-      <c r="E50" s="25">
-        <f>IF($B$46&gt;0,IF(LARGE($C$49:$F$49,$B$46)&lt;=E$49,1,0), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="F50" s="25">
-        <f>IF($B$46&gt;0,IF(LARGE($C$49:$F$49,$B$46)&lt;=F$49,1,0), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="G50" s="17" t="s">
+      <c r="D50" s="24">
+        <f>IF(($B$46-C50)&gt;0,IF(LARGE($C$49:$F$49,$B$46)&lt;=D$49,1,0), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="E50" s="24">
+        <f>IF(($B$46-SUM($C$50:$D$50))&gt;0,IF(LARGE($C$49:$F$49,$B$46)&lt;=E$49,1,0), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="F50" s="24">
+        <f>IF(($B$46-SUM($C$50:$D$51))&gt;0,IF(LARGE($C$49:$F$49,$B$46)&lt;=F$49,1,0), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="G50" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="H50" s="24" t="s">
+      <c r="H50" s="23" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A51" s="26" t="s">
+      <c r="A51" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="B51" s="27"/>
-      <c r="C51" s="28">
+      <c r="B51" s="26"/>
+      <c r="C51" s="27">
         <f>C43+C50</f>
-        <v>791</v>
-      </c>
-      <c r="D51" s="28">
+        <v>1081</v>
+      </c>
+      <c r="D51" s="27">
         <f>D43+D50</f>
-        <v>176</v>
-      </c>
-      <c r="E51" s="28">
+        <v>1080</v>
+      </c>
+      <c r="E51" s="27">
         <f>E43+E50</f>
         <v>0</v>
       </c>
-      <c r="F51" s="28">
+      <c r="F51" s="27">
         <f>F43+F50</f>
-        <v>295</v>
-      </c>
-      <c r="G51" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="G51" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="H51" s="26" t="s">
-        <v>135</v>
+      <c r="H51" s="25" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="1"/>
-      <c r="B52" s="85"/>
-      <c r="C52" s="23"/>
-      <c r="D52" s="23"/>
-      <c r="E52" s="23"/>
-      <c r="F52" s="23"/>
-      <c r="G52" s="17"/>
-      <c r="H52" s="24"/>
+      <c r="B52" s="84"/>
+      <c r="C52" s="22"/>
+      <c r="D52" s="22"/>
+      <c r="E52" s="22"/>
+      <c r="F52" s="22"/>
+      <c r="G52" s="16"/>
+      <c r="H52" s="23"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B53" s="33">
+      <c r="B53" s="32">
         <f>ROUND((B34-B48)/260,)</f>
         <v>0</v>
       </c>
-      <c r="C53" s="15"/>
-      <c r="D53" s="15"/>
-      <c r="E53" s="15"/>
-      <c r="F53" s="15"/>
-      <c r="G53" s="17" t="s">
+      <c r="C53" s="14"/>
+      <c r="D53" s="14"/>
+      <c r="E53" s="14"/>
+      <c r="F53" s="14"/>
+      <c r="G53" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="H53" s="24" t="s">
+      <c r="H53" s="23" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A54" s="78" t="s">
-        <v>141</v>
-      </c>
-      <c r="B54" s="84">
+      <c r="A54" s="77" t="s">
+        <v>140</v>
+      </c>
+      <c r="B54" s="83">
         <f>IF(B31 &gt; 0, MIN(1,B53/B31), 0)</f>
         <v>0</v>
       </c>
-      <c r="C54" s="80"/>
-      <c r="D54" s="79"/>
-      <c r="E54" s="79"/>
-      <c r="F54" s="79"/>
-      <c r="G54" s="81" t="s">
+      <c r="C54" s="79"/>
+      <c r="D54" s="78"/>
+      <c r="E54" s="78"/>
+      <c r="F54" s="78"/>
+      <c r="G54" s="80" t="s">
         <v>8</v>
       </c>
-      <c r="H54" s="79"/>
+      <c r="H54" s="78"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B55" s="31"/>
-      <c r="C55" s="16">
+      <c r="B55" s="30"/>
+      <c r="C55" s="15">
         <f>C39*$B$54</f>
         <v>0</v>
       </c>
-      <c r="D55" s="16">
+      <c r="D55" s="15">
         <f>D39*$B$54</f>
         <v>0</v>
       </c>
-      <c r="E55" s="16">
+      <c r="E55" s="15">
         <f>E39*$B$54</f>
         <v>0</v>
       </c>
-      <c r="F55" s="16">
+      <c r="F55" s="15">
         <f>F39*$B$54</f>
         <v>0</v>
       </c>
-      <c r="G55" s="17" t="s">
+      <c r="G55" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="H55" s="24" t="s">
+      <c r="H55" s="23" t="s">
         <v>46</v>
       </c>
     </row>
@@ -2380,44 +2430,44 @@
       <c r="A56" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B56" s="24"/>
-      <c r="C56" s="32">
+      <c r="B56" s="23"/>
+      <c r="C56" s="31">
         <f>FLOOR(C55, 1)</f>
         <v>0</v>
       </c>
-      <c r="D56" s="32">
+      <c r="D56" s="31">
         <f>FLOOR(D55, 1)</f>
         <v>0</v>
       </c>
-      <c r="E56" s="32">
+      <c r="E56" s="31">
         <f>FLOOR(E55, 1)</f>
         <v>0</v>
       </c>
-      <c r="F56" s="32">
+      <c r="F56" s="31">
         <f>FLOOR(F55, 1)</f>
         <v>0</v>
       </c>
-      <c r="G56" s="17" t="s">
+      <c r="G56" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="H56" s="24"/>
+      <c r="H56" s="23"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B57" s="36">
+      <c r="B57" s="35">
         <f>B53-SUM(C56:F56)</f>
         <v>0</v>
       </c>
-      <c r="C57" s="24"/>
-      <c r="D57" s="24"/>
-      <c r="E57" s="24"/>
-      <c r="F57" s="24"/>
-      <c r="G57" s="17" t="s">
+      <c r="C57" s="23"/>
+      <c r="D57" s="23"/>
+      <c r="E57" s="23"/>
+      <c r="F57" s="23"/>
+      <c r="G57" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="H57" s="24" t="s">
+      <c r="H57" s="23" t="s">
         <v>52</v>
       </c>
     </row>
@@ -2425,27 +2475,27 @@
       <c r="A58" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B58" s="33"/>
-      <c r="C58" s="23">
+      <c r="B58" s="32"/>
+      <c r="C58" s="22">
         <f>C55-TRUNC(C56)</f>
         <v>0</v>
       </c>
-      <c r="D58" s="23">
+      <c r="D58" s="22">
         <f>D55-TRUNC(D56)</f>
         <v>0</v>
       </c>
-      <c r="E58" s="23">
+      <c r="E58" s="22">
         <f>E55-TRUNC(E56)</f>
         <v>0</v>
       </c>
-      <c r="F58" s="23">
+      <c r="F58" s="22">
         <f>F55-TRUNC(F56)</f>
         <v>0</v>
       </c>
-      <c r="G58" s="17" t="s">
+      <c r="G58" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="H58" s="24" t="s">
+      <c r="H58" s="23" t="s">
         <v>48</v>
       </c>
     </row>
@@ -2453,88 +2503,88 @@
       <c r="A59" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B59" s="33"/>
-      <c r="C59" s="25">
+      <c r="B59" s="32"/>
+      <c r="C59" s="24">
         <f>IF($B$57&gt;0, IF(LARGE($C$58:$F$58,$B$57)&lt;=C$58,1,0), 0)</f>
         <v>0</v>
       </c>
-      <c r="D59" s="25">
+      <c r="D59" s="24">
         <f>IF($B$57&gt;0, IF(LARGE($C$58:$F$58,$B$57)&lt;=D$58,1,0), 0)</f>
         <v>0</v>
       </c>
-      <c r="E59" s="25">
+      <c r="E59" s="24">
         <f>IF($B$57&gt;0, IF(LARGE($C$58:$F$58,$B$57)&lt;=E$58,1,0), 0)</f>
         <v>0</v>
       </c>
-      <c r="F59" s="25">
+      <c r="F59" s="24">
         <f>IF($B$57&gt;0, IF(LARGE($C$58:$F$58,$B$57)&lt;=F$58,1,0), 0)</f>
         <v>0</v>
       </c>
-      <c r="G59" s="17" t="s">
+      <c r="G59" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="H59" s="24"/>
+      <c r="H59" s="23"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A60" s="26" t="s">
+      <c r="A60" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="B60" s="34"/>
-      <c r="C60" s="28">
+      <c r="B60" s="33"/>
+      <c r="C60" s="27">
         <f>C56+C59</f>
         <v>0</v>
       </c>
-      <c r="D60" s="28">
+      <c r="D60" s="27">
         <f>D56+D59</f>
         <v>0</v>
       </c>
-      <c r="E60" s="28">
+      <c r="E60" s="27">
         <f>E56+E59</f>
         <v>0</v>
       </c>
-      <c r="F60" s="28">
+      <c r="F60" s="27">
         <f>F56+F59</f>
         <v>0</v>
       </c>
-      <c r="G60" s="29" t="s">
+      <c r="G60" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="H60" s="35"/>
+      <c r="H60" s="34"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" s="1"/>
-      <c r="B61" s="33"/>
-      <c r="C61" s="25"/>
-      <c r="D61" s="25"/>
-      <c r="E61" s="25"/>
-      <c r="F61" s="25"/>
-      <c r="G61" s="17"/>
-      <c r="H61" s="24"/>
+      <c r="B61" s="32"/>
+      <c r="C61" s="24"/>
+      <c r="D61" s="24"/>
+      <c r="E61" s="24"/>
+      <c r="F61" s="24"/>
+      <c r="G61" s="16"/>
+      <c r="H61" s="23"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" s="1"/>
-      <c r="B62" s="33"/>
-      <c r="C62" s="24"/>
-      <c r="D62" s="24"/>
-      <c r="E62" s="24"/>
-      <c r="F62" s="24"/>
-      <c r="G62" s="17"/>
-      <c r="H62" s="24"/>
+      <c r="B62" s="32"/>
+      <c r="C62" s="23"/>
+      <c r="D62" s="23"/>
+      <c r="E62" s="23"/>
+      <c r="F62" s="23"/>
+      <c r="G62" s="16"/>
+      <c r="H62" s="23"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A63" s="26" t="s">
+      <c r="A63" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="B63" s="37">
+      <c r="B63" s="36">
         <f>B47+B53</f>
-        <v>1262</v>
-      </c>
-      <c r="C63" s="35"/>
-      <c r="D63" s="35"/>
-      <c r="E63" s="35"/>
-      <c r="F63" s="35"/>
-      <c r="G63" s="38"/>
-      <c r="H63" s="35"/>
+        <v>2161</v>
+      </c>
+      <c r="C63" s="34"/>
+      <c r="D63" s="34"/>
+      <c r="E63" s="34"/>
+      <c r="F63" s="34"/>
+      <c r="G63" s="37"/>
+      <c r="H63" s="34"/>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="H64" s="4"/>
@@ -2566,41 +2616,41 @@
     <col min="5" max="5" width="16.33203125" customWidth="1"/>
     <col min="6" max="6" width="17.33203125" customWidth="1"/>
     <col min="7" max="7" width="15.6640625" customWidth="1"/>
-    <col min="8" max="8" width="8.6640625" style="40" customWidth="1"/>
+    <col min="8" max="8" width="8.6640625" style="39" customWidth="1"/>
     <col min="9" max="9" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="43" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="41" t="s">
+    <row r="1" spans="1:9" s="42" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="40" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="41" t="s">
+      <c r="C1" s="40" t="s">
         <v>58</v>
       </c>
-      <c r="D1" s="42" t="s">
+      <c r="D1" s="41" t="s">
         <v>59</v>
       </c>
-      <c r="E1" s="42" t="s">
+      <c r="E1" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="F1" s="42" t="s">
+      <c r="F1" s="41" t="s">
         <v>61</v>
       </c>
-      <c r="G1" s="42" t="s">
+      <c r="G1" s="41" t="s">
         <v>62</v>
       </c>
-      <c r="H1" s="42" t="s">
+      <c r="H1" s="41" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="43"/>
+      <c r="A2" s="42"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="42" t="s">
         <v>7</v>
       </c>
       <c r="B3" t="s">
@@ -2618,12 +2668,12 @@
       <c r="G3" s="7">
         <v>0</v>
       </c>
-      <c r="H3" s="40" t="s">
+      <c r="H3" s="39" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="43"/>
+      <c r="A4" s="42"/>
       <c r="B4" t="s">
         <v>66</v>
       </c>
@@ -2643,42 +2693,42 @@
         <f>G3/SUM($D$3:$G$3)</f>
         <v>0</v>
       </c>
-      <c r="H4" s="40" t="s">
+      <c r="H4" s="39" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="43" t="s">
+      <c r="A5" s="42" t="s">
         <v>11</v>
       </c>
       <c r="B5" t="s">
         <v>67</v>
       </c>
-      <c r="D5" s="44">
+      <c r="D5" s="43">
         <f>D3*12/260</f>
         <v>969.23076923076928</v>
       </c>
-      <c r="E5" s="44">
+      <c r="E5" s="43">
         <f>E3*12/260</f>
         <v>461.53846153846155</v>
       </c>
-      <c r="F5" s="44">
+      <c r="F5" s="43">
         <f>F3*12/260</f>
         <v>1430.7692307692307</v>
       </c>
-      <c r="G5" s="44">
+      <c r="G5" s="43">
         <f>G3*12/260</f>
         <v>0</v>
       </c>
-      <c r="H5" s="40" t="s">
+      <c r="H5" s="39" t="s">
         <v>65</v>
       </c>
-      <c r="I5" s="45" t="s">
+      <c r="I5" s="44" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="43" t="s">
+      <c r="A6" s="42" t="s">
         <v>13</v>
       </c>
       <c r="B6" t="s">
@@ -2696,42 +2746,42 @@
       <c r="G6" s="10">
         <v>1</v>
       </c>
-      <c r="H6" s="40" t="s">
+      <c r="H6" s="39" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="43" t="s">
+      <c r="A7" s="42" t="s">
         <v>16</v>
       </c>
       <c r="B7" t="s">
         <v>71</v>
       </c>
-      <c r="D7" s="44">
+      <c r="D7" s="43">
         <f>D5*D6</f>
         <v>969.23076923076928</v>
       </c>
-      <c r="E7" s="44">
+      <c r="E7" s="43">
         <f>E5*E6</f>
         <v>461.53846153846155</v>
       </c>
-      <c r="F7" s="44">
+      <c r="F7" s="43">
         <f>F5*F6</f>
         <v>1430.7692307692307</v>
       </c>
-      <c r="G7" s="44">
+      <c r="G7" s="43">
         <f>G5*G6</f>
         <v>0</v>
       </c>
-      <c r="H7" s="40" t="s">
+      <c r="H7" s="39" t="s">
         <v>65</v>
       </c>
-      <c r="I7" s="46" t="s">
+      <c r="I7" s="45" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="43" t="s">
+      <c r="A8" s="42" t="s">
         <v>17</v>
       </c>
       <c r="B8" t="s">
@@ -2753,15 +2803,15 @@
         <f>MIN(G7,$C$15)</f>
         <v>0</v>
       </c>
-      <c r="H8" s="40" t="s">
+      <c r="H8" s="39" t="s">
         <v>70</v>
       </c>
-      <c r="I8" s="45" t="s">
+      <c r="I8" s="44" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="43" t="s">
+      <c r="A9" s="42" t="s">
         <v>18</v>
       </c>
       <c r="B9" t="s">
@@ -2779,39 +2829,39 @@
       <c r="G9" s="12">
         <v>1</v>
       </c>
-      <c r="H9" s="40" t="s">
+      <c r="H9" s="39" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="43" t="s">
+      <c r="A10" s="42" t="s">
         <v>20</v>
       </c>
       <c r="B10" t="s">
         <v>75</v>
       </c>
-      <c r="D10" s="44">
+      <c r="D10" s="43">
         <f>D7*D9</f>
         <v>484.61538461538464</v>
       </c>
-      <c r="E10" s="44">
+      <c r="E10" s="43">
         <f>E7*E9</f>
         <v>369.23076923076928</v>
       </c>
-      <c r="F10" s="44">
+      <c r="F10" s="43">
         <f>F7*F9</f>
         <v>286.15384615384613</v>
       </c>
-      <c r="G10" s="44">
+      <c r="G10" s="43">
         <f>G7*G9</f>
         <v>0</v>
       </c>
-      <c r="H10" s="40" t="s">
+      <c r="H10" s="39" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="43" t="s">
+      <c r="A11" s="42" t="s">
         <v>21</v>
       </c>
       <c r="B11" t="s">
@@ -2829,54 +2879,54 @@
       <c r="G11" s="10">
         <v>1</v>
       </c>
-      <c r="H11" s="40" t="s">
+      <c r="H11" s="39" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="43" t="s">
+      <c r="A12" s="42" t="s">
         <v>22</v>
       </c>
       <c r="B12" t="s">
         <v>77</v>
       </c>
-      <c r="D12" s="47">
+      <c r="D12" s="46">
         <f>D10*D11</f>
         <v>484.61538461538464</v>
       </c>
-      <c r="E12" s="47">
+      <c r="E12" s="46">
         <f>E10*E11</f>
         <v>332.30769230769238</v>
       </c>
-      <c r="F12" s="47">
+      <c r="F12" s="46">
         <f>F10*F11</f>
         <v>71.538461538461533</v>
       </c>
-      <c r="G12" s="47">
+      <c r="G12" s="46">
         <f>G10*G11</f>
         <v>0</v>
       </c>
-      <c r="H12" s="40" t="s">
+      <c r="H12" s="39" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="43" t="s">
+      <c r="A13" s="42" t="s">
         <v>23</v>
       </c>
       <c r="B13" t="s">
         <v>78</v>
       </c>
-      <c r="C13" s="48">
+      <c r="C13" s="47">
         <f>ROUND(SUM(D10:G10)/SUM(D7:G7),2)</f>
         <v>0.4</v>
       </c>
-      <c r="H13" s="40" t="s">
+      <c r="H13" s="39" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="43" t="s">
+      <c r="A14" s="42" t="s">
         <v>25</v>
       </c>
       <c r="B14" t="s">
@@ -2885,12 +2935,12 @@
       <c r="C14" s="7">
         <v>93634</v>
       </c>
-      <c r="H14" s="40" t="s">
+      <c r="H14" s="39" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="43" t="s">
+      <c r="A15" s="42" t="s">
         <v>27</v>
       </c>
       <c r="B15" t="s">
@@ -2900,15 +2950,15 @@
         <f>ROUND(6*C14/260, 0)</f>
         <v>2161</v>
       </c>
-      <c r="H15" s="40" t="s">
+      <c r="H15" s="39" t="s">
         <v>70</v>
       </c>
-      <c r="I15" s="45" t="s">
+      <c r="I15" s="44" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="43" t="s">
+      <c r="A16" s="42" t="s">
         <v>28</v>
       </c>
       <c r="B16" t="s">
@@ -2918,373 +2968,373 @@
         <f>ROUND(C13*C15,0)</f>
         <v>864</v>
       </c>
-      <c r="H16" s="40" t="s">
+      <c r="H16" s="39" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="49" t="s">
+      <c r="A17" s="48" t="s">
         <v>82</v>
       </c>
-      <c r="B17" s="50" t="s">
+      <c r="B17" s="49" t="s">
         <v>83</v>
       </c>
-      <c r="C17" s="51">
+      <c r="C17" s="50">
         <f>MIN(1, C16/SUM(D10:G10))</f>
         <v>0.75789473684210529</v>
       </c>
-      <c r="D17" s="52"/>
-      <c r="E17" s="52"/>
-      <c r="F17" s="52"/>
-      <c r="G17" s="52"/>
-      <c r="H17" s="53" t="s">
+      <c r="D17" s="51"/>
+      <c r="E17" s="51"/>
+      <c r="F17" s="51"/>
+      <c r="G17" s="51"/>
+      <c r="H17" s="52" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="49" t="s">
+      <c r="A18" s="48" t="s">
         <v>84</v>
       </c>
-      <c r="B18" s="50" t="s">
+      <c r="B18" s="49" t="s">
         <v>85</v>
       </c>
-      <c r="C18" s="50"/>
-      <c r="D18" s="52">
+      <c r="C18" s="49"/>
+      <c r="D18" s="51">
         <f>D10*ScalingFactor</f>
         <v>367.28744939271257</v>
       </c>
-      <c r="E18" s="52">
+      <c r="E18" s="51">
         <f>E10*ScalingFactor</f>
         <v>279.83805668016197</v>
       </c>
-      <c r="F18" s="52">
+      <c r="F18" s="51">
         <f>F10*ScalingFactor</f>
         <v>216.87449392712549</v>
       </c>
-      <c r="G18" s="52">
+      <c r="G18" s="51">
         <f>G10*ScalingFactor</f>
         <v>0</v>
       </c>
-      <c r="H18" s="53" t="s">
+      <c r="H18" s="52" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="49" t="s">
+      <c r="A19" s="48" t="s">
         <v>86</v>
       </c>
-      <c r="B19" s="50" t="s">
+      <c r="B19" s="49" t="s">
         <v>87</v>
       </c>
-      <c r="C19" s="50"/>
-      <c r="D19" s="52">
+      <c r="C19" s="49"/>
+      <c r="D19" s="51">
         <f>MIN(D18,D12)</f>
         <v>367.28744939271257</v>
       </c>
-      <c r="E19" s="52">
+      <c r="E19" s="51">
         <f>MIN(E18,E12)</f>
         <v>279.83805668016197</v>
       </c>
-      <c r="F19" s="52">
+      <c r="F19" s="51">
         <f>MIN(F18,F12)</f>
         <v>71.538461538461533</v>
       </c>
-      <c r="G19" s="52">
+      <c r="G19" s="51">
         <f>MIN(G18,G12)</f>
         <v>0</v>
       </c>
-      <c r="H19" s="53" t="s">
+      <c r="H19" s="52" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="49"/>
-      <c r="B20" s="50" t="s">
+      <c r="A20" s="48"/>
+      <c r="B20" s="49" t="s">
         <v>88</v>
       </c>
-      <c r="C20" s="50"/>
-      <c r="D20" s="52">
+      <c r="C20" s="49"/>
+      <c r="D20" s="51">
         <f>D19-D12</f>
         <v>-117.32793522267207</v>
       </c>
-      <c r="E20" s="52">
+      <c r="E20" s="51">
         <f>E19-E12</f>
         <v>-52.469635627530408</v>
       </c>
-      <c r="F20" s="52">
+      <c r="F20" s="51">
         <f>F19-F12</f>
         <v>0</v>
       </c>
-      <c r="G20" s="52">
+      <c r="G20" s="51">
         <f>G19-G12</f>
         <v>0</v>
       </c>
-      <c r="H20" s="53" t="s">
+      <c r="H20" s="52" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="49"/>
-      <c r="B21" s="50" t="s">
+      <c r="A21" s="48"/>
+      <c r="B21" s="49" t="s">
         <v>89</v>
       </c>
-      <c r="C21" s="50"/>
-      <c r="D21" s="51">
+      <c r="C21" s="49"/>
+      <c r="D21" s="50">
         <f>IF(D20 &lt; 0, D4, 0)</f>
         <v>0.33870967741935482</v>
       </c>
-      <c r="E21" s="51">
+      <c r="E21" s="50">
         <f>IF(E20 &lt; 0, E4, 0)</f>
         <v>0.16129032258064516</v>
       </c>
-      <c r="F21" s="51">
+      <c r="F21" s="50">
         <f>IF(F20 &lt; 0, F4, 0)</f>
         <v>0</v>
       </c>
-      <c r="G21" s="52"/>
-      <c r="H21" s="53" t="s">
+      <c r="G21" s="51"/>
+      <c r="H21" s="52" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="22" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="49" t="s">
+      <c r="A22" s="48" t="s">
         <v>90</v>
       </c>
-      <c r="B22" s="50" t="s">
+      <c r="B22" s="49" t="s">
         <v>91</v>
       </c>
-      <c r="C22" s="50"/>
-      <c r="D22" s="51">
+      <c r="C22" s="49"/>
+      <c r="D22" s="50">
         <f>IF(SUM(ShortfallIncomeRatioArb)=0,0,D21/SUM(ShortfallIncomeRatioArb))</f>
         <v>0.67741935483870963</v>
       </c>
-      <c r="E22" s="51">
+      <c r="E22" s="50">
         <f>IF(SUM(ShortfallIncomeRatioArb)=0,0,E21/SUM(ShortfallIncomeRatioArb))</f>
         <v>0.32258064516129031</v>
       </c>
-      <c r="F22" s="51">
+      <c r="F22" s="50">
         <f>IF(SUM(ShortfallIncomeRatioArb)=0,0,F21/SUM(ShortfallIncomeRatioArb))</f>
         <v>0</v>
       </c>
-      <c r="G22" s="51">
+      <c r="G22" s="50">
         <f>IF(SUM(ShortfallIncomeRatioArb)=0,0,G21/SUM(ShortfallIncomeRatioArb))</f>
         <v>0</v>
       </c>
-      <c r="H22" s="53" t="s">
+      <c r="H22" s="52" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="23" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="49"/>
-      <c r="B23" s="50" t="s">
+      <c r="A23" s="48"/>
+      <c r="B23" s="49" t="s">
         <v>92</v>
       </c>
-      <c r="C23" s="50"/>
-      <c r="D23" s="52">
+      <c r="C23" s="49"/>
+      <c r="D23" s="51">
         <f>D18-D19</f>
         <v>0</v>
       </c>
-      <c r="E23" s="52">
+      <c r="E23" s="51">
         <f>E18-E19</f>
         <v>0</v>
       </c>
-      <c r="F23" s="52">
+      <c r="F23" s="51">
         <f>F18-F19</f>
         <v>145.33603238866397</v>
       </c>
-      <c r="G23" s="52">
+      <c r="G23" s="51">
         <f>G18-G19</f>
         <v>0</v>
       </c>
-      <c r="H23" s="53" t="s">
+      <c r="H23" s="52" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="49" t="s">
+      <c r="A24" s="48" t="s">
         <v>93</v>
       </c>
-      <c r="B24" s="50" t="s">
+      <c r="B24" s="49" t="s">
         <v>94</v>
       </c>
-      <c r="C24" s="50"/>
-      <c r="D24" s="52">
+      <c r="C24" s="49"/>
+      <c r="D24" s="51">
         <f>MIN(-D20,IF(SUM($D$20:$G$20)&gt;=0, 0, SUM($D$23:$G$23)*D22))</f>
         <v>98.453441295546554</v>
       </c>
-      <c r="E24" s="52">
+      <c r="E24" s="51">
         <f>MIN(-E20,IF(SUM($D$20:$G$20)&gt;=0, 0, SUM($D$23:$G$23)*E22))</f>
         <v>46.882591093117405</v>
       </c>
-      <c r="F24" s="52">
+      <c r="F24" s="51">
         <f>MIN(-F20,IF(SUM($D$20:$G$20)&gt;=0, 0, SUM($D$23:$G$23)*F22))</f>
         <v>0</v>
       </c>
-      <c r="G24" s="52">
+      <c r="G24" s="51">
         <f>MIN(-G20,IF(SUM($D$20:$G$20)&gt;=0, 0, SUM($D$23:$G$23)*G22))</f>
         <v>0</v>
       </c>
-      <c r="H24" s="53" t="s">
+      <c r="H24" s="52" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="25" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="49"/>
-      <c r="B25" s="50" t="s">
+      <c r="A25" s="48"/>
+      <c r="B25" s="49" t="s">
         <v>95</v>
       </c>
-      <c r="C25" s="50"/>
-      <c r="D25" s="51">
+      <c r="C25" s="49"/>
+      <c r="D25" s="50">
         <f>IF(D23 = 0, 0, D4)</f>
         <v>0</v>
       </c>
-      <c r="E25" s="51">
+      <c r="E25" s="50">
         <f>IF(E23 = 0, 0, E4)</f>
         <v>0</v>
       </c>
-      <c r="F25" s="51">
+      <c r="F25" s="50">
         <f>IF(F23 = 0, 0, F4)</f>
         <v>0.5</v>
       </c>
-      <c r="G25" s="51">
+      <c r="G25" s="50">
         <f>IF(G23 = 0, 0, G4)</f>
         <v>0</v>
       </c>
-      <c r="H25" s="53" t="s">
+      <c r="H25" s="52" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="26" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="49"/>
-      <c r="B26" s="50" t="s">
+      <c r="A26" s="48"/>
+      <c r="B26" s="49" t="s">
         <v>96</v>
       </c>
-      <c r="C26" s="50"/>
-      <c r="D26" s="51">
+      <c r="C26" s="49"/>
+      <c r="D26" s="50">
         <f>IF(SUM(ShortfallIncomeRatioPerson)= 0, 0, D25/SUM(ShortfallIncomeRatioPerson))</f>
         <v>0</v>
       </c>
-      <c r="E26" s="51">
+      <c r="E26" s="50">
         <f>IF(SUM(ShortfallIncomeRatioPerson)= 0, 0, E25/SUM(ShortfallIncomeRatioPerson))</f>
         <v>0</v>
       </c>
-      <c r="F26" s="51">
+      <c r="F26" s="50">
         <f>IF(SUM(ShortfallIncomeRatioPerson)= 0, 0, F25/SUM(ShortfallIncomeRatioPerson))</f>
         <v>1</v>
       </c>
-      <c r="G26" s="51">
+      <c r="G26" s="50">
         <f>IF(SUM(ShortfallIncomeRatioPerson)= 0, 0, G25/SUM(ShortfallIncomeRatioPerson))</f>
         <v>0</v>
       </c>
-      <c r="H26" s="53" t="s">
+      <c r="H26" s="52" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="27" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="49" t="s">
+      <c r="A27" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="B27" s="50" t="s">
+      <c r="B27" s="49" t="s">
         <v>97</v>
       </c>
-      <c r="C27" s="50"/>
-      <c r="D27" s="54">
+      <c r="C27" s="49"/>
+      <c r="D27" s="53">
         <f>ROUND(D19+D24,0)</f>
         <v>466</v>
       </c>
-      <c r="E27" s="54">
+      <c r="E27" s="53">
         <f>ROUND(E19+E24,0)</f>
         <v>327</v>
       </c>
-      <c r="F27" s="54">
+      <c r="F27" s="53">
         <f>ROUND(F19+F24,0)</f>
         <v>72</v>
       </c>
-      <c r="G27" s="52">
+      <c r="G27" s="51">
         <f>ROUND(G19+G24,0)</f>
         <v>0</v>
       </c>
-      <c r="H27" s="53" t="s">
+      <c r="H27" s="52" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="28" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="49" t="s">
+      <c r="A28" s="48" t="s">
         <v>53</v>
       </c>
-      <c r="B28" s="50" t="s">
+      <c r="B28" s="49" t="s">
         <v>98</v>
       </c>
-      <c r="C28" s="50"/>
-      <c r="D28" s="50">
+      <c r="C28" s="49"/>
+      <c r="D28" s="49">
         <f>ROUND(D23-SUM(AdjustmentArb)*D26,0)</f>
         <v>0</v>
       </c>
-      <c r="E28" s="50">
+      <c r="E28" s="49">
         <f>ROUND(E23-SUM(AdjustmentArb)*E26,0)</f>
         <v>0</v>
       </c>
-      <c r="F28" s="50">
+      <c r="F28" s="49">
         <f>ROUND(F23-SUM(AdjustmentArb)*F26,0)</f>
         <v>0</v>
       </c>
-      <c r="G28" s="50">
+      <c r="G28" s="49">
         <f>ROUND(G23-SUM(AdjustmentArb)*G26,0)</f>
         <v>0</v>
       </c>
-      <c r="H28" s="53" t="s">
+      <c r="H28" s="52" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="29" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="49"/>
-      <c r="B29" s="50" t="s">
+      <c r="A29" s="48"/>
+      <c r="B29" s="49" t="s">
         <v>99</v>
       </c>
-      <c r="C29" s="55">
+      <c r="C29" s="54">
         <f>C16-SUM(D27:G28)</f>
         <v>-1</v>
       </c>
-      <c r="D29" s="50"/>
-      <c r="E29" s="50"/>
-      <c r="F29" s="50"/>
-      <c r="G29" s="50"/>
-      <c r="H29" s="53" t="s">
+      <c r="D29" s="49"/>
+      <c r="E29" s="49"/>
+      <c r="F29" s="49"/>
+      <c r="G29" s="49"/>
+      <c r="H29" s="52" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A30" s="43"/>
-      <c r="C30" s="39"/>
+      <c r="A30" s="42"/>
+      <c r="C30" s="38"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B31" s="18" t="s">
+      <c r="B31" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="C31" s="15"/>
-      <c r="D31" s="30">
+      <c r="C31" s="14"/>
+      <c r="D31" s="29">
         <f>ROUND(D10,0)</f>
         <v>485</v>
       </c>
-      <c r="E31" s="30">
+      <c r="E31" s="29">
         <f>ROUND(E10,0)</f>
         <v>369</v>
       </c>
-      <c r="F31" s="30">
+      <c r="F31" s="29">
         <f>ROUND(F10,0)</f>
         <v>286</v>
       </c>
-      <c r="G31" s="30">
+      <c r="G31" s="29">
         <f>ROUND(G10,0)</f>
         <v>0</v>
       </c>
-      <c r="H31" s="17" t="s">
+      <c r="H31" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="I31" s="46" t="s">
+      <c r="I31" s="45" t="s">
         <v>72</v>
       </c>
     </row>
@@ -3292,27 +3342,27 @@
       <c r="A32" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B32" s="18" t="s">
+      <c r="B32" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="C32" s="15"/>
-      <c r="D32" s="30">
+      <c r="C32" s="14"/>
+      <c r="D32" s="29">
         <f>ROUND(D12,0)</f>
         <v>485</v>
       </c>
-      <c r="E32" s="30">
+      <c r="E32" s="29">
         <f>ROUND(E12,0)</f>
         <v>332</v>
       </c>
-      <c r="F32" s="30">
+      <c r="F32" s="29">
         <f>ROUND(F12,0)</f>
         <v>72</v>
       </c>
-      <c r="G32" s="30">
+      <c r="G32" s="29">
         <f>ROUND(G12,0)</f>
         <v>0</v>
       </c>
-      <c r="H32" s="17" t="s">
+      <c r="H32" s="16" t="s">
         <v>70</v>
       </c>
     </row>
@@ -3320,162 +3370,162 @@
       <c r="A33" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B33" s="18" t="s">
+      <c r="B33" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="C33" s="15"/>
-      <c r="D33" s="30">
+      <c r="C33" s="14"/>
+      <c r="D33" s="29">
         <f>D31-D32</f>
         <v>0</v>
       </c>
-      <c r="E33" s="30">
+      <c r="E33" s="29">
         <f>E31-E32</f>
         <v>37</v>
       </c>
-      <c r="F33" s="30">
+      <c r="F33" s="29">
         <f>F31-F32</f>
         <v>214</v>
       </c>
-      <c r="G33" s="30">
+      <c r="G33" s="29">
         <f>G31-G32</f>
         <v>0</v>
       </c>
-      <c r="H33" s="17" t="s">
+      <c r="H33" s="16" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="1"/>
-      <c r="B34" s="56" t="s">
+      <c r="B34" s="55" t="s">
         <v>102</v>
       </c>
-      <c r="C34" s="99" t="str">
+      <c r="C34" s="97" t="str">
         <f>IF(SUM(D32:G33)&lt;=MAKSBELOP,"Everyone paid",IF(SUM(D32:G32)&lt;=MAKSBELOP,"Arbeidsgivere fully paid; Person partially paid by Person request", "Arbeidsgivere partial payment ratio by Arbeidsgiver request"))</f>
         <v>Arbeidsgivere partial payment ratio by Arbeidsgiver request</v>
       </c>
-      <c r="D34" s="99"/>
-      <c r="E34" s="99"/>
-      <c r="F34" s="99"/>
-      <c r="G34" s="99"/>
-      <c r="H34" s="17"/>
+      <c r="D34" s="97"/>
+      <c r="E34" s="97"/>
+      <c r="F34" s="97"/>
+      <c r="G34" s="97"/>
+      <c r="H34" s="16"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B35" s="18" t="s">
+      <c r="B35" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="C35" s="15"/>
-      <c r="D35" s="18">
+      <c r="C35" s="14"/>
+      <c r="D35" s="17">
         <f>IF(SUM($D$32:$G$33)&lt;=MAKSBELOP,D32,IF(SUM($D$32:$G$32)&lt;=MAKSBELOP,D32,ROUND(D32*MAKSBELOP/SUM($D$32:$G$32),0)))</f>
         <v>471</v>
       </c>
-      <c r="E35" s="18">
+      <c r="E35" s="17">
         <f>IF(SUM($D$32:$G$33)&lt;=MAKSBELOP,E32,IF(SUM($D$32:$G$32)&lt;=MAKSBELOP,E32,ROUND(E32*MAKSBELOP/SUM($D$32:$G$32),0)))</f>
         <v>323</v>
       </c>
-      <c r="F35" s="18">
+      <c r="F35" s="17">
         <f>IF(SUM($D$32:$G$33)&lt;=MAKSBELOP,F32,IF(SUM($D$32:$G$32)&lt;=MAKSBELOP,F32,ROUND(F32*MAKSBELOP/SUM($D$32:$G$32),0)))</f>
         <v>70</v>
       </c>
-      <c r="G35" s="18">
+      <c r="G35" s="17">
         <f>IF(SUM($D$32:$G$33)&lt;=MAKSBELOP,G32,IF(SUM($D$32:$G$32)&lt;=MAKSBELOP,G32,ROUND(G32*MAKSBELOP/SUM($D$32:$G$32),0)))</f>
         <v>0</v>
       </c>
-      <c r="H35" s="17" t="s">
+      <c r="H35" s="16" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="36" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="1"/>
-      <c r="B36" s="18" t="s">
+      <c r="B36" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="C36" s="15">
+      <c r="C36" s="14">
         <f>MAKSBELOP-SUM(D35:G35)</f>
         <v>0</v>
       </c>
-      <c r="D36" s="18"/>
-      <c r="E36" s="18"/>
-      <c r="F36" s="18"/>
-      <c r="G36" s="18"/>
-      <c r="H36" s="17"/>
+      <c r="D36" s="17"/>
+      <c r="E36" s="17"/>
+      <c r="F36" s="17"/>
+      <c r="G36" s="17"/>
+      <c r="H36" s="16"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B37" s="18" t="s">
+      <c r="B37" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18">
+      <c r="C37" s="17"/>
+      <c r="D37" s="17">
         <f>IF(SUM($D$32:$G$33)&lt;=MAKSBELOP,D33,IF(SUM($D$32:$G$32)&lt;=MAKSBELOP,ROUND(PersonRemainder*D33/SUM($D$33:$G$33),0),0))</f>
         <v>0</v>
       </c>
-      <c r="E37" s="18">
+      <c r="E37" s="17">
         <f>IF(SUM($D$32:$G$33)&lt;=MAKSBELOP,E33,IF(SUM($D$32:$G$32)&lt;=MAKSBELOP,ROUND(PersonRemainder*E33/SUM($D$33:$G$33),0),0))</f>
         <v>0</v>
       </c>
-      <c r="F37" s="18">
+      <c r="F37" s="17">
         <f>IF(SUM($D$32:$G$33)&lt;=MAKSBELOP,F33,IF(SUM($D$32:$G$32)&lt;=MAKSBELOP,ROUND(PersonRemainder*F33/SUM($D$33:$G$33),0),0))</f>
         <v>0</v>
       </c>
-      <c r="G37" s="18">
+      <c r="G37" s="17">
         <f>IF(SUM($D$32:$G$33)&lt;=MAKSBELOP,G33,IF(SUM($D$32:$G$32)&lt;=MAKSBELOP,ROUND(PersonRemainder*G33/SUM($D$33:$G$33),0),0))</f>
         <v>0</v>
       </c>
-      <c r="H37" s="17" t="s">
+      <c r="H37" s="16" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="1"/>
-      <c r="B38" s="18" t="s">
+      <c r="B38" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="C38" s="15">
+      <c r="C38" s="14">
         <f>MAKSBELOP-SUM(D35:G37)</f>
         <v>0</v>
       </c>
-      <c r="D38" s="18"/>
-      <c r="E38" s="18"/>
-      <c r="F38" s="18"/>
-      <c r="G38" s="18"/>
-      <c r="H38" s="17" t="s">
+      <c r="D38" s="17"/>
+      <c r="E38" s="17"/>
+      <c r="F38" s="17"/>
+      <c r="G38" s="17"/>
+      <c r="H38" s="16" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A40" s="57" t="s">
+      <c r="A40" s="56" t="s">
         <v>104</v>
       </c>
-      <c r="B40" s="58"/>
-      <c r="C40" s="59"/>
-      <c r="D40" s="60"/>
+      <c r="B40" s="57"/>
+      <c r="C40" s="58"/>
+      <c r="D40" s="59"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A41" s="100" t="s">
+      <c r="A41" s="98" t="s">
         <v>105</v>
       </c>
-      <c r="B41" s="100"/>
-      <c r="C41" s="100"/>
-      <c r="D41" s="100"/>
+      <c r="B41" s="98"/>
+      <c r="C41" s="98"/>
+      <c r="D41" s="98"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A43" s="61" t="s">
+      <c r="A43" s="60" t="s">
         <v>106</v>
       </c>
-      <c r="B43" s="62">
+      <c r="B43" s="61">
         <v>1430.76</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A44" s="61" t="s">
+      <c r="A44" s="60" t="s">
         <v>107</v>
       </c>
-      <c r="B44" s="62">
+      <c r="B44" s="61">
         <f>ROUND(B43*260/12,0)</f>
         <v>31000</v>
       </c>
@@ -3511,37 +3561,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="40" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="41" t="s">
+      <c r="C1" s="40" t="s">
         <v>58</v>
       </c>
-      <c r="D1" s="42" t="s">
+      <c r="D1" s="41" t="s">
         <v>59</v>
       </c>
-      <c r="E1" s="42" t="s">
+      <c r="E1" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="F1" s="42" t="s">
+      <c r="F1" s="41" t="s">
         <v>61</v>
       </c>
-      <c r="G1" s="42" t="s">
+      <c r="G1" s="41" t="s">
         <v>62</v>
       </c>
-      <c r="H1" s="42" t="s">
+      <c r="H1" s="41" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="43"/>
-      <c r="H2" s="40"/>
+      <c r="A2" s="42"/>
+      <c r="H2" s="39"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="42" t="s">
         <v>7</v>
       </c>
       <c r="B3" t="s">
@@ -3559,12 +3609,12 @@
       <c r="G3" s="7">
         <v>0</v>
       </c>
-      <c r="H3" s="40" t="s">
+      <c r="H3" s="39" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="43"/>
+      <c r="A4" s="42"/>
       <c r="B4" t="s">
         <v>66</v>
       </c>
@@ -3584,39 +3634,39 @@
         <f>G3/SUM($D$3:$G$3)</f>
         <v>0</v>
       </c>
-      <c r="H4" s="40" t="s">
+      <c r="H4" s="39" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="43" t="s">
+      <c r="A5" s="42" t="s">
         <v>11</v>
       </c>
       <c r="B5" t="s">
         <v>67</v>
       </c>
-      <c r="D5" s="44">
+      <c r="D5" s="43">
         <f>D3*12/260</f>
         <v>969.23076923076928</v>
       </c>
-      <c r="E5" s="44">
+      <c r="E5" s="43">
         <f>E3*12/260</f>
         <v>461.53846153846155</v>
       </c>
-      <c r="F5" s="44">
+      <c r="F5" s="43">
         <f>F3*12/260</f>
         <v>1430.7692307692307</v>
       </c>
-      <c r="G5" s="44">
+      <c r="G5" s="43">
         <f>G3*12/260</f>
         <v>0</v>
       </c>
-      <c r="H5" s="40" t="s">
+      <c r="H5" s="39" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="43" t="s">
+      <c r="A6" s="42" t="s">
         <v>13</v>
       </c>
       <c r="B6" t="s">
@@ -3634,39 +3684,39 @@
       <c r="G6" s="10">
         <v>1</v>
       </c>
-      <c r="H6" s="40" t="s">
+      <c r="H6" s="39" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="43" t="s">
+      <c r="A7" s="42" t="s">
         <v>16</v>
       </c>
       <c r="B7" t="s">
         <v>71</v>
       </c>
-      <c r="D7" s="44">
+      <c r="D7" s="43">
         <f>D5*D6</f>
         <v>969.23076923076928</v>
       </c>
-      <c r="E7" s="44">
+      <c r="E7" s="43">
         <f>E5*E6</f>
         <v>461.53846153846155</v>
       </c>
-      <c r="F7" s="44">
+      <c r="F7" s="43">
         <f>F5*F6</f>
         <v>1430.7692307692307</v>
       </c>
-      <c r="G7" s="44">
+      <c r="G7" s="43">
         <f>G5*G6</f>
         <v>0</v>
       </c>
-      <c r="H7" s="40" t="s">
+      <c r="H7" s="39" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="43" t="s">
+      <c r="A8" s="42" t="s">
         <v>17</v>
       </c>
       <c r="B8" t="s">
@@ -3688,12 +3738,12 @@
         <f>MIN(G7,$C$15)</f>
         <v>0</v>
       </c>
-      <c r="H8" s="40" t="s">
+      <c r="H8" s="39" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="43" t="s">
+      <c r="A9" s="42" t="s">
         <v>18</v>
       </c>
       <c r="B9" t="s">
@@ -3711,39 +3761,39 @@
       <c r="G9" s="12">
         <v>1</v>
       </c>
-      <c r="H9" s="40" t="s">
+      <c r="H9" s="39" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="43" t="s">
+      <c r="A10" s="42" t="s">
         <v>20</v>
       </c>
       <c r="B10" t="s">
         <v>75</v>
       </c>
-      <c r="D10" s="44">
+      <c r="D10" s="43">
         <f>D7*D9</f>
         <v>484.61538461538464</v>
       </c>
-      <c r="E10" s="44">
+      <c r="E10" s="43">
         <f>E7*E9</f>
         <v>369.23076923076928</v>
       </c>
-      <c r="F10" s="44">
+      <c r="F10" s="43">
         <f>F7*F9</f>
         <v>286.15384615384613</v>
       </c>
-      <c r="G10" s="44">
+      <c r="G10" s="43">
         <f>G7*G9</f>
         <v>0</v>
       </c>
-      <c r="H10" s="40" t="s">
+      <c r="H10" s="39" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="43" t="s">
+      <c r="A11" s="42" t="s">
         <v>21</v>
       </c>
       <c r="B11" t="s">
@@ -3761,54 +3811,54 @@
       <c r="G11" s="10">
         <v>1</v>
       </c>
-      <c r="H11" s="40" t="s">
+      <c r="H11" s="39" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="43" t="s">
+      <c r="A12" s="42" t="s">
         <v>22</v>
       </c>
       <c r="B12" t="s">
         <v>77</v>
       </c>
-      <c r="D12" s="47">
+      <c r="D12" s="46">
         <f>D10*D11</f>
         <v>484.61538461538464</v>
       </c>
-      <c r="E12" s="47">
+      <c r="E12" s="46">
         <f>E10*E11</f>
         <v>332.30769230769238</v>
       </c>
-      <c r="F12" s="47">
+      <c r="F12" s="46">
         <f>F10*F11</f>
         <v>71.538461538461533</v>
       </c>
-      <c r="G12" s="47">
+      <c r="G12" s="46">
         <f>G10*G11</f>
         <v>0</v>
       </c>
-      <c r="H12" s="40" t="s">
+      <c r="H12" s="39" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="43" t="s">
+      <c r="A13" s="42" t="s">
         <v>23</v>
       </c>
       <c r="B13" t="s">
         <v>78</v>
       </c>
-      <c r="C13" s="63">
+      <c r="C13" s="62">
         <f>SUM(D10:G10)/SUM(D7:G7)</f>
         <v>0.39838709677419348</v>
       </c>
-      <c r="H13" s="40" t="s">
+      <c r="H13" s="39" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="43" t="s">
+      <c r="A14" s="42" t="s">
         <v>25</v>
       </c>
       <c r="B14" t="s">
@@ -3817,401 +3867,401 @@
       <c r="C14" s="7">
         <v>101351</v>
       </c>
-      <c r="H14" s="40" t="s">
+      <c r="H14" s="39" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="43" t="s">
+      <c r="A15" s="42" t="s">
         <v>27</v>
       </c>
       <c r="B15" t="s">
         <v>80</v>
       </c>
-      <c r="C15" s="64">
+      <c r="C15" s="63">
         <f>6*C14/260</f>
         <v>2338.8692307692309</v>
       </c>
-      <c r="H15" s="40" t="s">
+      <c r="H15" s="39" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="43" t="s">
+      <c r="A16" s="42" t="s">
         <v>28</v>
       </c>
       <c r="B16" t="s">
         <v>81</v>
       </c>
-      <c r="C16" s="64">
+      <c r="C16" s="63">
         <f>C13*C15</f>
         <v>931.77532258064502</v>
       </c>
-      <c r="H16" s="40" t="s">
+      <c r="H16" s="39" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="49" t="s">
+      <c r="A17" s="48" t="s">
         <v>82</v>
       </c>
-      <c r="B17" s="50" t="s">
+      <c r="B17" s="49" t="s">
         <v>83</v>
       </c>
-      <c r="C17" s="51">
+      <c r="C17" s="50">
         <f>MIN(1, C16/SUM(D10:G10))</f>
         <v>0.81734677419354829</v>
       </c>
-      <c r="D17" s="52"/>
-      <c r="E17" s="52"/>
-      <c r="F17" s="52"/>
-      <c r="G17" s="52"/>
-      <c r="H17" s="53" t="s">
+      <c r="D17" s="51"/>
+      <c r="E17" s="51"/>
+      <c r="F17" s="51"/>
+      <c r="G17" s="51"/>
+      <c r="H17" s="52" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="49" t="s">
+      <c r="A18" s="48" t="s">
         <v>84</v>
       </c>
-      <c r="B18" s="50" t="s">
+      <c r="B18" s="49" t="s">
         <v>85</v>
       </c>
-      <c r="C18" s="50"/>
-      <c r="D18" s="52">
+      <c r="C18" s="49"/>
+      <c r="D18" s="51">
         <f>D10*ScalingFactor</f>
         <v>367.28744939271257</v>
       </c>
-      <c r="E18" s="52">
+      <c r="E18" s="51">
         <f>E10*ScalingFactor</f>
         <v>279.83805668016197</v>
       </c>
-      <c r="F18" s="52">
+      <c r="F18" s="51">
         <f>F10*ScalingFactor</f>
         <v>216.87449392712549</v>
       </c>
-      <c r="G18" s="52">
+      <c r="G18" s="51">
         <f>G10*ScalingFactor</f>
         <v>0</v>
       </c>
-      <c r="H18" s="53" t="s">
+      <c r="H18" s="52" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="49" t="s">
+      <c r="A19" s="48" t="s">
         <v>86</v>
       </c>
-      <c r="B19" s="50" t="s">
+      <c r="B19" s="49" t="s">
         <v>87</v>
       </c>
-      <c r="C19" s="50"/>
-      <c r="D19" s="52">
+      <c r="C19" s="49"/>
+      <c r="D19" s="51">
         <f>MIN(D18,D12)</f>
         <v>367.28744939271257</v>
       </c>
-      <c r="E19" s="52">
+      <c r="E19" s="51">
         <f>MIN(E18,E12)</f>
         <v>279.83805668016197</v>
       </c>
-      <c r="F19" s="52">
+      <c r="F19" s="51">
         <f>MIN(F18,F12)</f>
         <v>71.538461538461533</v>
       </c>
-      <c r="G19" s="52">
+      <c r="G19" s="51">
         <f>MIN(G18,G12)</f>
         <v>0</v>
       </c>
-      <c r="H19" s="53" t="s">
+      <c r="H19" s="52" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="49"/>
-      <c r="B20" s="50" t="s">
+      <c r="A20" s="48"/>
+      <c r="B20" s="49" t="s">
         <v>88</v>
       </c>
-      <c r="C20" s="50"/>
-      <c r="D20" s="52">
+      <c r="C20" s="49"/>
+      <c r="D20" s="51">
         <f>D19-D12</f>
         <v>-117.32793522267207</v>
       </c>
-      <c r="E20" s="52">
+      <c r="E20" s="51">
         <f>E19-E12</f>
         <v>-52.469635627530408</v>
       </c>
-      <c r="F20" s="52">
+      <c r="F20" s="51">
         <f>F19-F12</f>
         <v>0</v>
       </c>
-      <c r="G20" s="52">
+      <c r="G20" s="51">
         <f>G19-G12</f>
         <v>0</v>
       </c>
-      <c r="H20" s="53" t="s">
+      <c r="H20" s="52" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="49"/>
-      <c r="B21" s="50" t="s">
+      <c r="A21" s="48"/>
+      <c r="B21" s="49" t="s">
         <v>89</v>
       </c>
-      <c r="C21" s="50"/>
-      <c r="D21" s="51">
+      <c r="C21" s="49"/>
+      <c r="D21" s="50">
         <f>IF(D20 &lt; 0, D4, 0)</f>
         <v>0.33870967741935482</v>
       </c>
-      <c r="E21" s="51">
+      <c r="E21" s="50">
         <f>IF(E20 &lt; 0, E4, 0)</f>
         <v>0.16129032258064516</v>
       </c>
-      <c r="F21" s="51">
+      <c r="F21" s="50">
         <f>IF(F20 &lt; 0, F4, 0)</f>
         <v>0</v>
       </c>
-      <c r="G21" s="52"/>
-      <c r="H21" s="53" t="s">
+      <c r="G21" s="51"/>
+      <c r="H21" s="52" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="22" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="49" t="s">
+      <c r="A22" s="48" t="s">
         <v>90</v>
       </c>
-      <c r="B22" s="50" t="s">
+      <c r="B22" s="49" t="s">
         <v>91</v>
       </c>
-      <c r="C22" s="50"/>
-      <c r="D22" s="51">
+      <c r="C22" s="49"/>
+      <c r="D22" s="50">
         <f>IF(SUM(ShortfallIncomeRatioArb)=0,0,D21/SUM(ShortfallIncomeRatioArb))</f>
         <v>0.67741935483870963</v>
       </c>
-      <c r="E22" s="51">
+      <c r="E22" s="50">
         <f>IF(SUM(ShortfallIncomeRatioArb)=0,0,E21/SUM(ShortfallIncomeRatioArb))</f>
         <v>0.32258064516129031</v>
       </c>
-      <c r="F22" s="51">
+      <c r="F22" s="50">
         <f>IF(SUM(ShortfallIncomeRatioArb)=0,0,F21/SUM(ShortfallIncomeRatioArb))</f>
         <v>0</v>
       </c>
-      <c r="G22" s="51">
+      <c r="G22" s="50">
         <f>IF(SUM(ShortfallIncomeRatioArb)=0,0,G21/SUM(ShortfallIncomeRatioArb))</f>
         <v>0</v>
       </c>
-      <c r="H22" s="53" t="s">
+      <c r="H22" s="52" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="49"/>
-      <c r="B23" s="50" t="s">
+      <c r="A23" s="48"/>
+      <c r="B23" s="49" t="s">
         <v>92</v>
       </c>
-      <c r="C23" s="50"/>
-      <c r="D23" s="52">
+      <c r="C23" s="49"/>
+      <c r="D23" s="51">
         <f>D18-D19</f>
         <v>0</v>
       </c>
-      <c r="E23" s="52">
+      <c r="E23" s="51">
         <f>E18-E19</f>
         <v>0</v>
       </c>
-      <c r="F23" s="52">
+      <c r="F23" s="51">
         <f>F18-F19</f>
         <v>145.33603238866397</v>
       </c>
-      <c r="G23" s="52">
+      <c r="G23" s="51">
         <f>G18-G19</f>
         <v>0</v>
       </c>
-      <c r="H23" s="53" t="s">
+      <c r="H23" s="52" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="49" t="s">
+      <c r="A24" s="48" t="s">
         <v>93</v>
       </c>
-      <c r="B24" s="50" t="s">
+      <c r="B24" s="49" t="s">
         <v>94</v>
       </c>
-      <c r="C24" s="50"/>
-      <c r="D24" s="52">
+      <c r="C24" s="49"/>
+      <c r="D24" s="51">
         <f>MIN(-D20,IF(SUM($D$20:$G$20)&gt;=0, 0, SUM($D$23:$G$23)*D22))</f>
         <v>98.453441295546554</v>
       </c>
-      <c r="E24" s="52">
+      <c r="E24" s="51">
         <f>MIN(-E20,IF(SUM($D$20:$G$20)&gt;=0, 0, SUM($D$23:$G$23)*E22))</f>
         <v>46.882591093117405</v>
       </c>
-      <c r="F24" s="52">
+      <c r="F24" s="51">
         <f>MIN(-F20,IF(SUM($D$20:$G$20)&gt;=0, 0, SUM($D$23:$G$23)*F22))</f>
         <v>0</v>
       </c>
-      <c r="G24" s="52">
+      <c r="G24" s="51">
         <f>MIN(-G20,IF(SUM($D$20:$G$20)&gt;=0, 0, SUM($D$23:$G$23)*G22))</f>
         <v>0</v>
       </c>
-      <c r="H24" s="53" t="s">
+      <c r="H24" s="52" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="25" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="49"/>
-      <c r="B25" s="50" t="s">
+      <c r="A25" s="48"/>
+      <c r="B25" s="49" t="s">
         <v>95</v>
       </c>
-      <c r="C25" s="50"/>
-      <c r="D25" s="51">
+      <c r="C25" s="49"/>
+      <c r="D25" s="50">
         <f>IF(D23 = 0, 0, D4)</f>
         <v>0</v>
       </c>
-      <c r="E25" s="51">
+      <c r="E25" s="50">
         <f>IF(E23 = 0, 0, E4)</f>
         <v>0</v>
       </c>
-      <c r="F25" s="51">
+      <c r="F25" s="50">
         <f>IF(F23 = 0, 0, F4)</f>
         <v>0.5</v>
       </c>
-      <c r="G25" s="51">
+      <c r="G25" s="50">
         <f>IF(G23 = 0, 0, G4)</f>
         <v>0</v>
       </c>
-      <c r="H25" s="53" t="s">
+      <c r="H25" s="52" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="26" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="49"/>
-      <c r="B26" s="50" t="s">
+      <c r="A26" s="48"/>
+      <c r="B26" s="49" t="s">
         <v>96</v>
       </c>
-      <c r="C26" s="50"/>
-      <c r="D26" s="51">
+      <c r="C26" s="49"/>
+      <c r="D26" s="50">
         <f>IF(SUM(ShortfallIncomeRatioPerson)= 0, 0, D25/SUM(ShortfallIncomeRatioPerson))</f>
         <v>0</v>
       </c>
-      <c r="E26" s="51">
+      <c r="E26" s="50">
         <f>IF(SUM(ShortfallIncomeRatioPerson)= 0, 0, E25/SUM(ShortfallIncomeRatioPerson))</f>
         <v>0</v>
       </c>
-      <c r="F26" s="51">
+      <c r="F26" s="50">
         <f>IF(SUM(ShortfallIncomeRatioPerson)= 0, 0, F25/SUM(ShortfallIncomeRatioPerson))</f>
         <v>1</v>
       </c>
-      <c r="G26" s="51">
+      <c r="G26" s="50">
         <f>IF(SUM(ShortfallIncomeRatioPerson)= 0, 0, G25/SUM(ShortfallIncomeRatioPerson))</f>
         <v>0</v>
       </c>
-      <c r="H26" s="53" t="s">
+      <c r="H26" s="52" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="49" t="s">
+      <c r="A27" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="B27" s="50" t="s">
+      <c r="B27" s="49" t="s">
         <v>97</v>
       </c>
-      <c r="C27" s="50"/>
-      <c r="D27" s="54">
+      <c r="C27" s="49"/>
+      <c r="D27" s="53">
         <f>ROUND(D19+D24,0)</f>
         <v>466</v>
       </c>
-      <c r="E27" s="54">
+      <c r="E27" s="53">
         <f>ROUND(E19+E24,0)</f>
         <v>327</v>
       </c>
-      <c r="F27" s="54">
+      <c r="F27" s="53">
         <f>ROUND(F19+F24,0)</f>
         <v>72</v>
       </c>
-      <c r="G27" s="52">
+      <c r="G27" s="51">
         <f>ROUND(G19+G24,0)</f>
         <v>0</v>
       </c>
-      <c r="H27" s="53" t="s">
+      <c r="H27" s="52" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="28" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="49" t="s">
+      <c r="A28" s="48" t="s">
         <v>53</v>
       </c>
-      <c r="B28" s="50" t="s">
+      <c r="B28" s="49" t="s">
         <v>98</v>
       </c>
-      <c r="C28" s="50"/>
-      <c r="D28" s="50">
+      <c r="C28" s="49"/>
+      <c r="D28" s="49">
         <f>ROUND(D23-SUM(AdjustmentArb)*D26,0)</f>
         <v>0</v>
       </c>
-      <c r="E28" s="50">
+      <c r="E28" s="49">
         <f>ROUND(E23-SUM(AdjustmentArb)*E26,0)</f>
         <v>0</v>
       </c>
-      <c r="F28" s="50">
+      <c r="F28" s="49">
         <f>ROUND(F23-SUM(AdjustmentArb)*F26,0)</f>
         <v>0</v>
       </c>
-      <c r="G28" s="50">
+      <c r="G28" s="49">
         <f>ROUND(G23-SUM(AdjustmentArb)*G26,0)</f>
         <v>0</v>
       </c>
-      <c r="H28" s="53" t="s">
+      <c r="H28" s="52" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="29" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="49"/>
-      <c r="B29" s="50" t="s">
+      <c r="A29" s="48"/>
+      <c r="B29" s="49" t="s">
         <v>99</v>
       </c>
-      <c r="C29" s="55">
+      <c r="C29" s="54">
         <f>C16-SUM(D27:G28)</f>
         <v>66.775322580645025</v>
       </c>
-      <c r="D29" s="50"/>
-      <c r="E29" s="50"/>
-      <c r="F29" s="50"/>
-      <c r="G29" s="50"/>
-      <c r="H29" s="53" t="s">
+      <c r="D29" s="49"/>
+      <c r="E29" s="49"/>
+      <c r="F29" s="49"/>
+      <c r="G29" s="49"/>
+      <c r="H29" s="52" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A30" s="43"/>
-      <c r="C30" s="39"/>
-      <c r="H30" s="40"/>
+      <c r="A30" s="42"/>
+      <c r="C30" s="38"/>
+      <c r="H30" s="39"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B31" s="18" t="s">
+      <c r="B31" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="C31" s="15"/>
-      <c r="D31" s="65">
+      <c r="C31" s="14"/>
+      <c r="D31" s="64">
         <f>D10</f>
         <v>484.61538461538464</v>
       </c>
-      <c r="E31" s="65">
+      <c r="E31" s="64">
         <f>E10</f>
         <v>369.23076923076928</v>
       </c>
-      <c r="F31" s="65">
+      <c r="F31" s="64">
         <f>F10</f>
         <v>286.15384615384613</v>
       </c>
-      <c r="G31" s="30">
+      <c r="G31" s="29">
         <f>ROUND(G10,0)</f>
         <v>0</v>
       </c>
-      <c r="H31" s="17" t="s">
+      <c r="H31" s="16" t="s">
         <v>70</v>
       </c>
     </row>
@@ -4219,27 +4269,27 @@
       <c r="A32" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B32" s="18" t="s">
+      <c r="B32" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="C32" s="15"/>
-      <c r="D32" s="65">
+      <c r="C32" s="14"/>
+      <c r="D32" s="64">
         <f>D12</f>
         <v>484.61538461538464</v>
       </c>
-      <c r="E32" s="65">
+      <c r="E32" s="64">
         <f>E12</f>
         <v>332.30769230769238</v>
       </c>
-      <c r="F32" s="65">
+      <c r="F32" s="64">
         <f>F12</f>
         <v>71.538461538461533</v>
       </c>
-      <c r="G32" s="30">
+      <c r="G32" s="29">
         <f>ROUND(G12,0)</f>
         <v>0</v>
       </c>
-      <c r="H32" s="17" t="s">
+      <c r="H32" s="16" t="s">
         <v>70</v>
       </c>
     </row>
@@ -4247,130 +4297,130 @@
       <c r="A33" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B33" s="18" t="s">
+      <c r="B33" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="C33" s="15"/>
-      <c r="D33" s="65">
+      <c r="C33" s="14"/>
+      <c r="D33" s="64">
         <f>D31-D32</f>
         <v>0</v>
       </c>
-      <c r="E33" s="65">
+      <c r="E33" s="64">
         <f>E31-E32</f>
         <v>36.923076923076906</v>
       </c>
-      <c r="F33" s="65">
+      <c r="F33" s="64">
         <f>F31-F32</f>
         <v>214.61538461538458</v>
       </c>
-      <c r="G33" s="30">
+      <c r="G33" s="29">
         <f>G31-G32</f>
         <v>0</v>
       </c>
-      <c r="H33" s="17" t="s">
+      <c r="H33" s="16" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="1"/>
-      <c r="B34" s="56" t="s">
+      <c r="B34" s="55" t="s">
         <v>102</v>
       </c>
-      <c r="C34" s="99" t="str">
+      <c r="C34" s="97" t="str">
         <f>IF(SUM(D32:G33)&lt;=MAKSBELOP,"Everyone paid",IF(SUM(D32:G32)&lt;=MAKSBELOP,"Arbeidsgivere fully paid; Person partially paid by Person request", "Arbeidsgivere partial payment ratio by Arbeidsgiver request"))</f>
         <v>Arbeidsgivere partial payment ratio by Arbeidsgiver request</v>
       </c>
-      <c r="D34" s="99"/>
-      <c r="E34" s="99"/>
-      <c r="F34" s="99"/>
-      <c r="G34" s="99"/>
-      <c r="H34" s="17"/>
+      <c r="D34" s="97"/>
+      <c r="E34" s="97"/>
+      <c r="F34" s="97"/>
+      <c r="G34" s="97"/>
+      <c r="H34" s="16"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B35" s="18" t="s">
+      <c r="B35" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="C35" s="15"/>
-      <c r="D35" s="18">
+      <c r="C35" s="14"/>
+      <c r="D35" s="17">
         <f>IF(SUM($D$32:$G$33)&lt;=MAKSBELOP2,ROUND(D32,0),IF(SUM($D$32:$G$32)&lt;=MAKSBELOP2,ROUND(D32,0),ROUND(D32*MAKSBELOP2/SUM($D$32:$G$32),0)))</f>
         <v>485</v>
       </c>
-      <c r="E35" s="18">
+      <c r="E35" s="17">
         <f>IF(SUM($D$32:$G$33)&lt;=MAKSBELOP2,ROUND(E32,0),IF(SUM($D$32:$G$32)&lt;=MAKSBELOP2,ROUND(E32,0),ROUND(E32*MAKSBELOP2/SUM($D$32:$G$32),0)))</f>
         <v>332</v>
       </c>
-      <c r="F35" s="18">
+      <c r="F35" s="17">
         <f>IF(SUM($D$32:$G$33)&lt;=MAKSBELOP2,ROUND(F32,0),IF(SUM($D$32:$G$32)&lt;=MAKSBELOP2,ROUND(F32,0),ROUND(F32*MAKSBELOP2/SUM($D$32:$G$32),0)))</f>
         <v>72</v>
       </c>
-      <c r="G35" s="18">
+      <c r="G35" s="17">
         <f>IF(SUM($D$32:$G$33)&lt;=MAKSBELOP,G32,IF(SUM($D$32:$G$32)&lt;=MAKSBELOP,G32,ROUND(G32*MAKSBELOP/SUM($D$32:$G$32),0)))</f>
         <v>0</v>
       </c>
-      <c r="H35" s="17" t="s">
+      <c r="H35" s="16" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="1"/>
-      <c r="B36" s="18" t="s">
+      <c r="B36" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="C36" s="66">
+      <c r="C36" s="65">
         <f>MAKSBELOP2-SUM(D35:G35)</f>
         <v>42.775322580645025</v>
       </c>
-      <c r="D36" s="18"/>
-      <c r="E36" s="18"/>
-      <c r="F36" s="18"/>
-      <c r="G36" s="18"/>
-      <c r="H36" s="17"/>
+      <c r="D36" s="17"/>
+      <c r="E36" s="17"/>
+      <c r="F36" s="17"/>
+      <c r="G36" s="17"/>
+      <c r="H36" s="16"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B37" s="18" t="s">
+      <c r="B37" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="C37" s="18"/>
-      <c r="D37" s="25">
+      <c r="C37" s="17"/>
+      <c r="D37" s="24">
         <f>IF(SUM($D$32:$G$33)&lt;=MAKSBELOP2,ROUND(D33,0),IF(SUM($D$32:$G$32)&lt;=MAKSBELOP2,ROUND(PersonRemainder2*D33/SUM($D$33:$G$33),0),0))</f>
         <v>0</v>
       </c>
-      <c r="E37" s="25">
+      <c r="E37" s="24">
         <f>IF(SUM($D$32:$G$33)&lt;=MAKSBELOP2,ROUND(E33,0),IF(SUM($D$32:$G$32)&lt;=MAKSBELOP2,ROUND(PersonRemainder2*E33/SUM($D$33:$G$33),0),0))</f>
         <v>6</v>
       </c>
-      <c r="F37" s="25">
+      <c r="F37" s="24">
         <f>IF(SUM($D$32:$G$33)&lt;=MAKSBELOP2,ROUND(F33,0),IF(SUM($D$32:$G$32)&lt;=MAKSBELOP2,ROUND(PersonRemainder2*F33/SUM($D$33:$G$33),0),0))</f>
         <v>36</v>
       </c>
-      <c r="G37" s="18">
+      <c r="G37" s="17">
         <f>IF(SUM($D$32:$G$33)&lt;=MAKSBELOP,G33,IF(SUM($D$32:$G$32)&lt;=MAKSBELOP,ROUND(PersonRemainder*G33/SUM($D$33:$G$33),0),0))</f>
         <v>0</v>
       </c>
-      <c r="H37" s="17" t="s">
+      <c r="H37" s="16" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="1"/>
-      <c r="B38" s="18" t="s">
+      <c r="B38" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="C38" s="66">
+      <c r="C38" s="65">
         <f>MAKSBELOP2-SUM(D35:G37)</f>
         <v>0.77532258064502457</v>
       </c>
-      <c r="D38" s="18"/>
-      <c r="E38" s="18"/>
-      <c r="F38" s="18"/>
-      <c r="G38" s="18"/>
-      <c r="H38" s="17" t="s">
+      <c r="D38" s="17"/>
+      <c r="E38" s="17"/>
+      <c r="F38" s="17"/>
+      <c r="G38" s="17"/>
+      <c r="H38" s="16" t="s">
         <v>70</v>
       </c>
     </row>

</xml_diff>

<commit_message>
legger til tilkommen inntekt
det er en nedtrekksmeny som man sier "Ja" eller "Nei" på, også justeres sykepengegrunnlaget og total sykdomsgrad seg.
</commit_message>
<xml_diff>
--- a/doc/okonomi/Utbetaling.xlsx
+++ b/doc/okonomi/Utbetaling.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/david/dev/nav/helse-spleis/doc/okonomi/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C540BFB-4652-7A46-8CBA-F4AD86A75428}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98E76527-0CE8-9B4E-920B-4C7F4D958666}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8200" yWindow="5940" windowWidth="52940" windowHeight="32740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="36400" yWindow="500" windowWidth="52940" windowHeight="26600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Flere arbeidsgivere, ny " sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="156">
   <si>
     <t xml:space="preserve">Begrep	</t>
   </si>
@@ -527,6 +527,15 @@
   </si>
   <si>
     <t xml:space="preserve">Maks dagsats før reduksjon til 6G og reduksjon for total sykdomsgrad. </t>
+  </si>
+  <si>
+    <t>Arbeidsgrad</t>
+  </si>
+  <si>
+    <t>Nei</t>
+  </si>
+  <si>
+    <t>Tilkommen inntekt?</t>
   </si>
 </sst>
 </file>
@@ -730,31 +739,30 @@
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="111">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="9" fontId="0" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="10" fontId="0" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="10" fontId="0" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -768,7 +776,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -776,39 +783,35 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="3" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="5" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="5" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="168" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="165" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -818,28 +821,22 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="170" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="170" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="170" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="171" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -854,9 +851,8 @@
     <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -865,27 +861,23 @@
     <xf numFmtId="177" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="179" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="180" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="180" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="173" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="182" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1272,8 +1264,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1312,58 +1304,65 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="3"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="6"/>
+      <c r="A2" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="C2" t="s">
+        <v>154</v>
+      </c>
+      <c r="D2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E2" t="s">
+        <v>154</v>
+      </c>
+      <c r="F2" t="s">
+        <v>154</v>
+      </c>
+      <c r="G2" s="4"/>
+      <c r="H2" s="5"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="7">
+      <c r="C3" s="6">
         <v>31000</v>
       </c>
-      <c r="D3" s="7">
-        <v>31000</v>
-      </c>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="5" t="s">
+      <c r="D3" s="6">
+        <v>25000</v>
+      </c>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="3"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="8">
-        <f>C3/SUM($C$3:$F$3)</f>
-        <v>0.5</v>
-      </c>
-      <c r="D4" s="8">
-        <f>D3/SUM($C$3:$F$3)</f>
-        <v>0.5</v>
-      </c>
-      <c r="E4" s="8">
-        <f>E3/SUM($C$3:$F$3)</f>
-        <v>0</v>
-      </c>
-      <c r="F4" s="8">
-        <f>F3/SUM($C$3:$F$3)</f>
-        <v>0</v>
-      </c>
-      <c r="G4" s="5" t="s">
+      <c r="C4" s="7">
+        <f>C3*12/$B$10</f>
+        <v>0.5535714285714286</v>
+      </c>
+      <c r="D4" s="7">
+        <f>D3*12/$B$10</f>
+        <v>0.44642857142857145</v>
+      </c>
+      <c r="E4" s="7">
+        <f>E3*12/$B$10</f>
+        <v>0</v>
+      </c>
+      <c r="F4" s="7">
+        <f>F3*12/$B$10</f>
+        <v>0</v>
+      </c>
+      <c r="G4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="5" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1371,26 +1370,26 @@
       <c r="A5" t="s">
         <v>108</v>
       </c>
-      <c r="C5" s="38">
+      <c r="C5" s="36">
         <f>C3*12</f>
         <v>372000</v>
       </c>
-      <c r="D5" s="38">
+      <c r="D5" s="36">
         <f t="shared" ref="D5:F5" si="0">D3*12</f>
-        <v>372000</v>
-      </c>
-      <c r="E5" s="38">
+        <v>300000</v>
+      </c>
+      <c r="E5" s="36">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F5" s="38">
+      <c r="F5" s="36">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G5" s="69" t="s">
+      <c r="G5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="68" t="s">
+      <c r="H5" s="63" t="s">
         <v>110</v>
       </c>
     </row>
@@ -1398,1173 +1397,1197 @@
       <c r="A6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="107">
+      <c r="B6" s="65">
+        <f>SUM(C6:F6)</f>
+        <v>56000</v>
+      </c>
+      <c r="C6" s="65">
         <f>C3*1</f>
         <v>31000</v>
       </c>
-      <c r="D6" s="107">
-        <f>D3*1</f>
-        <v>31000</v>
-      </c>
-      <c r="E6" s="107">
+      <c r="D6" s="65">
+        <v>25000</v>
+      </c>
+      <c r="E6" s="65">
         <f>E3*0.25</f>
         <v>0</v>
       </c>
-      <c r="F6" s="107">
+      <c r="F6" s="65">
         <f>F3*0.3</f>
         <v>0</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="H6" s="5" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="67" t="s">
+      <c r="A7" s="39" t="s">
         <v>125</v>
       </c>
-      <c r="B7" s="71">
-        <f>SUM(C6:F6)*12</f>
-        <v>744000</v>
+      <c r="B7">
+        <f>B6*12</f>
+        <v>672000</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="12">
+      <c r="C8" s="11">
         <v>1</v>
       </c>
-      <c r="D8" s="12">
+      <c r="D8" s="11">
         <v>1</v>
       </c>
-      <c r="E8" s="12">
+      <c r="E8" s="11">
         <v>0.2</v>
       </c>
-      <c r="F8" s="12">
+      <c r="F8" s="11">
         <v>0.5</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="G8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="H8" s="5" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="67" t="s">
+      <c r="A9" s="97" t="s">
+        <v>153</v>
+      </c>
+      <c r="C9" s="66">
+        <f>1-C8</f>
+        <v>0</v>
+      </c>
+      <c r="D9" s="66">
+        <f t="shared" ref="D9:F9" si="1">1-D8</f>
+        <v>0</v>
+      </c>
+      <c r="E9" s="66">
+        <f t="shared" si="1"/>
+        <v>0.8</v>
+      </c>
+      <c r="F9" s="66">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="39" t="s">
         <v>113</v>
       </c>
-      <c r="B9" s="70">
-        <f>SUM(C5:F5)</f>
-        <v>744000</v>
-      </c>
-      <c r="G9" s="69" t="s">
+      <c r="B10" s="64">
+        <f>12*SUMIF(C2:F2,"Nei",C3:F3)</f>
+        <v>672000</v>
+      </c>
+      <c r="G10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H10" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="7">
+      <c r="B11" s="6">
         <v>93634</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="G11" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H10" s="6" t="s">
+      <c r="H11" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="67" t="s">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="38">
-        <f>B10*6</f>
+      <c r="B12" s="36">
+        <f>B11*6</f>
         <v>561804</v>
       </c>
-      <c r="G11" s="69" t="s">
+      <c r="G12" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H11" s="74" t="s">
+      <c r="H12" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="B12" s="108">
-        <f>ROUND(B11/260,)</f>
+      <c r="B13" s="94">
+        <f>ROUND(B12/260,)</f>
         <v>2161</v>
       </c>
-      <c r="G12" s="69" t="s">
+      <c r="G13" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H12" s="74" t="s">
+      <c r="H13" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="67" t="s">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="39" t="s">
         <v>109</v>
       </c>
-      <c r="B13" s="70">
-        <f>MIN(B9,B11)</f>
+      <c r="B14" s="64">
+        <f>MIN(B10,B12)</f>
         <v>561804</v>
       </c>
-      <c r="G13" s="69" t="s">
+      <c r="G14" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H13" s="74" t="s">
+      <c r="H14" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="67" t="s">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="39" t="s">
         <v>112</v>
       </c>
-      <c r="B14" s="71">
-        <f>ROUND(B13/260,0)</f>
+      <c r="B15" s="65">
+        <f>ROUND(B14/260,0)</f>
         <v>2161</v>
       </c>
-      <c r="G14" s="69" t="s">
+      <c r="G15" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H14" s="74" t="s">
+      <c r="H15" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="4"/>
-      <c r="C16" s="9">
+      <c r="C17" s="8">
         <f>C5/260</f>
         <v>1430.7692307692307</v>
       </c>
-      <c r="D16" s="9">
+      <c r="D17" s="8">
         <f>D5/260</f>
-        <v>1430.7692307692307</v>
-      </c>
-      <c r="E16" s="9">
+        <v>1153.8461538461538</v>
+      </c>
+      <c r="E17" s="8">
         <f>E5/260</f>
         <v>0</v>
       </c>
-      <c r="F16" s="9">
+      <c r="F17" s="8">
         <f>F5/260</f>
         <v>0</v>
       </c>
-      <c r="G16" s="5" t="s">
+      <c r="G17" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H16" s="6" t="s">
+      <c r="H17" s="5" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="10">
-        <v>1</v>
-      </c>
-      <c r="D17" s="10">
-        <v>1</v>
-      </c>
-      <c r="E17" s="10">
-        <v>1</v>
-      </c>
-      <c r="F17" s="10">
-        <v>1</v>
-      </c>
-      <c r="G17" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H17" s="6" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="9">
+        <v>1</v>
+      </c>
+      <c r="D18" s="9">
+        <v>1</v>
+      </c>
+      <c r="E18" s="9">
+        <v>1</v>
+      </c>
+      <c r="F18" s="9">
+        <v>1</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="4"/>
-      <c r="C18" s="108">
-        <f>C16*C17</f>
+      <c r="C19" s="94">
+        <f>C17*C18</f>
         <v>1430.7692307692307</v>
       </c>
-      <c r="D18" s="108">
-        <f t="shared" ref="D18:F18" si="1">D16*D17</f>
-        <v>1430.7692307692307</v>
-      </c>
-      <c r="E18" s="108">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F18" s="94">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G18" s="5" t="s">
+      <c r="D19" s="94">
+        <f t="shared" ref="D19:F19" si="2">D17*D18</f>
+        <v>1153.8461538461538</v>
+      </c>
+      <c r="E19" s="94">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F19" s="85">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G19" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H18" s="6" t="s">
+      <c r="H19" s="5" t="s">
         <v>152</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" s="72" t="s">
-        <v>114</v>
-      </c>
-      <c r="C19" s="73">
-        <f>C8*C4</f>
-        <v>0.5</v>
-      </c>
-      <c r="D19" s="73">
-        <f>D8*D4</f>
-        <v>0.5</v>
-      </c>
-      <c r="E19" s="73">
-        <f>E8*E4</f>
-        <v>0</v>
-      </c>
-      <c r="F19" s="73">
-        <f>F8*F4</f>
-        <v>0</v>
-      </c>
-      <c r="G19" s="69" t="s">
-        <v>8</v>
-      </c>
-      <c r="H19" s="74" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C20" s="66">
+        <f>C9*C4</f>
+        <v>0</v>
+      </c>
+      <c r="D20" s="66">
+        <f t="shared" ref="D20:F20" si="3">D9*D4</f>
+        <v>0</v>
+      </c>
+      <c r="E20" s="66">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F20" s="66">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H20" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="4"/>
-      <c r="C20" s="94">
-        <f>ROUND(C18*C8,0)</f>
+      <c r="C21" s="85">
+        <f>ROUND(C19*C8,0)</f>
         <v>1431</v>
       </c>
-      <c r="D20" s="94">
-        <f t="shared" ref="D20:F20" si="2">ROUND(D18*D8,0)</f>
-        <v>1431</v>
-      </c>
-      <c r="E20" s="94">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F20" s="94">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G20" s="5" t="s">
+      <c r="D21" s="85">
+        <f>ROUND(D19*D8,0)</f>
+        <v>1154</v>
+      </c>
+      <c r="E21" s="85">
+        <f>ROUND(E19*E8,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F21" s="85">
+        <f>ROUND(F19*F8,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G21" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H20" s="6" t="s">
+      <c r="H21" s="5" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" s="72" t="s">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="C21" s="95">
+      <c r="C22" s="86">
         <f>ROUND(C6*12/260*C8,0)</f>
         <v>1431</v>
       </c>
-      <c r="D21" s="95">
-        <f t="shared" ref="D21:F21" si="3">ROUND(D6*12/260*D8,0)</f>
-        <v>1431</v>
-      </c>
-      <c r="E21" s="95">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="F21" s="95">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G21" s="69" t="s">
+      <c r="D22" s="86">
+        <f>ROUND(D6*12/260*D8,0)</f>
+        <v>1154</v>
+      </c>
+      <c r="E22" s="86">
+        <f>ROUND(E6*12/260*E8,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F22" s="86">
+        <f>ROUND(F6*12/260*F8,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G22" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H21" s="74" t="s">
+      <c r="H22" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" s="72" t="s">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="B22" s="71">
-        <f>SUM(C20:F20)</f>
-        <v>2862</v>
-      </c>
-      <c r="G22" s="69" t="s">
+      <c r="B23" s="65">
+        <f>SUM(C21:F21)</f>
+        <v>2585</v>
+      </c>
+      <c r="G23" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H22" s="74" t="s">
+      <c r="H23" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" s="72" t="s">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="B23" s="71">
-        <f>B22*260</f>
-        <v>744120</v>
-      </c>
-      <c r="G23" s="69" t="s">
+      <c r="B24" s="65">
+        <f>B23*260</f>
+        <v>672100</v>
+      </c>
+      <c r="C24" s="66">
+        <f>C8*C4</f>
+        <v>0.5535714285714286</v>
+      </c>
+      <c r="D24" s="66">
+        <f>D8*D4</f>
+        <v>0.44642857142857145</v>
+      </c>
+      <c r="G24" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H23" s="74" t="s">
+      <c r="H24" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" s="72" t="s">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="B24" s="71">
-        <f>SUM(C21:F21)</f>
-        <v>2862</v>
-      </c>
-      <c r="C24" s="66"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" s="72" t="s">
-        <v>125</v>
-      </c>
-      <c r="B25" s="71">
-        <f>B24*260</f>
-        <v>744120</v>
-      </c>
+      <c r="B25" s="65">
+        <f>SUM(C22:F22)</f>
+        <v>2585</v>
+      </c>
+      <c r="C25" s="62"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B26" s="65">
+        <f>B25*260</f>
+        <v>672100</v>
+      </c>
+      <c r="C26" s="66"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B26" s="4"/>
-      <c r="C26" s="96">
-        <f>MIN(C20,C21)</f>
+      <c r="C27" s="86">
+        <f>MIN(C21,C22)</f>
         <v>1431</v>
       </c>
-      <c r="D26" s="96">
-        <f t="shared" ref="D26:F26" si="4">MIN(D20,D21)</f>
-        <v>1431</v>
-      </c>
-      <c r="E26" s="96">
-        <f>MIN(E20,E21)</f>
-        <v>0</v>
-      </c>
-      <c r="F26" s="96">
+      <c r="D27" s="86">
+        <f t="shared" ref="D27:F27" si="4">MIN(D21,D22)</f>
+        <v>1154</v>
+      </c>
+      <c r="E27" s="86">
+        <f>MIN(E21,E22)</f>
+        <v>0</v>
+      </c>
+      <c r="F27" s="86">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="G26" s="5" t="s">
+      <c r="G27" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H26" s="6" t="s">
+      <c r="H27" s="5" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" s="72" t="s">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="C27" s="101">
-        <f>C26/$B$24</f>
-        <v>0.5</v>
-      </c>
-      <c r="D27" s="97">
-        <f t="shared" ref="D27:F27" si="5">D26/$B$24</f>
-        <v>0.5</v>
-      </c>
-      <c r="E27" s="98">
-        <f>E26/$B$24</f>
-        <v>0</v>
-      </c>
-      <c r="F27" s="92">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="G27" s="69" t="s">
+      <c r="C28" s="88">
+        <f>C27/$B$25</f>
+        <v>0.55357833655706001</v>
+      </c>
+      <c r="D28" s="87">
+        <f>D27/$B$25</f>
+        <v>0.44642166344294004</v>
+      </c>
+      <c r="E28" s="88">
+        <f>E27/$B$25</f>
+        <v>0</v>
+      </c>
+      <c r="F28" s="83">
+        <f>F27/$B$25</f>
+        <v>0</v>
+      </c>
+      <c r="G28" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H27" s="74" t="s">
+      <c r="H28" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" s="72" t="s">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="C28" s="100">
-        <f>$B$35*C27</f>
-        <v>1080.5</v>
-      </c>
-      <c r="D28" s="66">
-        <f>$B$35*D27</f>
-        <v>1080.5</v>
-      </c>
-      <c r="E28" s="66">
-        <f>$B$35*E27</f>
-        <v>0</v>
-      </c>
-      <c r="F28" s="66">
-        <f>$B$35*F27</f>
-        <v>0</v>
-      </c>
-      <c r="H28" s="74" t="s">
+      <c r="C29" s="89">
+        <f>$B$36*C28</f>
+        <v>1196.2827852998066</v>
+      </c>
+      <c r="D29" s="62">
+        <f>$B$36*D28</f>
+        <v>964.71721470019338</v>
+      </c>
+      <c r="E29" s="62">
+        <f>$B$36*E28</f>
+        <v>0</v>
+      </c>
+      <c r="F29" s="62">
+        <f>$B$36*F28</f>
+        <v>0</v>
+      </c>
+      <c r="H29" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" s="72" t="s">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="B29" s="93">
-        <f>SUM(C26:F26)</f>
-        <v>2862</v>
-      </c>
-      <c r="C29" s="105"/>
-      <c r="D29" s="88"/>
-      <c r="E29" s="88"/>
-      <c r="F29" s="88"/>
-      <c r="G29" s="69" t="s">
+      <c r="B30" s="84">
+        <f>SUM(C27:F27)</f>
+        <v>2585</v>
+      </c>
+      <c r="C30" s="93"/>
+      <c r="D30" s="79"/>
+      <c r="E30" s="79"/>
+      <c r="F30" s="79"/>
+      <c r="G30" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H29" s="74" t="s">
+      <c r="H30" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A30" s="72" t="s">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="B30" s="71">
-        <f>B29*260</f>
-        <v>744120</v>
-      </c>
-      <c r="C30" s="66"/>
-      <c r="D30" s="66"/>
-      <c r="E30" s="66"/>
-      <c r="F30" s="66"/>
-      <c r="G30" s="69" t="s">
+      <c r="B31" s="65">
+        <f>B30*260</f>
+        <v>672100</v>
+      </c>
+      <c r="C31" s="62"/>
+      <c r="D31" s="62"/>
+      <c r="E31" s="62"/>
+      <c r="F31" s="62"/>
+      <c r="G31" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H30" s="74" t="s">
+      <c r="H31" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A31" s="72" t="s">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="B31" s="66">
-        <f>B22-B29</f>
-        <v>0</v>
-      </c>
-      <c r="C31" s="104"/>
-      <c r="D31" s="81"/>
-      <c r="F31" s="99"/>
-      <c r="G31" s="69" t="s">
+      <c r="B32" s="62">
+        <f>B23-B30</f>
+        <v>0</v>
+      </c>
+      <c r="C32" s="92"/>
+      <c r="D32" s="73"/>
+      <c r="G32" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H31" s="74" t="s">
+      <c r="H32" t="s">
         <v>132</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A32" s="72" t="s">
-        <v>125</v>
-      </c>
-      <c r="B32" s="71">
-        <f>B31*260</f>
-        <v>0</v>
-      </c>
-      <c r="C32" s="82"/>
-      <c r="D32" s="81"/>
-      <c r="G32" s="69" t="s">
-        <v>8</v>
-      </c>
-      <c r="H32" s="74" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B33" s="65">
+        <f>B32*260</f>
+        <v>0</v>
+      </c>
+      <c r="C33" s="74"/>
+      <c r="D33" s="73"/>
+      <c r="G33" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H33" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B33" s="13">
-        <f>SUM(C19:F19)</f>
+      <c r="B34" s="12">
+        <f>1-MIN(1,SUM(C20:F20))</f>
         <v>1</v>
       </c>
-      <c r="C33" s="86"/>
-      <c r="D33" s="106"/>
-      <c r="E33" s="87"/>
-      <c r="F33" s="85"/>
-      <c r="G33" s="5" t="s">
+      <c r="C34" s="77"/>
+      <c r="E34" s="78"/>
+      <c r="F34" s="73"/>
+      <c r="G34" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H33" s="6" t="s">
+      <c r="H34" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A34" s="72" t="s">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="B34" s="75">
-        <f>ROUND(B13*B33/260,)*260</f>
+      <c r="B35" s="67">
+        <f>ROUND(B14*B34/260,)*260</f>
         <v>561860</v>
       </c>
-      <c r="C34" s="85"/>
-      <c r="D34" s="81"/>
-      <c r="E34" s="85"/>
-      <c r="F34" s="4"/>
-      <c r="G34" s="69" t="s">
+      <c r="C35" s="73"/>
+      <c r="D35" s="73"/>
+      <c r="E35" s="73"/>
+      <c r="G35" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H34" s="74" t="s">
+      <c r="H35" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A35" s="72" t="s">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="B35" s="102">
-        <f>B34/260</f>
+      <c r="B36" s="90">
+        <f>B35/260</f>
         <v>2161</v>
       </c>
-      <c r="C35" s="81"/>
-      <c r="D35" s="103"/>
-      <c r="G35" s="69" t="s">
+      <c r="C36" s="73"/>
+      <c r="D36" s="91"/>
+      <c r="G36" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H35" s="74" t="s">
+      <c r="H36" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A36" s="72" t="s">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="B36" s="81">
-        <f>B34/MAX(B34,B30)</f>
-        <v>0.75506638714185881</v>
-      </c>
-      <c r="D36" s="99"/>
-      <c r="G36" s="69" t="s">
+      <c r="B37" s="73">
+        <f>B35/MAX(B35,B31)</f>
+        <v>0.83597678916827856</v>
+      </c>
+      <c r="G37" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H36" s="74" t="s">
+      <c r="H37" t="s">
         <v>124</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B37" s="14"/>
-      <c r="C37" s="15">
-        <f>C20</f>
-        <v>1431</v>
-      </c>
-      <c r="D37" s="15">
-        <f>D20</f>
-        <v>1431</v>
-      </c>
-      <c r="E37" s="15">
-        <f>E20</f>
-        <v>0</v>
-      </c>
-      <c r="F37" s="15">
-        <f>F20</f>
-        <v>0</v>
-      </c>
-      <c r="G37" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="H37" s="23" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B38" s="14"/>
-      <c r="C38" s="15">
-        <f>C26</f>
+        <v>20</v>
+      </c>
+      <c r="B38" s="13"/>
+      <c r="C38" s="14">
+        <f>C21</f>
         <v>1431</v>
       </c>
-      <c r="D38" s="15">
-        <f>D26</f>
-        <v>1431</v>
-      </c>
-      <c r="E38" s="15">
-        <f>E26</f>
-        <v>0</v>
-      </c>
-      <c r="F38" s="15">
-        <f>F26</f>
-        <v>0</v>
-      </c>
-      <c r="G38" s="16" t="s">
+      <c r="D38" s="14">
+        <f>D21</f>
+        <v>1154</v>
+      </c>
+      <c r="E38" s="14">
+        <f>E21</f>
+        <v>0</v>
+      </c>
+      <c r="F38" s="14">
+        <f>F21</f>
+        <v>0</v>
+      </c>
+      <c r="G38" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="H38" s="23" t="s">
-        <v>31</v>
+      <c r="H38" s="16" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B39" s="14"/>
-      <c r="C39" s="15">
-        <f>C37-C38</f>
-        <v>0</v>
-      </c>
-      <c r="D39" s="15">
-        <f>D37-D38</f>
-        <v>0</v>
-      </c>
-      <c r="E39" s="15">
-        <f>E37-E38</f>
-        <v>0</v>
-      </c>
-      <c r="F39" s="15">
-        <f>F37-F38</f>
-        <v>0</v>
-      </c>
-      <c r="G39" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B39" s="13"/>
+      <c r="C39" s="14">
+        <f>C27</f>
+        <v>1431</v>
+      </c>
+      <c r="D39" s="14">
+        <f>D27</f>
+        <v>1154</v>
+      </c>
+      <c r="E39" s="14">
+        <f>E27</f>
+        <v>0</v>
+      </c>
+      <c r="F39" s="14">
+        <f>F27</f>
+        <v>0</v>
+      </c>
+      <c r="G39" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="H39" s="23" t="s">
-        <v>135</v>
+      <c r="H39" s="16" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B40" s="13"/>
+      <c r="C40" s="14">
+        <f>C38-C39</f>
+        <v>0</v>
+      </c>
+      <c r="D40" s="14">
+        <f>D38-D39</f>
+        <v>0</v>
+      </c>
+      <c r="E40" s="14">
+        <f>E38-E39</f>
+        <v>0</v>
+      </c>
+      <c r="F40" s="14">
+        <f>F38-F39</f>
+        <v>0</v>
+      </c>
+      <c r="G40" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="H40" s="16" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B40" s="18" t="str">
-        <f>IF(B32&lt;=B34,"Arbeidsgiver og person blir refundert hele beløpet",IF(B30&lt;=B34,"Arbeidsgivere blir refundert hele beløpet; Person blir delvis refundert", "Arbeidsgivere blir delvis refundert"))</f>
+      <c r="B41" s="17" t="str">
+        <f>IF(B33&lt;=B35,"Arbeidsgiver og person blir refundert hele beløpet",IF(B31&lt;=B35,"Arbeidsgivere blir refundert hele beløpet; Person blir delvis refundert", "Arbeidsgivere blir delvis refundert"))</f>
         <v>Arbeidsgiver og person blir refundert hele beløpet</v>
       </c>
-      <c r="C40" s="18"/>
-      <c r="D40" s="18"/>
-      <c r="E40" s="18"/>
-      <c r="F40" s="18"/>
-      <c r="G40" s="16"/>
-      <c r="H40" s="23"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A41" s="1"/>
-      <c r="B41" s="19"/>
-      <c r="C41" s="76"/>
-      <c r="D41" s="20"/>
-      <c r="E41" s="20"/>
-      <c r="F41" s="21"/>
-      <c r="G41" s="16"/>
-      <c r="H41" s="23"/>
+      <c r="C41" s="17"/>
+      <c r="D41" s="17"/>
+      <c r="E41" s="17"/>
+      <c r="F41" s="17"/>
+      <c r="G41" s="15"/>
+      <c r="H41" s="16"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A42" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B42" s="19"/>
-      <c r="C42" s="22">
-        <f>C38*$B$36</f>
-        <v>1080.5</v>
-      </c>
-      <c r="D42" s="22">
-        <f>D38*$B$36</f>
-        <v>1080.5</v>
-      </c>
-      <c r="E42" s="22">
-        <f>E38*$B$36</f>
-        <v>0</v>
-      </c>
-      <c r="F42" s="22">
-        <f>F38*$B$36</f>
-        <v>0</v>
-      </c>
-      <c r="G42" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="H42" s="23" t="s">
-        <v>34</v>
-      </c>
+      <c r="A42" s="1"/>
+      <c r="B42" s="18"/>
+      <c r="C42" s="68"/>
+      <c r="D42" s="19"/>
+      <c r="E42" s="19"/>
+      <c r="F42" s="20"/>
+      <c r="G42" s="15"/>
+      <c r="H42" s="16"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B43" s="14"/>
-      <c r="C43" s="23">
-        <f>FLOOR(C42,1)</f>
-        <v>1080</v>
-      </c>
-      <c r="D43" s="23">
-        <f>FLOOR(D42,1)</f>
-        <v>1080</v>
-      </c>
-      <c r="E43" s="23">
-        <f>FLOOR(E42,1)</f>
-        <v>0</v>
-      </c>
-      <c r="F43" s="23">
-        <f>FLOOR(F42,1)</f>
-        <v>0</v>
-      </c>
-      <c r="G43" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="H43" s="23" t="s">
-        <v>36</v>
+        <v>34</v>
+      </c>
+      <c r="B43" s="18"/>
+      <c r="C43" s="21">
+        <f>C39*$B$37</f>
+        <v>1196.2827852998066</v>
+      </c>
+      <c r="D43" s="21">
+        <f>D39*$B$37</f>
+        <v>964.71721470019349</v>
+      </c>
+      <c r="E43" s="21">
+        <f>E39*$B$37</f>
+        <v>0</v>
+      </c>
+      <c r="F43" s="21">
+        <f>F39*$B$37</f>
+        <v>0</v>
+      </c>
+      <c r="G43" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="H43" s="16" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="B44" s="14">
-        <f>SUM(C43:F43)</f>
-        <v>2160</v>
-      </c>
-      <c r="C44" s="24"/>
-      <c r="D44" s="23"/>
-      <c r="E44" s="23"/>
-      <c r="F44" s="23"/>
-      <c r="G44" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="B44" s="13"/>
+      <c r="C44" s="16">
+        <f>FLOOR(C43,1)</f>
+        <v>1196</v>
+      </c>
+      <c r="D44" s="16">
+        <f>FLOOR(D43,1)</f>
+        <v>964</v>
+      </c>
+      <c r="E44" s="16">
+        <f>FLOOR(E43,1)</f>
+        <v>0</v>
+      </c>
+      <c r="F44" s="16">
+        <f>FLOOR(F43,1)</f>
+        <v>0</v>
+      </c>
+      <c r="G44" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="H44" s="23" t="s">
-        <v>137</v>
+      <c r="H44" s="16" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="B45" s="91">
-        <f>SUM(C42:F42)-B44</f>
-        <v>1</v>
-      </c>
-      <c r="C45" s="89"/>
-      <c r="D45" s="89"/>
-      <c r="E45" s="89"/>
-      <c r="F45" s="89"/>
-      <c r="G45" s="90" t="s">
-        <v>8</v>
-      </c>
-      <c r="H45" s="89" t="s">
-        <v>43</v>
+        <v>136</v>
+      </c>
+      <c r="B45" s="13">
+        <f>SUM(C44:F44)</f>
+        <v>2160</v>
+      </c>
+      <c r="C45" s="22"/>
+      <c r="D45" s="16"/>
+      <c r="E45" s="16"/>
+      <c r="F45" s="16"/>
+      <c r="G45" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="H45" s="16" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B46" s="29">
-        <f>ROUND(B45,)</f>
+        <v>148</v>
+      </c>
+      <c r="B46" s="82">
+        <f>SUM(C43:F43)-B45</f>
         <v>1</v>
       </c>
-      <c r="C46" s="23"/>
-      <c r="D46" s="23"/>
-      <c r="E46" s="23"/>
-      <c r="F46" s="23"/>
-      <c r="G46" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="H46" s="23" t="s">
+      <c r="C46" s="80"/>
+      <c r="D46" s="80"/>
+      <c r="E46" s="80"/>
+      <c r="F46" s="80"/>
+      <c r="G46" s="81" t="s">
+        <v>8</v>
+      </c>
+      <c r="H46" s="80" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B47" s="14">
-        <f>B44+B46</f>
-        <v>2161</v>
-      </c>
-      <c r="C47" s="24"/>
-      <c r="D47" s="23"/>
-      <c r="E47" s="23"/>
-      <c r="F47" s="23"/>
-      <c r="G47" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="B47" s="27">
+        <f>ROUND(B46,)</f>
+        <v>1</v>
+      </c>
+      <c r="C47" s="16"/>
+      <c r="D47" s="16"/>
+      <c r="E47" s="16"/>
+      <c r="F47" s="16"/>
+      <c r="G47" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="H47" s="23" t="s">
-        <v>138</v>
+      <c r="H47" s="16" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B48" s="14">
-        <f>B47*260</f>
-        <v>561860</v>
-      </c>
-      <c r="C48" s="24"/>
-      <c r="D48" s="23"/>
-      <c r="E48" s="23"/>
-      <c r="F48" s="23"/>
-      <c r="G48" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="B48" s="13">
+        <f>B45+B47</f>
+        <v>2161</v>
+      </c>
+      <c r="C48" s="22"/>
+      <c r="D48" s="16"/>
+      <c r="E48" s="16"/>
+      <c r="F48" s="16"/>
+      <c r="G48" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="H48" s="23" t="s">
-        <v>139</v>
+      <c r="H48" s="16" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B49" s="14"/>
-      <c r="C49" s="22">
-        <f>C42-TRUNC(C42)</f>
-        <v>0.5</v>
-      </c>
-      <c r="D49" s="22">
-        <f>D42-TRUNC(D42)</f>
-        <v>0.5</v>
-      </c>
-      <c r="E49" s="22">
-        <f>E42-TRUNC(E42)</f>
-        <v>0</v>
-      </c>
-      <c r="F49" s="22">
-        <f>F42-TRUNC(F42)</f>
-        <v>0</v>
-      </c>
-      <c r="G49" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="H49" s="23" t="s">
-        <v>38</v>
+        <v>125</v>
+      </c>
+      <c r="B49" s="13">
+        <f>B48*260</f>
+        <v>561860</v>
+      </c>
+      <c r="C49" s="22"/>
+      <c r="D49" s="16"/>
+      <c r="E49" s="16"/>
+      <c r="F49" s="16"/>
+      <c r="G49" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="H49" s="16" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B50" s="13"/>
+      <c r="C50" s="21">
+        <f>C43-TRUNC(C43)</f>
+        <v>0.28278529980661915</v>
+      </c>
+      <c r="D50" s="21">
+        <f>D43-TRUNC(D43)</f>
+        <v>0.71721470019349454</v>
+      </c>
+      <c r="E50" s="21">
+        <f>E43-TRUNC(E43)</f>
+        <v>0</v>
+      </c>
+      <c r="F50" s="21">
+        <f>F43-TRUNC(F43)</f>
+        <v>0</v>
+      </c>
+      <c r="G50" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="H50" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B50" s="14"/>
-      <c r="C50" s="24">
-        <f>IF($B$46&gt;0,IF(LARGE($C$49:$F$49,$B$46)&lt;=C$49,1,0), 0)</f>
+      <c r="B51" s="13"/>
+      <c r="C51" s="22">
+        <f>IF($B$47&gt;0,IF(LARGE($C$50:$F$50,$B$47)&lt;=C$50,1,0), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="D51" s="22">
+        <f>IF(($B$47-C51)&gt;0,IF(LARGE($C$50:$F$50,$B$47)&lt;=D$50,1,0), 0)</f>
         <v>1</v>
       </c>
-      <c r="D50" s="24">
-        <f>IF(($B$46-C50)&gt;0,IF(LARGE($C$49:$F$49,$B$46)&lt;=D$49,1,0), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="E50" s="24">
-        <f>IF(($B$46-SUM($C$50:$D$50))&gt;0,IF(LARGE($C$49:$F$49,$B$46)&lt;=E$49,1,0), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="F50" s="24">
-        <f>IF(($B$46-SUM($C$50:$D$51))&gt;0,IF(LARGE($C$49:$F$49,$B$46)&lt;=F$49,1,0), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="G50" s="16" t="s">
+      <c r="E51" s="22">
+        <f>IF(($B$47-SUM($C$51:$D$51))&gt;0,IF(LARGE($C$50:$F$50,$B$47)&lt;=E$50,1,0), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="F51" s="22">
+        <f>IF(($B$47-SUM($C$51:$D$52))&gt;0,IF(LARGE($C$50:$F$50,$B$47)&lt;=F$50,1,0), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="G51" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="H50" s="23" t="s">
+      <c r="H51" s="16" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A51" s="25" t="s">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A52" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="B51" s="26"/>
-      <c r="C51" s="27">
-        <f>C43+C50</f>
-        <v>1081</v>
-      </c>
-      <c r="D51" s="27">
-        <f>D43+D50</f>
-        <v>1080</v>
-      </c>
-      <c r="E51" s="27">
-        <f>E43+E50</f>
-        <v>0</v>
-      </c>
-      <c r="F51" s="27">
-        <f>F43+F50</f>
-        <v>0</v>
-      </c>
-      <c r="G51" s="28" t="s">
+      <c r="B52" s="24"/>
+      <c r="C52" s="25">
+        <f>C44+C51</f>
+        <v>1196</v>
+      </c>
+      <c r="D52" s="25">
+        <f>D44+D51</f>
+        <v>965</v>
+      </c>
+      <c r="E52" s="25">
+        <f>E44+E51</f>
+        <v>0</v>
+      </c>
+      <c r="F52" s="25">
+        <f>F44+F51</f>
+        <v>0</v>
+      </c>
+      <c r="G52" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="H51" s="25" t="s">
+      <c r="H52" s="23" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A52" s="1"/>
-      <c r="B52" s="84"/>
-      <c r="C52" s="22"/>
-      <c r="D52" s="22"/>
-      <c r="E52" s="22"/>
-      <c r="F52" s="22"/>
-      <c r="G52" s="16"/>
-      <c r="H52" s="23"/>
-    </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A53" s="1" t="s">
+      <c r="A53" s="1"/>
+      <c r="B53" s="76"/>
+      <c r="C53" s="21"/>
+      <c r="D53" s="21"/>
+      <c r="E53" s="21"/>
+      <c r="F53" s="21"/>
+      <c r="G53" s="15"/>
+      <c r="H53" s="16"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B53" s="32">
-        <f>ROUND((B34-B48)/260,)</f>
-        <v>0</v>
-      </c>
-      <c r="C53" s="14"/>
-      <c r="D53" s="14"/>
-      <c r="E53" s="14"/>
-      <c r="F53" s="14"/>
-      <c r="G53" s="16" t="s">
+      <c r="B54" s="30">
+        <f>ROUND((B35-B49)/260,)</f>
+        <v>0</v>
+      </c>
+      <c r="C54" s="13"/>
+      <c r="D54" s="13"/>
+      <c r="E54" s="13"/>
+      <c r="F54" s="13"/>
+      <c r="G54" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="H53" s="23" t="s">
+      <c r="H54" s="16" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A54" s="77" t="s">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A55" s="69" t="s">
         <v>140</v>
       </c>
-      <c r="B54" s="83">
-        <f>IF(B31 &gt; 0, MIN(1,B53/B31), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="C54" s="79"/>
-      <c r="D54" s="78"/>
-      <c r="E54" s="78"/>
-      <c r="F54" s="78"/>
-      <c r="G54" s="80" t="s">
+      <c r="B55" s="75">
+        <f>IF(B32 &gt; 0, MIN(1,B54/B32), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="C55" s="71"/>
+      <c r="D55" s="70"/>
+      <c r="E55" s="70"/>
+      <c r="F55" s="70"/>
+      <c r="G55" s="72" t="s">
         <v>8</v>
       </c>
-      <c r="H54" s="78"/>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A55" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B55" s="30"/>
-      <c r="C55" s="15">
-        <f>C39*$B$54</f>
-        <v>0</v>
-      </c>
-      <c r="D55" s="15">
-        <f>D39*$B$54</f>
-        <v>0</v>
-      </c>
-      <c r="E55" s="15">
-        <f>E39*$B$54</f>
-        <v>0</v>
-      </c>
-      <c r="F55" s="15">
-        <f>F39*$B$54</f>
-        <v>0</v>
-      </c>
-      <c r="G55" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="H55" s="23" t="s">
-        <v>46</v>
-      </c>
+      <c r="H55" s="70"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B56" s="23"/>
-      <c r="C56" s="31">
-        <f>FLOOR(C55, 1)</f>
-        <v>0</v>
-      </c>
-      <c r="D56" s="31">
-        <f>FLOOR(D55, 1)</f>
-        <v>0</v>
-      </c>
-      <c r="E56" s="31">
-        <f>FLOOR(E55, 1)</f>
-        <v>0</v>
-      </c>
-      <c r="F56" s="31">
-        <f>FLOOR(F55, 1)</f>
-        <v>0</v>
-      </c>
-      <c r="G56" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="H56" s="23"/>
+        <v>45</v>
+      </c>
+      <c r="B56" s="28"/>
+      <c r="C56" s="14">
+        <f>C40*$B$55</f>
+        <v>0</v>
+      </c>
+      <c r="D56" s="14">
+        <f>D40*$B$55</f>
+        <v>0</v>
+      </c>
+      <c r="E56" s="14">
+        <f>E40*$B$55</f>
+        <v>0</v>
+      </c>
+      <c r="F56" s="14">
+        <f>F40*$B$55</f>
+        <v>0</v>
+      </c>
+      <c r="G56" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="H56" s="16" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B57" s="35">
-        <f>B53-SUM(C56:F56)</f>
-        <v>0</v>
-      </c>
-      <c r="C57" s="23"/>
-      <c r="D57" s="23"/>
-      <c r="E57" s="23"/>
-      <c r="F57" s="23"/>
-      <c r="G57" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B57" s="16"/>
+      <c r="C57" s="29">
+        <f>FLOOR(C56, 1)</f>
+        <v>0</v>
+      </c>
+      <c r="D57" s="29">
+        <f>FLOOR(D56, 1)</f>
+        <v>0</v>
+      </c>
+      <c r="E57" s="29">
+        <f>FLOOR(E56, 1)</f>
+        <v>0</v>
+      </c>
+      <c r="F57" s="29">
+        <f>FLOOR(F56, 1)</f>
+        <v>0</v>
+      </c>
+      <c r="G57" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="H57" s="23" t="s">
-        <v>52</v>
-      </c>
+      <c r="H57" s="16"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B58" s="32"/>
-      <c r="C58" s="22">
-        <f>C55-TRUNC(C56)</f>
-        <v>0</v>
-      </c>
-      <c r="D58" s="22">
-        <f>D55-TRUNC(D56)</f>
-        <v>0</v>
-      </c>
-      <c r="E58" s="22">
-        <f>E55-TRUNC(E56)</f>
-        <v>0</v>
-      </c>
-      <c r="F58" s="22">
-        <f>F55-TRUNC(F56)</f>
-        <v>0</v>
-      </c>
-      <c r="G58" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="H58" s="23" t="s">
-        <v>48</v>
+        <v>51</v>
+      </c>
+      <c r="B58" s="33">
+        <f>B54-SUM(C57:F57)</f>
+        <v>0</v>
+      </c>
+      <c r="C58" s="16"/>
+      <c r="D58" s="16"/>
+      <c r="E58" s="16"/>
+      <c r="F58" s="16"/>
+      <c r="G58" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="H58" s="16" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B59" s="30"/>
+      <c r="C59" s="21">
+        <f>C56-TRUNC(C57)</f>
+        <v>0</v>
+      </c>
+      <c r="D59" s="21">
+        <f>D56-TRUNC(D57)</f>
+        <v>0</v>
+      </c>
+      <c r="E59" s="21">
+        <f>E56-TRUNC(E57)</f>
+        <v>0</v>
+      </c>
+      <c r="F59" s="21">
+        <f>F56-TRUNC(F57)</f>
+        <v>0</v>
+      </c>
+      <c r="G59" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="H59" s="16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A60" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B59" s="32"/>
-      <c r="C59" s="24">
-        <f>IF($B$57&gt;0, IF(LARGE($C$58:$F$58,$B$57)&lt;=C$58,1,0), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="D59" s="24">
-        <f>IF($B$57&gt;0, IF(LARGE($C$58:$F$58,$B$57)&lt;=D$58,1,0), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="E59" s="24">
-        <f>IF($B$57&gt;0, IF(LARGE($C$58:$F$58,$B$57)&lt;=E$58,1,0), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="F59" s="24">
-        <f>IF($B$57&gt;0, IF(LARGE($C$58:$F$58,$B$57)&lt;=F$58,1,0), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="G59" s="16" t="s">
+      <c r="B60" s="30"/>
+      <c r="C60" s="22">
+        <f>IF($B$58&gt;0, IF(LARGE($C$59:$F$59,$B$58)&lt;=C$59,1,0), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="D60" s="22">
+        <f>IF($B$58&gt;0, IF(LARGE($C$59:$F$59,$B$58)&lt;=D$59,1,0), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="E60" s="22">
+        <f>IF($B$58&gt;0, IF(LARGE($C$59:$F$59,$B$58)&lt;=E$59,1,0), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="F60" s="22">
+        <f>IF($B$58&gt;0, IF(LARGE($C$59:$F$59,$B$58)&lt;=F$59,1,0), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="G60" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="H59" s="23"/>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A60" s="25" t="s">
+      <c r="H60" s="16"/>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A61" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="B60" s="33"/>
-      <c r="C60" s="27">
-        <f>C56+C59</f>
-        <v>0</v>
-      </c>
-      <c r="D60" s="27">
-        <f>D56+D59</f>
-        <v>0</v>
-      </c>
-      <c r="E60" s="27">
-        <f>E56+E59</f>
-        <v>0</v>
-      </c>
-      <c r="F60" s="27">
-        <f>F56+F59</f>
-        <v>0</v>
-      </c>
-      <c r="G60" s="28" t="s">
+      <c r="B61" s="31"/>
+      <c r="C61" s="25">
+        <f>C57+C60</f>
+        <v>0</v>
+      </c>
+      <c r="D61" s="25">
+        <f>D57+D60</f>
+        <v>0</v>
+      </c>
+      <c r="E61" s="25">
+        <f>E57+E60</f>
+        <v>0</v>
+      </c>
+      <c r="F61" s="25">
+        <f>F57+F60</f>
+        <v>0</v>
+      </c>
+      <c r="G61" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="H60" s="34"/>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A61" s="1"/>
-      <c r="B61" s="32"/>
-      <c r="C61" s="24"/>
-      <c r="D61" s="24"/>
-      <c r="E61" s="24"/>
-      <c r="F61" s="24"/>
-      <c r="G61" s="16"/>
-      <c r="H61" s="23"/>
+      <c r="H61" s="32"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" s="1"/>
-      <c r="B62" s="32"/>
-      <c r="C62" s="23"/>
-      <c r="D62" s="23"/>
-      <c r="E62" s="23"/>
-      <c r="F62" s="23"/>
-      <c r="G62" s="16"/>
-      <c r="H62" s="23"/>
+      <c r="B62" s="30"/>
+      <c r="C62" s="22"/>
+      <c r="D62" s="22"/>
+      <c r="E62" s="22"/>
+      <c r="F62" s="22"/>
+      <c r="G62" s="15"/>
+      <c r="H62" s="16"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A63" s="25" t="s">
+      <c r="A63" s="1"/>
+      <c r="B63" s="30"/>
+      <c r="C63" s="16"/>
+      <c r="D63" s="16"/>
+      <c r="E63" s="16"/>
+      <c r="F63" s="16"/>
+      <c r="G63" s="15"/>
+      <c r="H63" s="16"/>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A64" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="B63" s="36">
-        <f>B47+B53</f>
+      <c r="B64" s="34">
+        <f>B48+B54</f>
         <v>2161</v>
       </c>
-      <c r="C63" s="34"/>
-      <c r="D63" s="34"/>
-      <c r="E63" s="34"/>
-      <c r="F63" s="34"/>
-      <c r="G63" s="37"/>
-      <c r="H63" s="34"/>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="H64" s="4"/>
+      <c r="C64" s="32"/>
+      <c r="D64" s="32"/>
+      <c r="E64" s="32"/>
+      <c r="F64" s="32"/>
+      <c r="G64" s="35"/>
+      <c r="H64" s="32"/>
     </row>
   </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2" xr:uid="{F6473A73-E798-8B4E-9BD5-79C536C252F3}">
+      <formula1>"Nei, Ja"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:F2" xr:uid="{9F11E83E-224A-EB44-9967-5889595FBD51}">
+      <formula1>"Nei,Ja"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <ignoredErrors>
-    <ignoredError sqref="B24" formula="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
 
@@ -2586,725 +2609,725 @@
     <col min="5" max="5" width="16.33203125" customWidth="1"/>
     <col min="6" max="6" width="17.33203125" customWidth="1"/>
     <col min="7" max="7" width="15.6640625" customWidth="1"/>
-    <col min="8" max="8" width="8.6640625" style="39" customWidth="1"/>
+    <col min="8" max="8" width="8.6640625" style="4" customWidth="1"/>
     <col min="9" max="9" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="42" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="40" t="s">
+    <row r="1" spans="1:9" s="39" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="37" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="40" t="s">
+      <c r="C1" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="D1" s="41" t="s">
+      <c r="D1" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="E1" s="41" t="s">
+      <c r="E1" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="F1" s="41" t="s">
+      <c r="F1" s="38" t="s">
         <v>61</v>
       </c>
-      <c r="G1" s="41" t="s">
+      <c r="G1" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="H1" s="41" t="s">
+      <c r="H1" s="38" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="42"/>
+      <c r="A2" s="39"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="39" t="s">
         <v>7</v>
       </c>
       <c r="B3" t="s">
         <v>64</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="6">
         <v>21000</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="6">
         <v>10000</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="6">
         <v>31000</v>
       </c>
-      <c r="G3" s="7">
-        <v>0</v>
-      </c>
-      <c r="H3" s="39" t="s">
+      <c r="G3" s="6">
+        <v>0</v>
+      </c>
+      <c r="H3" s="4" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="42"/>
+      <c r="A4" s="39"/>
       <c r="B4" t="s">
         <v>66</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="7">
         <f>D3/SUM($D$3:$G$3)</f>
         <v>0.33870967741935482</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="7">
         <f>E3/SUM($D$3:$G$3)</f>
         <v>0.16129032258064516</v>
       </c>
-      <c r="F4" s="8">
+      <c r="F4" s="7">
         <f>F3/SUM($D$3:$G$3)</f>
         <v>0.5</v>
       </c>
-      <c r="G4" s="8">
+      <c r="G4" s="7">
         <f>G3/SUM($D$3:$G$3)</f>
         <v>0</v>
       </c>
-      <c r="H4" s="39" t="s">
+      <c r="H4" s="4" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="42" t="s">
+      <c r="A5" s="39" t="s">
         <v>11</v>
       </c>
       <c r="B5" t="s">
         <v>67</v>
       </c>
-      <c r="D5" s="43">
+      <c r="D5" s="40">
         <f>D3*12/260</f>
         <v>969.23076923076928</v>
       </c>
-      <c r="E5" s="43">
+      <c r="E5" s="40">
         <f>E3*12/260</f>
         <v>461.53846153846155</v>
       </c>
-      <c r="F5" s="43">
+      <c r="F5" s="40">
         <f>F3*12/260</f>
         <v>1430.7692307692307</v>
       </c>
-      <c r="G5" s="43">
+      <c r="G5" s="40">
         <f>G3*12/260</f>
         <v>0</v>
       </c>
-      <c r="H5" s="39" t="s">
+      <c r="H5" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="I5" s="44" t="s">
+      <c r="I5" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="42" t="s">
+      <c r="A6" s="39" t="s">
         <v>13</v>
       </c>
       <c r="B6" t="s">
         <v>69</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="9">
         <v>1</v>
       </c>
-      <c r="E6" s="10">
+      <c r="E6" s="9">
         <v>1</v>
       </c>
-      <c r="F6" s="10">
+      <c r="F6" s="9">
         <v>1</v>
       </c>
-      <c r="G6" s="10">
+      <c r="G6" s="9">
         <v>1</v>
       </c>
-      <c r="H6" s="39" t="s">
+      <c r="H6" s="4" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="42" t="s">
+      <c r="A7" s="39" t="s">
         <v>16</v>
       </c>
       <c r="B7" t="s">
         <v>71</v>
       </c>
-      <c r="D7" s="43">
+      <c r="D7" s="40">
         <f>D5*D6</f>
         <v>969.23076923076928</v>
       </c>
-      <c r="E7" s="43">
+      <c r="E7" s="40">
         <f>E5*E6</f>
         <v>461.53846153846155</v>
       </c>
-      <c r="F7" s="43">
+      <c r="F7" s="40">
         <f>F5*F6</f>
         <v>1430.7692307692307</v>
       </c>
-      <c r="G7" s="43">
+      <c r="G7" s="40">
         <f>G5*G6</f>
         <v>0</v>
       </c>
-      <c r="H7" s="39" t="s">
+      <c r="H7" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="I7" s="45" t="s">
+      <c r="I7" s="41" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="42" t="s">
+      <c r="A8" s="39" t="s">
         <v>17</v>
       </c>
       <c r="B8" t="s">
         <v>73</v>
       </c>
-      <c r="D8" s="11">
+      <c r="D8" s="10">
         <f>MIN(D7,$C$15)</f>
         <v>969.23076923076928</v>
       </c>
-      <c r="E8" s="11">
+      <c r="E8" s="10">
         <f>MIN(E7,$C$15)</f>
         <v>461.53846153846155</v>
       </c>
-      <c r="F8" s="11">
+      <c r="F8" s="10">
         <f>MIN(F7,$C$15)</f>
         <v>1430.7692307692307</v>
       </c>
-      <c r="G8" s="11">
+      <c r="G8" s="10">
         <f>MIN(G7,$C$15)</f>
         <v>0</v>
       </c>
-      <c r="H8" s="39" t="s">
+      <c r="H8" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="I8" s="44" t="s">
+      <c r="I8" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="42" t="s">
+      <c r="A9" s="39" t="s">
         <v>18</v>
       </c>
       <c r="B9" t="s">
         <v>74</v>
       </c>
-      <c r="D9" s="12">
+      <c r="D9" s="11">
         <v>0.5</v>
       </c>
-      <c r="E9" s="12">
+      <c r="E9" s="11">
         <v>0.8</v>
       </c>
-      <c r="F9" s="12">
+      <c r="F9" s="11">
         <v>0.2</v>
       </c>
-      <c r="G9" s="12">
+      <c r="G9" s="11">
         <v>1</v>
       </c>
-      <c r="H9" s="39" t="s">
+      <c r="H9" s="4" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="42" t="s">
+      <c r="A10" s="39" t="s">
         <v>20</v>
       </c>
       <c r="B10" t="s">
         <v>75</v>
       </c>
-      <c r="D10" s="43">
+      <c r="D10" s="40">
         <f>D7*D9</f>
         <v>484.61538461538464</v>
       </c>
-      <c r="E10" s="43">
+      <c r="E10" s="40">
         <f>E7*E9</f>
         <v>369.23076923076928</v>
       </c>
-      <c r="F10" s="43">
+      <c r="F10" s="40">
         <f>F7*F9</f>
         <v>286.15384615384613</v>
       </c>
-      <c r="G10" s="43">
+      <c r="G10" s="40">
         <f>G7*G9</f>
         <v>0</v>
       </c>
-      <c r="H10" s="39" t="s">
+      <c r="H10" s="4" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="42" t="s">
+      <c r="A11" s="39" t="s">
         <v>21</v>
       </c>
       <c r="B11" t="s">
         <v>76</v>
       </c>
-      <c r="D11" s="10">
+      <c r="D11" s="9">
         <v>1</v>
       </c>
-      <c r="E11" s="10">
+      <c r="E11" s="9">
         <v>0.9</v>
       </c>
-      <c r="F11" s="10">
+      <c r="F11" s="9">
         <v>0.25</v>
       </c>
-      <c r="G11" s="10">
+      <c r="G11" s="9">
         <v>1</v>
       </c>
-      <c r="H11" s="39" t="s">
+      <c r="H11" s="4" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="42" t="s">
+      <c r="A12" s="39" t="s">
         <v>22</v>
       </c>
       <c r="B12" t="s">
         <v>77</v>
       </c>
-      <c r="D12" s="46">
+      <c r="D12" s="42">
         <f>D10*D11</f>
         <v>484.61538461538464</v>
       </c>
-      <c r="E12" s="46">
+      <c r="E12" s="42">
         <f>E10*E11</f>
         <v>332.30769230769238</v>
       </c>
-      <c r="F12" s="46">
+      <c r="F12" s="42">
         <f>F10*F11</f>
         <v>71.538461538461533</v>
       </c>
-      <c r="G12" s="46">
+      <c r="G12" s="42">
         <f>G10*G11</f>
         <v>0</v>
       </c>
-      <c r="H12" s="39" t="s">
+      <c r="H12" s="4" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="42" t="s">
+      <c r="A13" s="39" t="s">
         <v>23</v>
       </c>
       <c r="B13" t="s">
         <v>78</v>
       </c>
-      <c r="C13" s="47">
+      <c r="C13" s="43">
         <f>ROUND(SUM(D10:G10)/SUM(D7:G7),2)</f>
         <v>0.4</v>
       </c>
-      <c r="H13" s="39" t="s">
+      <c r="H13" s="4" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="42" t="s">
+      <c r="A14" s="39" t="s">
         <v>25</v>
       </c>
       <c r="B14" t="s">
         <v>79</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C14" s="6">
         <v>93634</v>
       </c>
-      <c r="H14" s="39" t="s">
+      <c r="H14" s="4" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="42" t="s">
+      <c r="A15" s="39" t="s">
         <v>27</v>
       </c>
       <c r="B15" t="s">
         <v>80</v>
       </c>
-      <c r="C15" s="11">
+      <c r="C15" s="10">
         <f>ROUND(6*C14/260, 0)</f>
         <v>2161</v>
       </c>
-      <c r="H15" s="39" t="s">
+      <c r="H15" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="I15" s="44" t="s">
+      <c r="I15" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="42" t="s">
+      <c r="A16" s="39" t="s">
         <v>28</v>
       </c>
       <c r="B16" t="s">
         <v>81</v>
       </c>
-      <c r="C16" s="11">
+      <c r="C16" s="10">
         <f>ROUND(C13*C15,0)</f>
         <v>864</v>
       </c>
-      <c r="H16" s="39" t="s">
+      <c r="H16" s="4" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="48" t="s">
+      <c r="A17" s="44" t="s">
         <v>82</v>
       </c>
-      <c r="B17" s="49" t="s">
+      <c r="B17" s="45" t="s">
         <v>83</v>
       </c>
-      <c r="C17" s="50">
+      <c r="C17" s="46">
         <f>MIN(1, C16/SUM(D10:G10))</f>
         <v>0.75789473684210529</v>
       </c>
-      <c r="D17" s="51"/>
-      <c r="E17" s="51"/>
-      <c r="F17" s="51"/>
-      <c r="G17" s="51"/>
-      <c r="H17" s="52" t="s">
+      <c r="D17" s="47"/>
+      <c r="E17" s="47"/>
+      <c r="F17" s="47"/>
+      <c r="G17" s="47"/>
+      <c r="H17" s="48" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="48" t="s">
+      <c r="A18" s="44" t="s">
         <v>84</v>
       </c>
-      <c r="B18" s="49" t="s">
+      <c r="B18" s="45" t="s">
         <v>85</v>
       </c>
-      <c r="C18" s="49"/>
-      <c r="D18" s="51">
+      <c r="C18" s="45"/>
+      <c r="D18" s="47">
         <f>D10*ScalingFactor</f>
         <v>367.28744939271257</v>
       </c>
-      <c r="E18" s="51">
+      <c r="E18" s="47">
         <f>E10*ScalingFactor</f>
         <v>279.83805668016197</v>
       </c>
-      <c r="F18" s="51">
+      <c r="F18" s="47">
         <f>F10*ScalingFactor</f>
         <v>216.87449392712549</v>
       </c>
-      <c r="G18" s="51">
+      <c r="G18" s="47">
         <f>G10*ScalingFactor</f>
         <v>0</v>
       </c>
-      <c r="H18" s="52" t="s">
+      <c r="H18" s="48" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="48" t="s">
+      <c r="A19" s="44" t="s">
         <v>86</v>
       </c>
-      <c r="B19" s="49" t="s">
+      <c r="B19" s="45" t="s">
         <v>87</v>
       </c>
-      <c r="C19" s="49"/>
-      <c r="D19" s="51">
+      <c r="C19" s="45"/>
+      <c r="D19" s="47">
         <f>MIN(D18,D12)</f>
         <v>367.28744939271257</v>
       </c>
-      <c r="E19" s="51">
+      <c r="E19" s="47">
         <f>MIN(E18,E12)</f>
         <v>279.83805668016197</v>
       </c>
-      <c r="F19" s="51">
+      <c r="F19" s="47">
         <f>MIN(F18,F12)</f>
         <v>71.538461538461533</v>
       </c>
-      <c r="G19" s="51">
+      <c r="G19" s="47">
         <f>MIN(G18,G12)</f>
         <v>0</v>
       </c>
-      <c r="H19" s="52" t="s">
+      <c r="H19" s="48" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="48"/>
-      <c r="B20" s="49" t="s">
+      <c r="A20" s="44"/>
+      <c r="B20" s="45" t="s">
         <v>88</v>
       </c>
-      <c r="C20" s="49"/>
-      <c r="D20" s="51">
+      <c r="C20" s="45"/>
+      <c r="D20" s="47">
         <f>D19-D12</f>
         <v>-117.32793522267207</v>
       </c>
-      <c r="E20" s="51">
+      <c r="E20" s="47">
         <f>E19-E12</f>
         <v>-52.469635627530408</v>
       </c>
-      <c r="F20" s="51">
+      <c r="F20" s="47">
         <f>F19-F12</f>
         <v>0</v>
       </c>
-      <c r="G20" s="51">
+      <c r="G20" s="47">
         <f>G19-G12</f>
         <v>0</v>
       </c>
-      <c r="H20" s="52" t="s">
+      <c r="H20" s="48" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="48"/>
-      <c r="B21" s="49" t="s">
+      <c r="A21" s="44"/>
+      <c r="B21" s="45" t="s">
         <v>89</v>
       </c>
-      <c r="C21" s="49"/>
-      <c r="D21" s="50">
+      <c r="C21" s="45"/>
+      <c r="D21" s="46">
         <f>IF(D20 &lt; 0, D4, 0)</f>
         <v>0.33870967741935482</v>
       </c>
-      <c r="E21" s="50">
+      <c r="E21" s="46">
         <f>IF(E20 &lt; 0, E4, 0)</f>
         <v>0.16129032258064516</v>
       </c>
-      <c r="F21" s="50">
+      <c r="F21" s="46">
         <f>IF(F20 &lt; 0, F4, 0)</f>
         <v>0</v>
       </c>
-      <c r="G21" s="51"/>
-      <c r="H21" s="52" t="s">
+      <c r="G21" s="47"/>
+      <c r="H21" s="48" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="22" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="48" t="s">
+      <c r="A22" s="44" t="s">
         <v>90</v>
       </c>
-      <c r="B22" s="49" t="s">
+      <c r="B22" s="45" t="s">
         <v>91</v>
       </c>
-      <c r="C22" s="49"/>
-      <c r="D22" s="50">
+      <c r="C22" s="45"/>
+      <c r="D22" s="46">
         <f>IF(SUM(ShortfallIncomeRatioArb)=0,0,D21/SUM(ShortfallIncomeRatioArb))</f>
         <v>0.67741935483870963</v>
       </c>
-      <c r="E22" s="50">
+      <c r="E22" s="46">
         <f>IF(SUM(ShortfallIncomeRatioArb)=0,0,E21/SUM(ShortfallIncomeRatioArb))</f>
         <v>0.32258064516129031</v>
       </c>
-      <c r="F22" s="50">
+      <c r="F22" s="46">
         <f>IF(SUM(ShortfallIncomeRatioArb)=0,0,F21/SUM(ShortfallIncomeRatioArb))</f>
         <v>0</v>
       </c>
-      <c r="G22" s="50">
+      <c r="G22" s="46">
         <f>IF(SUM(ShortfallIncomeRatioArb)=0,0,G21/SUM(ShortfallIncomeRatioArb))</f>
         <v>0</v>
       </c>
-      <c r="H22" s="52" t="s">
+      <c r="H22" s="48" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="23" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="48"/>
-      <c r="B23" s="49" t="s">
+      <c r="A23" s="44"/>
+      <c r="B23" s="45" t="s">
         <v>92</v>
       </c>
-      <c r="C23" s="49"/>
-      <c r="D23" s="51">
+      <c r="C23" s="45"/>
+      <c r="D23" s="47">
         <f>D18-D19</f>
         <v>0</v>
       </c>
-      <c r="E23" s="51">
+      <c r="E23" s="47">
         <f>E18-E19</f>
         <v>0</v>
       </c>
-      <c r="F23" s="51">
+      <c r="F23" s="47">
         <f>F18-F19</f>
         <v>145.33603238866397</v>
       </c>
-      <c r="G23" s="51">
+      <c r="G23" s="47">
         <f>G18-G19</f>
         <v>0</v>
       </c>
-      <c r="H23" s="52" t="s">
+      <c r="H23" s="48" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="48" t="s">
+      <c r="A24" s="44" t="s">
         <v>93</v>
       </c>
-      <c r="B24" s="49" t="s">
+      <c r="B24" s="45" t="s">
         <v>94</v>
       </c>
-      <c r="C24" s="49"/>
-      <c r="D24" s="51">
+      <c r="C24" s="45"/>
+      <c r="D24" s="47">
         <f>MIN(-D20,IF(SUM($D$20:$G$20)&gt;=0, 0, SUM($D$23:$G$23)*D22))</f>
         <v>98.453441295546554</v>
       </c>
-      <c r="E24" s="51">
+      <c r="E24" s="47">
         <f>MIN(-E20,IF(SUM($D$20:$G$20)&gt;=0, 0, SUM($D$23:$G$23)*E22))</f>
         <v>46.882591093117405</v>
       </c>
-      <c r="F24" s="51">
+      <c r="F24" s="47">
         <f>MIN(-F20,IF(SUM($D$20:$G$20)&gt;=0, 0, SUM($D$23:$G$23)*F22))</f>
         <v>0</v>
       </c>
-      <c r="G24" s="51">
+      <c r="G24" s="47">
         <f>MIN(-G20,IF(SUM($D$20:$G$20)&gt;=0, 0, SUM($D$23:$G$23)*G22))</f>
         <v>0</v>
       </c>
-      <c r="H24" s="52" t="s">
+      <c r="H24" s="48" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="25" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="48"/>
-      <c r="B25" s="49" t="s">
+      <c r="A25" s="44"/>
+      <c r="B25" s="45" t="s">
         <v>95</v>
       </c>
-      <c r="C25" s="49"/>
-      <c r="D25" s="50">
+      <c r="C25" s="45"/>
+      <c r="D25" s="46">
         <f>IF(D23 = 0, 0, D4)</f>
         <v>0</v>
       </c>
-      <c r="E25" s="50">
+      <c r="E25" s="46">
         <f>IF(E23 = 0, 0, E4)</f>
         <v>0</v>
       </c>
-      <c r="F25" s="50">
+      <c r="F25" s="46">
         <f>IF(F23 = 0, 0, F4)</f>
         <v>0.5</v>
       </c>
-      <c r="G25" s="50">
+      <c r="G25" s="46">
         <f>IF(G23 = 0, 0, G4)</f>
         <v>0</v>
       </c>
-      <c r="H25" s="52" t="s">
+      <c r="H25" s="48" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="26" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="48"/>
-      <c r="B26" s="49" t="s">
+      <c r="A26" s="44"/>
+      <c r="B26" s="45" t="s">
         <v>96</v>
       </c>
-      <c r="C26" s="49"/>
-      <c r="D26" s="50">
+      <c r="C26" s="45"/>
+      <c r="D26" s="46">
         <f>IF(SUM(ShortfallIncomeRatioPerson)= 0, 0, D25/SUM(ShortfallIncomeRatioPerson))</f>
         <v>0</v>
       </c>
-      <c r="E26" s="50">
+      <c r="E26" s="46">
         <f>IF(SUM(ShortfallIncomeRatioPerson)= 0, 0, E25/SUM(ShortfallIncomeRatioPerson))</f>
         <v>0</v>
       </c>
-      <c r="F26" s="50">
+      <c r="F26" s="46">
         <f>IF(SUM(ShortfallIncomeRatioPerson)= 0, 0, F25/SUM(ShortfallIncomeRatioPerson))</f>
         <v>1</v>
       </c>
-      <c r="G26" s="50">
+      <c r="G26" s="46">
         <f>IF(SUM(ShortfallIncomeRatioPerson)= 0, 0, G25/SUM(ShortfallIncomeRatioPerson))</f>
         <v>0</v>
       </c>
-      <c r="H26" s="52" t="s">
+      <c r="H26" s="48" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="27" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="48" t="s">
+      <c r="A27" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="B27" s="49" t="s">
+      <c r="B27" s="45" t="s">
         <v>97</v>
       </c>
-      <c r="C27" s="49"/>
-      <c r="D27" s="53">
+      <c r="C27" s="45"/>
+      <c r="D27" s="49">
         <f>ROUND(D19+D24,0)</f>
         <v>466</v>
       </c>
-      <c r="E27" s="53">
+      <c r="E27" s="49">
         <f>ROUND(E19+E24,0)</f>
         <v>327</v>
       </c>
-      <c r="F27" s="53">
+      <c r="F27" s="49">
         <f>ROUND(F19+F24,0)</f>
         <v>72</v>
       </c>
-      <c r="G27" s="51">
+      <c r="G27" s="47">
         <f>ROUND(G19+G24,0)</f>
         <v>0</v>
       </c>
-      <c r="H27" s="52" t="s">
+      <c r="H27" s="48" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="28" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="48" t="s">
+      <c r="A28" s="44" t="s">
         <v>53</v>
       </c>
-      <c r="B28" s="49" t="s">
+      <c r="B28" s="45" t="s">
         <v>98</v>
       </c>
-      <c r="C28" s="49"/>
-      <c r="D28" s="49">
+      <c r="C28" s="45"/>
+      <c r="D28" s="45">
         <f>ROUND(D23-SUM(AdjustmentArb)*D26,0)</f>
         <v>0</v>
       </c>
-      <c r="E28" s="49">
+      <c r="E28" s="45">
         <f>ROUND(E23-SUM(AdjustmentArb)*E26,0)</f>
         <v>0</v>
       </c>
-      <c r="F28" s="49">
+      <c r="F28" s="45">
         <f>ROUND(F23-SUM(AdjustmentArb)*F26,0)</f>
         <v>0</v>
       </c>
-      <c r="G28" s="49">
+      <c r="G28" s="45">
         <f>ROUND(G23-SUM(AdjustmentArb)*G26,0)</f>
         <v>0</v>
       </c>
-      <c r="H28" s="52" t="s">
+      <c r="H28" s="48" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="29" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="48"/>
-      <c r="B29" s="49" t="s">
+      <c r="A29" s="44"/>
+      <c r="B29" s="45" t="s">
         <v>99</v>
       </c>
-      <c r="C29" s="54">
+      <c r="C29" s="50">
         <f>C16-SUM(D27:G28)</f>
         <v>-1</v>
       </c>
-      <c r="D29" s="49"/>
-      <c r="E29" s="49"/>
-      <c r="F29" s="49"/>
-      <c r="G29" s="49"/>
-      <c r="H29" s="52" t="s">
+      <c r="D29" s="45"/>
+      <c r="E29" s="45"/>
+      <c r="F29" s="45"/>
+      <c r="G29" s="45"/>
+      <c r="H29" s="48" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A30" s="42"/>
-      <c r="C30" s="38"/>
+      <c r="A30" s="39"/>
+      <c r="C30" s="36"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B31" s="17" t="s">
+      <c r="B31" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="C31" s="14"/>
-      <c r="D31" s="29">
+      <c r="C31" s="13"/>
+      <c r="D31" s="27">
         <f>ROUND(D10,0)</f>
         <v>485</v>
       </c>
-      <c r="E31" s="29">
+      <c r="E31" s="27">
         <f>ROUND(E10,0)</f>
         <v>369</v>
       </c>
-      <c r="F31" s="29">
+      <c r="F31" s="27">
         <f>ROUND(F10,0)</f>
         <v>286</v>
       </c>
-      <c r="G31" s="29">
+      <c r="G31" s="27">
         <f>ROUND(G10,0)</f>
         <v>0</v>
       </c>
-      <c r="H31" s="16" t="s">
+      <c r="H31" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="I31" s="45" t="s">
+      <c r="I31" s="41" t="s">
         <v>72</v>
       </c>
     </row>
@@ -3312,27 +3335,27 @@
       <c r="A32" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B32" s="17" t="s">
+      <c r="B32" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="C32" s="14"/>
-      <c r="D32" s="29">
+      <c r="C32" s="13"/>
+      <c r="D32" s="27">
         <f>ROUND(D12,0)</f>
         <v>485</v>
       </c>
-      <c r="E32" s="29">
+      <c r="E32" s="27">
         <f>ROUND(E12,0)</f>
         <v>332</v>
       </c>
-      <c r="F32" s="29">
+      <c r="F32" s="27">
         <f>ROUND(F12,0)</f>
         <v>72</v>
       </c>
-      <c r="G32" s="29">
+      <c r="G32" s="27">
         <f>ROUND(G12,0)</f>
         <v>0</v>
       </c>
-      <c r="H32" s="16" t="s">
+      <c r="H32" s="15" t="s">
         <v>70</v>
       </c>
     </row>
@@ -3340,162 +3363,162 @@
       <c r="A33" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B33" s="17" t="s">
+      <c r="B33" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="C33" s="14"/>
-      <c r="D33" s="29">
+      <c r="C33" s="13"/>
+      <c r="D33" s="27">
         <f>D31-D32</f>
         <v>0</v>
       </c>
-      <c r="E33" s="29">
+      <c r="E33" s="27">
         <f>E31-E32</f>
         <v>37</v>
       </c>
-      <c r="F33" s="29">
+      <c r="F33" s="27">
         <f>F31-F32</f>
         <v>214</v>
       </c>
-      <c r="G33" s="29">
+      <c r="G33" s="27">
         <f>G31-G32</f>
         <v>0</v>
       </c>
-      <c r="H33" s="16" t="s">
+      <c r="H33" s="15" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="1"/>
-      <c r="B34" s="55" t="s">
+      <c r="B34" s="51" t="s">
         <v>102</v>
       </c>
-      <c r="C34" s="109" t="str">
+      <c r="C34" s="95" t="str">
         <f>IF(SUM(D32:G33)&lt;=MAKSBELOP,"Everyone paid",IF(SUM(D32:G32)&lt;=MAKSBELOP,"Arbeidsgivere fully paid; Person partially paid by Person request", "Arbeidsgivere partial payment ratio by Arbeidsgiver request"))</f>
         <v>Arbeidsgivere partial payment ratio by Arbeidsgiver request</v>
       </c>
-      <c r="D34" s="109"/>
-      <c r="E34" s="109"/>
-      <c r="F34" s="109"/>
-      <c r="G34" s="109"/>
-      <c r="H34" s="16"/>
+      <c r="D34" s="95"/>
+      <c r="E34" s="95"/>
+      <c r="F34" s="95"/>
+      <c r="G34" s="95"/>
+      <c r="H34" s="15"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B35" s="17" t="s">
+      <c r="B35" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="C35" s="14"/>
-      <c r="D35" s="17">
+      <c r="C35" s="13"/>
+      <c r="D35" s="16">
         <f>IF(SUM($D$32:$G$33)&lt;=MAKSBELOP,D32,IF(SUM($D$32:$G$32)&lt;=MAKSBELOP,D32,ROUND(D32*MAKSBELOP/SUM($D$32:$G$32),0)))</f>
         <v>471</v>
       </c>
-      <c r="E35" s="17">
+      <c r="E35" s="16">
         <f>IF(SUM($D$32:$G$33)&lt;=MAKSBELOP,E32,IF(SUM($D$32:$G$32)&lt;=MAKSBELOP,E32,ROUND(E32*MAKSBELOP/SUM($D$32:$G$32),0)))</f>
         <v>323</v>
       </c>
-      <c r="F35" s="17">
+      <c r="F35" s="16">
         <f>IF(SUM($D$32:$G$33)&lt;=MAKSBELOP,F32,IF(SUM($D$32:$G$32)&lt;=MAKSBELOP,F32,ROUND(F32*MAKSBELOP/SUM($D$32:$G$32),0)))</f>
         <v>70</v>
       </c>
-      <c r="G35" s="17">
+      <c r="G35" s="16">
         <f>IF(SUM($D$32:$G$33)&lt;=MAKSBELOP,G32,IF(SUM($D$32:$G$32)&lt;=MAKSBELOP,G32,ROUND(G32*MAKSBELOP/SUM($D$32:$G$32),0)))</f>
         <v>0</v>
       </c>
-      <c r="H35" s="16" t="s">
+      <c r="H35" s="15" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="36" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="1"/>
-      <c r="B36" s="17" t="s">
+      <c r="B36" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="C36" s="14">
+      <c r="C36" s="13">
         <f>MAKSBELOP-SUM(D35:G35)</f>
         <v>0</v>
       </c>
-      <c r="D36" s="17"/>
-      <c r="E36" s="17"/>
-      <c r="F36" s="17"/>
-      <c r="G36" s="17"/>
-      <c r="H36" s="16"/>
+      <c r="D36" s="16"/>
+      <c r="E36" s="16"/>
+      <c r="F36" s="16"/>
+      <c r="G36" s="16"/>
+      <c r="H36" s="15"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B37" s="17" t="s">
+      <c r="B37" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="C37" s="17"/>
-      <c r="D37" s="17">
+      <c r="C37" s="16"/>
+      <c r="D37" s="16">
         <f>IF(SUM($D$32:$G$33)&lt;=MAKSBELOP,D33,IF(SUM($D$32:$G$32)&lt;=MAKSBELOP,ROUND(PersonRemainder*D33/SUM($D$33:$G$33),0),0))</f>
         <v>0</v>
       </c>
-      <c r="E37" s="17">
+      <c r="E37" s="16">
         <f>IF(SUM($D$32:$G$33)&lt;=MAKSBELOP,E33,IF(SUM($D$32:$G$32)&lt;=MAKSBELOP,ROUND(PersonRemainder*E33/SUM($D$33:$G$33),0),0))</f>
         <v>0</v>
       </c>
-      <c r="F37" s="17">
+      <c r="F37" s="16">
         <f>IF(SUM($D$32:$G$33)&lt;=MAKSBELOP,F33,IF(SUM($D$32:$G$32)&lt;=MAKSBELOP,ROUND(PersonRemainder*F33/SUM($D$33:$G$33),0),0))</f>
         <v>0</v>
       </c>
-      <c r="G37" s="17">
+      <c r="G37" s="16">
         <f>IF(SUM($D$32:$G$33)&lt;=MAKSBELOP,G33,IF(SUM($D$32:$G$32)&lt;=MAKSBELOP,ROUND(PersonRemainder*G33/SUM($D$33:$G$33),0),0))</f>
         <v>0</v>
       </c>
-      <c r="H37" s="16" t="s">
+      <c r="H37" s="15" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="1"/>
-      <c r="B38" s="17" t="s">
+      <c r="B38" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="C38" s="14">
+      <c r="C38" s="13">
         <f>MAKSBELOP-SUM(D35:G37)</f>
         <v>0</v>
       </c>
-      <c r="D38" s="17"/>
-      <c r="E38" s="17"/>
-      <c r="F38" s="17"/>
-      <c r="G38" s="17"/>
-      <c r="H38" s="16" t="s">
+      <c r="D38" s="16"/>
+      <c r="E38" s="16"/>
+      <c r="F38" s="16"/>
+      <c r="G38" s="16"/>
+      <c r="H38" s="15" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A40" s="56" t="s">
+      <c r="A40" s="52" t="s">
         <v>104</v>
       </c>
-      <c r="B40" s="57"/>
-      <c r="C40" s="58"/>
-      <c r="D40" s="59"/>
+      <c r="B40" s="53"/>
+      <c r="C40" s="54"/>
+      <c r="D40" s="55"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A41" s="110" t="s">
+      <c r="A41" s="96" t="s">
         <v>105</v>
       </c>
-      <c r="B41" s="110"/>
-      <c r="C41" s="110"/>
-      <c r="D41" s="110"/>
+      <c r="B41" s="96"/>
+      <c r="C41" s="96"/>
+      <c r="D41" s="96"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A43" s="60" t="s">
+      <c r="A43" s="56" t="s">
         <v>106</v>
       </c>
-      <c r="B43" s="61">
+      <c r="B43" s="57">
         <v>1430.76</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A44" s="60" t="s">
+      <c r="A44" s="56" t="s">
         <v>107</v>
       </c>
-      <c r="B44" s="61">
+      <c r="B44" s="57">
         <f>ROUND(B43*260/12,0)</f>
         <v>31000</v>
       </c>
@@ -3531,707 +3554,707 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="37" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="40" t="s">
+      <c r="C1" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="D1" s="41" t="s">
+      <c r="D1" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="E1" s="41" t="s">
+      <c r="E1" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="F1" s="41" t="s">
+      <c r="F1" s="38" t="s">
         <v>61</v>
       </c>
-      <c r="G1" s="41" t="s">
+      <c r="G1" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="H1" s="41" t="s">
+      <c r="H1" s="38" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="42"/>
-      <c r="H2" s="39"/>
+      <c r="A2" s="39"/>
+      <c r="H2" s="4"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="39" t="s">
         <v>7</v>
       </c>
       <c r="B3" t="s">
         <v>64</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="6">
         <v>21000</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="6">
         <v>10000</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="6">
         <v>31000</v>
       </c>
-      <c r="G3" s="7">
-        <v>0</v>
-      </c>
-      <c r="H3" s="39" t="s">
+      <c r="G3" s="6">
+        <v>0</v>
+      </c>
+      <c r="H3" s="4" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="42"/>
+      <c r="A4" s="39"/>
       <c r="B4" t="s">
         <v>66</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="7">
         <f>D3/SUM($D$3:$G$3)</f>
         <v>0.33870967741935482</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="7">
         <f>E3/SUM($D$3:$G$3)</f>
         <v>0.16129032258064516</v>
       </c>
-      <c r="F4" s="8">
+      <c r="F4" s="7">
         <f>F3/SUM($D$3:$G$3)</f>
         <v>0.5</v>
       </c>
-      <c r="G4" s="8">
+      <c r="G4" s="7">
         <f>G3/SUM($D$3:$G$3)</f>
         <v>0</v>
       </c>
-      <c r="H4" s="39" t="s">
+      <c r="H4" s="4" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="42" t="s">
+      <c r="A5" s="39" t="s">
         <v>11</v>
       </c>
       <c r="B5" t="s">
         <v>67</v>
       </c>
-      <c r="D5" s="43">
+      <c r="D5" s="40">
         <f>D3*12/260</f>
         <v>969.23076923076928</v>
       </c>
-      <c r="E5" s="43">
+      <c r="E5" s="40">
         <f>E3*12/260</f>
         <v>461.53846153846155</v>
       </c>
-      <c r="F5" s="43">
+      <c r="F5" s="40">
         <f>F3*12/260</f>
         <v>1430.7692307692307</v>
       </c>
-      <c r="G5" s="43">
+      <c r="G5" s="40">
         <f>G3*12/260</f>
         <v>0</v>
       </c>
-      <c r="H5" s="39" t="s">
+      <c r="H5" s="4" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="42" t="s">
+      <c r="A6" s="39" t="s">
         <v>13</v>
       </c>
       <c r="B6" t="s">
         <v>69</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="9">
         <v>1</v>
       </c>
-      <c r="E6" s="10">
+      <c r="E6" s="9">
         <v>1</v>
       </c>
-      <c r="F6" s="10">
+      <c r="F6" s="9">
         <v>1</v>
       </c>
-      <c r="G6" s="10">
+      <c r="G6" s="9">
         <v>1</v>
       </c>
-      <c r="H6" s="39" t="s">
+      <c r="H6" s="4" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="42" t="s">
+      <c r="A7" s="39" t="s">
         <v>16</v>
       </c>
       <c r="B7" t="s">
         <v>71</v>
       </c>
-      <c r="D7" s="43">
+      <c r="D7" s="40">
         <f>D5*D6</f>
         <v>969.23076923076928</v>
       </c>
-      <c r="E7" s="43">
+      <c r="E7" s="40">
         <f>E5*E6</f>
         <v>461.53846153846155</v>
       </c>
-      <c r="F7" s="43">
+      <c r="F7" s="40">
         <f>F5*F6</f>
         <v>1430.7692307692307</v>
       </c>
-      <c r="G7" s="43">
+      <c r="G7" s="40">
         <f>G5*G6</f>
         <v>0</v>
       </c>
-      <c r="H7" s="39" t="s">
+      <c r="H7" s="4" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="42" t="s">
+      <c r="A8" s="39" t="s">
         <v>17</v>
       </c>
       <c r="B8" t="s">
         <v>73</v>
       </c>
-      <c r="D8" s="11">
+      <c r="D8" s="10">
         <f>MIN(D7,$C$15)</f>
         <v>969.23076923076928</v>
       </c>
-      <c r="E8" s="11">
+      <c r="E8" s="10">
         <f>MIN(E7,$C$15)</f>
         <v>461.53846153846155</v>
       </c>
-      <c r="F8" s="11">
+      <c r="F8" s="10">
         <f>MIN(F7,$C$15)</f>
         <v>1430.7692307692307</v>
       </c>
-      <c r="G8" s="11">
+      <c r="G8" s="10">
         <f>MIN(G7,$C$15)</f>
         <v>0</v>
       </c>
-      <c r="H8" s="39" t="s">
+      <c r="H8" s="4" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="42" t="s">
+      <c r="A9" s="39" t="s">
         <v>18</v>
       </c>
       <c r="B9" t="s">
         <v>74</v>
       </c>
-      <c r="D9" s="12">
+      <c r="D9" s="11">
         <v>0.5</v>
       </c>
-      <c r="E9" s="12">
+      <c r="E9" s="11">
         <v>0.8</v>
       </c>
-      <c r="F9" s="12">
+      <c r="F9" s="11">
         <v>0.2</v>
       </c>
-      <c r="G9" s="12">
+      <c r="G9" s="11">
         <v>1</v>
       </c>
-      <c r="H9" s="39" t="s">
+      <c r="H9" s="4" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="42" t="s">
+      <c r="A10" s="39" t="s">
         <v>20</v>
       </c>
       <c r="B10" t="s">
         <v>75</v>
       </c>
-      <c r="D10" s="43">
+      <c r="D10" s="40">
         <f>D7*D9</f>
         <v>484.61538461538464</v>
       </c>
-      <c r="E10" s="43">
+      <c r="E10" s="40">
         <f>E7*E9</f>
         <v>369.23076923076928</v>
       </c>
-      <c r="F10" s="43">
+      <c r="F10" s="40">
         <f>F7*F9</f>
         <v>286.15384615384613</v>
       </c>
-      <c r="G10" s="43">
+      <c r="G10" s="40">
         <f>G7*G9</f>
         <v>0</v>
       </c>
-      <c r="H10" s="39" t="s">
+      <c r="H10" s="4" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="42" t="s">
+      <c r="A11" s="39" t="s">
         <v>21</v>
       </c>
       <c r="B11" t="s">
         <v>76</v>
       </c>
-      <c r="D11" s="10">
+      <c r="D11" s="9">
         <v>1</v>
       </c>
-      <c r="E11" s="10">
+      <c r="E11" s="9">
         <v>0.9</v>
       </c>
-      <c r="F11" s="10">
+      <c r="F11" s="9">
         <v>0.25</v>
       </c>
-      <c r="G11" s="10">
+      <c r="G11" s="9">
         <v>1</v>
       </c>
-      <c r="H11" s="39" t="s">
+      <c r="H11" s="4" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="42" t="s">
+      <c r="A12" s="39" t="s">
         <v>22</v>
       </c>
       <c r="B12" t="s">
         <v>77</v>
       </c>
-      <c r="D12" s="46">
+      <c r="D12" s="42">
         <f>D10*D11</f>
         <v>484.61538461538464</v>
       </c>
-      <c r="E12" s="46">
+      <c r="E12" s="42">
         <f>E10*E11</f>
         <v>332.30769230769238</v>
       </c>
-      <c r="F12" s="46">
+      <c r="F12" s="42">
         <f>F10*F11</f>
         <v>71.538461538461533</v>
       </c>
-      <c r="G12" s="46">
+      <c r="G12" s="42">
         <f>G10*G11</f>
         <v>0</v>
       </c>
-      <c r="H12" s="39" t="s">
+      <c r="H12" s="4" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="42" t="s">
+      <c r="A13" s="39" t="s">
         <v>23</v>
       </c>
       <c r="B13" t="s">
         <v>78</v>
       </c>
-      <c r="C13" s="62">
+      <c r="C13" s="58">
         <f>SUM(D10:G10)/SUM(D7:G7)</f>
         <v>0.39838709677419348</v>
       </c>
-      <c r="H13" s="39" t="s">
+      <c r="H13" s="4" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="42" t="s">
+      <c r="A14" s="39" t="s">
         <v>25</v>
       </c>
       <c r="B14" t="s">
         <v>79</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C14" s="6">
         <v>101351</v>
       </c>
-      <c r="H14" s="39" t="s">
+      <c r="H14" s="4" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="42" t="s">
+      <c r="A15" s="39" t="s">
         <v>27</v>
       </c>
       <c r="B15" t="s">
         <v>80</v>
       </c>
-      <c r="C15" s="63">
+      <c r="C15" s="59">
         <f>6*C14/260</f>
         <v>2338.8692307692309</v>
       </c>
-      <c r="H15" s="39" t="s">
+      <c r="H15" s="4" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="42" t="s">
+      <c r="A16" s="39" t="s">
         <v>28</v>
       </c>
       <c r="B16" t="s">
         <v>81</v>
       </c>
-      <c r="C16" s="63">
+      <c r="C16" s="59">
         <f>C13*C15</f>
         <v>931.77532258064502</v>
       </c>
-      <c r="H16" s="39" t="s">
+      <c r="H16" s="4" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="48" t="s">
+      <c r="A17" s="44" t="s">
         <v>82</v>
       </c>
-      <c r="B17" s="49" t="s">
+      <c r="B17" s="45" t="s">
         <v>83</v>
       </c>
-      <c r="C17" s="50">
+      <c r="C17" s="46">
         <f>MIN(1, C16/SUM(D10:G10))</f>
         <v>0.81734677419354829</v>
       </c>
-      <c r="D17" s="51"/>
-      <c r="E17" s="51"/>
-      <c r="F17" s="51"/>
-      <c r="G17" s="51"/>
-      <c r="H17" s="52" t="s">
+      <c r="D17" s="47"/>
+      <c r="E17" s="47"/>
+      <c r="F17" s="47"/>
+      <c r="G17" s="47"/>
+      <c r="H17" s="48" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="48" t="s">
+      <c r="A18" s="44" t="s">
         <v>84</v>
       </c>
-      <c r="B18" s="49" t="s">
+      <c r="B18" s="45" t="s">
         <v>85</v>
       </c>
-      <c r="C18" s="49"/>
-      <c r="D18" s="51">
+      <c r="C18" s="45"/>
+      <c r="D18" s="47">
         <f>D10*ScalingFactor</f>
         <v>367.28744939271257</v>
       </c>
-      <c r="E18" s="51">
+      <c r="E18" s="47">
         <f>E10*ScalingFactor</f>
         <v>279.83805668016197</v>
       </c>
-      <c r="F18" s="51">
+      <c r="F18" s="47">
         <f>F10*ScalingFactor</f>
         <v>216.87449392712549</v>
       </c>
-      <c r="G18" s="51">
+      <c r="G18" s="47">
         <f>G10*ScalingFactor</f>
         <v>0</v>
       </c>
-      <c r="H18" s="52" t="s">
+      <c r="H18" s="48" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="48" t="s">
+      <c r="A19" s="44" t="s">
         <v>86</v>
       </c>
-      <c r="B19" s="49" t="s">
+      <c r="B19" s="45" t="s">
         <v>87</v>
       </c>
-      <c r="C19" s="49"/>
-      <c r="D19" s="51">
+      <c r="C19" s="45"/>
+      <c r="D19" s="47">
         <f>MIN(D18,D12)</f>
         <v>367.28744939271257</v>
       </c>
-      <c r="E19" s="51">
+      <c r="E19" s="47">
         <f>MIN(E18,E12)</f>
         <v>279.83805668016197</v>
       </c>
-      <c r="F19" s="51">
+      <c r="F19" s="47">
         <f>MIN(F18,F12)</f>
         <v>71.538461538461533</v>
       </c>
-      <c r="G19" s="51">
+      <c r="G19" s="47">
         <f>MIN(G18,G12)</f>
         <v>0</v>
       </c>
-      <c r="H19" s="52" t="s">
+      <c r="H19" s="48" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="48"/>
-      <c r="B20" s="49" t="s">
+      <c r="A20" s="44"/>
+      <c r="B20" s="45" t="s">
         <v>88</v>
       </c>
-      <c r="C20" s="49"/>
-      <c r="D20" s="51">
+      <c r="C20" s="45"/>
+      <c r="D20" s="47">
         <f>D19-D12</f>
         <v>-117.32793522267207</v>
       </c>
-      <c r="E20" s="51">
+      <c r="E20" s="47">
         <f>E19-E12</f>
         <v>-52.469635627530408</v>
       </c>
-      <c r="F20" s="51">
+      <c r="F20" s="47">
         <f>F19-F12</f>
         <v>0</v>
       </c>
-      <c r="G20" s="51">
+      <c r="G20" s="47">
         <f>G19-G12</f>
         <v>0</v>
       </c>
-      <c r="H20" s="52" t="s">
+      <c r="H20" s="48" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="48"/>
-      <c r="B21" s="49" t="s">
+      <c r="A21" s="44"/>
+      <c r="B21" s="45" t="s">
         <v>89</v>
       </c>
-      <c r="C21" s="49"/>
-      <c r="D21" s="50">
+      <c r="C21" s="45"/>
+      <c r="D21" s="46">
         <f>IF(D20 &lt; 0, D4, 0)</f>
         <v>0.33870967741935482</v>
       </c>
-      <c r="E21" s="50">
+      <c r="E21" s="46">
         <f>IF(E20 &lt; 0, E4, 0)</f>
         <v>0.16129032258064516</v>
       </c>
-      <c r="F21" s="50">
+      <c r="F21" s="46">
         <f>IF(F20 &lt; 0, F4, 0)</f>
         <v>0</v>
       </c>
-      <c r="G21" s="51"/>
-      <c r="H21" s="52" t="s">
+      <c r="G21" s="47"/>
+      <c r="H21" s="48" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="22" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="48" t="s">
+      <c r="A22" s="44" t="s">
         <v>90</v>
       </c>
-      <c r="B22" s="49" t="s">
+      <c r="B22" s="45" t="s">
         <v>91</v>
       </c>
-      <c r="C22" s="49"/>
-      <c r="D22" s="50">
+      <c r="C22" s="45"/>
+      <c r="D22" s="46">
         <f>IF(SUM(ShortfallIncomeRatioArb)=0,0,D21/SUM(ShortfallIncomeRatioArb))</f>
         <v>0.67741935483870963</v>
       </c>
-      <c r="E22" s="50">
+      <c r="E22" s="46">
         <f>IF(SUM(ShortfallIncomeRatioArb)=0,0,E21/SUM(ShortfallIncomeRatioArb))</f>
         <v>0.32258064516129031</v>
       </c>
-      <c r="F22" s="50">
+      <c r="F22" s="46">
         <f>IF(SUM(ShortfallIncomeRatioArb)=0,0,F21/SUM(ShortfallIncomeRatioArb))</f>
         <v>0</v>
       </c>
-      <c r="G22" s="50">
+      <c r="G22" s="46">
         <f>IF(SUM(ShortfallIncomeRatioArb)=0,0,G21/SUM(ShortfallIncomeRatioArb))</f>
         <v>0</v>
       </c>
-      <c r="H22" s="52" t="s">
+      <c r="H22" s="48" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="48"/>
-      <c r="B23" s="49" t="s">
+      <c r="A23" s="44"/>
+      <c r="B23" s="45" t="s">
         <v>92</v>
       </c>
-      <c r="C23" s="49"/>
-      <c r="D23" s="51">
+      <c r="C23" s="45"/>
+      <c r="D23" s="47">
         <f>D18-D19</f>
         <v>0</v>
       </c>
-      <c r="E23" s="51">
+      <c r="E23" s="47">
         <f>E18-E19</f>
         <v>0</v>
       </c>
-      <c r="F23" s="51">
+      <c r="F23" s="47">
         <f>F18-F19</f>
         <v>145.33603238866397</v>
       </c>
-      <c r="G23" s="51">
+      <c r="G23" s="47">
         <f>G18-G19</f>
         <v>0</v>
       </c>
-      <c r="H23" s="52" t="s">
+      <c r="H23" s="48" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="48" t="s">
+      <c r="A24" s="44" t="s">
         <v>93</v>
       </c>
-      <c r="B24" s="49" t="s">
+      <c r="B24" s="45" t="s">
         <v>94</v>
       </c>
-      <c r="C24" s="49"/>
-      <c r="D24" s="51">
+      <c r="C24" s="45"/>
+      <c r="D24" s="47">
         <f>MIN(-D20,IF(SUM($D$20:$G$20)&gt;=0, 0, SUM($D$23:$G$23)*D22))</f>
         <v>98.453441295546554</v>
       </c>
-      <c r="E24" s="51">
+      <c r="E24" s="47">
         <f>MIN(-E20,IF(SUM($D$20:$G$20)&gt;=0, 0, SUM($D$23:$G$23)*E22))</f>
         <v>46.882591093117405</v>
       </c>
-      <c r="F24" s="51">
+      <c r="F24" s="47">
         <f>MIN(-F20,IF(SUM($D$20:$G$20)&gt;=0, 0, SUM($D$23:$G$23)*F22))</f>
         <v>0</v>
       </c>
-      <c r="G24" s="51">
+      <c r="G24" s="47">
         <f>MIN(-G20,IF(SUM($D$20:$G$20)&gt;=0, 0, SUM($D$23:$G$23)*G22))</f>
         <v>0</v>
       </c>
-      <c r="H24" s="52" t="s">
+      <c r="H24" s="48" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="25" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="48"/>
-      <c r="B25" s="49" t="s">
+      <c r="A25" s="44"/>
+      <c r="B25" s="45" t="s">
         <v>95</v>
       </c>
-      <c r="C25" s="49"/>
-      <c r="D25" s="50">
+      <c r="C25" s="45"/>
+      <c r="D25" s="46">
         <f>IF(D23 = 0, 0, D4)</f>
         <v>0</v>
       </c>
-      <c r="E25" s="50">
+      <c r="E25" s="46">
         <f>IF(E23 = 0, 0, E4)</f>
         <v>0</v>
       </c>
-      <c r="F25" s="50">
+      <c r="F25" s="46">
         <f>IF(F23 = 0, 0, F4)</f>
         <v>0.5</v>
       </c>
-      <c r="G25" s="50">
+      <c r="G25" s="46">
         <f>IF(G23 = 0, 0, G4)</f>
         <v>0</v>
       </c>
-      <c r="H25" s="52" t="s">
+      <c r="H25" s="48" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="26" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="48"/>
-      <c r="B26" s="49" t="s">
+      <c r="A26" s="44"/>
+      <c r="B26" s="45" t="s">
         <v>96</v>
       </c>
-      <c r="C26" s="49"/>
-      <c r="D26" s="50">
+      <c r="C26" s="45"/>
+      <c r="D26" s="46">
         <f>IF(SUM(ShortfallIncomeRatioPerson)= 0, 0, D25/SUM(ShortfallIncomeRatioPerson))</f>
         <v>0</v>
       </c>
-      <c r="E26" s="50">
+      <c r="E26" s="46">
         <f>IF(SUM(ShortfallIncomeRatioPerson)= 0, 0, E25/SUM(ShortfallIncomeRatioPerson))</f>
         <v>0</v>
       </c>
-      <c r="F26" s="50">
+      <c r="F26" s="46">
         <f>IF(SUM(ShortfallIncomeRatioPerson)= 0, 0, F25/SUM(ShortfallIncomeRatioPerson))</f>
         <v>1</v>
       </c>
-      <c r="G26" s="50">
+      <c r="G26" s="46">
         <f>IF(SUM(ShortfallIncomeRatioPerson)= 0, 0, G25/SUM(ShortfallIncomeRatioPerson))</f>
         <v>0</v>
       </c>
-      <c r="H26" s="52" t="s">
+      <c r="H26" s="48" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="48" t="s">
+      <c r="A27" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="B27" s="49" t="s">
+      <c r="B27" s="45" t="s">
         <v>97</v>
       </c>
-      <c r="C27" s="49"/>
-      <c r="D27" s="53">
+      <c r="C27" s="45"/>
+      <c r="D27" s="49">
         <f>ROUND(D19+D24,0)</f>
         <v>466</v>
       </c>
-      <c r="E27" s="53">
+      <c r="E27" s="49">
         <f>ROUND(E19+E24,0)</f>
         <v>327</v>
       </c>
-      <c r="F27" s="53">
+      <c r="F27" s="49">
         <f>ROUND(F19+F24,0)</f>
         <v>72</v>
       </c>
-      <c r="G27" s="51">
+      <c r="G27" s="47">
         <f>ROUND(G19+G24,0)</f>
         <v>0</v>
       </c>
-      <c r="H27" s="52" t="s">
+      <c r="H27" s="48" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="28" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="48" t="s">
+      <c r="A28" s="44" t="s">
         <v>53</v>
       </c>
-      <c r="B28" s="49" t="s">
+      <c r="B28" s="45" t="s">
         <v>98</v>
       </c>
-      <c r="C28" s="49"/>
-      <c r="D28" s="49">
+      <c r="C28" s="45"/>
+      <c r="D28" s="45">
         <f>ROUND(D23-SUM(AdjustmentArb)*D26,0)</f>
         <v>0</v>
       </c>
-      <c r="E28" s="49">
+      <c r="E28" s="45">
         <f>ROUND(E23-SUM(AdjustmentArb)*E26,0)</f>
         <v>0</v>
       </c>
-      <c r="F28" s="49">
+      <c r="F28" s="45">
         <f>ROUND(F23-SUM(AdjustmentArb)*F26,0)</f>
         <v>0</v>
       </c>
-      <c r="G28" s="49">
+      <c r="G28" s="45">
         <f>ROUND(G23-SUM(AdjustmentArb)*G26,0)</f>
         <v>0</v>
       </c>
-      <c r="H28" s="52" t="s">
+      <c r="H28" s="48" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="29" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="48"/>
-      <c r="B29" s="49" t="s">
+      <c r="A29" s="44"/>
+      <c r="B29" s="45" t="s">
         <v>99</v>
       </c>
-      <c r="C29" s="54">
+      <c r="C29" s="50">
         <f>C16-SUM(D27:G28)</f>
         <v>66.775322580645025</v>
       </c>
-      <c r="D29" s="49"/>
-      <c r="E29" s="49"/>
-      <c r="F29" s="49"/>
-      <c r="G29" s="49"/>
-      <c r="H29" s="52" t="s">
+      <c r="D29" s="45"/>
+      <c r="E29" s="45"/>
+      <c r="F29" s="45"/>
+      <c r="G29" s="45"/>
+      <c r="H29" s="48" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A30" s="42"/>
-      <c r="C30" s="38"/>
-      <c r="H30" s="39"/>
+      <c r="A30" s="39"/>
+      <c r="C30" s="36"/>
+      <c r="H30" s="4"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B31" s="17" t="s">
+      <c r="B31" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="C31" s="14"/>
-      <c r="D31" s="64">
+      <c r="C31" s="13"/>
+      <c r="D31" s="60">
         <f>D10</f>
         <v>484.61538461538464</v>
       </c>
-      <c r="E31" s="64">
+      <c r="E31" s="60">
         <f>E10</f>
         <v>369.23076923076928</v>
       </c>
-      <c r="F31" s="64">
+      <c r="F31" s="60">
         <f>F10</f>
         <v>286.15384615384613</v>
       </c>
-      <c r="G31" s="29">
+      <c r="G31" s="27">
         <f>ROUND(G10,0)</f>
         <v>0</v>
       </c>
-      <c r="H31" s="16" t="s">
+      <c r="H31" s="15" t="s">
         <v>70</v>
       </c>
     </row>
@@ -4239,27 +4262,27 @@
       <c r="A32" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B32" s="17" t="s">
+      <c r="B32" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="C32" s="14"/>
-      <c r="D32" s="64">
+      <c r="C32" s="13"/>
+      <c r="D32" s="60">
         <f>D12</f>
         <v>484.61538461538464</v>
       </c>
-      <c r="E32" s="64">
+      <c r="E32" s="60">
         <f>E12</f>
         <v>332.30769230769238</v>
       </c>
-      <c r="F32" s="64">
+      <c r="F32" s="60">
         <f>F12</f>
         <v>71.538461538461533</v>
       </c>
-      <c r="G32" s="29">
+      <c r="G32" s="27">
         <f>ROUND(G12,0)</f>
         <v>0</v>
       </c>
-      <c r="H32" s="16" t="s">
+      <c r="H32" s="15" t="s">
         <v>70</v>
       </c>
     </row>
@@ -4267,130 +4290,130 @@
       <c r="A33" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B33" s="17" t="s">
+      <c r="B33" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="C33" s="14"/>
-      <c r="D33" s="64">
+      <c r="C33" s="13"/>
+      <c r="D33" s="60">
         <f>D31-D32</f>
         <v>0</v>
       </c>
-      <c r="E33" s="64">
+      <c r="E33" s="60">
         <f>E31-E32</f>
         <v>36.923076923076906</v>
       </c>
-      <c r="F33" s="64">
+      <c r="F33" s="60">
         <f>F31-F32</f>
         <v>214.61538461538458</v>
       </c>
-      <c r="G33" s="29">
+      <c r="G33" s="27">
         <f>G31-G32</f>
         <v>0</v>
       </c>
-      <c r="H33" s="16" t="s">
+      <c r="H33" s="15" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="1"/>
-      <c r="B34" s="55" t="s">
+      <c r="B34" s="51" t="s">
         <v>102</v>
       </c>
-      <c r="C34" s="109" t="str">
+      <c r="C34" s="95" t="str">
         <f>IF(SUM(D32:G33)&lt;=MAKSBELOP,"Everyone paid",IF(SUM(D32:G32)&lt;=MAKSBELOP,"Arbeidsgivere fully paid; Person partially paid by Person request", "Arbeidsgivere partial payment ratio by Arbeidsgiver request"))</f>
         <v>Arbeidsgivere partial payment ratio by Arbeidsgiver request</v>
       </c>
-      <c r="D34" s="109"/>
-      <c r="E34" s="109"/>
-      <c r="F34" s="109"/>
-      <c r="G34" s="109"/>
-      <c r="H34" s="16"/>
+      <c r="D34" s="95"/>
+      <c r="E34" s="95"/>
+      <c r="F34" s="95"/>
+      <c r="G34" s="95"/>
+      <c r="H34" s="15"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B35" s="17" t="s">
+      <c r="B35" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="C35" s="14"/>
-      <c r="D35" s="17">
+      <c r="C35" s="13"/>
+      <c r="D35" s="16">
         <f>IF(SUM($D$32:$G$33)&lt;=MAKSBELOP2,ROUND(D32,0),IF(SUM($D$32:$G$32)&lt;=MAKSBELOP2,ROUND(D32,0),ROUND(D32*MAKSBELOP2/SUM($D$32:$G$32),0)))</f>
         <v>485</v>
       </c>
-      <c r="E35" s="17">
+      <c r="E35" s="16">
         <f>IF(SUM($D$32:$G$33)&lt;=MAKSBELOP2,ROUND(E32,0),IF(SUM($D$32:$G$32)&lt;=MAKSBELOP2,ROUND(E32,0),ROUND(E32*MAKSBELOP2/SUM($D$32:$G$32),0)))</f>
         <v>332</v>
       </c>
-      <c r="F35" s="17">
+      <c r="F35" s="16">
         <f>IF(SUM($D$32:$G$33)&lt;=MAKSBELOP2,ROUND(F32,0),IF(SUM($D$32:$G$32)&lt;=MAKSBELOP2,ROUND(F32,0),ROUND(F32*MAKSBELOP2/SUM($D$32:$G$32),0)))</f>
         <v>72</v>
       </c>
-      <c r="G35" s="17">
+      <c r="G35" s="16">
         <f>IF(SUM($D$32:$G$33)&lt;=MAKSBELOP,G32,IF(SUM($D$32:$G$32)&lt;=MAKSBELOP,G32,ROUND(G32*MAKSBELOP/SUM($D$32:$G$32),0)))</f>
         <v>0</v>
       </c>
-      <c r="H35" s="16" t="s">
+      <c r="H35" s="15" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="1"/>
-      <c r="B36" s="17" t="s">
+      <c r="B36" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="C36" s="65">
+      <c r="C36" s="61">
         <f>MAKSBELOP2-SUM(D35:G35)</f>
         <v>42.775322580645025</v>
       </c>
-      <c r="D36" s="17"/>
-      <c r="E36" s="17"/>
-      <c r="F36" s="17"/>
-      <c r="G36" s="17"/>
-      <c r="H36" s="16"/>
+      <c r="D36" s="16"/>
+      <c r="E36" s="16"/>
+      <c r="F36" s="16"/>
+      <c r="G36" s="16"/>
+      <c r="H36" s="15"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B37" s="17" t="s">
+      <c r="B37" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="C37" s="17"/>
-      <c r="D37" s="24">
+      <c r="C37" s="16"/>
+      <c r="D37" s="22">
         <f>IF(SUM($D$32:$G$33)&lt;=MAKSBELOP2,ROUND(D33,0),IF(SUM($D$32:$G$32)&lt;=MAKSBELOP2,ROUND(PersonRemainder2*D33/SUM($D$33:$G$33),0),0))</f>
         <v>0</v>
       </c>
-      <c r="E37" s="24">
+      <c r="E37" s="22">
         <f>IF(SUM($D$32:$G$33)&lt;=MAKSBELOP2,ROUND(E33,0),IF(SUM($D$32:$G$32)&lt;=MAKSBELOP2,ROUND(PersonRemainder2*E33/SUM($D$33:$G$33),0),0))</f>
         <v>6</v>
       </c>
-      <c r="F37" s="24">
+      <c r="F37" s="22">
         <f>IF(SUM($D$32:$G$33)&lt;=MAKSBELOP2,ROUND(F33,0),IF(SUM($D$32:$G$32)&lt;=MAKSBELOP2,ROUND(PersonRemainder2*F33/SUM($D$33:$G$33),0),0))</f>
         <v>36</v>
       </c>
-      <c r="G37" s="17">
+      <c r="G37" s="16">
         <f>IF(SUM($D$32:$G$33)&lt;=MAKSBELOP,G33,IF(SUM($D$32:$G$32)&lt;=MAKSBELOP,ROUND(PersonRemainder*G33/SUM($D$33:$G$33),0),0))</f>
         <v>0</v>
       </c>
-      <c r="H37" s="16" t="s">
+      <c r="H37" s="15" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="1"/>
-      <c r="B38" s="17" t="s">
+      <c r="B38" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="C38" s="65">
+      <c r="C38" s="61">
         <f>MAKSBELOP2-SUM(D35:G37)</f>
         <v>0.77532258064502457</v>
       </c>
-      <c r="D38" s="17"/>
-      <c r="E38" s="17"/>
-      <c r="F38" s="17"/>
-      <c r="G38" s="17"/>
-      <c r="H38" s="16" t="s">
+      <c r="D38" s="16"/>
+      <c r="E38" s="16"/>
+      <c r="F38" s="16"/>
+      <c r="G38" s="16"/>
+      <c r="H38" s="15" t="s">
         <v>70</v>
       </c>
     </row>

</xml_diff>